<commit_message>
RPA datasets push 2023-10-14
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="124">
   <si>
     <t>상장일</t>
   </si>
@@ -69,6 +69,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2023-10-13</t>
+  </si>
+  <si>
     <t>2023-10-05</t>
   </si>
   <si>
@@ -108,150 +111,150 @@
     <t>2023-08-22</t>
   </si>
   <si>
+    <t>에이치엠씨제6호스팩</t>
+  </si>
+  <si>
+    <t>두산로보틱스</t>
+  </si>
+  <si>
+    <t>신한제11호스팩</t>
+  </si>
+  <si>
+    <t>한싹</t>
+  </si>
+  <si>
+    <t>레뷰코퍼레이션</t>
+  </si>
+  <si>
+    <t>아이엠티</t>
+  </si>
+  <si>
+    <t>밀리의서재</t>
+  </si>
+  <si>
+    <t>인스웨이브시스템즈</t>
+  </si>
+  <si>
+    <t>상상인제4호스팩</t>
+  </si>
+  <si>
+    <t>한화플러스제4호스팩</t>
+  </si>
+  <si>
+    <t>대신밸런스제16호스팩</t>
+  </si>
+  <si>
+    <t>유안타제11호스팩</t>
+  </si>
+  <si>
+    <t>한국제12호스팩</t>
+  </si>
+  <si>
+    <t>대신밸런스제15호스팩</t>
+  </si>
+  <si>
+    <t>시큐레터</t>
+  </si>
+  <si>
+    <t>스마트레이더시스템</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>코스피</t>
+  </si>
+  <si>
+    <t>현대차</t>
+  </si>
+  <si>
+    <t>한국</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>키움</t>
+  </si>
+  <si>
+    <t>신영</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>유비에스</t>
+  </si>
+  <si>
+    <t>신한</t>
+  </si>
+  <si>
+    <t>삼성</t>
+  </si>
+  <si>
+    <t>유안타</t>
+  </si>
+  <si>
+    <t>유진</t>
+  </si>
+  <si>
+    <t>상상인</t>
+  </si>
+  <si>
+    <t>한화</t>
+  </si>
+  <si>
+    <t>대신</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>공동대표</t>
+  </si>
+  <si>
+    <t>공동</t>
+  </si>
+  <si>
+    <t>인수</t>
+  </si>
+  <si>
+    <t>2023-09-21</t>
+  </si>
+  <si>
+    <t>2023-09-19</t>
+  </si>
+  <si>
+    <t>2023-09-18</t>
+  </si>
+  <si>
+    <t>2023-08-29</t>
+  </si>
+  <si>
+    <t>2023-08-23</t>
+  </si>
+  <si>
     <t>2023-08-21</t>
   </si>
   <si>
-    <t>두산로보틱스</t>
-  </si>
-  <si>
-    <t>신한제11호스팩</t>
-  </si>
-  <si>
-    <t>한싹</t>
-  </si>
-  <si>
-    <t>레뷰코퍼레이션</t>
-  </si>
-  <si>
-    <t>아이엠티</t>
-  </si>
-  <si>
-    <t>밀리의서재</t>
-  </si>
-  <si>
-    <t>인스웨이브시스템즈</t>
-  </si>
-  <si>
-    <t>상상인제4호스팩</t>
-  </si>
-  <si>
-    <t>한화플러스제4호스팩</t>
-  </si>
-  <si>
-    <t>대신밸런스제16호스팩</t>
-  </si>
-  <si>
-    <t>유안타제11호스팩</t>
-  </si>
-  <si>
-    <t>한국제12호스팩</t>
-  </si>
-  <si>
-    <t>대신밸런스제15호스팩</t>
-  </si>
-  <si>
-    <t>시큐레터</t>
-  </si>
-  <si>
-    <t>스마트레이더시스템</t>
-  </si>
-  <si>
-    <t>넥스틸</t>
-  </si>
-  <si>
-    <t>코스피</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>한국</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>KB</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t>키움</t>
-  </si>
-  <si>
-    <t>신영</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>유비에스</t>
-  </si>
-  <si>
-    <t>신한</t>
-  </si>
-  <si>
-    <t>삼성</t>
-  </si>
-  <si>
-    <t>유안타</t>
-  </si>
-  <si>
-    <t>유진</t>
-  </si>
-  <si>
-    <t>상상인</t>
-  </si>
-  <si>
-    <t>한화</t>
-  </si>
-  <si>
-    <t>대신</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>공동대표</t>
-  </si>
-  <si>
-    <t>공동</t>
-  </si>
-  <si>
-    <t>인수</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>2023-09-21</t>
-  </si>
-  <si>
-    <t>2023-09-19</t>
-  </si>
-  <si>
-    <t>2023-09-18</t>
-  </si>
-  <si>
-    <t>2023-08-29</t>
-  </si>
-  <si>
-    <t>2023-08-23</t>
-  </si>
-  <si>
     <t>2023-08-14</t>
   </si>
   <si>
     <t>2023-08-10</t>
   </si>
   <si>
-    <t>2023-08-09</t>
-  </si>
-  <si>
     <t>2023-09-26</t>
   </si>
   <si>
@@ -324,6 +327,9 @@
     <t>한국, 미래</t>
   </si>
   <si>
+    <t>61.15 : 1</t>
+  </si>
+  <si>
     <t>519.6 : 1</t>
   </si>
   <si>
@@ -367,9 +373,6 @@
   </si>
   <si>
     <t>1366 : 1</t>
-  </si>
-  <si>
-    <t>4.63 : 1</t>
   </si>
   <si>
     <t>인수기관</t>
@@ -812,57 +815,57 @@
         <v>47</v>
       </c>
       <c r="D2">
-        <v>4212</v>
+        <v>80</v>
       </c>
       <c r="E2" t="s">
         <v>49</v>
       </c>
       <c r="F2">
-        <v>1263.6</v>
+        <v>80</v>
       </c>
       <c r="G2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M2">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="N2">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="P2" t="s">
-        <v>78</v>
+        <v>19</v>
       </c>
       <c r="Q2">
-        <v>87871545</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D3">
         <v>4212</v>
@@ -874,22 +877,22 @@
         <v>1263.6</v>
       </c>
       <c r="G3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M3">
         <v>26000</v>
@@ -898,10 +901,10 @@
         <v>30</v>
       </c>
       <c r="O3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="P3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="Q3">
         <v>87871545</v>
@@ -909,13 +912,13 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D4">
         <v>4212</v>
@@ -924,37 +927,37 @@
         <v>51</v>
       </c>
       <c r="F4">
-        <v>421.2</v>
+        <v>1263.6</v>
       </c>
       <c r="G4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M4">
         <v>26000</v>
       </c>
       <c r="N4">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="O4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="P4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="Q4">
         <v>87871545</v>
@@ -962,13 +965,13 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D5">
         <v>4212</v>
@@ -980,22 +983,22 @@
         <v>421.2</v>
       </c>
       <c r="G5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M5">
         <v>26000</v>
@@ -1004,10 +1007,10 @@
         <v>10</v>
       </c>
       <c r="O5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="P5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="Q5">
         <v>87871545</v>
@@ -1015,13 +1018,13 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D6">
         <v>4212</v>
@@ -1033,22 +1036,22 @@
         <v>421.2</v>
       </c>
       <c r="G6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M6">
         <v>26000</v>
@@ -1057,10 +1060,10 @@
         <v>10</v>
       </c>
       <c r="O6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="P6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="Q6">
         <v>87871545</v>
@@ -1068,13 +1071,13 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D7">
         <v>4212</v>
@@ -1083,37 +1086,37 @@
         <v>54</v>
       </c>
       <c r="F7">
-        <v>126.36</v>
+        <v>421.2</v>
       </c>
       <c r="G7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="L7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M7">
         <v>26000</v>
       </c>
       <c r="N7">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="O7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="P7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="Q7">
         <v>87871545</v>
@@ -1121,13 +1124,13 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D8">
         <v>4212</v>
@@ -1139,22 +1142,22 @@
         <v>126.36</v>
       </c>
       <c r="G8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K8" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M8">
         <v>26000</v>
@@ -1163,10 +1166,10 @@
         <v>3</v>
       </c>
       <c r="O8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="P8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="Q8">
         <v>87871545</v>
@@ -1174,13 +1177,13 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D9">
         <v>4212</v>
@@ -1192,22 +1195,22 @@
         <v>126.36</v>
       </c>
       <c r="G9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K9" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M9">
         <v>26000</v>
@@ -1216,10 +1219,10 @@
         <v>3</v>
       </c>
       <c r="O9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="P9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="Q9">
         <v>87871545</v>
@@ -1227,13 +1230,13 @@
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D10">
         <v>4212</v>
@@ -1242,37 +1245,37 @@
         <v>57</v>
       </c>
       <c r="F10">
-        <v>42.12</v>
+        <v>126.36</v>
       </c>
       <c r="G10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K10" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M10">
         <v>26000</v>
       </c>
       <c r="N10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="P10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="Q10">
         <v>87871545</v>
@@ -1289,37 +1292,37 @@
         <v>48</v>
       </c>
       <c r="D11">
-        <v>360</v>
+        <v>4212</v>
       </c>
       <c r="E11" t="s">
         <v>58</v>
       </c>
       <c r="F11">
-        <v>360</v>
+        <v>42.12</v>
       </c>
       <c r="G11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M11">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="N11">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="O11" t="s">
         <v>71</v>
@@ -1328,60 +1331,60 @@
         <v>79</v>
       </c>
       <c r="Q11">
-        <v>13500000</v>
+        <v>87871545</v>
       </c>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
         <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D12">
-        <v>187.5</v>
+        <v>360</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="F12">
-        <v>187.5</v>
+        <v>360</v>
       </c>
       <c r="G12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M12">
-        <v>12500</v>
+        <v>2000</v>
       </c>
       <c r="N12">
         <v>100</v>
       </c>
       <c r="O12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="P12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="Q12">
-        <v>1020000</v>
+        <v>13500000</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1392,49 +1395,49 @@
         <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D13">
-        <v>336</v>
+        <v>187.5</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F13">
-        <v>336</v>
+        <v>187.5</v>
       </c>
       <c r="G13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M13">
-        <v>15000</v>
+        <v>12500</v>
       </c>
       <c r="N13">
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="P13" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="Q13">
-        <v>1619200</v>
+        <v>1020000</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1445,60 +1448,60 @@
         <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D14">
-        <v>221.2</v>
+        <v>336</v>
       </c>
       <c r="E14" t="s">
         <v>60</v>
       </c>
       <c r="F14">
-        <v>154.84</v>
+        <v>336</v>
       </c>
       <c r="G14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M14">
-        <v>14000</v>
+        <v>15000</v>
       </c>
       <c r="N14">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="O14" t="s">
         <v>72</v>
       </c>
       <c r="P14" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="Q14">
-        <v>2370000</v>
+        <v>1619200</v>
       </c>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D15">
         <v>221.2</v>
@@ -1507,37 +1510,37 @@
         <v>61</v>
       </c>
       <c r="F15">
-        <v>66.36</v>
+        <v>154.84</v>
       </c>
       <c r="G15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M15">
         <v>14000</v>
       </c>
       <c r="N15">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="O15" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="P15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Q15">
         <v>2370000</v>
@@ -1551,49 +1554,49 @@
         <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D16">
-        <v>345</v>
+        <v>221.2</v>
       </c>
       <c r="E16" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="F16">
-        <v>345</v>
+        <v>66.36</v>
       </c>
       <c r="G16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K16" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M16">
-        <v>23000</v>
+        <v>14000</v>
       </c>
       <c r="N16">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="O16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="P16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Q16">
-        <v>1125000</v>
+        <v>2370000</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1604,49 +1607,49 @@
         <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D17">
-        <v>264</v>
+        <v>345</v>
       </c>
       <c r="E17" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F17">
-        <v>264</v>
+        <v>345</v>
       </c>
       <c r="G17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M17">
-        <v>24000</v>
+        <v>23000</v>
       </c>
       <c r="N17">
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="P17" t="s">
         <v>71</v>
       </c>
       <c r="Q17">
-        <v>825000</v>
+        <v>1125000</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -1657,49 +1660,49 @@
         <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18">
-        <v>90</v>
+        <v>264</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F18">
-        <v>90</v>
+        <v>264</v>
       </c>
       <c r="G18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M18">
-        <v>2000</v>
+        <v>24000</v>
       </c>
       <c r="N18">
         <v>100</v>
       </c>
       <c r="O18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P18" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="Q18">
-        <v>3375000</v>
+        <v>825000</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1710,34 +1713,34 @@
         <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D19">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E19" t="s">
         <v>63</v>
       </c>
       <c r="F19">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M19">
         <v>2000</v>
@@ -1746,13 +1749,13 @@
         <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="P19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q19">
-        <v>3562500</v>
+        <v>3375000</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -1763,34 +1766,34 @@
         <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D20">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="E20" t="s">
         <v>64</v>
       </c>
       <c r="F20">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="G20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M20">
         <v>2000</v>
@@ -1802,10 +1805,10 @@
         <v>74</v>
       </c>
       <c r="P20" t="s">
-        <v>80</v>
+        <v>27</v>
       </c>
       <c r="Q20">
-        <v>4875000</v>
+        <v>3562500</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1816,34 +1819,34 @@
         <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D21">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="E21" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F21">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="G21" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H21" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I21" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J21" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L21" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M21">
         <v>2000</v>
@@ -1852,13 +1855,13 @@
         <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="P21" t="s">
         <v>81</v>
       </c>
       <c r="Q21">
-        <v>3750000</v>
+        <v>4875000</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1869,34 +1872,34 @@
         <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D22">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E22" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="F22">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="G22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M22">
         <v>2000</v>
@@ -1908,48 +1911,48 @@
         <v>30</v>
       </c>
       <c r="P22" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="Q22">
-        <v>3000000</v>
+        <v>3750000</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D23">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="E23" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="F23">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="G23" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H23" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I23" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J23" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L23" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M23">
         <v>2000</v>
@@ -1958,13 +1961,13 @@
         <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="P23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q23">
-        <v>4875000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -1975,49 +1978,49 @@
         <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D24">
-        <v>160.0662</v>
+        <v>130</v>
       </c>
       <c r="E24" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F24">
-        <v>160.0662</v>
+        <v>130</v>
       </c>
       <c r="G24" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H24" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I24" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J24" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K24" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L24" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M24">
-        <v>12000</v>
+        <v>2000</v>
       </c>
       <c r="N24">
         <v>100</v>
       </c>
       <c r="O24" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="P24" t="s">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="Q24">
-        <v>1000414</v>
+        <v>4875000</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -2028,49 +2031,49 @@
         <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D25">
-        <v>177.6</v>
+        <v>160.0662</v>
       </c>
       <c r="E25" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F25">
-        <v>177.6</v>
+        <v>160.0662</v>
       </c>
       <c r="G25" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H25" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I25" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J25" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L25" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M25">
-        <v>8000</v>
+        <v>12000</v>
       </c>
       <c r="N25">
         <v>100</v>
       </c>
       <c r="O25" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="P25" t="s">
         <v>83</v>
       </c>
       <c r="Q25">
-        <v>1665000</v>
+        <v>1000414</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -2084,46 +2087,46 @@
         <v>47</v>
       </c>
       <c r="D26">
-        <v>805</v>
+        <v>177.6</v>
       </c>
       <c r="E26" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="F26">
-        <v>805</v>
+        <v>177.6</v>
       </c>
       <c r="G26" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H26" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I26" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J26" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L26" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M26">
-        <v>11500</v>
+        <v>8000</v>
       </c>
       <c r="N26">
         <v>100</v>
       </c>
       <c r="O26" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="P26" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="Q26">
-        <v>5239200</v>
+        <v>1665000</v>
       </c>
     </row>
   </sheetData>
@@ -2144,10 +2147,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -2156,111 +2159,111 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
       </c>
       <c r="F2">
-        <v>421200000</v>
+        <v>8000000</v>
       </c>
       <c r="G2">
-        <v>16200000</v>
+        <v>4000000</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I2">
-        <v>21000</v>
+        <v>2000</v>
       </c>
       <c r="J2">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="K2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L2">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="M2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="S2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="T2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -2271,7 +2274,7 @@
         <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="D3" t="s">
         <v>79</v>
@@ -2280,173 +2283,173 @@
         <v>18</v>
       </c>
       <c r="F3">
-        <v>36000000</v>
+        <v>421200000</v>
       </c>
       <c r="G3">
-        <v>18000000</v>
+        <v>16200000</v>
       </c>
       <c r="H3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I3">
-        <v>2000</v>
+        <v>21000</v>
       </c>
       <c r="J3">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="K3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L3">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="M3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="S3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="T3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
         <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4">
-        <v>18750000</v>
+        <v>36000000</v>
       </c>
       <c r="G4">
-        <v>1500000</v>
+        <v>18000000</v>
       </c>
       <c r="H4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I4">
-        <v>8900</v>
+        <v>2000</v>
       </c>
       <c r="J4">
-        <v>11000</v>
+        <v>2000</v>
       </c>
       <c r="K4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L4">
-        <v>12500</v>
+        <v>2000</v>
       </c>
       <c r="M4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="S4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="T4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
         <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
       </c>
       <c r="F5">
-        <v>33600000</v>
+        <v>18750000</v>
       </c>
       <c r="G5">
-        <v>2240000</v>
+        <v>1500000</v>
       </c>
       <c r="H5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I5">
-        <v>11500</v>
+        <v>8900</v>
       </c>
       <c r="J5">
-        <v>13200</v>
+        <v>11000</v>
       </c>
       <c r="K5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L5">
-        <v>15000</v>
+        <v>12500</v>
       </c>
       <c r="M5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O5">
-        <v>26.78571428571428</v>
+        <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="S5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="T5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -2460,128 +2463,128 @@
         <v>60</v>
       </c>
       <c r="D6" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="E6" t="s">
         <v>20</v>
       </c>
       <c r="F6">
-        <v>22120000</v>
+        <v>33600000</v>
       </c>
       <c r="G6">
-        <v>1580000</v>
+        <v>2240000</v>
       </c>
       <c r="H6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I6">
-        <v>10500</v>
+        <v>11500</v>
       </c>
       <c r="J6">
-        <v>12000</v>
+        <v>13200</v>
       </c>
       <c r="K6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L6">
-        <v>14000</v>
+        <v>15000</v>
       </c>
       <c r="M6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O6">
-        <v>0</v>
+        <v>26.78571428571428</v>
       </c>
       <c r="P6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="S6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="T6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
         <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="D7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E7" t="s">
         <v>21</v>
       </c>
       <c r="F7">
-        <v>34500000</v>
+        <v>22120000</v>
       </c>
       <c r="G7">
-        <v>1500000</v>
+        <v>1580000</v>
       </c>
       <c r="H7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I7">
-        <v>20000</v>
+        <v>10500</v>
       </c>
       <c r="J7">
-        <v>23000</v>
+        <v>12000</v>
       </c>
       <c r="K7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L7">
-        <v>23000</v>
+        <v>14000</v>
       </c>
       <c r="M7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="S7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="T7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="B8" t="s">
         <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
         <v>71</v>
@@ -2590,116 +2593,116 @@
         <v>22</v>
       </c>
       <c r="F8">
-        <v>26400000</v>
+        <v>34500000</v>
       </c>
       <c r="G8">
-        <v>1100000</v>
+        <v>1500000</v>
       </c>
       <c r="H8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I8">
         <v>20000</v>
       </c>
       <c r="J8">
-        <v>24000</v>
+        <v>23000</v>
       </c>
       <c r="K8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L8">
-        <v>24000</v>
+        <v>23000</v>
       </c>
       <c r="M8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O8">
-        <v>18.18181818181818</v>
+        <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="S8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="T8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
         <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="E9" t="s">
         <v>23</v>
       </c>
       <c r="F9">
-        <v>9000000</v>
+        <v>26400000</v>
       </c>
       <c r="G9">
-        <v>4500000</v>
+        <v>1100000</v>
       </c>
       <c r="H9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I9">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="J9">
-        <v>2000</v>
+        <v>24000</v>
       </c>
       <c r="K9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L9">
-        <v>2000</v>
+        <v>24000</v>
       </c>
       <c r="M9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O9">
-        <v>0</v>
+        <v>18.18181818181818</v>
       </c>
       <c r="P9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="S9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="T9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
         <v>39</v>
@@ -2708,19 +2711,19 @@
         <v>63</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
         <v>24</v>
       </c>
       <c r="F10">
-        <v>9500000</v>
+        <v>9000000</v>
       </c>
       <c r="G10">
-        <v>4750000</v>
+        <v>4500000</v>
       </c>
       <c r="H10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I10">
         <v>2000</v>
@@ -2729,34 +2732,34 @@
         <v>2000</v>
       </c>
       <c r="K10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L10">
         <v>2000</v>
       </c>
       <c r="M10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="S10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="T10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -2770,19 +2773,19 @@
         <v>64</v>
       </c>
       <c r="D11" t="s">
-        <v>80</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
         <v>25</v>
       </c>
       <c r="F11">
-        <v>13000000</v>
+        <v>9500000</v>
       </c>
       <c r="G11">
-        <v>6500000</v>
+        <v>4750000</v>
       </c>
       <c r="H11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I11">
         <v>2000</v>
@@ -2791,45 +2794,45 @@
         <v>2000</v>
       </c>
       <c r="K11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L11">
         <v>2000</v>
       </c>
       <c r="M11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="S11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="T11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="B12" t="s">
         <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D12" t="s">
         <v>81</v>
@@ -2838,13 +2841,13 @@
         <v>26</v>
       </c>
       <c r="F12">
-        <v>10000000</v>
+        <v>13000000</v>
       </c>
       <c r="G12">
-        <v>5000000</v>
+        <v>6500000</v>
       </c>
       <c r="H12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I12">
         <v>2000</v>
@@ -2853,34 +2856,34 @@
         <v>2000</v>
       </c>
       <c r="K12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L12">
         <v>2000</v>
       </c>
       <c r="M12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="S12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="T12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -2891,22 +2894,22 @@
         <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="E13" t="s">
         <v>27</v>
       </c>
       <c r="F13">
-        <v>8000000</v>
+        <v>10000000</v>
       </c>
       <c r="G13">
-        <v>4000000</v>
+        <v>5000000</v>
       </c>
       <c r="H13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I13">
         <v>2000</v>
@@ -2915,60 +2918,60 @@
         <v>2000</v>
       </c>
       <c r="K13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L13">
         <v>2000</v>
       </c>
       <c r="M13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R13" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="S13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="T13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
         <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" t="s">
         <v>28</v>
       </c>
-      <c r="E14" t="s">
-        <v>27</v>
-      </c>
       <c r="F14">
-        <v>13000000</v>
+        <v>8000000</v>
       </c>
       <c r="G14">
-        <v>6500000</v>
+        <v>4000000</v>
       </c>
       <c r="H14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I14">
         <v>2000</v>
@@ -2977,107 +2980,107 @@
         <v>2000</v>
       </c>
       <c r="K14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L14">
         <v>2000</v>
       </c>
       <c r="M14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R14" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="S14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="T14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
         <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D15" t="s">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
         <v>28</v>
       </c>
       <c r="F15">
-        <v>16006620</v>
+        <v>13000000</v>
       </c>
       <c r="G15">
-        <v>1333885</v>
+        <v>6500000</v>
       </c>
       <c r="H15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I15">
-        <v>9200</v>
+        <v>2000</v>
       </c>
       <c r="J15">
-        <v>10600</v>
+        <v>2000</v>
       </c>
       <c r="K15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L15">
-        <v>12000</v>
+        <v>2000</v>
       </c>
       <c r="M15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R15" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="S15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="T15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
         <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D16" t="s">
         <v>83</v>
@@ -3086,111 +3089,111 @@
         <v>29</v>
       </c>
       <c r="F16">
-        <v>17760000</v>
+        <v>16006620</v>
       </c>
       <c r="G16">
-        <v>2220000</v>
+        <v>1333885</v>
       </c>
       <c r="H16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I16">
-        <v>5800</v>
+        <v>9200</v>
       </c>
       <c r="J16">
-        <v>6800</v>
+        <v>10600</v>
       </c>
       <c r="K16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L16">
-        <v>8000</v>
+        <v>12000</v>
       </c>
       <c r="M16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R16" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="S16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="T16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B17" t="s">
         <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E17" t="s">
         <v>30</v>
       </c>
       <c r="F17">
-        <v>80500000</v>
+        <v>17760000</v>
       </c>
       <c r="G17">
-        <v>7000000</v>
+        <v>2220000</v>
       </c>
       <c r="H17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I17">
-        <v>11500</v>
+        <v>5800</v>
       </c>
       <c r="J17">
-        <v>12500</v>
+        <v>6800</v>
       </c>
       <c r="K17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L17">
-        <v>11500</v>
+        <v>8000</v>
       </c>
       <c r="M17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O17">
-        <v>47.85714285714286</v>
+        <v>0</v>
       </c>
       <c r="P17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="S17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="T17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -3208,16 +3211,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -3229,10 +3232,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -3241,30 +3244,30 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2">
         <v>42120</v>
@@ -3284,25 +3287,25 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H3">
         <v>42120</v>
@@ -3322,25 +3325,25 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H4">
         <v>18750</v>
@@ -3360,25 +3363,25 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H5">
         <v>42120</v>
@@ -3398,34 +3401,34 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" t="s">
         <v>30</v>
       </c>
-      <c r="C6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" t="s">
-        <v>27</v>
-      </c>
       <c r="H6">
-        <v>13000</v>
+        <v>17760</v>
       </c>
       <c r="I6">
-        <v>6500000</v>
+        <v>2220000</v>
       </c>
       <c r="J6">
-        <v>2000</v>
+        <v>8000</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -3436,34 +3439,34 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
         <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F7" t="s">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="G7" t="s">
         <v>28</v>
       </c>
       <c r="H7">
-        <v>16006.62</v>
+        <v>13000</v>
       </c>
       <c r="I7">
-        <v>1333885</v>
+        <v>6500000</v>
       </c>
       <c r="J7">
-        <v>12000</v>
+        <v>2000</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -3474,25 +3477,25 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H8">
         <v>13000</v>
@@ -3512,19 +3515,19 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
         <v>45</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F9" t="s">
         <v>83</v>
@@ -3533,13 +3536,13 @@
         <v>29</v>
       </c>
       <c r="H9">
-        <v>17760</v>
+        <v>16006.62</v>
       </c>
       <c r="I9">
-        <v>2220000</v>
+        <v>1333885</v>
       </c>
       <c r="J9">
-        <v>8000</v>
+        <v>12000</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -3550,25 +3553,25 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E10" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H10">
         <v>126360</v>
@@ -3588,25 +3591,25 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H11">
         <v>34500</v>
@@ -3626,25 +3629,25 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H12">
         <v>33600</v>
@@ -3664,25 +3667,25 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" t="s">
         <v>25</v>
       </c>
-      <c r="C13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" t="s">
-        <v>62</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>24</v>
-      </c>
-      <c r="G13" t="s">
-        <v>23</v>
       </c>
       <c r="H13">
         <v>9000</v>
@@ -3702,25 +3705,25 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E14" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H14">
         <v>12636</v>
@@ -3740,25 +3743,25 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" t="s">
         <v>23</v>
-      </c>
-      <c r="C15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G15" t="s">
-        <v>22</v>
       </c>
       <c r="H15">
         <v>26400</v>
@@ -3778,25 +3781,25 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H16">
         <v>36000</v>
@@ -3816,25 +3819,25 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E17" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F17" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H17">
         <v>4212</v>
@@ -3854,25 +3857,25 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E18" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H18">
         <v>15484</v>
@@ -3892,25 +3895,25 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H19">
         <v>10000</v>
@@ -3930,25 +3933,25 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
         <v>61</v>
       </c>
-      <c r="B20" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" t="s">
-        <v>60</v>
-      </c>
       <c r="E20" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H20">
         <v>6636</v>
@@ -3968,25 +3971,25 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E21" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F21" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G21" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H21">
         <v>12636</v>
@@ -4006,183 +4009,183 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="E22" t="s">
-        <v>56</v>
+        <v>122</v>
       </c>
       <c r="F22" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G22" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="H22">
-        <v>80500</v>
+        <v>12636</v>
       </c>
       <c r="I22">
-        <v>7000000</v>
+        <v>16200000</v>
       </c>
       <c r="J22">
-        <v>11500</v>
+        <v>26000</v>
       </c>
       <c r="K22">
         <v>0</v>
       </c>
       <c r="L22">
-        <v>100</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="D23" t="s">
-        <v>101</v>
+        <v>50</v>
       </c>
       <c r="E23" t="s">
-        <v>121</v>
+        <v>50</v>
       </c>
       <c r="F23" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="G23" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="H23">
-        <v>12636</v>
+        <v>8000</v>
       </c>
       <c r="I23">
-        <v>16200000</v>
+        <v>4000000</v>
       </c>
       <c r="J23">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="K23">
         <v>0</v>
       </c>
       <c r="L23">
-        <v>3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D24" t="s">
-        <v>49</v>
+        <v>102</v>
       </c>
       <c r="E24" t="s">
-        <v>49</v>
+        <v>122</v>
       </c>
       <c r="F24" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="G24" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="H24">
-        <v>8000</v>
+        <v>126360</v>
       </c>
       <c r="I24">
-        <v>4000000</v>
+        <v>16200000</v>
       </c>
       <c r="J24">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="K24">
         <v>0</v>
       </c>
       <c r="L24">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C25" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D25" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="E25" t="s">
-        <v>121</v>
+        <v>64</v>
       </c>
       <c r="F25" t="s">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="G25" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="H25">
-        <v>126360</v>
+        <v>9500</v>
       </c>
       <c r="I25">
-        <v>16200000</v>
+        <v>4750000</v>
       </c>
       <c r="J25">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="K25">
         <v>0</v>
       </c>
       <c r="L25">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D26" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="E26" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="F26" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G26" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="H26">
-        <v>9500</v>
+        <v>8000</v>
       </c>
       <c r="I26">
-        <v>4750000</v>
+        <v>4000000</v>
       </c>
       <c r="J26">
         <v>2000</v>

</xml_diff>

<commit_message>
RPA datasets push 2023-10-16
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="120">
   <si>
     <t>상장일</t>
   </si>
@@ -108,153 +108,147 @@
     <t>2023-08-24</t>
   </si>
   <si>
+    <t>에이치엠씨제6호스팩</t>
+  </si>
+  <si>
+    <t>두산로보틱스</t>
+  </si>
+  <si>
+    <t>신한제11호스팩</t>
+  </si>
+  <si>
+    <t>한싹</t>
+  </si>
+  <si>
+    <t>레뷰코퍼레이션</t>
+  </si>
+  <si>
+    <t>아이엠티</t>
+  </si>
+  <si>
+    <t>밀리의서재</t>
+  </si>
+  <si>
+    <t>인스웨이브시스템즈</t>
+  </si>
+  <si>
+    <t>상상인제4호스팩</t>
+  </si>
+  <si>
+    <t>한화플러스제4호스팩</t>
+  </si>
+  <si>
+    <t>대신밸런스제16호스팩</t>
+  </si>
+  <si>
+    <t>유안타제11호스팩</t>
+  </si>
+  <si>
+    <t>한국제12호스팩</t>
+  </si>
+  <si>
+    <t>대신밸런스제15호스팩</t>
+  </si>
+  <si>
+    <t>시큐레터</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>코스피</t>
+  </si>
+  <si>
+    <t>현대차</t>
+  </si>
+  <si>
+    <t>한국</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>키움</t>
+  </si>
+  <si>
+    <t>신영</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>유비에스</t>
+  </si>
+  <si>
+    <t>신한</t>
+  </si>
+  <si>
+    <t>삼성</t>
+  </si>
+  <si>
+    <t>유안타</t>
+  </si>
+  <si>
+    <t>유진</t>
+  </si>
+  <si>
+    <t>상상인</t>
+  </si>
+  <si>
+    <t>한화</t>
+  </si>
+  <si>
+    <t>대신</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>공동대표</t>
+  </si>
+  <si>
+    <t>공동</t>
+  </si>
+  <si>
+    <t>인수</t>
+  </si>
+  <si>
+    <t>2023-09-21</t>
+  </si>
+  <si>
+    <t>2023-09-19</t>
+  </si>
+  <si>
+    <t>2023-09-18</t>
+  </si>
+  <si>
+    <t>2023-08-29</t>
+  </si>
+  <si>
+    <t>2023-08-23</t>
+  </si>
+  <si>
     <t>2023-08-22</t>
   </si>
   <si>
-    <t>에이치엠씨제6호스팩</t>
-  </si>
-  <si>
-    <t>두산로보틱스</t>
-  </si>
-  <si>
-    <t>신한제11호스팩</t>
-  </si>
-  <si>
-    <t>한싹</t>
-  </si>
-  <si>
-    <t>레뷰코퍼레이션</t>
-  </si>
-  <si>
-    <t>아이엠티</t>
-  </si>
-  <si>
-    <t>밀리의서재</t>
-  </si>
-  <si>
-    <t>인스웨이브시스템즈</t>
-  </si>
-  <si>
-    <t>상상인제4호스팩</t>
-  </si>
-  <si>
-    <t>한화플러스제4호스팩</t>
-  </si>
-  <si>
-    <t>대신밸런스제16호스팩</t>
-  </si>
-  <si>
-    <t>유안타제11호스팩</t>
-  </si>
-  <si>
-    <t>한국제12호스팩</t>
-  </si>
-  <si>
-    <t>대신밸런스제15호스팩</t>
-  </si>
-  <si>
-    <t>시큐레터</t>
-  </si>
-  <si>
-    <t>스마트레이더시스템</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>코스피</t>
-  </si>
-  <si>
-    <t>현대차</t>
-  </si>
-  <si>
-    <t>한국</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>KB</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t>키움</t>
-  </si>
-  <si>
-    <t>신영</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>유비에스</t>
-  </si>
-  <si>
-    <t>신한</t>
-  </si>
-  <si>
-    <t>삼성</t>
-  </si>
-  <si>
-    <t>유안타</t>
-  </si>
-  <si>
-    <t>유진</t>
-  </si>
-  <si>
-    <t>상상인</t>
-  </si>
-  <si>
-    <t>한화</t>
-  </si>
-  <si>
-    <t>대신</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>공동대표</t>
-  </si>
-  <si>
-    <t>공동</t>
-  </si>
-  <si>
-    <t>인수</t>
-  </si>
-  <si>
-    <t>2023-09-21</t>
-  </si>
-  <si>
-    <t>2023-09-19</t>
-  </si>
-  <si>
-    <t>2023-09-18</t>
-  </si>
-  <si>
-    <t>2023-08-29</t>
-  </si>
-  <si>
-    <t>2023-08-23</t>
-  </si>
-  <si>
     <t>2023-08-21</t>
   </si>
   <si>
     <t>2023-08-14</t>
   </si>
   <si>
-    <t>2023-08-10</t>
-  </si>
-  <si>
     <t>2023-09-26</t>
   </si>
   <si>
@@ -270,9 +264,6 @@
     <t>2023-08-18</t>
   </si>
   <si>
-    <t>2023-08-16</t>
-  </si>
-  <si>
     <t>회사명</t>
   </si>
   <si>
@@ -370,9 +361,6 @@
   </si>
   <si>
     <t>1698.41 : 1</t>
-  </si>
-  <si>
-    <t>1366 : 1</t>
   </si>
   <si>
     <t>인수기관</t>
@@ -745,7 +733,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -809,37 +797,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D2">
         <v>80</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F2">
         <v>80</v>
       </c>
       <c r="G2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M2">
         <v>2000</v>
@@ -862,37 +850,37 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D3">
         <v>4212</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F3">
         <v>1263.6</v>
       </c>
       <c r="G3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K3" t="s">
         <v>66</v>
       </c>
-      <c r="H3" t="s">
-        <v>66</v>
-      </c>
-      <c r="I3" t="s">
-        <v>66</v>
-      </c>
-      <c r="J3" t="s">
-        <v>66</v>
-      </c>
-      <c r="K3" t="s">
-        <v>68</v>
-      </c>
       <c r="L3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M3">
         <v>26000</v>
@@ -901,10 +889,10 @@
         <v>30</v>
       </c>
       <c r="O3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q3">
         <v>87871545</v>
@@ -915,37 +903,37 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D4">
         <v>4212</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F4">
         <v>1263.6</v>
       </c>
       <c r="G4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K4" t="s">
         <v>66</v>
       </c>
-      <c r="H4" t="s">
-        <v>66</v>
-      </c>
-      <c r="I4" t="s">
-        <v>66</v>
-      </c>
-      <c r="J4" t="s">
-        <v>66</v>
-      </c>
-      <c r="K4" t="s">
-        <v>68</v>
-      </c>
       <c r="L4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M4">
         <v>26000</v>
@@ -954,10 +942,10 @@
         <v>30</v>
       </c>
       <c r="O4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q4">
         <v>87871545</v>
@@ -968,37 +956,37 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D5">
         <v>4212</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F5">
         <v>421.2</v>
       </c>
       <c r="G5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M5">
         <v>26000</v>
@@ -1007,10 +995,10 @@
         <v>10</v>
       </c>
       <c r="O5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q5">
         <v>87871545</v>
@@ -1021,37 +1009,37 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D6">
         <v>4212</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F6">
         <v>421.2</v>
       </c>
       <c r="G6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M6">
         <v>26000</v>
@@ -1060,10 +1048,10 @@
         <v>10</v>
       </c>
       <c r="O6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q6">
         <v>87871545</v>
@@ -1074,37 +1062,37 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D7">
         <v>4212</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F7">
         <v>421.2</v>
       </c>
       <c r="G7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M7">
         <v>26000</v>
@@ -1113,10 +1101,10 @@
         <v>10</v>
       </c>
       <c r="O7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q7">
         <v>87871545</v>
@@ -1127,37 +1115,37 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D8">
         <v>4212</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F8">
         <v>126.36</v>
       </c>
       <c r="G8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M8">
         <v>26000</v>
@@ -1166,10 +1154,10 @@
         <v>3</v>
       </c>
       <c r="O8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q8">
         <v>87871545</v>
@@ -1180,37 +1168,37 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D9">
         <v>4212</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F9">
         <v>126.36</v>
       </c>
       <c r="G9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M9">
         <v>26000</v>
@@ -1219,10 +1207,10 @@
         <v>3</v>
       </c>
       <c r="O9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q9">
         <v>87871545</v>
@@ -1233,37 +1221,37 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D10">
         <v>4212</v>
       </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F10">
         <v>126.36</v>
       </c>
       <c r="G10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M10">
         <v>26000</v>
@@ -1272,10 +1260,10 @@
         <v>3</v>
       </c>
       <c r="O10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q10">
         <v>87871545</v>
@@ -1286,37 +1274,37 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D11">
         <v>4212</v>
       </c>
       <c r="E11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F11">
         <v>42.12</v>
       </c>
       <c r="G11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M11">
         <v>26000</v>
@@ -1325,10 +1313,10 @@
         <v>1</v>
       </c>
       <c r="O11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q11">
         <v>87871545</v>
@@ -1339,37 +1327,37 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D12">
         <v>360</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F12">
         <v>360</v>
       </c>
       <c r="G12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M12">
         <v>2000</v>
@@ -1378,10 +1366,10 @@
         <v>100</v>
       </c>
       <c r="O12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q12">
         <v>13500000</v>
@@ -1392,37 +1380,37 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D13">
         <v>187.5</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F13">
         <v>187.5</v>
       </c>
       <c r="G13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M13">
         <v>12500</v>
@@ -1431,10 +1419,10 @@
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q13">
         <v>1020000</v>
@@ -1445,37 +1433,37 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D14">
         <v>336</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F14">
         <v>336</v>
       </c>
       <c r="G14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M14">
         <v>15000</v>
@@ -1484,10 +1472,10 @@
         <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q14">
         <v>1619200</v>
@@ -1498,37 +1486,37 @@
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D15">
         <v>221.2</v>
       </c>
       <c r="E15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F15">
         <v>154.84</v>
       </c>
       <c r="G15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M15">
         <v>14000</v>
@@ -1537,10 +1525,10 @@
         <v>70</v>
       </c>
       <c r="O15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="P15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Q15">
         <v>2370000</v>
@@ -1551,37 +1539,37 @@
         <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D16">
         <v>221.2</v>
       </c>
       <c r="E16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F16">
         <v>66.36</v>
       </c>
       <c r="G16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M16">
         <v>14000</v>
@@ -1590,10 +1578,10 @@
         <v>30</v>
       </c>
       <c r="O16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="P16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Q16">
         <v>2370000</v>
@@ -1604,37 +1592,37 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D17">
         <v>345</v>
       </c>
       <c r="E17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F17">
         <v>345</v>
       </c>
       <c r="G17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M17">
         <v>23000</v>
@@ -1643,10 +1631,10 @@
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="P17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Q17">
         <v>1125000</v>
@@ -1657,37 +1645,37 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D18">
         <v>264</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F18">
         <v>264</v>
       </c>
       <c r="G18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M18">
         <v>24000</v>
@@ -1699,7 +1687,7 @@
         <v>24</v>
       </c>
       <c r="P18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Q18">
         <v>825000</v>
@@ -1710,37 +1698,37 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D19">
         <v>90</v>
       </c>
       <c r="E19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F19">
         <v>90</v>
       </c>
       <c r="G19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M19">
         <v>2000</v>
@@ -1763,37 +1751,37 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D20">
         <v>95</v>
       </c>
       <c r="E20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F20">
         <v>95</v>
       </c>
       <c r="G20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M20">
         <v>2000</v>
@@ -1802,7 +1790,7 @@
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="P20" t="s">
         <v>27</v>
@@ -1816,37 +1804,37 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D21">
         <v>130</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F21">
         <v>130</v>
       </c>
       <c r="G21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M21">
         <v>2000</v>
@@ -1855,10 +1843,10 @@
         <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q21">
         <v>4875000</v>
@@ -1869,37 +1857,37 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D22">
         <v>100</v>
       </c>
       <c r="E22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F22">
         <v>100</v>
       </c>
       <c r="G22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M22">
         <v>2000</v>
@@ -1908,10 +1896,10 @@
         <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="P22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q22">
         <v>3750000</v>
@@ -1922,37 +1910,37 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D23">
         <v>80</v>
       </c>
       <c r="E23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F23">
         <v>80</v>
       </c>
       <c r="G23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M23">
         <v>2000</v>
@@ -1961,7 +1949,7 @@
         <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P23" t="s">
         <v>29</v>
@@ -1975,37 +1963,37 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D24">
         <v>130</v>
       </c>
       <c r="E24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F24">
         <v>130</v>
       </c>
       <c r="G24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M24">
         <v>2000</v>
@@ -2014,7 +2002,7 @@
         <v>100</v>
       </c>
       <c r="O24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P24" t="s">
         <v>29</v>
@@ -2028,37 +2016,37 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s">
         <v>45</v>
-      </c>
-      <c r="C25" t="s">
-        <v>47</v>
       </c>
       <c r="D25">
         <v>160.0662</v>
       </c>
       <c r="E25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F25">
         <v>160.0662</v>
       </c>
       <c r="G25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M25">
         <v>12000</v>
@@ -2067,66 +2055,13 @@
         <v>100</v>
       </c>
       <c r="O25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P25" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q25">
         <v>1000414</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17">
-      <c r="A26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26">
-        <v>177.6</v>
-      </c>
-      <c r="E26" t="s">
-        <v>65</v>
-      </c>
-      <c r="F26">
-        <v>177.6</v>
-      </c>
-      <c r="G26" t="s">
-        <v>66</v>
-      </c>
-      <c r="H26" t="s">
-        <v>66</v>
-      </c>
-      <c r="I26" t="s">
-        <v>66</v>
-      </c>
-      <c r="J26" t="s">
-        <v>66</v>
-      </c>
-      <c r="K26" t="s">
-        <v>67</v>
-      </c>
-      <c r="L26" t="s">
-        <v>66</v>
-      </c>
-      <c r="M26">
-        <v>8000</v>
-      </c>
-      <c r="N26">
-        <v>100</v>
-      </c>
-      <c r="O26" t="s">
-        <v>78</v>
-      </c>
-      <c r="P26" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q26">
-        <v>1665000</v>
       </c>
     </row>
   </sheetData>
@@ -2136,7 +2071,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2147,10 +2082,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -2159,49 +2094,49 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -2209,10 +2144,10 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -2227,7 +2162,7 @@
         <v>4000000</v>
       </c>
       <c r="H2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I2">
         <v>2000</v>
@@ -2236,48 +2171,48 @@
         <v>2000</v>
       </c>
       <c r="K2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L2">
         <v>2000</v>
       </c>
       <c r="M2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="R2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="S2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="T2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
@@ -2289,7 +2224,7 @@
         <v>16200000</v>
       </c>
       <c r="H3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I3">
         <v>21000</v>
@@ -2298,48 +2233,48 @@
         <v>26000</v>
       </c>
       <c r="K3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L3">
         <v>26000</v>
       </c>
       <c r="M3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="R3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="S3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="T3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
@@ -2351,7 +2286,7 @@
         <v>18000000</v>
       </c>
       <c r="H4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I4">
         <v>2000</v>
@@ -2360,48 +2295,48 @@
         <v>2000</v>
       </c>
       <c r="K4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L4">
         <v>2000</v>
       </c>
       <c r="M4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="R4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="S4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="T4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
@@ -2413,7 +2348,7 @@
         <v>1500000</v>
       </c>
       <c r="H5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I5">
         <v>8900</v>
@@ -2422,48 +2357,48 @@
         <v>11000</v>
       </c>
       <c r="K5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L5">
         <v>12500</v>
       </c>
       <c r="M5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="R5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="S5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="T5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E6" t="s">
         <v>20</v>
@@ -2475,7 +2410,7 @@
         <v>2240000</v>
       </c>
       <c r="H6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I6">
         <v>11500</v>
@@ -2484,48 +2419,48 @@
         <v>13200</v>
       </c>
       <c r="K6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L6">
         <v>15000</v>
       </c>
       <c r="M6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O6">
         <v>26.78571428571428</v>
       </c>
       <c r="P6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="R6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="S6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="T6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E7" t="s">
         <v>21</v>
@@ -2537,7 +2472,7 @@
         <v>1580000</v>
       </c>
       <c r="H7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I7">
         <v>10500</v>
@@ -2546,48 +2481,48 @@
         <v>12000</v>
       </c>
       <c r="K7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L7">
         <v>14000</v>
       </c>
       <c r="M7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="R7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="S7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="T7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
         <v>22</v>
@@ -2599,7 +2534,7 @@
         <v>1500000</v>
       </c>
       <c r="H8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I8">
         <v>20000</v>
@@ -2608,34 +2543,34 @@
         <v>23000</v>
       </c>
       <c r="K8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L8">
         <v>23000</v>
       </c>
       <c r="M8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="R8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="S8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="T8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -2643,13 +2578,13 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E9" t="s">
         <v>23</v>
@@ -2661,7 +2596,7 @@
         <v>1100000</v>
       </c>
       <c r="H9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I9">
         <v>20000</v>
@@ -2670,34 +2605,34 @@
         <v>24000</v>
       </c>
       <c r="K9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L9">
         <v>24000</v>
       </c>
       <c r="M9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O9">
         <v>18.18181818181818</v>
       </c>
       <c r="P9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="R9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="S9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="T9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -2705,10 +2640,10 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
         <v>25</v>
@@ -2723,7 +2658,7 @@
         <v>4500000</v>
       </c>
       <c r="H10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I10">
         <v>2000</v>
@@ -2732,45 +2667,45 @@
         <v>2000</v>
       </c>
       <c r="K10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L10">
         <v>2000</v>
       </c>
       <c r="M10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="R10" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="S10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="T10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D11" t="s">
         <v>27</v>
@@ -2785,7 +2720,7 @@
         <v>4750000</v>
       </c>
       <c r="H11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I11">
         <v>2000</v>
@@ -2794,48 +2729,48 @@
         <v>2000</v>
       </c>
       <c r="K11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L11">
         <v>2000</v>
       </c>
       <c r="M11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="R11" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="S11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="T11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E12" t="s">
         <v>26</v>
@@ -2847,7 +2782,7 @@
         <v>6500000</v>
       </c>
       <c r="H12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I12">
         <v>2000</v>
@@ -2856,48 +2791,48 @@
         <v>2000</v>
       </c>
       <c r="K12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L12">
         <v>2000</v>
       </c>
       <c r="M12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="R12" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="S12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="T12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E13" t="s">
         <v>27</v>
@@ -2909,7 +2844,7 @@
         <v>5000000</v>
       </c>
       <c r="H13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I13">
         <v>2000</v>
@@ -2918,45 +2853,45 @@
         <v>2000</v>
       </c>
       <c r="K13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L13">
         <v>2000</v>
       </c>
       <c r="M13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="R13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="S13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="T13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D14" t="s">
         <v>29</v>
@@ -2971,7 +2906,7 @@
         <v>4000000</v>
       </c>
       <c r="H14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I14">
         <v>2000</v>
@@ -2980,45 +2915,45 @@
         <v>2000</v>
       </c>
       <c r="K14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L14">
         <v>2000</v>
       </c>
       <c r="M14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="R14" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="S14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="T14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D15" t="s">
         <v>29</v>
@@ -3033,7 +2968,7 @@
         <v>6500000</v>
       </c>
       <c r="H15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I15">
         <v>2000</v>
@@ -3042,48 +2977,48 @@
         <v>2000</v>
       </c>
       <c r="K15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L15">
         <v>2000</v>
       </c>
       <c r="M15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="R15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="S15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="T15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E16" t="s">
         <v>29</v>
@@ -3095,7 +3030,7 @@
         <v>1333885</v>
       </c>
       <c r="H16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I16">
         <v>9200</v>
@@ -3104,96 +3039,34 @@
         <v>10600</v>
       </c>
       <c r="K16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L16">
         <v>12000</v>
       </c>
       <c r="M16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="R16" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="S16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="T16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20">
-      <c r="A17" t="s">
-        <v>78</v>
-      </c>
-      <c r="B17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" t="s">
-        <v>84</v>
-      </c>
-      <c r="E17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17">
-        <v>17760000</v>
-      </c>
-      <c r="G17">
-        <v>2220000</v>
-      </c>
-      <c r="H17" t="s">
-        <v>66</v>
-      </c>
-      <c r="I17">
-        <v>5800</v>
-      </c>
-      <c r="J17">
-        <v>6800</v>
-      </c>
-      <c r="K17" t="s">
-        <v>66</v>
-      </c>
-      <c r="L17">
-        <v>8000</v>
-      </c>
-      <c r="M17" t="s">
-        <v>66</v>
-      </c>
-      <c r="N17" t="s">
-        <v>66</v>
-      </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>66</v>
-      </c>
-      <c r="R17" t="s">
-        <v>118</v>
-      </c>
-      <c r="S17" t="s">
-        <v>66</v>
-      </c>
-      <c r="T17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -3203,7 +3076,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3211,16 +3084,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -3232,10 +3105,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -3244,27 +3117,27 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s">
         <v>18</v>
@@ -3287,98 +3160,98 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s">
-        <v>122</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H3">
-        <v>42120</v>
+        <v>18750</v>
       </c>
       <c r="I3">
-        <v>16200000</v>
+        <v>1500000</v>
       </c>
       <c r="J3">
-        <v>26000</v>
+        <v>12500</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H4">
-        <v>18750</v>
+        <v>42120</v>
       </c>
       <c r="I4">
-        <v>1500000</v>
+        <v>16200000</v>
       </c>
       <c r="J4">
-        <v>12500</v>
+        <v>26000</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G5" t="s">
         <v>18</v>
@@ -3401,34 +3274,34 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H6">
-        <v>17760</v>
+        <v>13000</v>
       </c>
       <c r="I6">
-        <v>2220000</v>
+        <v>6500000</v>
       </c>
       <c r="J6">
-        <v>8000</v>
+        <v>2000</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -3439,19 +3312,19 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F7" t="s">
         <v>29</v>
@@ -3477,34 +3350,34 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F8" t="s">
         <v>81</v>
       </c>
       <c r="G8" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H8">
-        <v>13000</v>
+        <v>16006.62</v>
       </c>
       <c r="I8">
-        <v>6500000</v>
+        <v>1333885</v>
       </c>
       <c r="J8">
-        <v>2000</v>
+        <v>12000</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -3515,34 +3388,34 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E9" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="F9" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="G9" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="H9">
-        <v>16006.62</v>
+        <v>34500</v>
       </c>
       <c r="I9">
-        <v>1333885</v>
+        <v>1500000</v>
       </c>
       <c r="J9">
-        <v>12000</v>
+        <v>23000</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -3553,22 +3426,22 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G10" t="s">
         <v>18</v>
@@ -3591,34 +3464,34 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="F11" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="G11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H11">
-        <v>34500</v>
+        <v>33600</v>
       </c>
       <c r="I11">
-        <v>1500000</v>
+        <v>2240000</v>
       </c>
       <c r="J11">
-        <v>23000</v>
+        <v>15000</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -3629,34 +3502,34 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F12" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="G12" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H12">
-        <v>33600</v>
+        <v>9000</v>
       </c>
       <c r="I12">
-        <v>2240000</v>
+        <v>4500000</v>
       </c>
       <c r="J12">
-        <v>15000</v>
+        <v>2000</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -3667,34 +3540,34 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E13" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F13" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="G13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H13">
-        <v>9000</v>
+        <v>26400</v>
       </c>
       <c r="I13">
-        <v>4500000</v>
+        <v>1100000</v>
       </c>
       <c r="J13">
-        <v>2000</v>
+        <v>24000</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -3705,22 +3578,22 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E14" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G14" t="s">
         <v>18</v>
@@ -3743,34 +3616,34 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F15" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="G15" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H15">
-        <v>26400</v>
+        <v>36000</v>
       </c>
       <c r="I15">
-        <v>1100000</v>
+        <v>18000000</v>
       </c>
       <c r="J15">
-        <v>24000</v>
+        <v>2000</v>
       </c>
       <c r="K15">
         <v>0</v>
@@ -3781,192 +3654,192 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
       <c r="E16" t="s">
-        <v>59</v>
+        <v>118</v>
       </c>
       <c r="F16" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H16">
-        <v>36000</v>
+        <v>4212</v>
       </c>
       <c r="I16">
-        <v>18000000</v>
+        <v>16200000</v>
       </c>
       <c r="J16">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
         <v>71</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D17" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="E17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F17" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G17" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H17">
-        <v>4212</v>
+        <v>15484</v>
       </c>
       <c r="I17">
-        <v>16200000</v>
+        <v>1580000</v>
       </c>
       <c r="J17">
-        <v>26000</v>
+        <v>14000</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
-        <v>1</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E18" t="s">
-        <v>123</v>
+        <v>59</v>
       </c>
       <c r="F18" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="G18" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="H18">
-        <v>15484</v>
+        <v>10000</v>
       </c>
       <c r="I18">
-        <v>1580000</v>
+        <v>5000000</v>
       </c>
       <c r="J18">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18">
-        <v>70</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="C19" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
       <c r="F19" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="G19" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H19">
-        <v>10000</v>
+        <v>6636</v>
       </c>
       <c r="I19">
-        <v>5000000</v>
+        <v>1580000</v>
       </c>
       <c r="J19">
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="K19">
         <v>0</v>
       </c>
       <c r="L19">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="E20" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F20" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="G20" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H20">
-        <v>6636</v>
+        <v>12636</v>
       </c>
       <c r="I20">
-        <v>1580000</v>
+        <v>16200000</v>
       </c>
       <c r="J20">
-        <v>14000</v>
+        <v>26000</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
       <c r="L20">
-        <v>30</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -3974,19 +3847,19 @@
         <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E21" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G21" t="s">
         <v>18</v>
@@ -4009,28 +3882,28 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D22" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E22" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G22" t="s">
         <v>18</v>
       </c>
       <c r="H22">
-        <v>12636</v>
+        <v>126360</v>
       </c>
       <c r="I22">
         <v>16200000</v>
@@ -4042,24 +3915,24 @@
         <v>0</v>
       </c>
       <c r="L22">
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F23" t="s">
         <v>29</v>
@@ -4085,69 +3958,69 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D24" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="E24" t="s">
-        <v>122</v>
+        <v>62</v>
       </c>
       <c r="F24" t="s">
-        <v>79</v>
+        <v>27</v>
       </c>
       <c r="G24" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="H24">
-        <v>126360</v>
+        <v>9500</v>
       </c>
       <c r="I24">
-        <v>16200000</v>
+        <v>4750000</v>
       </c>
       <c r="J24">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="K24">
         <v>0</v>
       </c>
       <c r="L24">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="E25" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="F25" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="G25" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="H25">
-        <v>9500</v>
+        <v>8000</v>
       </c>
       <c r="I25">
-        <v>4750000</v>
+        <v>4000000</v>
       </c>
       <c r="J25">
         <v>2000</v>
@@ -4156,44 +4029,6 @@
         <v>0</v>
       </c>
       <c r="L25">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" t="s">
-        <v>49</v>
-      </c>
-      <c r="F26" t="s">
-        <v>19</v>
-      </c>
-      <c r="G26" t="s">
-        <v>17</v>
-      </c>
-      <c r="H26">
-        <v>8000</v>
-      </c>
-      <c r="I26">
-        <v>4000000</v>
-      </c>
-      <c r="J26">
-        <v>2000</v>
-      </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-      <c r="L26">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2023-10-18
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="116">
   <si>
     <t>상장일</t>
   </si>
@@ -105,165 +105,156 @@
     <t>2023-08-30</t>
   </si>
   <si>
+    <t>에이치엠씨제6호스팩</t>
+  </si>
+  <si>
+    <t>두산로보틱스</t>
+  </si>
+  <si>
+    <t>신한제11호스팩</t>
+  </si>
+  <si>
+    <t>한싹</t>
+  </si>
+  <si>
+    <t>레뷰코퍼레이션</t>
+  </si>
+  <si>
+    <t>아이엠티</t>
+  </si>
+  <si>
+    <t>밀리의서재</t>
+  </si>
+  <si>
+    <t>인스웨이브시스템즈</t>
+  </si>
+  <si>
+    <t>상상인제4호스팩</t>
+  </si>
+  <si>
+    <t>한화플러스제4호스팩</t>
+  </si>
+  <si>
+    <t>대신밸런스제16호스팩</t>
+  </si>
+  <si>
+    <t>유안타제11호스팩</t>
+  </si>
+  <si>
+    <t>한국제12호스팩</t>
+  </si>
+  <si>
+    <t>대신밸런스제15호스팩</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>코스피</t>
+  </si>
+  <si>
+    <t>현대차</t>
+  </si>
+  <si>
+    <t>한국</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>키움</t>
+  </si>
+  <si>
+    <t>신영</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>유비에스</t>
+  </si>
+  <si>
+    <t>신한</t>
+  </si>
+  <si>
+    <t>삼성</t>
+  </si>
+  <si>
+    <t>유안타</t>
+  </si>
+  <si>
+    <t>유진</t>
+  </si>
+  <si>
+    <t>상상인</t>
+  </si>
+  <si>
+    <t>한화</t>
+  </si>
+  <si>
+    <t>대신</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>공동대표</t>
+  </si>
+  <si>
+    <t>공동</t>
+  </si>
+  <si>
+    <t>인수</t>
+  </si>
+  <si>
+    <t>2023-09-21</t>
+  </si>
+  <si>
+    <t>2023-09-19</t>
+  </si>
+  <si>
+    <t>2023-09-18</t>
+  </si>
+  <si>
+    <t>2023-08-29</t>
+  </si>
+  <si>
+    <t>2023-08-23</t>
+  </si>
+  <si>
+    <t>2023-08-22</t>
+  </si>
+  <si>
+    <t>2023-08-21</t>
+  </si>
+  <si>
+    <t>2023-09-26</t>
+  </si>
+  <si>
+    <t>2023-09-22</t>
+  </si>
+  <si>
+    <t>2023-08-28</t>
+  </si>
+  <si>
+    <t>2023-08-25</t>
+  </si>
+  <si>
     <t>2023-08-24</t>
   </si>
   <si>
-    <t>에이치엠씨제6호스팩</t>
-  </si>
-  <si>
-    <t>두산로보틱스</t>
-  </si>
-  <si>
-    <t>신한제11호스팩</t>
-  </si>
-  <si>
-    <t>한싹</t>
-  </si>
-  <si>
-    <t>레뷰코퍼레이션</t>
-  </si>
-  <si>
-    <t>아이엠티</t>
-  </si>
-  <si>
-    <t>밀리의서재</t>
-  </si>
-  <si>
-    <t>인스웨이브시스템즈</t>
-  </si>
-  <si>
-    <t>상상인제4호스팩</t>
-  </si>
-  <si>
-    <t>한화플러스제4호스팩</t>
-  </si>
-  <si>
-    <t>대신밸런스제16호스팩</t>
-  </si>
-  <si>
-    <t>유안타제11호스팩</t>
-  </si>
-  <si>
-    <t>한국제12호스팩</t>
-  </si>
-  <si>
-    <t>대신밸런스제15호스팩</t>
-  </si>
-  <si>
-    <t>시큐레터</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>코스피</t>
-  </si>
-  <si>
-    <t>현대차</t>
-  </si>
-  <si>
-    <t>한국</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>KB</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t>키움</t>
-  </si>
-  <si>
-    <t>신영</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>유비에스</t>
-  </si>
-  <si>
-    <t>신한</t>
-  </si>
-  <si>
-    <t>삼성</t>
-  </si>
-  <si>
-    <t>유안타</t>
-  </si>
-  <si>
-    <t>유진</t>
-  </si>
-  <si>
-    <t>상상인</t>
-  </si>
-  <si>
-    <t>한화</t>
-  </si>
-  <si>
-    <t>대신</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>공동대표</t>
-  </si>
-  <si>
-    <t>공동</t>
-  </si>
-  <si>
-    <t>인수</t>
-  </si>
-  <si>
-    <t>2023-09-21</t>
-  </si>
-  <si>
-    <t>2023-09-19</t>
-  </si>
-  <si>
-    <t>2023-09-18</t>
-  </si>
-  <si>
-    <t>2023-08-29</t>
-  </si>
-  <si>
-    <t>2023-08-23</t>
-  </si>
-  <si>
-    <t>2023-08-22</t>
-  </si>
-  <si>
-    <t>2023-08-21</t>
-  </si>
-  <si>
-    <t>2023-08-14</t>
-  </si>
-  <si>
-    <t>2023-09-26</t>
-  </si>
-  <si>
-    <t>2023-09-22</t>
-  </si>
-  <si>
-    <t>2023-08-28</t>
-  </si>
-  <si>
-    <t>2023-08-25</t>
-  </si>
-  <si>
-    <t>2023-08-18</t>
-  </si>
-  <si>
     <t>회사명</t>
   </si>
   <si>
@@ -358,9 +349,6 @@
   </si>
   <si>
     <t>548.99 : 1</t>
-  </si>
-  <si>
-    <t>1698.41 : 1</t>
   </si>
   <si>
     <t>인수기관</t>
@@ -733,7 +721,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -797,37 +785,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D2">
         <v>80</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F2">
         <v>80</v>
       </c>
       <c r="G2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M2">
         <v>2000</v>
@@ -850,37 +838,37 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3">
         <v>4212</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F3">
         <v>1263.6</v>
       </c>
       <c r="G3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K3" t="s">
         <v>64</v>
       </c>
-      <c r="H3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I3" t="s">
-        <v>64</v>
-      </c>
-      <c r="J3" t="s">
-        <v>64</v>
-      </c>
-      <c r="K3" t="s">
-        <v>66</v>
-      </c>
       <c r="L3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M3">
         <v>26000</v>
@@ -889,10 +877,10 @@
         <v>30</v>
       </c>
       <c r="O3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Q3">
         <v>87871545</v>
@@ -903,37 +891,37 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D4">
         <v>4212</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F4">
         <v>1263.6</v>
       </c>
       <c r="G4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K4" t="s">
         <v>64</v>
       </c>
-      <c r="H4" t="s">
-        <v>64</v>
-      </c>
-      <c r="I4" t="s">
-        <v>64</v>
-      </c>
-      <c r="J4" t="s">
-        <v>64</v>
-      </c>
-      <c r="K4" t="s">
-        <v>66</v>
-      </c>
       <c r="L4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M4">
         <v>26000</v>
@@ -942,10 +930,10 @@
         <v>30</v>
       </c>
       <c r="O4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Q4">
         <v>87871545</v>
@@ -956,37 +944,37 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5">
         <v>4212</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F5">
         <v>421.2</v>
       </c>
       <c r="G5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M5">
         <v>26000</v>
@@ -995,10 +983,10 @@
         <v>10</v>
       </c>
       <c r="O5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Q5">
         <v>87871545</v>
@@ -1009,37 +997,37 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D6">
         <v>4212</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F6">
         <v>421.2</v>
       </c>
       <c r="G6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M6">
         <v>26000</v>
@@ -1048,10 +1036,10 @@
         <v>10</v>
       </c>
       <c r="O6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Q6">
         <v>87871545</v>
@@ -1062,37 +1050,37 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7">
         <v>4212</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F7">
         <v>421.2</v>
       </c>
       <c r="G7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M7">
         <v>26000</v>
@@ -1101,10 +1089,10 @@
         <v>10</v>
       </c>
       <c r="O7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Q7">
         <v>87871545</v>
@@ -1115,37 +1103,37 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D8">
         <v>4212</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F8">
         <v>126.36</v>
       </c>
       <c r="G8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M8">
         <v>26000</v>
@@ -1154,10 +1142,10 @@
         <v>3</v>
       </c>
       <c r="O8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Q8">
         <v>87871545</v>
@@ -1168,37 +1156,37 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D9">
         <v>4212</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F9">
         <v>126.36</v>
       </c>
       <c r="G9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M9">
         <v>26000</v>
@@ -1207,10 +1195,10 @@
         <v>3</v>
       </c>
       <c r="O9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Q9">
         <v>87871545</v>
@@ -1221,37 +1209,37 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D10">
         <v>4212</v>
       </c>
       <c r="E10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F10">
         <v>126.36</v>
       </c>
       <c r="G10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M10">
         <v>26000</v>
@@ -1260,10 +1248,10 @@
         <v>3</v>
       </c>
       <c r="O10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P10" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Q10">
         <v>87871545</v>
@@ -1274,37 +1262,37 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D11">
         <v>4212</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F11">
         <v>42.12</v>
       </c>
       <c r="G11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M11">
         <v>26000</v>
@@ -1313,10 +1301,10 @@
         <v>1</v>
       </c>
       <c r="O11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Q11">
         <v>87871545</v>
@@ -1327,37 +1315,37 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D12">
         <v>360</v>
       </c>
       <c r="E12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F12">
         <v>360</v>
       </c>
       <c r="G12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M12">
         <v>2000</v>
@@ -1366,10 +1354,10 @@
         <v>100</v>
       </c>
       <c r="O12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="Q12">
         <v>13500000</v>
@@ -1380,37 +1368,37 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D13">
         <v>187.5</v>
       </c>
       <c r="E13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F13">
         <v>187.5</v>
       </c>
       <c r="G13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M13">
         <v>12500</v>
@@ -1419,10 +1407,10 @@
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="Q13">
         <v>1020000</v>
@@ -1433,37 +1421,37 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D14">
         <v>336</v>
       </c>
       <c r="E14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F14">
         <v>336</v>
       </c>
       <c r="G14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M14">
         <v>15000</v>
@@ -1472,10 +1460,10 @@
         <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="Q14">
         <v>1619200</v>
@@ -1486,37 +1474,37 @@
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D15">
         <v>221.2</v>
       </c>
       <c r="E15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F15">
         <v>154.84</v>
       </c>
       <c r="G15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M15">
         <v>14000</v>
@@ -1525,10 +1513,10 @@
         <v>70</v>
       </c>
       <c r="O15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q15">
         <v>2370000</v>
@@ -1539,37 +1527,37 @@
         <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D16">
         <v>221.2</v>
       </c>
       <c r="E16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F16">
         <v>66.36</v>
       </c>
       <c r="G16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M16">
         <v>14000</v>
@@ -1578,10 +1566,10 @@
         <v>30</v>
       </c>
       <c r="O16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q16">
         <v>2370000</v>
@@ -1592,37 +1580,37 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D17">
         <v>345</v>
       </c>
       <c r="E17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F17">
         <v>345</v>
       </c>
       <c r="G17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M17">
         <v>23000</v>
@@ -1631,10 +1619,10 @@
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q17">
         <v>1125000</v>
@@ -1645,37 +1633,37 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D18">
         <v>264</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F18">
         <v>264</v>
       </c>
       <c r="G18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M18">
         <v>24000</v>
@@ -1687,7 +1675,7 @@
         <v>24</v>
       </c>
       <c r="P18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Q18">
         <v>825000</v>
@@ -1698,37 +1686,37 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D19">
         <v>90</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F19">
         <v>90</v>
       </c>
       <c r="G19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M19">
         <v>2000</v>
@@ -1751,37 +1739,37 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D20">
         <v>95</v>
       </c>
       <c r="E20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F20">
         <v>95</v>
       </c>
       <c r="G20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M20">
         <v>2000</v>
@@ -1790,7 +1778,7 @@
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P20" t="s">
         <v>27</v>
@@ -1804,37 +1792,37 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D21">
         <v>130</v>
       </c>
       <c r="E21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F21">
         <v>130</v>
       </c>
       <c r="G21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M21">
         <v>2000</v>
@@ -1843,10 +1831,10 @@
         <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="P21" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="Q21">
         <v>4875000</v>
@@ -1857,37 +1845,37 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D22">
         <v>100</v>
       </c>
       <c r="E22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F22">
         <v>100</v>
       </c>
       <c r="G22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M22">
         <v>2000</v>
@@ -1896,10 +1884,10 @@
         <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="P22" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="Q22">
         <v>3750000</v>
@@ -1910,37 +1898,37 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D23">
         <v>80</v>
       </c>
       <c r="E23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F23">
         <v>80</v>
       </c>
       <c r="G23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M23">
         <v>2000</v>
@@ -1949,10 +1937,10 @@
         <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P23" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="Q23">
         <v>3000000</v>
@@ -1963,37 +1951,37 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" t="s">
         <v>43</v>
-      </c>
-      <c r="C24" t="s">
-        <v>45</v>
       </c>
       <c r="D24">
         <v>130</v>
       </c>
       <c r="E24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F24">
         <v>130</v>
       </c>
       <c r="G24" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H24" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I24" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J24" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L24" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M24">
         <v>2000</v>
@@ -2002,66 +1990,13 @@
         <v>100</v>
       </c>
       <c r="O24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P24" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="Q24">
         <v>4875000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17">
-      <c r="A25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" t="s">
-        <v>45</v>
-      </c>
-      <c r="D25">
-        <v>160.0662</v>
-      </c>
-      <c r="E25" t="s">
-        <v>63</v>
-      </c>
-      <c r="F25">
-        <v>160.0662</v>
-      </c>
-      <c r="G25" t="s">
-        <v>64</v>
-      </c>
-      <c r="H25" t="s">
-        <v>64</v>
-      </c>
-      <c r="I25" t="s">
-        <v>64</v>
-      </c>
-      <c r="J25" t="s">
-        <v>64</v>
-      </c>
-      <c r="K25" t="s">
-        <v>65</v>
-      </c>
-      <c r="L25" t="s">
-        <v>64</v>
-      </c>
-      <c r="M25">
-        <v>12000</v>
-      </c>
-      <c r="N25">
-        <v>100</v>
-      </c>
-      <c r="O25" t="s">
-        <v>76</v>
-      </c>
-      <c r="P25" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q25">
-        <v>1000414</v>
       </c>
     </row>
   </sheetData>
@@ -2071,7 +2006,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2082,10 +2017,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -2094,49 +2029,49 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -2144,10 +2079,10 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -2162,7 +2097,7 @@
         <v>4000000</v>
       </c>
       <c r="H2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I2">
         <v>2000</v>
@@ -2171,48 +2106,48 @@
         <v>2000</v>
       </c>
       <c r="K2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L2">
         <v>2000</v>
       </c>
       <c r="M2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="R2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="S2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="T2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
@@ -2224,7 +2159,7 @@
         <v>16200000</v>
       </c>
       <c r="H3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I3">
         <v>21000</v>
@@ -2233,48 +2168,48 @@
         <v>26000</v>
       </c>
       <c r="K3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L3">
         <v>26000</v>
       </c>
       <c r="M3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="R3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="S3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="T3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
@@ -2286,7 +2221,7 @@
         <v>18000000</v>
       </c>
       <c r="H4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I4">
         <v>2000</v>
@@ -2295,48 +2230,48 @@
         <v>2000</v>
       </c>
       <c r="K4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L4">
         <v>2000</v>
       </c>
       <c r="M4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="R4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="S4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="T4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
@@ -2348,7 +2283,7 @@
         <v>1500000</v>
       </c>
       <c r="H5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I5">
         <v>8900</v>
@@ -2357,48 +2292,48 @@
         <v>11000</v>
       </c>
       <c r="K5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L5">
         <v>12500</v>
       </c>
       <c r="M5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="R5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="S5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="T5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E6" t="s">
         <v>20</v>
@@ -2410,7 +2345,7 @@
         <v>2240000</v>
       </c>
       <c r="H6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I6">
         <v>11500</v>
@@ -2419,48 +2354,48 @@
         <v>13200</v>
       </c>
       <c r="K6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L6">
         <v>15000</v>
       </c>
       <c r="M6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O6">
         <v>26.78571428571428</v>
       </c>
       <c r="P6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="R6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="S6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="T6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
         <v>21</v>
@@ -2472,7 +2407,7 @@
         <v>1580000</v>
       </c>
       <c r="H7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I7">
         <v>10500</v>
@@ -2481,48 +2416,48 @@
         <v>12000</v>
       </c>
       <c r="K7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L7">
         <v>14000</v>
       </c>
       <c r="M7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="R7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="S7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="T7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E8" t="s">
         <v>22</v>
@@ -2534,7 +2469,7 @@
         <v>1500000</v>
       </c>
       <c r="H8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I8">
         <v>20000</v>
@@ -2543,34 +2478,34 @@
         <v>23000</v>
       </c>
       <c r="K8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L8">
         <v>23000</v>
       </c>
       <c r="M8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="R8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="S8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="T8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -2578,13 +2513,13 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E9" t="s">
         <v>23</v>
@@ -2596,7 +2531,7 @@
         <v>1100000</v>
       </c>
       <c r="H9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I9">
         <v>20000</v>
@@ -2605,34 +2540,34 @@
         <v>24000</v>
       </c>
       <c r="K9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L9">
         <v>24000</v>
       </c>
       <c r="M9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O9">
         <v>18.18181818181818</v>
       </c>
       <c r="P9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="R9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="S9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="T9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -2640,10 +2575,10 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
         <v>25</v>
@@ -2658,7 +2593,7 @@
         <v>4500000</v>
       </c>
       <c r="H10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I10">
         <v>2000</v>
@@ -2667,45 +2602,45 @@
         <v>2000</v>
       </c>
       <c r="K10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L10">
         <v>2000</v>
       </c>
       <c r="M10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="R10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="S10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="T10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D11" t="s">
         <v>27</v>
@@ -2720,7 +2655,7 @@
         <v>4750000</v>
       </c>
       <c r="H11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I11">
         <v>2000</v>
@@ -2729,48 +2664,48 @@
         <v>2000</v>
       </c>
       <c r="K11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L11">
         <v>2000</v>
       </c>
       <c r="M11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="R11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="S11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="T11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E12" t="s">
         <v>26</v>
@@ -2782,7 +2717,7 @@
         <v>6500000</v>
       </c>
       <c r="H12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I12">
         <v>2000</v>
@@ -2791,48 +2726,48 @@
         <v>2000</v>
       </c>
       <c r="K12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L12">
         <v>2000</v>
       </c>
       <c r="M12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="R12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="S12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="T12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E13" t="s">
         <v>27</v>
@@ -2844,7 +2779,7 @@
         <v>5000000</v>
       </c>
       <c r="H13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I13">
         <v>2000</v>
@@ -2853,48 +2788,48 @@
         <v>2000</v>
       </c>
       <c r="K13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L13">
         <v>2000</v>
       </c>
       <c r="M13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="R13" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="S13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="T13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="E14" t="s">
         <v>28</v>
@@ -2906,7 +2841,7 @@
         <v>4000000</v>
       </c>
       <c r="H14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I14">
         <v>2000</v>
@@ -2915,48 +2850,48 @@
         <v>2000</v>
       </c>
       <c r="K14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L14">
         <v>2000</v>
       </c>
       <c r="M14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="R14" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="S14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="T14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D15" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="E15" t="s">
         <v>28</v>
@@ -2968,7 +2903,7 @@
         <v>6500000</v>
       </c>
       <c r="H15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I15">
         <v>2000</v>
@@ -2977,96 +2912,34 @@
         <v>2000</v>
       </c>
       <c r="K15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L15">
         <v>2000</v>
       </c>
       <c r="M15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="R15" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="S15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="T15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20">
-      <c r="A16" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" t="s">
-        <v>81</v>
-      </c>
-      <c r="E16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16">
-        <v>16006620</v>
-      </c>
-      <c r="G16">
-        <v>1333885</v>
-      </c>
-      <c r="H16" t="s">
-        <v>64</v>
-      </c>
-      <c r="I16">
-        <v>9200</v>
-      </c>
-      <c r="J16">
-        <v>10600</v>
-      </c>
-      <c r="K16" t="s">
-        <v>64</v>
-      </c>
-      <c r="L16">
-        <v>12000</v>
-      </c>
-      <c r="M16" t="s">
-        <v>64</v>
-      </c>
-      <c r="N16" t="s">
-        <v>64</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>64</v>
-      </c>
-      <c r="R16" t="s">
-        <v>114</v>
-      </c>
-      <c r="S16" t="s">
-        <v>64</v>
-      </c>
-      <c r="T16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -3076,7 +2949,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3084,16 +2957,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -3105,10 +2978,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -3117,27 +2990,27 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G2" t="s">
         <v>18</v>
@@ -3160,22 +3033,22 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G3" t="s">
         <v>19</v>
@@ -3198,22 +3071,22 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G4" t="s">
         <v>18</v>
@@ -3236,22 +3109,22 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G5" t="s">
         <v>18</v>
@@ -3274,22 +3147,22 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G6" t="s">
         <v>26</v>
@@ -3312,22 +3185,22 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="G7" t="s">
         <v>28</v>
@@ -3350,60 +3223,60 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="E8" t="s">
-        <v>63</v>
+        <v>114</v>
       </c>
       <c r="F8" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="H8">
-        <v>16006.62</v>
+        <v>126360</v>
       </c>
       <c r="I8">
-        <v>1333885</v>
+        <v>16200000</v>
       </c>
       <c r="J8">
-        <v>12000</v>
+        <v>26000</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G9" t="s">
         <v>22</v>
@@ -3426,72 +3299,72 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>99</v>
+        <v>56</v>
       </c>
       <c r="E10" t="s">
-        <v>118</v>
+        <v>56</v>
       </c>
       <c r="F10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H10">
-        <v>126360</v>
+        <v>33600</v>
       </c>
       <c r="I10">
-        <v>16200000</v>
+        <v>2240000</v>
       </c>
       <c r="J10">
-        <v>26000</v>
+        <v>15000</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F11" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="G11" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H11">
-        <v>33600</v>
+        <v>9000</v>
       </c>
       <c r="I11">
-        <v>2240000</v>
+        <v>4500000</v>
       </c>
       <c r="J11">
-        <v>15000</v>
+        <v>2000</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -3502,60 +3375,60 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="E12" t="s">
-        <v>61</v>
+        <v>114</v>
       </c>
       <c r="F12" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="G12" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H12">
-        <v>9000</v>
+        <v>12636</v>
       </c>
       <c r="I12">
-        <v>4500000</v>
+        <v>16200000</v>
       </c>
       <c r="J12">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12">
-        <v>100</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B13" t="s">
         <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G13" t="s">
         <v>23</v>
@@ -3578,136 +3451,136 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
         <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="E14" t="s">
-        <v>118</v>
+        <v>55</v>
       </c>
       <c r="F14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H14">
-        <v>12636</v>
+        <v>36000</v>
       </c>
       <c r="I14">
-        <v>16200000</v>
+        <v>18000000</v>
       </c>
       <c r="J14">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14">
-        <v>3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>96</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>114</v>
       </c>
       <c r="F15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H15">
-        <v>36000</v>
+        <v>4212</v>
       </c>
       <c r="I15">
-        <v>18000000</v>
+        <v>16200000</v>
       </c>
       <c r="J15">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>99</v>
+        <v>57</v>
       </c>
       <c r="E16" t="s">
-        <v>118</v>
+        <v>57</v>
       </c>
       <c r="F16" t="s">
         <v>77</v>
       </c>
       <c r="G16" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="H16">
-        <v>4212</v>
+        <v>10000</v>
       </c>
       <c r="I16">
-        <v>16200000</v>
+        <v>5000000</v>
       </c>
       <c r="J16">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G17" t="s">
         <v>21</v>
@@ -3730,78 +3603,78 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>115</v>
       </c>
       <c r="F18" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="G18" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H18">
-        <v>10000</v>
+        <v>6636</v>
       </c>
       <c r="I18">
-        <v>5000000</v>
+        <v>1580000</v>
       </c>
       <c r="J18">
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>96</v>
       </c>
       <c r="E19" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F19" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="G19" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H19">
-        <v>6636</v>
+        <v>12636</v>
       </c>
       <c r="I19">
-        <v>1580000</v>
+        <v>16200000</v>
       </c>
       <c r="J19">
-        <v>14000</v>
+        <v>26000</v>
       </c>
       <c r="K19">
         <v>0</v>
       </c>
       <c r="L19">
-        <v>30</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -3809,19 +3682,19 @@
         <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E20" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F20" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G20" t="s">
         <v>18</v>
@@ -3844,28 +3717,28 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D21" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E21" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F21" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G21" t="s">
         <v>18</v>
       </c>
       <c r="H21">
-        <v>12636</v>
+        <v>126360</v>
       </c>
       <c r="I21">
         <v>16200000</v>
@@ -3877,74 +3750,74 @@
         <v>0</v>
       </c>
       <c r="L21">
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="D22" t="s">
-        <v>99</v>
+        <v>46</v>
       </c>
       <c r="E22" t="s">
-        <v>118</v>
+        <v>46</v>
       </c>
       <c r="F22" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G22" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="H22">
-        <v>126360</v>
+        <v>8000</v>
       </c>
       <c r="I22">
-        <v>16200000</v>
+        <v>4000000</v>
       </c>
       <c r="J22">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="K22">
         <v>0</v>
       </c>
       <c r="L22">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B23" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D23" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="E23" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="F23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G23" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H23">
-        <v>8000</v>
+        <v>9500</v>
       </c>
       <c r="I23">
-        <v>4000000</v>
+        <v>4750000</v>
       </c>
       <c r="J23">
         <v>2000</v>
@@ -3958,31 +3831,31 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D24" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="E24" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="F24" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="G24" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="H24">
-        <v>9500</v>
+        <v>8000</v>
       </c>
       <c r="I24">
-        <v>4750000</v>
+        <v>4000000</v>
       </c>
       <c r="J24">
         <v>2000</v>
@@ -3991,44 +3864,6 @@
         <v>0</v>
       </c>
       <c r="L24">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" t="s">
-        <v>47</v>
-      </c>
-      <c r="E25" t="s">
-        <v>47</v>
-      </c>
-      <c r="F25" t="s">
-        <v>19</v>
-      </c>
-      <c r="G25" t="s">
-        <v>17</v>
-      </c>
-      <c r="H25">
-        <v>8000</v>
-      </c>
-      <c r="I25">
-        <v>4000000</v>
-      </c>
-      <c r="J25">
-        <v>2000</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-      <c r="L25">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2023-10-19
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="120">
   <si>
     <t>상장일</t>
   </si>
@@ -69,6 +69,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2023-10-18</t>
+  </si>
+  <si>
     <t>2023-10-13</t>
   </si>
   <si>
@@ -105,6 +108,9 @@
     <t>2023-08-30</t>
   </si>
   <si>
+    <t>퓨릿</t>
+  </si>
+  <si>
     <t>에이치엠씨제6호스팩</t>
   </si>
   <si>
@@ -153,15 +159,15 @@
     <t>코스피</t>
   </si>
   <si>
+    <t>미래</t>
+  </si>
+  <si>
     <t>현대차</t>
   </si>
   <si>
     <t>한국</t>
   </si>
   <si>
-    <t>미래</t>
-  </si>
-  <si>
     <t>NH</t>
   </si>
   <si>
@@ -240,6 +246,9 @@
     <t>2023-08-21</t>
   </si>
   <si>
+    <t>2023-10-11</t>
+  </si>
+  <si>
     <t>2023-09-26</t>
   </si>
   <si>
@@ -307,6 +316,9 @@
   </si>
   <si>
     <t>한국, 미래</t>
+  </si>
+  <si>
+    <t>1415.77 : 1</t>
   </si>
   <si>
     <t>61.15 : 1</t>
@@ -721,7 +733,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q24"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -785,52 +797,52 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D2">
-        <v>80</v>
+        <v>442.659</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F2">
-        <v>80</v>
+        <v>442.659</v>
       </c>
       <c r="G2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M2">
-        <v>2000</v>
+        <v>10700</v>
       </c>
       <c r="N2">
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="P2" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="Q2">
-        <v>3000000</v>
+        <v>3102750</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -838,90 +850,90 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D3">
-        <v>4212</v>
+        <v>80</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F3">
-        <v>1263.6</v>
+        <v>80</v>
       </c>
       <c r="G3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="L3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M3">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="N3">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="P3" t="s">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="Q3">
-        <v>87871545</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D4">
         <v>4212</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F4">
         <v>1263.6</v>
       </c>
       <c r="G4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M4">
         <v>26000</v>
@@ -930,10 +942,10 @@
         <v>30</v>
       </c>
       <c r="O4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="P4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="Q4">
         <v>87871545</v>
@@ -941,52 +953,52 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D5">
         <v>4212</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F5">
-        <v>421.2</v>
+        <v>1263.6</v>
       </c>
       <c r="G5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M5">
         <v>26000</v>
       </c>
       <c r="N5">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="O5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="P5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="Q5">
         <v>87871545</v>
@@ -994,40 +1006,40 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D6">
         <v>4212</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F6">
         <v>421.2</v>
       </c>
       <c r="G6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M6">
         <v>26000</v>
@@ -1036,10 +1048,10 @@
         <v>10</v>
       </c>
       <c r="O6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="P6" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="Q6">
         <v>87871545</v>
@@ -1047,40 +1059,40 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D7">
         <v>4212</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F7">
         <v>421.2</v>
       </c>
       <c r="G7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M7">
         <v>26000</v>
@@ -1089,10 +1101,10 @@
         <v>10</v>
       </c>
       <c r="O7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="P7" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="Q7">
         <v>87871545</v>
@@ -1100,52 +1112,52 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D8">
         <v>4212</v>
       </c>
       <c r="E8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F8">
-        <v>126.36</v>
+        <v>421.2</v>
       </c>
       <c r="G8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M8">
         <v>26000</v>
       </c>
       <c r="N8">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="O8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="P8" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="Q8">
         <v>87871545</v>
@@ -1153,40 +1165,40 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D9">
         <v>4212</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F9">
         <v>126.36</v>
       </c>
       <c r="G9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M9">
         <v>26000</v>
@@ -1195,10 +1207,10 @@
         <v>3</v>
       </c>
       <c r="O9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="P9" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="Q9">
         <v>87871545</v>
@@ -1206,40 +1218,40 @@
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D10">
         <v>4212</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F10">
         <v>126.36</v>
       </c>
       <c r="G10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M10">
         <v>26000</v>
@@ -1248,10 +1260,10 @@
         <v>3</v>
       </c>
       <c r="O10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="P10" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="Q10">
         <v>87871545</v>
@@ -1259,52 +1271,52 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D11">
         <v>4212</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F11">
-        <v>42.12</v>
+        <v>126.36</v>
       </c>
       <c r="G11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M11">
         <v>26000</v>
       </c>
       <c r="N11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="P11" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="Q11">
         <v>87871545</v>
@@ -1315,105 +1327,105 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D12">
-        <v>360</v>
+        <v>4212</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F12">
-        <v>360</v>
+        <v>42.12</v>
       </c>
       <c r="G12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K12" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="L12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M12">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="N12">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="O12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P12" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="Q12">
-        <v>13500000</v>
+        <v>87871545</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D13">
-        <v>187.5</v>
+        <v>360</v>
       </c>
       <c r="E13" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="F13">
-        <v>187.5</v>
+        <v>360</v>
       </c>
       <c r="G13" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H13" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I13" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J13" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L13" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M13">
-        <v>12500</v>
+        <v>2000</v>
       </c>
       <c r="N13">
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="P13" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="Q13">
-        <v>1020000</v>
+        <v>13500000</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1421,52 +1433,52 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D14">
-        <v>336</v>
+        <v>187.5</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F14">
-        <v>336</v>
+        <v>187.5</v>
       </c>
       <c r="G14" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H14" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I14" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J14" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L14" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M14">
-        <v>15000</v>
+        <v>12500</v>
       </c>
       <c r="N14">
         <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="P14" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="Q14">
-        <v>1619200</v>
+        <v>1020000</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1474,102 +1486,102 @@
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D15">
-        <v>221.2</v>
+        <v>336</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F15">
-        <v>154.84</v>
+        <v>336</v>
       </c>
       <c r="G15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M15">
-        <v>14000</v>
+        <v>15000</v>
       </c>
       <c r="N15">
+        <v>100</v>
+      </c>
+      <c r="O15" t="s">
         <v>70</v>
       </c>
-      <c r="O15" t="s">
-        <v>69</v>
-      </c>
       <c r="P15" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="Q15">
-        <v>2370000</v>
+        <v>1619200</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D16">
         <v>221.2</v>
       </c>
       <c r="E16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F16">
-        <v>66.36</v>
+        <v>154.84</v>
       </c>
       <c r="G16" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H16" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I16" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J16" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L16" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M16">
         <v>14000</v>
       </c>
       <c r="N16">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="O16" t="s">
+        <v>71</v>
+      </c>
+      <c r="P16" t="s">
         <v>69</v>
-      </c>
-      <c r="P16" t="s">
-        <v>67</v>
       </c>
       <c r="Q16">
         <v>2370000</v>
@@ -1580,52 +1592,52 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D17">
-        <v>345</v>
+        <v>221.2</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="F17">
-        <v>345</v>
+        <v>66.36</v>
       </c>
       <c r="G17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K17" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="L17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M17">
-        <v>23000</v>
+        <v>14000</v>
       </c>
       <c r="N17">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="O17" t="s">
+        <v>71</v>
+      </c>
+      <c r="P17" t="s">
         <v>69</v>
       </c>
-      <c r="P17" t="s">
-        <v>67</v>
-      </c>
       <c r="Q17">
-        <v>1125000</v>
+        <v>2370000</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -1633,52 +1645,52 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D18">
-        <v>264</v>
+        <v>345</v>
       </c>
       <c r="E18" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F18">
-        <v>264</v>
+        <v>345</v>
       </c>
       <c r="G18" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H18" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I18" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J18" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L18" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M18">
-        <v>24000</v>
+        <v>23000</v>
       </c>
       <c r="N18">
         <v>100</v>
       </c>
       <c r="O18" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="P18" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="Q18">
-        <v>825000</v>
+        <v>1125000</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1686,52 +1698,52 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D19">
-        <v>90</v>
+        <v>264</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F19">
-        <v>90</v>
+        <v>264</v>
       </c>
       <c r="G19" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H19" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I19" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J19" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K19" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L19" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M19">
-        <v>2000</v>
+        <v>24000</v>
       </c>
       <c r="N19">
         <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P19" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="Q19">
-        <v>3375000</v>
+        <v>825000</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -1739,37 +1751,37 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D20">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E20" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F20">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G20" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H20" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I20" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J20" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K20" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L20" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M20">
         <v>2000</v>
@@ -1778,13 +1790,13 @@
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="P20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q20">
-        <v>3562500</v>
+        <v>3375000</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1792,37 +1804,37 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D21">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="E21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F21">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="G21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K21" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M21">
         <v>2000</v>
@@ -1831,13 +1843,13 @@
         <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="P21" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="Q21">
-        <v>4875000</v>
+        <v>3562500</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1845,37 +1857,37 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D22">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="E22" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="F22">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="G22" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H22" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I22" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J22" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K22" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L22" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M22">
         <v>2000</v>
@@ -1884,13 +1896,13 @@
         <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="P22" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="Q22">
-        <v>3750000</v>
+        <v>4875000</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1898,37 +1910,37 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D23">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E23" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="F23">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="G23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K23" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M23">
         <v>2000</v>
@@ -1937,51 +1949,51 @@
         <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="P23" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="Q23">
-        <v>3000000</v>
+        <v>3750000</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D24">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="E24" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F24">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="G24" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H24" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I24" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J24" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K24" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L24" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M24">
         <v>2000</v>
@@ -1990,12 +2002,65 @@
         <v>100</v>
       </c>
       <c r="O24" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="P24" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="Q24">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25">
+        <v>130</v>
+      </c>
+      <c r="E25" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25">
+        <v>130</v>
+      </c>
+      <c r="G25" t="s">
+        <v>64</v>
+      </c>
+      <c r="H25" t="s">
+        <v>64</v>
+      </c>
+      <c r="I25" t="s">
+        <v>64</v>
+      </c>
+      <c r="J25" t="s">
+        <v>64</v>
+      </c>
+      <c r="K25" t="s">
+        <v>65</v>
+      </c>
+      <c r="L25" t="s">
+        <v>64</v>
+      </c>
+      <c r="M25">
+        <v>2000</v>
+      </c>
+      <c r="N25">
+        <v>100</v>
+      </c>
+      <c r="O25" t="s">
+        <v>75</v>
+      </c>
+      <c r="P25" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q25">
         <v>4875000</v>
       </c>
     </row>
@@ -2006,7 +2071,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T15"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2017,10 +2082,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -2029,633 +2094,633 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
       </c>
       <c r="F2">
-        <v>8000000</v>
+        <v>44265900</v>
       </c>
       <c r="G2">
-        <v>4000000</v>
+        <v>4137000</v>
       </c>
       <c r="H2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I2">
-        <v>2000</v>
+        <v>8800</v>
       </c>
       <c r="J2">
-        <v>2000</v>
+        <v>10700</v>
       </c>
       <c r="K2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L2">
-        <v>2000</v>
+        <v>10700</v>
       </c>
       <c r="M2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>30.21513173797438</v>
       </c>
       <c r="P2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="R2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="T2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
       </c>
       <c r="F3">
-        <v>421200000</v>
+        <v>8000000</v>
       </c>
       <c r="G3">
-        <v>16200000</v>
+        <v>4000000</v>
       </c>
       <c r="H3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I3">
-        <v>21000</v>
+        <v>2000</v>
       </c>
       <c r="J3">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="K3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L3">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="M3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="R3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="S3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="T3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
       </c>
       <c r="F4">
-        <v>36000000</v>
+        <v>421200000</v>
       </c>
       <c r="G4">
-        <v>18000000</v>
+        <v>16200000</v>
       </c>
       <c r="H4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I4">
-        <v>2000</v>
+        <v>21000</v>
       </c>
       <c r="J4">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="K4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L4">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="M4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="R4" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="S4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="T4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F5">
-        <v>18750000</v>
+        <v>36000000</v>
       </c>
       <c r="G5">
-        <v>1500000</v>
+        <v>18000000</v>
       </c>
       <c r="H5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I5">
-        <v>8900</v>
+        <v>2000</v>
       </c>
       <c r="J5">
-        <v>11000</v>
+        <v>2000</v>
       </c>
       <c r="K5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L5">
-        <v>12500</v>
+        <v>2000</v>
       </c>
       <c r="M5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="R5" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="S5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="T5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E6" t="s">
         <v>20</v>
       </c>
       <c r="F6">
-        <v>33600000</v>
+        <v>18750000</v>
       </c>
       <c r="G6">
-        <v>2240000</v>
+        <v>1500000</v>
       </c>
       <c r="H6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I6">
-        <v>11500</v>
+        <v>8900</v>
       </c>
       <c r="J6">
-        <v>13200</v>
+        <v>11000</v>
       </c>
       <c r="K6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L6">
-        <v>15000</v>
+        <v>12500</v>
       </c>
       <c r="M6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O6">
-        <v>26.78571428571428</v>
+        <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="R6" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="S6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="T6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="E7" t="s">
         <v>21</v>
       </c>
       <c r="F7">
-        <v>22120000</v>
+        <v>33600000</v>
       </c>
       <c r="G7">
-        <v>1580000</v>
+        <v>2240000</v>
       </c>
       <c r="H7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I7">
-        <v>10500</v>
+        <v>11500</v>
       </c>
       <c r="J7">
-        <v>12000</v>
+        <v>13200</v>
       </c>
       <c r="K7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L7">
-        <v>14000</v>
+        <v>15000</v>
       </c>
       <c r="M7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O7">
-        <v>0</v>
+        <v>26.78571428571428</v>
       </c>
       <c r="P7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="R7" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="S7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="T7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" t="s">
         <v>69</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" t="s">
-        <v>67</v>
       </c>
       <c r="E8" t="s">
         <v>22</v>
       </c>
       <c r="F8">
-        <v>34500000</v>
+        <v>22120000</v>
       </c>
       <c r="G8">
-        <v>1500000</v>
+        <v>1580000</v>
       </c>
       <c r="H8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I8">
-        <v>20000</v>
+        <v>10500</v>
       </c>
       <c r="J8">
-        <v>23000</v>
+        <v>12000</v>
       </c>
       <c r="K8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L8">
-        <v>23000</v>
+        <v>14000</v>
       </c>
       <c r="M8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="R8" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="S8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="T8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
         <v>23</v>
       </c>
       <c r="F9">
-        <v>26400000</v>
+        <v>34500000</v>
       </c>
       <c r="G9">
-        <v>1100000</v>
+        <v>1500000</v>
       </c>
       <c r="H9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I9">
         <v>20000</v>
       </c>
       <c r="J9">
-        <v>24000</v>
+        <v>23000</v>
       </c>
       <c r="K9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L9">
-        <v>24000</v>
+        <v>23000</v>
       </c>
       <c r="M9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O9">
-        <v>18.18181818181818</v>
+        <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="R9" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="S9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="T9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="E10" t="s">
         <v>24</v>
       </c>
       <c r="F10">
-        <v>9000000</v>
+        <v>26400000</v>
       </c>
       <c r="G10">
-        <v>4500000</v>
+        <v>1100000</v>
       </c>
       <c r="H10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I10">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="J10">
-        <v>2000</v>
+        <v>24000</v>
       </c>
       <c r="K10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L10">
-        <v>2000</v>
+        <v>24000</v>
       </c>
       <c r="M10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O10">
-        <v>0</v>
+        <v>18.18181818181818</v>
       </c>
       <c r="P10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="R10" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="S10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="T10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s">
         <v>25</v>
       </c>
       <c r="F11">
-        <v>9500000</v>
+        <v>9000000</v>
       </c>
       <c r="G11">
-        <v>4750000</v>
+        <v>4500000</v>
       </c>
       <c r="H11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I11">
         <v>2000</v>
@@ -2664,60 +2729,60 @@
         <v>2000</v>
       </c>
       <c r="K11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L11">
         <v>2000</v>
       </c>
       <c r="M11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="R11" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="S11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="T11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s">
         <v>26</v>
       </c>
       <c r="F12">
-        <v>13000000</v>
+        <v>9500000</v>
       </c>
       <c r="G12">
-        <v>6500000</v>
+        <v>4750000</v>
       </c>
       <c r="H12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I12">
         <v>2000</v>
@@ -2726,60 +2791,60 @@
         <v>2000</v>
       </c>
       <c r="K12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L12">
         <v>2000</v>
       </c>
       <c r="M12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="R12" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="S12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="T12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D13" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E13" t="s">
         <v>27</v>
       </c>
       <c r="F13">
-        <v>10000000</v>
+        <v>13000000</v>
       </c>
       <c r="G13">
-        <v>5000000</v>
+        <v>6500000</v>
       </c>
       <c r="H13" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I13">
         <v>2000</v>
@@ -2788,60 +2853,60 @@
         <v>2000</v>
       </c>
       <c r="K13" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L13">
         <v>2000</v>
       </c>
       <c r="M13" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N13" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q13" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="R13" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="S13" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="T13" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E14" t="s">
         <v>28</v>
       </c>
       <c r="F14">
-        <v>8000000</v>
+        <v>10000000</v>
       </c>
       <c r="G14">
-        <v>4000000</v>
+        <v>5000000</v>
       </c>
       <c r="H14" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I14">
         <v>2000</v>
@@ -2850,60 +2915,60 @@
         <v>2000</v>
       </c>
       <c r="K14" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L14">
         <v>2000</v>
       </c>
       <c r="M14" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N14" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q14" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="R14" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="S14" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="T14" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F15">
-        <v>13000000</v>
+        <v>8000000</v>
       </c>
       <c r="G15">
-        <v>6500000</v>
+        <v>4000000</v>
       </c>
       <c r="H15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I15">
         <v>2000</v>
@@ -2912,34 +2977,96 @@
         <v>2000</v>
       </c>
       <c r="K15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L15">
         <v>2000</v>
       </c>
       <c r="M15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="R15" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="S15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="T15" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16">
+        <v>13000000</v>
+      </c>
+      <c r="G16">
+        <v>6500000</v>
+      </c>
+      <c r="H16" t="s">
+        <v>64</v>
+      </c>
+      <c r="I16">
+        <v>2000</v>
+      </c>
+      <c r="J16">
+        <v>2000</v>
+      </c>
+      <c r="K16" t="s">
+        <v>64</v>
+      </c>
+      <c r="L16">
+        <v>2000</v>
+      </c>
+      <c r="M16" t="s">
+        <v>64</v>
+      </c>
+      <c r="N16" t="s">
+        <v>64</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>64</v>
+      </c>
+      <c r="R16" t="s">
+        <v>114</v>
+      </c>
+      <c r="S16" t="s">
+        <v>64</v>
+      </c>
+      <c r="T16" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2949,7 +3076,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2957,16 +3084,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -2978,10 +3105,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -2990,30 +3117,30 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E2" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H2">
         <v>42120</v>
@@ -3033,25 +3160,25 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H3">
         <v>18750</v>
@@ -3071,25 +3198,25 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E4" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H4">
         <v>42120</v>
@@ -3109,25 +3236,25 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E5" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H5">
         <v>42120</v>
@@ -3147,25 +3274,25 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F6" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H6">
         <v>13000</v>
@@ -3185,25 +3312,25 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
         <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7">
         <v>13000</v>
@@ -3226,37 +3353,37 @@
         <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>96</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H8">
-        <v>126360</v>
+        <v>34500</v>
       </c>
       <c r="I8">
-        <v>16200000</v>
+        <v>1500000</v>
       </c>
       <c r="J8">
-        <v>26000</v>
+        <v>23000</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -3264,10 +3391,10 @@
         <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
         <v>47</v>
@@ -3276,19 +3403,19 @@
         <v>47</v>
       </c>
       <c r="F9" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="G9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="H9">
-        <v>34500</v>
+        <v>44265.9</v>
       </c>
       <c r="I9">
-        <v>1500000</v>
+        <v>4137000</v>
       </c>
       <c r="J9">
-        <v>23000</v>
+        <v>10700</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -3299,72 +3426,72 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>118</v>
       </c>
       <c r="F10" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H10">
-        <v>33600</v>
+        <v>126360</v>
       </c>
       <c r="I10">
-        <v>2240000</v>
+        <v>16200000</v>
       </c>
       <c r="J10">
-        <v>15000</v>
+        <v>26000</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
+        <v>78</v>
       </c>
       <c r="G11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H11">
-        <v>9000</v>
+        <v>33600</v>
       </c>
       <c r="I11">
-        <v>4500000</v>
+        <v>2240000</v>
       </c>
       <c r="J11">
-        <v>2000</v>
+        <v>15000</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -3375,110 +3502,110 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
-        <v>114</v>
+        <v>61</v>
       </c>
       <c r="F12" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="G12" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="H12">
-        <v>12636</v>
+        <v>9000</v>
       </c>
       <c r="I12">
-        <v>16200000</v>
+        <v>4500000</v>
       </c>
       <c r="J12">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12">
-        <v>3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>118</v>
       </c>
       <c r="F13" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="G13" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H13">
-        <v>26400</v>
+        <v>12636</v>
       </c>
       <c r="I13">
-        <v>1100000</v>
+        <v>16200000</v>
       </c>
       <c r="J13">
-        <v>24000</v>
+        <v>26000</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="L13">
-        <v>100</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F14" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G14" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="H14">
-        <v>36000</v>
+        <v>26400</v>
       </c>
       <c r="I14">
-        <v>18000000</v>
+        <v>1100000</v>
       </c>
       <c r="J14">
-        <v>2000</v>
+        <v>24000</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -3489,101 +3616,101 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>114</v>
+        <v>57</v>
       </c>
       <c r="F15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="G15" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H15">
-        <v>4212</v>
+        <v>36000</v>
       </c>
       <c r="I15">
-        <v>16200000</v>
+        <v>18000000</v>
       </c>
       <c r="J15">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
       <c r="E16" t="s">
-        <v>57</v>
+        <v>118</v>
       </c>
       <c r="F16" t="s">
         <v>77</v>
       </c>
       <c r="G16" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H16">
-        <v>10000</v>
+        <v>4212</v>
       </c>
       <c r="I16">
-        <v>5000000</v>
+        <v>16200000</v>
       </c>
       <c r="J16">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" t="s">
+        <v>119</v>
+      </c>
+      <c r="F17" t="s">
         <v>69</v>
       </c>
-      <c r="C17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" t="s">
-        <v>115</v>
-      </c>
-      <c r="F17" t="s">
-        <v>67</v>
-      </c>
       <c r="G17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H17">
         <v>15484</v>
@@ -3603,78 +3730,78 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E18" t="s">
-        <v>115</v>
+        <v>59</v>
       </c>
       <c r="F18" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="G18" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="H18">
-        <v>6636</v>
+        <v>10000</v>
       </c>
       <c r="I18">
-        <v>1580000</v>
+        <v>5000000</v>
       </c>
       <c r="J18">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="E19" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="F19" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G19" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H19">
-        <v>12636</v>
+        <v>6636</v>
       </c>
       <c r="I19">
-        <v>16200000</v>
+        <v>1580000</v>
       </c>
       <c r="J19">
-        <v>26000</v>
+        <v>14000</v>
       </c>
       <c r="K19">
         <v>0</v>
       </c>
       <c r="L19">
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -3682,22 +3809,22 @@
         <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D20" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E20" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F20" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H20">
         <v>12636</v>
@@ -3717,28 +3844,28 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E21" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F21" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G21" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H21">
-        <v>126360</v>
+        <v>12636</v>
       </c>
       <c r="I21">
         <v>16200000</v>
@@ -3750,30 +3877,30 @@
         <v>0</v>
       </c>
       <c r="L21">
-        <v>30</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D22" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E22" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F22" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H22">
         <v>8000</v>
@@ -3793,69 +3920,69 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>60</v>
+        <v>99</v>
       </c>
       <c r="E23" t="s">
-        <v>60</v>
+        <v>118</v>
       </c>
       <c r="F23" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="G23" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H23">
-        <v>9500</v>
+        <v>126360</v>
       </c>
       <c r="I23">
-        <v>4750000</v>
+        <v>16200000</v>
       </c>
       <c r="J23">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="K23">
         <v>0</v>
       </c>
       <c r="L23">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="C24" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="D24" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="E24" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="F24" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="G24" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="H24">
-        <v>8000</v>
+        <v>9500</v>
       </c>
       <c r="I24">
-        <v>4000000</v>
+        <v>4750000</v>
       </c>
       <c r="J24">
         <v>2000</v>
@@ -3864,6 +3991,44 @@
         <v>0</v>
       </c>
       <c r="L24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25">
+        <v>8000</v>
+      </c>
+      <c r="I25">
+        <v>4000000</v>
+      </c>
+      <c r="J25">
+        <v>2000</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2023-10-20
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="123">
   <si>
     <t>상장일</t>
   </si>
@@ -69,6 +69,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2023-10-19</t>
+  </si>
+  <si>
     <t>2023-10-18</t>
   </si>
   <si>
@@ -108,6 +111,9 @@
     <t>2023-08-30</t>
   </si>
   <si>
+    <t>신성에스티</t>
+  </si>
+  <si>
     <t>퓨릿</t>
   </si>
   <si>
@@ -316,6 +322,9 @@
   </si>
   <si>
     <t>한국, 미래</t>
+  </si>
+  <si>
+    <t>1891.4 : 1</t>
   </si>
   <si>
     <t>1415.77 : 1</t>
@@ -733,7 +742,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -797,52 +806,52 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D2">
-        <v>442.659</v>
+        <v>520</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F2">
-        <v>442.659</v>
+        <v>520</v>
       </c>
       <c r="G2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M2">
-        <v>10700</v>
+        <v>26000</v>
       </c>
       <c r="N2">
         <v>100</v>
       </c>
       <c r="O2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" t="s">
         <v>19</v>
       </c>
-      <c r="P2" t="s">
-        <v>76</v>
-      </c>
       <c r="Q2">
-        <v>3102750</v>
+        <v>1300000</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -850,52 +859,52 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D3">
-        <v>80</v>
+        <v>442.659</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F3">
-        <v>80</v>
+        <v>442.659</v>
       </c>
       <c r="G3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M3">
-        <v>2000</v>
+        <v>10700</v>
       </c>
       <c r="N3">
         <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="P3" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="Q3">
-        <v>3000000</v>
+        <v>3102750</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -903,90 +912,90 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D4">
-        <v>4212</v>
+        <v>80</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F4">
-        <v>1263.6</v>
+        <v>80</v>
       </c>
       <c r="G4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M4">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="N4">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="P4" t="s">
-        <v>77</v>
+        <v>21</v>
       </c>
       <c r="Q4">
-        <v>87871545</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D5">
         <v>4212</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F5">
         <v>1263.6</v>
       </c>
       <c r="G5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M5">
         <v>26000</v>
@@ -995,10 +1004,10 @@
         <v>30</v>
       </c>
       <c r="O5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="P5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="Q5">
         <v>87871545</v>
@@ -1006,52 +1015,52 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D6">
         <v>4212</v>
       </c>
       <c r="E6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F6">
-        <v>421.2</v>
+        <v>1263.6</v>
       </c>
       <c r="G6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M6">
         <v>26000</v>
       </c>
       <c r="N6">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="O6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="P6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="Q6">
         <v>87871545</v>
@@ -1059,40 +1068,40 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D7">
         <v>4212</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F7">
         <v>421.2</v>
       </c>
       <c r="G7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M7">
         <v>26000</v>
@@ -1101,10 +1110,10 @@
         <v>10</v>
       </c>
       <c r="O7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="P7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="Q7">
         <v>87871545</v>
@@ -1112,40 +1121,40 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D8">
         <v>4212</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F8">
         <v>421.2</v>
       </c>
       <c r="G8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M8">
         <v>26000</v>
@@ -1154,10 +1163,10 @@
         <v>10</v>
       </c>
       <c r="O8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="P8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="Q8">
         <v>87871545</v>
@@ -1165,52 +1174,52 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D9">
         <v>4212</v>
       </c>
       <c r="E9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F9">
-        <v>126.36</v>
+        <v>421.2</v>
       </c>
       <c r="G9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="L9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M9">
         <v>26000</v>
       </c>
       <c r="N9">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="O9" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="P9" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="Q9">
         <v>87871545</v>
@@ -1218,40 +1227,40 @@
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D10">
         <v>4212</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F10">
         <v>126.36</v>
       </c>
       <c r="G10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K10" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M10">
         <v>26000</v>
@@ -1260,10 +1269,10 @@
         <v>3</v>
       </c>
       <c r="O10" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="P10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="Q10">
         <v>87871545</v>
@@ -1271,40 +1280,40 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D11">
         <v>4212</v>
       </c>
       <c r="E11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F11">
         <v>126.36</v>
       </c>
       <c r="G11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K11" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M11">
         <v>26000</v>
@@ -1313,10 +1322,10 @@
         <v>3</v>
       </c>
       <c r="O11" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="P11" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="Q11">
         <v>87871545</v>
@@ -1324,52 +1333,52 @@
     </row>
     <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D12">
         <v>4212</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F12">
-        <v>42.12</v>
+        <v>126.36</v>
       </c>
       <c r="G12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K12" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M12">
         <v>26000</v>
       </c>
       <c r="N12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="P12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="Q12">
         <v>87871545</v>
@@ -1380,105 +1389,105 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D13">
-        <v>360</v>
+        <v>4212</v>
       </c>
       <c r="E13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F13">
-        <v>360</v>
+        <v>42.12</v>
       </c>
       <c r="G13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K13" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="L13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M13">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="N13">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="O13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="P13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="Q13">
-        <v>13500000</v>
+        <v>87871545</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D14">
-        <v>187.5</v>
+        <v>360</v>
       </c>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="F14">
-        <v>187.5</v>
+        <v>360</v>
       </c>
       <c r="G14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K14" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M14">
-        <v>12500</v>
+        <v>2000</v>
       </c>
       <c r="N14">
         <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="P14" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="Q14">
-        <v>1020000</v>
+        <v>13500000</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1486,52 +1495,52 @@
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D15">
-        <v>336</v>
+        <v>187.5</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F15">
-        <v>336</v>
+        <v>187.5</v>
       </c>
       <c r="G15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K15" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M15">
-        <v>15000</v>
+        <v>12500</v>
       </c>
       <c r="N15">
         <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="P15" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="Q15">
-        <v>1619200</v>
+        <v>1020000</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1539,102 +1548,102 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D16">
-        <v>221.2</v>
+        <v>336</v>
       </c>
       <c r="E16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F16">
-        <v>154.84</v>
+        <v>336</v>
       </c>
       <c r="G16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K16" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M16">
-        <v>14000</v>
+        <v>15000</v>
       </c>
       <c r="N16">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="P16" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="Q16">
-        <v>2370000</v>
+        <v>1619200</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D17">
         <v>221.2</v>
       </c>
       <c r="E17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F17">
-        <v>66.36</v>
+        <v>154.84</v>
       </c>
       <c r="G17" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H17" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I17" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J17" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L17" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M17">
         <v>14000</v>
       </c>
       <c r="N17">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="O17" t="s">
+        <v>73</v>
+      </c>
+      <c r="P17" t="s">
         <v>71</v>
-      </c>
-      <c r="P17" t="s">
-        <v>69</v>
       </c>
       <c r="Q17">
         <v>2370000</v>
@@ -1645,52 +1654,52 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D18">
-        <v>345</v>
+        <v>221.2</v>
       </c>
       <c r="E18" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="F18">
-        <v>345</v>
+        <v>66.36</v>
       </c>
       <c r="G18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K18" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="L18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M18">
-        <v>23000</v>
+        <v>14000</v>
       </c>
       <c r="N18">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="O18" t="s">
+        <v>73</v>
+      </c>
+      <c r="P18" t="s">
         <v>71</v>
       </c>
-      <c r="P18" t="s">
-        <v>69</v>
-      </c>
       <c r="Q18">
-        <v>1125000</v>
+        <v>2370000</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1698,52 +1707,52 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D19">
-        <v>264</v>
+        <v>345</v>
       </c>
       <c r="E19" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F19">
-        <v>264</v>
+        <v>345</v>
       </c>
       <c r="G19" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H19" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I19" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J19" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K19" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L19" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M19">
-        <v>24000</v>
+        <v>23000</v>
       </c>
       <c r="N19">
         <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="P19" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Q19">
-        <v>825000</v>
+        <v>1125000</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -1751,52 +1760,52 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D20">
-        <v>90</v>
+        <v>264</v>
       </c>
       <c r="E20" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F20">
-        <v>90</v>
+        <v>264</v>
       </c>
       <c r="G20" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H20" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I20" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J20" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K20" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L20" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M20">
-        <v>2000</v>
+        <v>24000</v>
       </c>
       <c r="N20">
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P20" t="s">
-        <v>26</v>
+        <v>72</v>
       </c>
       <c r="Q20">
-        <v>3375000</v>
+        <v>825000</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1804,37 +1813,37 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D21">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E21" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F21">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G21" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H21" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I21" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J21" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K21" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L21" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M21">
         <v>2000</v>
@@ -1843,13 +1852,13 @@
         <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="P21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q21">
-        <v>3562500</v>
+        <v>3375000</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1857,37 +1866,37 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D22">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="E22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F22">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="G22" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H22" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I22" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J22" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K22" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L22" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M22">
         <v>2000</v>
@@ -1896,13 +1905,13 @@
         <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="P22" t="s">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="Q22">
-        <v>4875000</v>
+        <v>3562500</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1910,37 +1919,37 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D23">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="E23" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F23">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="G23" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H23" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I23" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J23" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L23" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M23">
         <v>2000</v>
@@ -1949,13 +1958,13 @@
         <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="P23" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Q23">
-        <v>3750000</v>
+        <v>4875000</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -1963,37 +1972,37 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D24">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E24" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="F24">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="G24" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H24" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I24" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J24" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K24" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L24" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M24">
         <v>2000</v>
@@ -2002,51 +2011,51 @@
         <v>100</v>
       </c>
       <c r="O24" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="P24" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="Q24">
-        <v>3000000</v>
+        <v>3750000</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D25">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="E25" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F25">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="G25" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H25" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I25" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J25" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K25" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L25" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M25">
         <v>2000</v>
@@ -2055,12 +2064,65 @@
         <v>100</v>
       </c>
       <c r="O25" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="P25" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="Q25">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26">
+        <v>130</v>
+      </c>
+      <c r="E26" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26">
+        <v>130</v>
+      </c>
+      <c r="G26" t="s">
+        <v>66</v>
+      </c>
+      <c r="H26" t="s">
+        <v>66</v>
+      </c>
+      <c r="I26" t="s">
+        <v>66</v>
+      </c>
+      <c r="J26" t="s">
+        <v>66</v>
+      </c>
+      <c r="K26" t="s">
+        <v>67</v>
+      </c>
+      <c r="L26" t="s">
+        <v>66</v>
+      </c>
+      <c r="M26">
+        <v>2000</v>
+      </c>
+      <c r="N26">
+        <v>100</v>
+      </c>
+      <c r="O26" t="s">
+        <v>77</v>
+      </c>
+      <c r="P26" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q26">
         <v>4875000</v>
       </c>
     </row>
@@ -2071,7 +2133,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2082,10 +2144,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -2094,695 +2156,695 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
         <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="s">
-        <v>76</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
       </c>
       <c r="F2">
-        <v>44265900</v>
+        <v>52000000</v>
       </c>
       <c r="G2">
-        <v>4137000</v>
+        <v>2000000</v>
       </c>
       <c r="H2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I2">
-        <v>8800</v>
+        <v>22000</v>
       </c>
       <c r="J2">
-        <v>10700</v>
+        <v>25000</v>
       </c>
       <c r="K2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L2">
-        <v>10700</v>
+        <v>26000</v>
       </c>
       <c r="M2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="O2">
-        <v>30.21513173797438</v>
+        <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="Q2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="R2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="S2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="T2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
       </c>
       <c r="F3">
-        <v>8000000</v>
+        <v>44265900</v>
       </c>
       <c r="G3">
-        <v>4000000</v>
+        <v>4137000</v>
       </c>
       <c r="H3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I3">
-        <v>2000</v>
+        <v>8800</v>
       </c>
       <c r="J3">
-        <v>2000</v>
+        <v>10700</v>
       </c>
       <c r="K3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L3">
-        <v>2000</v>
+        <v>10700</v>
       </c>
       <c r="M3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>30.21513173797438</v>
       </c>
       <c r="P3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="Q3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="R3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="S3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="T3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
       </c>
       <c r="F4">
-        <v>421200000</v>
+        <v>8000000</v>
       </c>
       <c r="G4">
-        <v>16200000</v>
+        <v>4000000</v>
       </c>
       <c r="H4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I4">
-        <v>21000</v>
+        <v>2000</v>
       </c>
       <c r="J4">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="K4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L4">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="M4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="Q4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="R4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="S4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="T4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
       </c>
       <c r="F5">
-        <v>36000000</v>
+        <v>421200000</v>
       </c>
       <c r="G5">
-        <v>18000000</v>
+        <v>16200000</v>
       </c>
       <c r="H5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I5">
-        <v>2000</v>
+        <v>21000</v>
       </c>
       <c r="J5">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="K5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L5">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="M5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="Q5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="R5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="S5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="T5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F6">
-        <v>18750000</v>
+        <v>36000000</v>
       </c>
       <c r="G6">
-        <v>1500000</v>
+        <v>18000000</v>
       </c>
       <c r="H6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I6">
-        <v>8900</v>
+        <v>2000</v>
       </c>
       <c r="J6">
-        <v>11000</v>
+        <v>2000</v>
       </c>
       <c r="K6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L6">
-        <v>12500</v>
+        <v>2000</v>
       </c>
       <c r="M6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="Q6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="R6" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="S6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="T6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E7" t="s">
         <v>21</v>
       </c>
       <c r="F7">
-        <v>33600000</v>
+        <v>18750000</v>
       </c>
       <c r="G7">
-        <v>2240000</v>
+        <v>1500000</v>
       </c>
       <c r="H7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I7">
-        <v>11500</v>
+        <v>8900</v>
       </c>
       <c r="J7">
-        <v>13200</v>
+        <v>11000</v>
       </c>
       <c r="K7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L7">
-        <v>15000</v>
+        <v>12500</v>
       </c>
       <c r="M7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="O7">
-        <v>26.78571428571428</v>
+        <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="Q7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="R7" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="S7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="T7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E8" t="s">
         <v>22</v>
       </c>
       <c r="F8">
-        <v>22120000</v>
+        <v>33600000</v>
       </c>
       <c r="G8">
-        <v>1580000</v>
+        <v>2240000</v>
       </c>
       <c r="H8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I8">
-        <v>10500</v>
+        <v>11500</v>
       </c>
       <c r="J8">
-        <v>12000</v>
+        <v>13200</v>
       </c>
       <c r="K8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L8">
-        <v>14000</v>
+        <v>15000</v>
       </c>
       <c r="M8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="O8">
-        <v>0</v>
+        <v>26.78571428571428</v>
       </c>
       <c r="P8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="Q8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="R8" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="S8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="T8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" t="s">
         <v>71</v>
-      </c>
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" t="s">
-        <v>69</v>
       </c>
       <c r="E9" t="s">
         <v>23</v>
       </c>
       <c r="F9">
-        <v>34500000</v>
+        <v>22120000</v>
       </c>
       <c r="G9">
-        <v>1500000</v>
+        <v>1580000</v>
       </c>
       <c r="H9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I9">
-        <v>20000</v>
+        <v>10500</v>
       </c>
       <c r="J9">
-        <v>23000</v>
+        <v>12000</v>
       </c>
       <c r="K9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L9">
-        <v>23000</v>
+        <v>14000</v>
       </c>
       <c r="M9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="Q9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="R9" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="S9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="T9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E10" t="s">
         <v>24</v>
       </c>
       <c r="F10">
-        <v>26400000</v>
+        <v>34500000</v>
       </c>
       <c r="G10">
-        <v>1100000</v>
+        <v>1500000</v>
       </c>
       <c r="H10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I10">
         <v>20000</v>
       </c>
       <c r="J10">
-        <v>24000</v>
+        <v>23000</v>
       </c>
       <c r="K10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L10">
-        <v>24000</v>
+        <v>23000</v>
       </c>
       <c r="M10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="O10">
-        <v>18.18181818181818</v>
+        <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="Q10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="R10" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="S10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="T10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>72</v>
       </c>
       <c r="E11" t="s">
         <v>25</v>
       </c>
       <c r="F11">
-        <v>9000000</v>
+        <v>26400000</v>
       </c>
       <c r="G11">
-        <v>4500000</v>
+        <v>1100000</v>
       </c>
       <c r="H11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I11">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="J11">
-        <v>2000</v>
+        <v>24000</v>
       </c>
       <c r="K11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L11">
-        <v>2000</v>
+        <v>24000</v>
       </c>
       <c r="M11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>18.18181818181818</v>
       </c>
       <c r="P11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="Q11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="R11" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="S11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="T11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E12" t="s">
         <v>26</v>
       </c>
       <c r="F12">
-        <v>9500000</v>
+        <v>9000000</v>
       </c>
       <c r="G12">
-        <v>4750000</v>
+        <v>4500000</v>
       </c>
       <c r="H12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I12">
         <v>2000</v>
@@ -2791,60 +2853,60 @@
         <v>2000</v>
       </c>
       <c r="K12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L12">
         <v>2000</v>
       </c>
       <c r="M12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="Q12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="R12" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="S12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="T12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
         <v>27</v>
       </c>
       <c r="F13">
-        <v>13000000</v>
+        <v>9500000</v>
       </c>
       <c r="G13">
-        <v>6500000</v>
+        <v>4750000</v>
       </c>
       <c r="H13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I13">
         <v>2000</v>
@@ -2853,60 +2915,60 @@
         <v>2000</v>
       </c>
       <c r="K13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L13">
         <v>2000</v>
       </c>
       <c r="M13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="Q13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="R13" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="S13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="T13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="D14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E14" t="s">
         <v>28</v>
       </c>
       <c r="F14">
-        <v>10000000</v>
+        <v>13000000</v>
       </c>
       <c r="G14">
-        <v>5000000</v>
+        <v>6500000</v>
       </c>
       <c r="H14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I14">
         <v>2000</v>
@@ -2915,60 +2977,60 @@
         <v>2000</v>
       </c>
       <c r="K14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L14">
         <v>2000</v>
       </c>
       <c r="M14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="Q14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="R14" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="S14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="T14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="D15" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E15" t="s">
         <v>29</v>
       </c>
       <c r="F15">
-        <v>8000000</v>
+        <v>10000000</v>
       </c>
       <c r="G15">
-        <v>4000000</v>
+        <v>5000000</v>
       </c>
       <c r="H15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I15">
         <v>2000</v>
@@ -2977,60 +3039,60 @@
         <v>2000</v>
       </c>
       <c r="K15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L15">
         <v>2000</v>
       </c>
       <c r="M15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="Q15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="R15" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="S15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="T15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="D16" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F16">
-        <v>13000000</v>
+        <v>8000000</v>
       </c>
       <c r="G16">
-        <v>6500000</v>
+        <v>4000000</v>
       </c>
       <c r="H16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I16">
         <v>2000</v>
@@ -3039,34 +3101,96 @@
         <v>2000</v>
       </c>
       <c r="K16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L16">
         <v>2000</v>
       </c>
       <c r="M16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="Q16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="R16" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="S16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="T16" t="s">
-        <v>64</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17">
+        <v>13000000</v>
+      </c>
+      <c r="G17">
+        <v>6500000</v>
+      </c>
+      <c r="H17" t="s">
+        <v>66</v>
+      </c>
+      <c r="I17">
+        <v>2000</v>
+      </c>
+      <c r="J17">
+        <v>2000</v>
+      </c>
+      <c r="K17" t="s">
+        <v>66</v>
+      </c>
+      <c r="L17">
+        <v>2000</v>
+      </c>
+      <c r="M17" t="s">
+        <v>66</v>
+      </c>
+      <c r="N17" t="s">
+        <v>66</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>66</v>
+      </c>
+      <c r="R17" t="s">
+        <v>117</v>
+      </c>
+      <c r="S17" t="s">
+        <v>66</v>
+      </c>
+      <c r="T17" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -3076,7 +3200,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3084,16 +3208,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -3105,10 +3229,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -3117,30 +3241,30 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H2">
         <v>42120</v>
@@ -3160,25 +3284,25 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H3">
         <v>18750</v>
@@ -3198,25 +3322,25 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E4" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H4">
         <v>42120</v>
@@ -3236,25 +3360,25 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E5" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H5">
         <v>42120</v>
@@ -3274,25 +3398,25 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H6">
         <v>13000</v>
@@ -3312,25 +3436,25 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H7">
         <v>13000</v>
@@ -3350,25 +3474,25 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" t="s">
         <v>71</v>
       </c>
-      <c r="C8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" t="s">
-        <v>69</v>
-      </c>
       <c r="G8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H8">
         <v>34500</v>
@@ -3388,34 +3512,34 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" t="s">
         <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" t="s">
-        <v>76</v>
       </c>
       <c r="G9" t="s">
         <v>17</v>
       </c>
       <c r="H9">
-        <v>44265.9</v>
+        <v>52000</v>
       </c>
       <c r="I9">
-        <v>4137000</v>
+        <v>2000000</v>
       </c>
       <c r="J9">
-        <v>10700</v>
+        <v>26000</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -3426,110 +3550,110 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
         <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>99</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
-        <v>118</v>
+        <v>49</v>
       </c>
       <c r="F10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H10">
-        <v>126360</v>
+        <v>44265.9</v>
       </c>
       <c r="I10">
-        <v>16200000</v>
+        <v>4137000</v>
       </c>
       <c r="J10">
-        <v>26000</v>
+        <v>10700</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
       <c r="E11" t="s">
-        <v>58</v>
+        <v>121</v>
       </c>
       <c r="F11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H11">
-        <v>33600</v>
+        <v>126360</v>
       </c>
       <c r="I11">
-        <v>2240000</v>
+        <v>16200000</v>
       </c>
       <c r="J11">
-        <v>15000</v>
+        <v>26000</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F12" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
       <c r="G12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H12">
-        <v>9000</v>
+        <v>33600</v>
       </c>
       <c r="I12">
-        <v>4500000</v>
+        <v>2240000</v>
       </c>
       <c r="J12">
-        <v>2000</v>
+        <v>15000</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -3540,110 +3664,110 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="E13" t="s">
-        <v>118</v>
+        <v>63</v>
       </c>
       <c r="F13" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="G13" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="H13">
-        <v>12636</v>
+        <v>9000</v>
       </c>
       <c r="I13">
-        <v>16200000</v>
+        <v>4500000</v>
       </c>
       <c r="J13">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="L13">
-        <v>3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
+        <v>101</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>121</v>
       </c>
       <c r="F14" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="G14" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H14">
-        <v>26400</v>
+        <v>12636</v>
       </c>
       <c r="I14">
-        <v>1100000</v>
+        <v>16200000</v>
       </c>
       <c r="J14">
-        <v>24000</v>
+        <v>26000</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14">
-        <v>100</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F15" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G15" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H15">
-        <v>36000</v>
+        <v>26400</v>
       </c>
       <c r="I15">
-        <v>18000000</v>
+        <v>1100000</v>
       </c>
       <c r="J15">
-        <v>2000</v>
+        <v>24000</v>
       </c>
       <c r="K15">
         <v>0</v>
@@ -3654,101 +3778,101 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="E16" t="s">
-        <v>118</v>
+        <v>59</v>
       </c>
       <c r="F16" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G16" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H16">
-        <v>4212</v>
+        <v>36000</v>
       </c>
       <c r="I16">
-        <v>16200000</v>
+        <v>18000000</v>
       </c>
       <c r="J16">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
         <v>71</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="E17" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F17" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="G17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H17">
-        <v>15484</v>
+        <v>4212</v>
       </c>
       <c r="I17">
-        <v>1580000</v>
+        <v>16200000</v>
       </c>
       <c r="J17">
-        <v>14000</v>
+        <v>26000</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
-        <v>70</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F18" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H18">
         <v>10000</v>
@@ -3768,28 +3892,28 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" t="s">
+        <v>122</v>
+      </c>
+      <c r="F19" t="s">
         <v>71</v>
       </c>
-      <c r="C19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" t="s">
-        <v>119</v>
-      </c>
-      <c r="F19" t="s">
-        <v>69</v>
-      </c>
       <c r="G19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H19">
-        <v>6636</v>
+        <v>15484</v>
       </c>
       <c r="I19">
         <v>1580000</v>
@@ -3801,45 +3925,45 @@
         <v>0</v>
       </c>
       <c r="L19">
-        <v>30</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>99</v>
+        <v>61</v>
       </c>
       <c r="E20" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="F20" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G20" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H20">
-        <v>12636</v>
+        <v>6636</v>
       </c>
       <c r="I20">
-        <v>16200000</v>
+        <v>1580000</v>
       </c>
       <c r="J20">
-        <v>26000</v>
+        <v>14000</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
       <c r="L20">
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -3847,22 +3971,22 @@
         <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E21" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F21" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H21">
         <v>12636</v>
@@ -3882,63 +4006,63 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>49</v>
+        <v>101</v>
       </c>
       <c r="E22" t="s">
-        <v>49</v>
+        <v>121</v>
       </c>
       <c r="F22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G22" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="H22">
-        <v>8000</v>
+        <v>12636</v>
       </c>
       <c r="I22">
-        <v>4000000</v>
+        <v>16200000</v>
       </c>
       <c r="J22">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="K22">
         <v>0</v>
       </c>
       <c r="L22">
-        <v>100</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E23" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F23" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G23" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H23">
         <v>126360</v>
@@ -3958,31 +4082,31 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D24" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E24" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F24" t="s">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="G24" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="H24">
-        <v>9500</v>
+        <v>8000</v>
       </c>
       <c r="I24">
-        <v>4750000</v>
+        <v>4000000</v>
       </c>
       <c r="J24">
         <v>2000</v>
@@ -3996,31 +4120,31 @@
     </row>
     <row r="25" spans="1:12">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="C25" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="D25" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="E25" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="F25" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="G25" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="H25">
-        <v>8000</v>
+        <v>9500</v>
       </c>
       <c r="I25">
-        <v>4000000</v>
+        <v>4750000</v>
       </c>
       <c r="J25">
         <v>2000</v>
@@ -4029,6 +4153,44 @@
         <v>0</v>
       </c>
       <c r="L25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" t="s">
+        <v>19</v>
+      </c>
+      <c r="H26">
+        <v>8000</v>
+      </c>
+      <c r="I26">
+        <v>4000000</v>
+      </c>
+      <c r="J26">
+        <v>2000</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2023-10-22
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="126">
   <si>
     <t>상장일</t>
   </si>
@@ -69,6 +69,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2023-10-20</t>
+  </si>
+  <si>
     <t>2023-10-19</t>
   </si>
   <si>
@@ -111,6 +114,9 @@
     <t>2023-08-30</t>
   </si>
   <si>
+    <t>에스엘에스바이오</t>
+  </si>
+  <si>
     <t>신성에스티</t>
   </si>
   <si>
@@ -165,6 +171,9 @@
     <t>코스피</t>
   </si>
   <si>
+    <t>하나</t>
+  </si>
+  <si>
     <t>미래</t>
   </si>
   <si>
@@ -189,9 +198,6 @@
     <t>신영</t>
   </si>
   <si>
-    <t>하나</t>
-  </si>
-  <si>
     <t>유비에스</t>
   </si>
   <si>
@@ -322,6 +328,9 @@
   </si>
   <si>
     <t>한국, 미래</t>
+  </si>
+  <si>
+    <t>345.96 : 1</t>
   </si>
   <si>
     <t>1891.4 : 1</t>
@@ -742,7 +751,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -806,52 +815,52 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D2">
-        <v>520</v>
+        <v>53.9</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F2">
-        <v>520</v>
+        <v>53.9</v>
       </c>
       <c r="G2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M2">
-        <v>26000</v>
+        <v>7000</v>
       </c>
       <c r="N2">
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q2">
-        <v>1300000</v>
+        <v>577500</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -859,52 +868,52 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D3">
-        <v>442.659</v>
+        <v>520</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F3">
-        <v>442.659</v>
+        <v>520</v>
       </c>
       <c r="G3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M3">
-        <v>10700</v>
+        <v>26000</v>
       </c>
       <c r="N3">
         <v>100</v>
       </c>
       <c r="O3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" t="s">
         <v>20</v>
       </c>
-      <c r="P3" t="s">
-        <v>78</v>
-      </c>
       <c r="Q3">
-        <v>3102750</v>
+        <v>1300000</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -912,52 +921,52 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D4">
-        <v>80</v>
+        <v>442.659</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F4">
-        <v>80</v>
+        <v>442.659</v>
       </c>
       <c r="G4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M4">
-        <v>2000</v>
+        <v>10700</v>
       </c>
       <c r="N4">
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="P4" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="Q4">
-        <v>3000000</v>
+        <v>3102750</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -965,90 +974,90 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D5">
-        <v>4212</v>
+        <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F5">
-        <v>1263.6</v>
+        <v>80</v>
       </c>
       <c r="G5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="L5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M5">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="N5">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="P5" t="s">
-        <v>79</v>
+        <v>22</v>
       </c>
       <c r="Q5">
-        <v>87871545</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D6">
         <v>4212</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="F6">
         <v>1263.6</v>
       </c>
       <c r="G6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M6">
         <v>26000</v>
@@ -1057,10 +1066,10 @@
         <v>30</v>
       </c>
       <c r="O6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="P6" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="Q6">
         <v>87871545</v>
@@ -1068,13 +1077,13 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D7">
         <v>4212</v>
@@ -1083,37 +1092,37 @@
         <v>52</v>
       </c>
       <c r="F7">
-        <v>421.2</v>
+        <v>1263.6</v>
       </c>
       <c r="G7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M7">
         <v>26000</v>
       </c>
       <c r="N7">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="O7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="P7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="Q7">
         <v>87871545</v>
@@ -1121,40 +1130,40 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D8">
         <v>4212</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F8">
         <v>421.2</v>
       </c>
       <c r="G8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="L8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M8">
         <v>26000</v>
@@ -1163,10 +1172,10 @@
         <v>10</v>
       </c>
       <c r="O8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="P8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="Q8">
         <v>87871545</v>
@@ -1174,40 +1183,40 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D9">
         <v>4212</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F9">
         <v>421.2</v>
       </c>
       <c r="G9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K9" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="L9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M9">
         <v>26000</v>
@@ -1216,10 +1225,10 @@
         <v>10</v>
       </c>
       <c r="O9" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="P9" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="Q9">
         <v>87871545</v>
@@ -1227,52 +1236,52 @@
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D10">
         <v>4212</v>
       </c>
       <c r="E10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F10">
-        <v>126.36</v>
+        <v>421.2</v>
       </c>
       <c r="G10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M10">
         <v>26000</v>
       </c>
       <c r="N10">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="O10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="P10" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="Q10">
         <v>87871545</v>
@@ -1280,40 +1289,40 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D11">
         <v>4212</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F11">
         <v>126.36</v>
       </c>
       <c r="G11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K11" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="L11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M11">
         <v>26000</v>
@@ -1322,10 +1331,10 @@
         <v>3</v>
       </c>
       <c r="O11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="P11" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="Q11">
         <v>87871545</v>
@@ -1333,40 +1342,40 @@
     </row>
     <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D12">
         <v>4212</v>
       </c>
       <c r="E12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F12">
         <v>126.36</v>
       </c>
       <c r="G12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K12" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="L12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M12">
         <v>26000</v>
@@ -1375,10 +1384,10 @@
         <v>3</v>
       </c>
       <c r="O12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="P12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="Q12">
         <v>87871545</v>
@@ -1386,52 +1395,52 @@
     </row>
     <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D13">
         <v>4212</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="F13">
-        <v>42.12</v>
+        <v>126.36</v>
       </c>
       <c r="G13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="L13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M13">
         <v>26000</v>
       </c>
       <c r="N13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O13" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="P13" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="Q13">
         <v>87871545</v>
@@ -1442,105 +1451,105 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D14">
-        <v>360</v>
+        <v>4212</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F14">
-        <v>360</v>
+        <v>42.12</v>
       </c>
       <c r="G14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K14" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="L14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M14">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="N14">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="O14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="P14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Q14">
-        <v>13500000</v>
+        <v>87871545</v>
       </c>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D15">
-        <v>187.5</v>
+        <v>360</v>
       </c>
       <c r="E15" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="F15">
-        <v>187.5</v>
+        <v>360</v>
       </c>
       <c r="G15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M15">
-        <v>12500</v>
+        <v>2000</v>
       </c>
       <c r="N15">
         <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="P15" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="Q15">
-        <v>1020000</v>
+        <v>13500000</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1548,52 +1557,52 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D16">
-        <v>336</v>
+        <v>187.5</v>
       </c>
       <c r="E16" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F16">
-        <v>336</v>
+        <v>187.5</v>
       </c>
       <c r="G16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K16" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M16">
-        <v>15000</v>
+        <v>12500</v>
       </c>
       <c r="N16">
         <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="P16" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="Q16">
-        <v>1619200</v>
+        <v>1020000</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1601,102 +1610,102 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D17">
-        <v>221.2</v>
+        <v>336</v>
       </c>
       <c r="E17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F17">
-        <v>154.84</v>
+        <v>336</v>
       </c>
       <c r="G17" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H17" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I17" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J17" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L17" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M17">
-        <v>14000</v>
+        <v>15000</v>
       </c>
       <c r="N17">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="P17" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="Q17">
-        <v>2370000</v>
+        <v>1619200</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D18">
         <v>221.2</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F18">
-        <v>66.36</v>
+        <v>154.84</v>
       </c>
       <c r="G18" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H18" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I18" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J18" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L18" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M18">
         <v>14000</v>
       </c>
       <c r="N18">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="O18" t="s">
+        <v>75</v>
+      </c>
+      <c r="P18" t="s">
         <v>73</v>
-      </c>
-      <c r="P18" t="s">
-        <v>71</v>
       </c>
       <c r="Q18">
         <v>2370000</v>
@@ -1707,52 +1716,52 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D19">
-        <v>345</v>
+        <v>221.2</v>
       </c>
       <c r="E19" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="F19">
-        <v>345</v>
+        <v>66.36</v>
       </c>
       <c r="G19" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H19" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I19" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J19" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K19" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="L19" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M19">
-        <v>23000</v>
+        <v>14000</v>
       </c>
       <c r="N19">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="O19" t="s">
+        <v>75</v>
+      </c>
+      <c r="P19" t="s">
         <v>73</v>
       </c>
-      <c r="P19" t="s">
-        <v>71</v>
-      </c>
       <c r="Q19">
-        <v>1125000</v>
+        <v>2370000</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -1760,52 +1769,52 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D20">
-        <v>264</v>
+        <v>345</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F20">
-        <v>264</v>
+        <v>345</v>
       </c>
       <c r="G20" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H20" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I20" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J20" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K20" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L20" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M20">
-        <v>24000</v>
+        <v>23000</v>
       </c>
       <c r="N20">
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="P20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q20">
-        <v>825000</v>
+        <v>1125000</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1813,52 +1822,52 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D21">
-        <v>90</v>
+        <v>264</v>
       </c>
       <c r="E21" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F21">
-        <v>90</v>
+        <v>264</v>
       </c>
       <c r="G21" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H21" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I21" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J21" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K21" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L21" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M21">
-        <v>2000</v>
+        <v>24000</v>
       </c>
       <c r="N21">
         <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P21" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="Q21">
-        <v>3375000</v>
+        <v>825000</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1866,37 +1875,37 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D22">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F22">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G22" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H22" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I22" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J22" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K22" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L22" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M22">
         <v>2000</v>
@@ -1905,13 +1914,13 @@
         <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
       <c r="P22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q22">
-        <v>3562500</v>
+        <v>3375000</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1919,37 +1928,37 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D23">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="E23" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F23">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="G23" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H23" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I23" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J23" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K23" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L23" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M23">
         <v>2000</v>
@@ -1958,13 +1967,13 @@
         <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="P23" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="Q23">
-        <v>4875000</v>
+        <v>3562500</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -1972,37 +1981,37 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D24">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="E24" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="F24">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="G24" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H24" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I24" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J24" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K24" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L24" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M24">
         <v>2000</v>
@@ -2011,13 +2020,13 @@
         <v>100</v>
       </c>
       <c r="O24" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="P24" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="Q24">
-        <v>3750000</v>
+        <v>4875000</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -2025,37 +2034,37 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D25">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E25" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="F25">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="G25" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H25" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I25" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J25" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K25" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L25" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M25">
         <v>2000</v>
@@ -2064,51 +2073,51 @@
         <v>100</v>
       </c>
       <c r="O25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="P25" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="Q25">
-        <v>3000000</v>
+        <v>3750000</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C26" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D26">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="E26" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="F26">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="G26" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H26" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I26" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J26" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K26" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L26" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M26">
         <v>2000</v>
@@ -2117,12 +2126,65 @@
         <v>100</v>
       </c>
       <c r="O26" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="P26" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="Q26">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27">
+        <v>130</v>
+      </c>
+      <c r="E27" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27">
+        <v>130</v>
+      </c>
+      <c r="G27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H27" t="s">
+        <v>68</v>
+      </c>
+      <c r="I27" t="s">
+        <v>68</v>
+      </c>
+      <c r="J27" t="s">
+        <v>68</v>
+      </c>
+      <c r="K27" t="s">
+        <v>69</v>
+      </c>
+      <c r="L27" t="s">
+        <v>68</v>
+      </c>
+      <c r="M27">
+        <v>2000</v>
+      </c>
+      <c r="N27">
+        <v>100</v>
+      </c>
+      <c r="O27" t="s">
+        <v>79</v>
+      </c>
+      <c r="P27" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q27">
         <v>4875000</v>
       </c>
     </row>
@@ -2133,7 +2195,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2144,10 +2206,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -2156,757 +2218,757 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
       </c>
       <c r="F2">
-        <v>52000000</v>
+        <v>5390000</v>
       </c>
       <c r="G2">
-        <v>2000000</v>
+        <v>770000</v>
       </c>
       <c r="H2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I2">
-        <v>22000</v>
+        <v>8200</v>
       </c>
       <c r="J2">
-        <v>25000</v>
+        <v>9400</v>
       </c>
       <c r="K2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L2">
-        <v>26000</v>
+        <v>7000</v>
       </c>
       <c r="M2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="Q2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="R2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="S2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="T2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
         <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" t="s">
-        <v>78</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
       </c>
       <c r="F3">
-        <v>44265900</v>
+        <v>52000000</v>
       </c>
       <c r="G3">
-        <v>4137000</v>
+        <v>2000000</v>
       </c>
       <c r="H3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I3">
-        <v>8800</v>
+        <v>22000</v>
       </c>
       <c r="J3">
-        <v>10700</v>
+        <v>25000</v>
       </c>
       <c r="K3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L3">
-        <v>10700</v>
+        <v>26000</v>
       </c>
       <c r="M3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="O3">
-        <v>30.21513173797438</v>
+        <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="Q3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="R3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="S3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="T3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
       </c>
       <c r="F4">
-        <v>8000000</v>
+        <v>44265900</v>
       </c>
       <c r="G4">
-        <v>4000000</v>
+        <v>4137000</v>
       </c>
       <c r="H4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I4">
-        <v>2000</v>
+        <v>8800</v>
       </c>
       <c r="J4">
-        <v>2000</v>
+        <v>10700</v>
       </c>
       <c r="K4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L4">
-        <v>2000</v>
+        <v>10700</v>
       </c>
       <c r="M4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>30.21513173797438</v>
       </c>
       <c r="P4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="Q4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="R4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="S4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="T4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
       </c>
       <c r="F5">
-        <v>421200000</v>
+        <v>8000000</v>
       </c>
       <c r="G5">
-        <v>16200000</v>
+        <v>4000000</v>
       </c>
       <c r="H5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I5">
-        <v>21000</v>
+        <v>2000</v>
       </c>
       <c r="J5">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="K5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L5">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="M5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="Q5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="R5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="S5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="T5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>103</v>
       </c>
       <c r="D6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
       </c>
       <c r="F6">
-        <v>36000000</v>
+        <v>421200000</v>
       </c>
       <c r="G6">
-        <v>18000000</v>
+        <v>16200000</v>
       </c>
       <c r="H6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I6">
-        <v>2000</v>
+        <v>21000</v>
       </c>
       <c r="J6">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="K6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L6">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="M6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="Q6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="R6" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="S6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="T6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F7">
-        <v>18750000</v>
+        <v>36000000</v>
       </c>
       <c r="G7">
-        <v>1500000</v>
+        <v>18000000</v>
       </c>
       <c r="H7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I7">
-        <v>8900</v>
+        <v>2000</v>
       </c>
       <c r="J7">
-        <v>11000</v>
+        <v>2000</v>
       </c>
       <c r="K7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L7">
-        <v>12500</v>
+        <v>2000</v>
       </c>
       <c r="M7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="Q7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="R7" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="S7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="T7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E8" t="s">
         <v>22</v>
       </c>
       <c r="F8">
-        <v>33600000</v>
+        <v>18750000</v>
       </c>
       <c r="G8">
-        <v>2240000</v>
+        <v>1500000</v>
       </c>
       <c r="H8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I8">
-        <v>11500</v>
+        <v>8900</v>
       </c>
       <c r="J8">
-        <v>13200</v>
+        <v>11000</v>
       </c>
       <c r="K8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L8">
-        <v>15000</v>
+        <v>12500</v>
       </c>
       <c r="M8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="O8">
-        <v>26.78571428571428</v>
+        <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="Q8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="R8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="S8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="T8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D9" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="E9" t="s">
         <v>23</v>
       </c>
       <c r="F9">
-        <v>22120000</v>
+        <v>33600000</v>
       </c>
       <c r="G9">
-        <v>1580000</v>
+        <v>2240000</v>
       </c>
       <c r="H9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I9">
-        <v>10500</v>
+        <v>11500</v>
       </c>
       <c r="J9">
-        <v>12000</v>
+        <v>13200</v>
       </c>
       <c r="K9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L9">
-        <v>14000</v>
+        <v>15000</v>
       </c>
       <c r="M9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="O9">
-        <v>0</v>
+        <v>26.78571428571428</v>
       </c>
       <c r="P9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="Q9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="R9" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="S9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="T9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" t="s">
         <v>73</v>
-      </c>
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" t="s">
-        <v>71</v>
       </c>
       <c r="E10" t="s">
         <v>24</v>
       </c>
       <c r="F10">
-        <v>34500000</v>
+        <v>22120000</v>
       </c>
       <c r="G10">
-        <v>1500000</v>
+        <v>1580000</v>
       </c>
       <c r="H10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I10">
-        <v>20000</v>
+        <v>10500</v>
       </c>
       <c r="J10">
-        <v>23000</v>
+        <v>12000</v>
       </c>
       <c r="K10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L10">
-        <v>23000</v>
+        <v>14000</v>
       </c>
       <c r="M10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="Q10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="R10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="S10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="T10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E11" t="s">
         <v>25</v>
       </c>
       <c r="F11">
-        <v>26400000</v>
+        <v>34500000</v>
       </c>
       <c r="G11">
-        <v>1100000</v>
+        <v>1500000</v>
       </c>
       <c r="H11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I11">
         <v>20000</v>
       </c>
       <c r="J11">
-        <v>24000</v>
+        <v>23000</v>
       </c>
       <c r="K11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L11">
-        <v>24000</v>
+        <v>23000</v>
       </c>
       <c r="M11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="O11">
-        <v>18.18181818181818</v>
+        <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="Q11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="R11" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="S11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="T11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="E12" t="s">
         <v>26</v>
       </c>
       <c r="F12">
-        <v>9000000</v>
+        <v>26400000</v>
       </c>
       <c r="G12">
-        <v>4500000</v>
+        <v>1100000</v>
       </c>
       <c r="H12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I12">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="J12">
-        <v>2000</v>
+        <v>24000</v>
       </c>
       <c r="K12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L12">
-        <v>2000</v>
+        <v>24000</v>
       </c>
       <c r="M12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="O12">
-        <v>0</v>
+        <v>18.18181818181818</v>
       </c>
       <c r="P12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="Q12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="R12" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="S12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="T12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E13" t="s">
         <v>27</v>
       </c>
       <c r="F13">
-        <v>9500000</v>
+        <v>9000000</v>
       </c>
       <c r="G13">
-        <v>4750000</v>
+        <v>4500000</v>
       </c>
       <c r="H13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I13">
         <v>2000</v>
@@ -2915,60 +2977,60 @@
         <v>2000</v>
       </c>
       <c r="K13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L13">
         <v>2000</v>
       </c>
       <c r="M13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="Q13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="R13" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="S13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="T13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D14" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="E14" t="s">
         <v>28</v>
       </c>
       <c r="F14">
-        <v>13000000</v>
+        <v>9500000</v>
       </c>
       <c r="G14">
-        <v>6500000</v>
+        <v>4750000</v>
       </c>
       <c r="H14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I14">
         <v>2000</v>
@@ -2977,60 +3039,60 @@
         <v>2000</v>
       </c>
       <c r="K14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L14">
         <v>2000</v>
       </c>
       <c r="M14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="Q14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="R14" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="S14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="T14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D15" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E15" t="s">
         <v>29</v>
       </c>
       <c r="F15">
-        <v>10000000</v>
+        <v>13000000</v>
       </c>
       <c r="G15">
-        <v>5000000</v>
+        <v>6500000</v>
       </c>
       <c r="H15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I15">
         <v>2000</v>
@@ -3039,60 +3101,60 @@
         <v>2000</v>
       </c>
       <c r="K15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L15">
         <v>2000</v>
       </c>
       <c r="M15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="Q15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="R15" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="S15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="T15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E16" t="s">
         <v>30</v>
       </c>
       <c r="F16">
-        <v>8000000</v>
+        <v>10000000</v>
       </c>
       <c r="G16">
-        <v>4000000</v>
+        <v>5000000</v>
       </c>
       <c r="H16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I16">
         <v>2000</v>
@@ -3101,60 +3163,60 @@
         <v>2000</v>
       </c>
       <c r="K16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L16">
         <v>2000</v>
       </c>
       <c r="M16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="Q16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="R16" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="S16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="T16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F17">
-        <v>13000000</v>
+        <v>8000000</v>
       </c>
       <c r="G17">
-        <v>6500000</v>
+        <v>4000000</v>
       </c>
       <c r="H17" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I17">
         <v>2000</v>
@@ -3163,34 +3225,96 @@
         <v>2000</v>
       </c>
       <c r="K17" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L17">
         <v>2000</v>
       </c>
       <c r="M17" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N17" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="O17">
         <v>0</v>
       </c>
       <c r="P17" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="Q17" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="R17" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="S17" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="T17" t="s">
-        <v>66</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18">
+        <v>13000000</v>
+      </c>
+      <c r="G18">
+        <v>6500000</v>
+      </c>
+      <c r="H18" t="s">
+        <v>68</v>
+      </c>
+      <c r="I18">
+        <v>2000</v>
+      </c>
+      <c r="J18">
+        <v>2000</v>
+      </c>
+      <c r="K18" t="s">
+        <v>68</v>
+      </c>
+      <c r="L18">
+        <v>2000</v>
+      </c>
+      <c r="M18" t="s">
+        <v>68</v>
+      </c>
+      <c r="N18" t="s">
+        <v>68</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>68</v>
+      </c>
+      <c r="R18" t="s">
+        <v>120</v>
+      </c>
+      <c r="S18" t="s">
+        <v>68</v>
+      </c>
+      <c r="T18" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -3200,7 +3324,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3208,16 +3332,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -3229,10 +3353,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -3241,30 +3365,30 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2">
         <v>42120</v>
@@ -3284,101 +3408,101 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>103</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>124</v>
       </c>
       <c r="F3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G3" t="s">
         <v>21</v>
       </c>
       <c r="H3">
-        <v>18750</v>
+        <v>42120</v>
       </c>
       <c r="I3">
-        <v>1500000</v>
+        <v>16200000</v>
       </c>
       <c r="J3">
-        <v>12500</v>
+        <v>26000</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>101</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
-        <v>121</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H4">
-        <v>42120</v>
+        <v>18750</v>
       </c>
       <c r="I4">
-        <v>16200000</v>
+        <v>1500000</v>
       </c>
       <c r="J4">
-        <v>26000</v>
+        <v>12500</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E5" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H5">
         <v>42120</v>
@@ -3398,25 +3522,25 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H6">
         <v>13000</v>
@@ -3436,25 +3560,25 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H7">
         <v>13000</v>
@@ -3474,34 +3598,34 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F8" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H8">
-        <v>34500</v>
+        <v>52000</v>
       </c>
       <c r="I8">
-        <v>1500000</v>
+        <v>2000000</v>
       </c>
       <c r="J8">
-        <v>23000</v>
+        <v>26000</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -3512,34 +3636,34 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" t="s">
         <v>19</v>
       </c>
-      <c r="G9" t="s">
-        <v>17</v>
-      </c>
       <c r="H9">
-        <v>52000</v>
+        <v>44265.9</v>
       </c>
       <c r="I9">
-        <v>2000000</v>
+        <v>4137000</v>
       </c>
       <c r="J9">
-        <v>26000</v>
+        <v>10700</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -3550,101 +3674,101 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
       <c r="E10" t="s">
-        <v>49</v>
+        <v>124</v>
       </c>
       <c r="F10" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H10">
-        <v>44265.9</v>
+        <v>126360</v>
       </c>
       <c r="I10">
-        <v>4137000</v>
+        <v>16200000</v>
       </c>
       <c r="J10">
-        <v>10700</v>
+        <v>26000</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>101</v>
+        <v>52</v>
       </c>
       <c r="E11" t="s">
-        <v>121</v>
+        <v>52</v>
       </c>
       <c r="F11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G11" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H11">
-        <v>126360</v>
+        <v>34500</v>
       </c>
       <c r="I11">
-        <v>16200000</v>
+        <v>1500000</v>
       </c>
       <c r="J11">
-        <v>26000</v>
+        <v>23000</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F12" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H12">
         <v>33600</v>
@@ -3664,25 +3788,25 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" t="s">
         <v>28</v>
       </c>
-      <c r="C13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" t="s">
-        <v>63</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>27</v>
-      </c>
-      <c r="G13" t="s">
-        <v>26</v>
       </c>
       <c r="H13">
         <v>9000</v>
@@ -3702,101 +3826,101 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>101</v>
+        <v>59</v>
       </c>
       <c r="E14" t="s">
-        <v>121</v>
+        <v>59</v>
       </c>
       <c r="F14" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G14" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H14">
-        <v>12636</v>
+        <v>26400</v>
       </c>
       <c r="I14">
-        <v>16200000</v>
+        <v>1100000</v>
       </c>
       <c r="J14">
-        <v>26000</v>
+        <v>24000</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14">
-        <v>3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>103</v>
       </c>
       <c r="E15" t="s">
-        <v>56</v>
+        <v>124</v>
       </c>
       <c r="F15" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="G15" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H15">
-        <v>26400</v>
+        <v>12636</v>
       </c>
       <c r="I15">
-        <v>1100000</v>
+        <v>16200000</v>
       </c>
       <c r="J15">
-        <v>24000</v>
+        <v>26000</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15">
-        <v>100</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E16" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F16" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H16">
         <v>36000</v>
@@ -3816,25 +3940,25 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E17" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F17" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H17">
         <v>4212</v>
@@ -3854,101 +3978,101 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E18" t="s">
-        <v>61</v>
+        <v>125</v>
       </c>
       <c r="F18" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="G18" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H18">
-        <v>10000</v>
+        <v>15484</v>
       </c>
       <c r="I18">
-        <v>5000000</v>
+        <v>1580000</v>
       </c>
       <c r="J18">
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18">
-        <v>100</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E19" t="s">
-        <v>122</v>
+        <v>63</v>
       </c>
       <c r="F19" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="G19" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="H19">
-        <v>15484</v>
+        <v>10000</v>
       </c>
       <c r="I19">
-        <v>1580000</v>
+        <v>5000000</v>
       </c>
       <c r="J19">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="K19">
         <v>0</v>
       </c>
       <c r="L19">
-        <v>70</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" t="s">
+        <v>125</v>
+      </c>
+      <c r="F20" t="s">
         <v>73</v>
       </c>
-      <c r="C20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" t="s">
-        <v>122</v>
-      </c>
-      <c r="F20" t="s">
-        <v>71</v>
-      </c>
       <c r="G20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H20">
         <v>6636</v>
@@ -3968,25 +4092,25 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D21" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E21" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F21" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H21">
         <v>12636</v>
@@ -4006,25 +4130,25 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E22" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F22" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H22">
         <v>12636</v>
@@ -4047,104 +4171,104 @@
         <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="E23" t="s">
-        <v>121</v>
+        <v>51</v>
       </c>
       <c r="F23" t="s">
-        <v>79</v>
+        <v>20</v>
       </c>
       <c r="G23" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H23">
-        <v>126360</v>
+        <v>5390</v>
       </c>
       <c r="I23">
-        <v>16200000</v>
+        <v>770000</v>
       </c>
       <c r="J23">
-        <v>26000</v>
+        <v>7000</v>
       </c>
       <c r="K23">
         <v>0</v>
       </c>
       <c r="L23">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D24" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
       <c r="E24" t="s">
-        <v>51</v>
+        <v>124</v>
       </c>
       <c r="F24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G24" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="H24">
-        <v>8000</v>
+        <v>126360</v>
       </c>
       <c r="I24">
-        <v>4000000</v>
+        <v>16200000</v>
       </c>
       <c r="J24">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="K24">
         <v>0</v>
       </c>
       <c r="L24">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C25" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D25" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="E25" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="F25" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="G25" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="H25">
-        <v>9500</v>
+        <v>8000</v>
       </c>
       <c r="I25">
-        <v>4750000</v>
+        <v>4000000</v>
       </c>
       <c r="J25">
         <v>2000</v>
@@ -4158,31 +4282,31 @@
     </row>
     <row r="26" spans="1:12">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D26" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="E26" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="F26" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G26" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="H26">
-        <v>8000</v>
+        <v>9500</v>
       </c>
       <c r="I26">
-        <v>4000000</v>
+        <v>4750000</v>
       </c>
       <c r="J26">
         <v>2000</v>
@@ -4191,6 +4315,44 @@
         <v>0</v>
       </c>
       <c r="L26">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27">
+        <v>8000</v>
+      </c>
+      <c r="I27">
+        <v>4000000</v>
+      </c>
+      <c r="J27">
+        <v>2000</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2023-10-24
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="119">
   <si>
     <t>상장일</t>
   </si>
@@ -111,9 +111,6 @@
     <t>2023-09-01</t>
   </si>
   <si>
-    <t>2023-08-30</t>
-  </si>
-  <si>
     <t>에스엘에스바이오</t>
   </si>
   <si>
@@ -159,12 +156,6 @@
     <t>유안타제11호스팩</t>
   </si>
   <si>
-    <t>한국제12호스팩</t>
-  </si>
-  <si>
-    <t>대신밸런스제15호스팩</t>
-  </si>
-  <si>
     <t>코스닥</t>
   </si>
   <si>
@@ -255,9 +246,6 @@
     <t>2023-08-22</t>
   </si>
   <si>
-    <t>2023-08-21</t>
-  </si>
-  <si>
     <t>2023-10-11</t>
   </si>
   <si>
@@ -273,9 +261,6 @@
     <t>2023-08-25</t>
   </si>
   <si>
-    <t>2023-08-24</t>
-  </si>
-  <si>
     <t>회사명</t>
   </si>
   <si>
@@ -373,12 +358,6 @@
   </si>
   <si>
     <t>296.2 : 1</t>
-  </si>
-  <si>
-    <t>872.19 : 1</t>
-  </si>
-  <si>
-    <t>548.99 : 1</t>
   </si>
   <si>
     <t>인수기관</t>
@@ -751,7 +730,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -815,37 +794,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D2">
         <v>53.9</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F2">
         <v>53.9</v>
       </c>
       <c r="G2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M2">
         <v>7000</v>
@@ -868,37 +847,37 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D3">
         <v>520</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F3">
         <v>520</v>
       </c>
       <c r="G3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M3">
         <v>26000</v>
@@ -921,37 +900,37 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D4">
         <v>442.659</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F4">
         <v>442.659</v>
       </c>
       <c r="G4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M4">
         <v>10700</v>
@@ -963,7 +942,7 @@
         <v>21</v>
       </c>
       <c r="P4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="Q4">
         <v>3102750</v>
@@ -974,37 +953,37 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D5">
         <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F5">
         <v>80</v>
       </c>
       <c r="G5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M5">
         <v>2000</v>
@@ -1027,37 +1006,37 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D6">
         <v>4212</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F6">
         <v>1263.6</v>
       </c>
       <c r="G6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="L6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M6">
         <v>26000</v>
@@ -1066,10 +1045,10 @@
         <v>30</v>
       </c>
       <c r="O6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="P6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="Q6">
         <v>87871545</v>
@@ -1080,37 +1059,37 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D7">
         <v>4212</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F7">
         <v>1263.6</v>
       </c>
       <c r="G7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="L7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M7">
         <v>26000</v>
@@ -1119,10 +1098,10 @@
         <v>30</v>
       </c>
       <c r="O7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="P7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="Q7">
         <v>87871545</v>
@@ -1133,37 +1112,37 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D8">
         <v>4212</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F8">
         <v>421.2</v>
       </c>
       <c r="G8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I8" t="s">
+        <v>65</v>
+      </c>
+      <c r="J8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K8" t="s">
         <v>68</v>
       </c>
-      <c r="H8" t="s">
-        <v>68</v>
-      </c>
-      <c r="I8" t="s">
-        <v>68</v>
-      </c>
-      <c r="J8" t="s">
-        <v>68</v>
-      </c>
-      <c r="K8" t="s">
-        <v>71</v>
-      </c>
       <c r="L8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M8">
         <v>26000</v>
@@ -1172,10 +1151,10 @@
         <v>10</v>
       </c>
       <c r="O8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="P8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="Q8">
         <v>87871545</v>
@@ -1186,37 +1165,37 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D9">
         <v>4212</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F9">
         <v>421.2</v>
       </c>
       <c r="G9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J9" t="s">
+        <v>65</v>
+      </c>
+      <c r="K9" t="s">
         <v>68</v>
       </c>
-      <c r="H9" t="s">
-        <v>68</v>
-      </c>
-      <c r="I9" t="s">
-        <v>68</v>
-      </c>
-      <c r="J9" t="s">
-        <v>68</v>
-      </c>
-      <c r="K9" t="s">
-        <v>71</v>
-      </c>
       <c r="L9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M9">
         <v>26000</v>
@@ -1225,10 +1204,10 @@
         <v>10</v>
       </c>
       <c r="O9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="P9" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="Q9">
         <v>87871545</v>
@@ -1239,37 +1218,37 @@
         <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D10">
         <v>4212</v>
       </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F10">
         <v>421.2</v>
       </c>
       <c r="G10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I10" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K10" t="s">
         <v>68</v>
       </c>
-      <c r="H10" t="s">
-        <v>68</v>
-      </c>
-      <c r="I10" t="s">
-        <v>68</v>
-      </c>
-      <c r="J10" t="s">
-        <v>68</v>
-      </c>
-      <c r="K10" t="s">
-        <v>71</v>
-      </c>
       <c r="L10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M10">
         <v>26000</v>
@@ -1278,10 +1257,10 @@
         <v>10</v>
       </c>
       <c r="O10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="P10" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="Q10">
         <v>87871545</v>
@@ -1292,37 +1271,37 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D11">
         <v>4212</v>
       </c>
       <c r="E11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F11">
         <v>126.36</v>
       </c>
       <c r="G11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M11">
         <v>26000</v>
@@ -1331,10 +1310,10 @@
         <v>3</v>
       </c>
       <c r="O11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="P11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="Q11">
         <v>87871545</v>
@@ -1345,37 +1324,37 @@
         <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D12">
         <v>4212</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F12">
         <v>126.36</v>
       </c>
       <c r="G12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M12">
         <v>26000</v>
@@ -1384,10 +1363,10 @@
         <v>3</v>
       </c>
       <c r="O12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="P12" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="Q12">
         <v>87871545</v>
@@ -1398,37 +1377,37 @@
         <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D13">
         <v>4212</v>
       </c>
       <c r="E13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F13">
         <v>126.36</v>
       </c>
       <c r="G13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M13">
         <v>26000</v>
@@ -1437,10 +1416,10 @@
         <v>3</v>
       </c>
       <c r="O13" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="P13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="Q13">
         <v>87871545</v>
@@ -1451,37 +1430,37 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D14">
         <v>4212</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F14">
         <v>42.12</v>
       </c>
       <c r="G14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M14">
         <v>26000</v>
@@ -1490,10 +1469,10 @@
         <v>1</v>
       </c>
       <c r="O14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="P14" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="Q14">
         <v>87871545</v>
@@ -1504,37 +1483,37 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D15">
         <v>360</v>
       </c>
       <c r="E15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F15">
         <v>360</v>
       </c>
       <c r="G15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M15">
         <v>2000</v>
@@ -1543,10 +1522,10 @@
         <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="P15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="Q15">
         <v>13500000</v>
@@ -1557,37 +1536,37 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D16">
         <v>187.5</v>
       </c>
       <c r="E16" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F16">
         <v>187.5</v>
       </c>
       <c r="G16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M16">
         <v>12500</v>
@@ -1596,10 +1575,10 @@
         <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="P16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="Q16">
         <v>1020000</v>
@@ -1610,37 +1589,37 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D17">
         <v>336</v>
       </c>
       <c r="E17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F17">
         <v>336</v>
       </c>
       <c r="G17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M17">
         <v>15000</v>
@@ -1649,10 +1628,10 @@
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="P17" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="Q17">
         <v>1619200</v>
@@ -1663,37 +1642,37 @@
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D18">
         <v>221.2</v>
       </c>
       <c r="E18" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F18">
         <v>154.84</v>
       </c>
       <c r="G18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K18" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M18">
         <v>14000</v>
@@ -1702,10 +1681,10 @@
         <v>70</v>
       </c>
       <c r="O18" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="P18" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="Q18">
         <v>2370000</v>
@@ -1716,37 +1695,37 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D19">
         <v>221.2</v>
       </c>
       <c r="E19" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F19">
         <v>66.36</v>
       </c>
       <c r="G19" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H19" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I19" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J19" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L19" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M19">
         <v>14000</v>
@@ -1755,10 +1734,10 @@
         <v>30</v>
       </c>
       <c r="O19" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="P19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="Q19">
         <v>2370000</v>
@@ -1769,37 +1748,37 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D20">
         <v>345</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F20">
         <v>345</v>
       </c>
       <c r="G20" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H20" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I20" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J20" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K20" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L20" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M20">
         <v>23000</v>
@@ -1808,10 +1787,10 @@
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="P20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="Q20">
         <v>1125000</v>
@@ -1822,37 +1801,37 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D21">
         <v>264</v>
       </c>
       <c r="E21" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F21">
         <v>264</v>
       </c>
       <c r="G21" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H21" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I21" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J21" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K21" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L21" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M21">
         <v>24000</v>
@@ -1864,7 +1843,7 @@
         <v>27</v>
       </c>
       <c r="P21" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="Q21">
         <v>825000</v>
@@ -1875,37 +1854,37 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D22">
         <v>90</v>
       </c>
       <c r="E22" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F22">
         <v>90</v>
       </c>
       <c r="G22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K22" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M22">
         <v>2000</v>
@@ -1928,37 +1907,37 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D23">
         <v>95</v>
       </c>
       <c r="E23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F23">
         <v>95</v>
       </c>
       <c r="G23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K23" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M23">
         <v>2000</v>
@@ -1967,7 +1946,7 @@
         <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P23" t="s">
         <v>30</v>
@@ -1981,37 +1960,37 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D24">
         <v>130</v>
       </c>
       <c r="E24" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F24">
         <v>130</v>
       </c>
       <c r="G24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K24" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M24">
         <v>2000</v>
@@ -2020,10 +1999,10 @@
         <v>100</v>
       </c>
       <c r="O24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P24" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="Q24">
         <v>4875000</v>
@@ -2034,37 +2013,37 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" t="s">
         <v>46</v>
-      </c>
-      <c r="C25" t="s">
-        <v>49</v>
       </c>
       <c r="D25">
         <v>100</v>
       </c>
       <c r="E25" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F25">
         <v>100</v>
       </c>
       <c r="G25" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H25" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I25" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J25" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K25" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L25" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M25">
         <v>2000</v>
@@ -2073,119 +2052,13 @@
         <v>100</v>
       </c>
       <c r="O25" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="P25" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="Q25">
         <v>3750000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17">
-      <c r="A26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26">
-        <v>80</v>
-      </c>
-      <c r="E26" t="s">
-        <v>54</v>
-      </c>
-      <c r="F26">
-        <v>80</v>
-      </c>
-      <c r="G26" t="s">
-        <v>68</v>
-      </c>
-      <c r="H26" t="s">
-        <v>68</v>
-      </c>
-      <c r="I26" t="s">
-        <v>68</v>
-      </c>
-      <c r="J26" t="s">
-        <v>68</v>
-      </c>
-      <c r="K26" t="s">
-        <v>69</v>
-      </c>
-      <c r="L26" t="s">
-        <v>68</v>
-      </c>
-      <c r="M26">
-        <v>2000</v>
-      </c>
-      <c r="N26">
-        <v>100</v>
-      </c>
-      <c r="O26" t="s">
-        <v>79</v>
-      </c>
-      <c r="P26" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q26">
-        <v>3000000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17">
-      <c r="A27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" t="s">
-        <v>49</v>
-      </c>
-      <c r="D27">
-        <v>130</v>
-      </c>
-      <c r="E27" t="s">
-        <v>67</v>
-      </c>
-      <c r="F27">
-        <v>130</v>
-      </c>
-      <c r="G27" t="s">
-        <v>68</v>
-      </c>
-      <c r="H27" t="s">
-        <v>68</v>
-      </c>
-      <c r="I27" t="s">
-        <v>68</v>
-      </c>
-      <c r="J27" t="s">
-        <v>68</v>
-      </c>
-      <c r="K27" t="s">
-        <v>69</v>
-      </c>
-      <c r="L27" t="s">
-        <v>68</v>
-      </c>
-      <c r="M27">
-        <v>2000</v>
-      </c>
-      <c r="N27">
-        <v>100</v>
-      </c>
-      <c r="O27" t="s">
-        <v>79</v>
-      </c>
-      <c r="P27" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q27">
-        <v>4875000</v>
       </c>
     </row>
   </sheetData>
@@ -2195,7 +2068,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T18"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2206,10 +2079,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -2218,49 +2091,49 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -2268,10 +2141,10 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>
@@ -2286,7 +2159,7 @@
         <v>770000</v>
       </c>
       <c r="H2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I2">
         <v>8200</v>
@@ -2295,34 +2168,34 @@
         <v>9400</v>
       </c>
       <c r="K2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L2">
         <v>7000</v>
       </c>
       <c r="M2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="N2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="Q2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="R2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="S2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="T2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -2330,10 +2203,10 @@
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
@@ -2348,7 +2221,7 @@
         <v>2000000</v>
       </c>
       <c r="H3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I3">
         <v>22000</v>
@@ -2357,34 +2230,34 @@
         <v>25000</v>
       </c>
       <c r="K3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L3">
         <v>26000</v>
       </c>
       <c r="M3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="N3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="Q3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="R3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="S3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="T3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -2392,13 +2265,13 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
@@ -2410,7 +2283,7 @@
         <v>4137000</v>
       </c>
       <c r="H4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I4">
         <v>8800</v>
@@ -2419,34 +2292,34 @@
         <v>10700</v>
       </c>
       <c r="K4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L4">
         <v>10700</v>
       </c>
       <c r="M4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="N4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="O4">
         <v>30.21513173797438</v>
       </c>
       <c r="P4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="Q4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="R4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="S4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="T4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -2454,10 +2327,10 @@
         <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
         <v>22</v>
@@ -2472,7 +2345,7 @@
         <v>4000000</v>
       </c>
       <c r="H5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I5">
         <v>2000</v>
@@ -2481,48 +2354,48 @@
         <v>2000</v>
       </c>
       <c r="K5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L5">
         <v>2000</v>
       </c>
       <c r="M5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="N5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="Q5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="R5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="S5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="T5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
@@ -2534,7 +2407,7 @@
         <v>16200000</v>
       </c>
       <c r="H6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I6">
         <v>21000</v>
@@ -2543,48 +2416,48 @@
         <v>26000</v>
       </c>
       <c r="K6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L6">
         <v>26000</v>
       </c>
       <c r="M6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="N6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="Q6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="R6" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="S6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="T6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E7" t="s">
         <v>22</v>
@@ -2596,7 +2469,7 @@
         <v>18000000</v>
       </c>
       <c r="H7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I7">
         <v>2000</v>
@@ -2605,48 +2478,48 @@
         <v>2000</v>
       </c>
       <c r="K7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L7">
         <v>2000</v>
       </c>
       <c r="M7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="N7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="Q7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="R7" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="S7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="T7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E8" t="s">
         <v>22</v>
@@ -2658,7 +2531,7 @@
         <v>1500000</v>
       </c>
       <c r="H8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I8">
         <v>8900</v>
@@ -2667,48 +2540,48 @@
         <v>11000</v>
       </c>
       <c r="K8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L8">
         <v>12500</v>
       </c>
       <c r="M8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="N8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="Q8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="R8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="S8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="T8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E9" t="s">
         <v>23</v>
@@ -2720,7 +2593,7 @@
         <v>2240000</v>
       </c>
       <c r="H9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I9">
         <v>11500</v>
@@ -2729,48 +2602,48 @@
         <v>13200</v>
       </c>
       <c r="K9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L9">
         <v>15000</v>
       </c>
       <c r="M9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="N9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="O9">
         <v>26.78571428571428</v>
       </c>
       <c r="P9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="Q9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="R9" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="S9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="T9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E10" t="s">
         <v>24</v>
@@ -2782,7 +2655,7 @@
         <v>1580000</v>
       </c>
       <c r="H10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I10">
         <v>10500</v>
@@ -2791,48 +2664,48 @@
         <v>12000</v>
       </c>
       <c r="K10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L10">
         <v>14000</v>
       </c>
       <c r="M10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="N10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="Q10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="R10" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="S10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="T10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E11" t="s">
         <v>25</v>
@@ -2844,7 +2717,7 @@
         <v>1500000</v>
       </c>
       <c r="H11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I11">
         <v>20000</v>
@@ -2853,34 +2726,34 @@
         <v>23000</v>
       </c>
       <c r="K11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L11">
         <v>23000</v>
       </c>
       <c r="M11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="N11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="Q11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="R11" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="S11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="T11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -2888,13 +2761,13 @@
         <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E12" t="s">
         <v>26</v>
@@ -2906,7 +2779,7 @@
         <v>1100000</v>
       </c>
       <c r="H12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I12">
         <v>20000</v>
@@ -2915,34 +2788,34 @@
         <v>24000</v>
       </c>
       <c r="K12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L12">
         <v>24000</v>
       </c>
       <c r="M12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="N12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="O12">
         <v>18.18181818181818</v>
       </c>
       <c r="P12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="Q12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="R12" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="S12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="T12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -2950,10 +2823,10 @@
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D13" t="s">
         <v>28</v>
@@ -2968,7 +2841,7 @@
         <v>4500000</v>
       </c>
       <c r="H13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I13">
         <v>2000</v>
@@ -2977,45 +2850,45 @@
         <v>2000</v>
       </c>
       <c r="K13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L13">
         <v>2000</v>
       </c>
       <c r="M13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="N13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="Q13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="R13" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="S13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="T13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D14" t="s">
         <v>30</v>
@@ -3030,7 +2903,7 @@
         <v>4750000</v>
       </c>
       <c r="H14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I14">
         <v>2000</v>
@@ -3039,48 +2912,48 @@
         <v>2000</v>
       </c>
       <c r="K14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L14">
         <v>2000</v>
       </c>
       <c r="M14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="N14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="Q14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="R14" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="S14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="T14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D15" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E15" t="s">
         <v>29</v>
@@ -3092,7 +2965,7 @@
         <v>6500000</v>
       </c>
       <c r="H15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I15">
         <v>2000</v>
@@ -3101,48 +2974,48 @@
         <v>2000</v>
       </c>
       <c r="K15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L15">
         <v>2000</v>
       </c>
       <c r="M15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="N15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="Q15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="R15" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="S15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="T15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D16" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E16" t="s">
         <v>30</v>
@@ -3154,7 +3027,7 @@
         <v>5000000</v>
       </c>
       <c r="H16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I16">
         <v>2000</v>
@@ -3163,158 +3036,34 @@
         <v>2000</v>
       </c>
       <c r="K16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L16">
         <v>2000</v>
       </c>
       <c r="M16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="N16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="Q16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="R16" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="S16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="T16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20">
-      <c r="A17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" t="s">
-        <v>85</v>
-      </c>
-      <c r="E17" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17">
-        <v>8000000</v>
-      </c>
-      <c r="G17">
-        <v>4000000</v>
-      </c>
-      <c r="H17" t="s">
-        <v>68</v>
-      </c>
-      <c r="I17">
-        <v>2000</v>
-      </c>
-      <c r="J17">
-        <v>2000</v>
-      </c>
-      <c r="K17" t="s">
-        <v>68</v>
-      </c>
-      <c r="L17">
-        <v>2000</v>
-      </c>
-      <c r="M17" t="s">
-        <v>68</v>
-      </c>
-      <c r="N17" t="s">
-        <v>68</v>
-      </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>68</v>
-      </c>
-      <c r="R17" t="s">
-        <v>119</v>
-      </c>
-      <c r="S17" t="s">
-        <v>68</v>
-      </c>
-      <c r="T17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20">
-      <c r="A18" t="s">
-        <v>79</v>
-      </c>
-      <c r="B18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" t="s">
-        <v>85</v>
-      </c>
-      <c r="E18" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18">
-        <v>13000000</v>
-      </c>
-      <c r="G18">
-        <v>6500000</v>
-      </c>
-      <c r="H18" t="s">
-        <v>68</v>
-      </c>
-      <c r="I18">
-        <v>2000</v>
-      </c>
-      <c r="J18">
-        <v>2000</v>
-      </c>
-      <c r="K18" t="s">
-        <v>68</v>
-      </c>
-      <c r="L18">
-        <v>2000</v>
-      </c>
-      <c r="M18" t="s">
-        <v>68</v>
-      </c>
-      <c r="N18" t="s">
-        <v>68</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>68</v>
-      </c>
-      <c r="R18" t="s">
-        <v>120</v>
-      </c>
-      <c r="S18" t="s">
-        <v>68</v>
-      </c>
-      <c r="T18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -3324,7 +3073,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3332,16 +3081,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -3353,10 +3102,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -3365,27 +3114,27 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E2" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s">
         <v>21</v>
@@ -3408,22 +3157,22 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E3" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G3" t="s">
         <v>21</v>
@@ -3446,22 +3195,22 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G4" t="s">
         <v>22</v>
@@ -3484,22 +3233,22 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E5" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G5" t="s">
         <v>21</v>
@@ -3522,25 +3271,25 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" t="s">
         <v>79</v>
       </c>
-      <c r="C6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6" t="s">
-        <v>85</v>
-      </c>
       <c r="G6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H6">
         <v>13000</v>
@@ -3560,34 +3309,34 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="E7" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="F7" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="G7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H7">
-        <v>13000</v>
+        <v>34500</v>
       </c>
       <c r="I7">
-        <v>6500000</v>
+        <v>1500000</v>
       </c>
       <c r="J7">
-        <v>2000</v>
+        <v>23000</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -3598,19 +3347,19 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
         <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F8" t="s">
         <v>20</v>
@@ -3636,22 +3385,22 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F9" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G9" t="s">
         <v>19</v>
@@ -3674,22 +3423,22 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E10" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F10" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G10" t="s">
         <v>21</v>
@@ -3712,34 +3461,34 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="F11" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="G11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H11">
-        <v>34500</v>
+        <v>33600</v>
       </c>
       <c r="I11">
-        <v>1500000</v>
+        <v>2240000</v>
       </c>
       <c r="J11">
-        <v>23000</v>
+        <v>15000</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -3753,10 +3502,10 @@
         <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
         <v>62</v>
@@ -3765,19 +3514,19 @@
         <v>62</v>
       </c>
       <c r="F12" t="s">
-        <v>82</v>
+        <v>28</v>
       </c>
       <c r="G12" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H12">
-        <v>33600</v>
+        <v>9000</v>
       </c>
       <c r="I12">
-        <v>2240000</v>
+        <v>4500000</v>
       </c>
       <c r="J12">
-        <v>15000</v>
+        <v>2000</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -3788,34 +3537,34 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E13" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="F13" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="G13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H13">
-        <v>9000</v>
+        <v>26400</v>
       </c>
       <c r="I13">
-        <v>4500000</v>
+        <v>1100000</v>
       </c>
       <c r="J13">
-        <v>2000</v>
+        <v>24000</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -3826,116 +3575,116 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>117</v>
       </c>
       <c r="F14" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G14" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="H14">
-        <v>26400</v>
+        <v>12636</v>
       </c>
       <c r="I14">
-        <v>1100000</v>
+        <v>16200000</v>
       </c>
       <c r="J14">
-        <v>24000</v>
+        <v>26000</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14">
-        <v>100</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C15" t="s">
         <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>103</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
-        <v>124</v>
+        <v>58</v>
       </c>
       <c r="F15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H15">
-        <v>12636</v>
+        <v>36000</v>
       </c>
       <c r="I15">
-        <v>16200000</v>
+        <v>18000000</v>
       </c>
       <c r="J15">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15">
-        <v>3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
+        <v>98</v>
       </c>
       <c r="E16" t="s">
-        <v>61</v>
+        <v>117</v>
       </c>
       <c r="F16" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H16">
-        <v>36000</v>
+        <v>4212</v>
       </c>
       <c r="I16">
-        <v>18000000</v>
+        <v>16200000</v>
       </c>
       <c r="J16">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -3943,209 +3692,209 @@
         <v>60</v>
       </c>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="E17" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F17" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="G17" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H17">
-        <v>4212</v>
+        <v>15484</v>
       </c>
       <c r="I17">
-        <v>16200000</v>
+        <v>1580000</v>
       </c>
       <c r="J17">
-        <v>26000</v>
+        <v>14000</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
-        <v>1</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s">
         <v>75</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D18" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E18" t="s">
-        <v>125</v>
+        <v>60</v>
       </c>
       <c r="F18" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="G18" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H18">
-        <v>15484</v>
+        <v>10000</v>
       </c>
       <c r="I18">
-        <v>1580000</v>
+        <v>5000000</v>
       </c>
       <c r="J18">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18">
-        <v>70</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E19" t="s">
-        <v>63</v>
+        <v>118</v>
       </c>
       <c r="F19" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="G19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H19">
-        <v>10000</v>
+        <v>6636</v>
       </c>
       <c r="I19">
-        <v>5000000</v>
+        <v>1580000</v>
       </c>
       <c r="J19">
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="K19">
         <v>0</v>
       </c>
       <c r="L19">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="E20" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="F20" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G20" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H20">
-        <v>6636</v>
+        <v>12636</v>
       </c>
       <c r="I20">
-        <v>1580000</v>
+        <v>16200000</v>
       </c>
       <c r="J20">
-        <v>14000</v>
+        <v>26000</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
       <c r="L20">
-        <v>30</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>103</v>
+        <v>48</v>
       </c>
       <c r="E21" t="s">
-        <v>124</v>
+        <v>48</v>
       </c>
       <c r="F21" t="s">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="G21" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H21">
-        <v>12636</v>
+        <v>5390</v>
       </c>
       <c r="I21">
-        <v>16200000</v>
+        <v>770000</v>
       </c>
       <c r="J21">
-        <v>26000</v>
+        <v>7000</v>
       </c>
       <c r="K21">
         <v>0</v>
       </c>
       <c r="L21">
-        <v>3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D22" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E22" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F22" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G22" t="s">
         <v>21</v>
@@ -4171,98 +3920,98 @@
         <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D23" t="s">
-        <v>51</v>
+        <v>98</v>
       </c>
       <c r="E23" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="F23" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="G23" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H23">
-        <v>5390</v>
+        <v>126360</v>
       </c>
       <c r="I23">
-        <v>770000</v>
+        <v>16200000</v>
       </c>
       <c r="J23">
-        <v>7000</v>
+        <v>26000</v>
       </c>
       <c r="K23">
         <v>0</v>
       </c>
       <c r="L23">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B24" t="s">
         <v>73</v>
       </c>
       <c r="C24" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D24" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="E24" t="s">
-        <v>124</v>
+        <v>63</v>
       </c>
       <c r="F24" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="G24" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="H24">
-        <v>126360</v>
+        <v>9500</v>
       </c>
       <c r="I24">
-        <v>16200000</v>
+        <v>4750000</v>
       </c>
       <c r="J24">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="K24">
         <v>0</v>
       </c>
       <c r="L24">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
-        <v>79</v>
+        <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F25" t="s">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="G25" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="H25">
         <v>8000</v>
@@ -4277,82 +4026,6 @@
         <v>0</v>
       </c>
       <c r="L25">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" t="s">
-        <v>66</v>
-      </c>
-      <c r="B26" t="s">
-        <v>76</v>
-      </c>
-      <c r="C26" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" t="s">
-        <v>66</v>
-      </c>
-      <c r="E26" t="s">
-        <v>66</v>
-      </c>
-      <c r="F26" t="s">
-        <v>30</v>
-      </c>
-      <c r="G26" t="s">
-        <v>28</v>
-      </c>
-      <c r="H26">
-        <v>9500</v>
-      </c>
-      <c r="I26">
-        <v>4750000</v>
-      </c>
-      <c r="J26">
-        <v>2000</v>
-      </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-      <c r="L26">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27" t="s">
-        <v>53</v>
-      </c>
-      <c r="E27" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" t="s">
-        <v>22</v>
-      </c>
-      <c r="G27" t="s">
-        <v>20</v>
-      </c>
-      <c r="H27">
-        <v>8000</v>
-      </c>
-      <c r="I27">
-        <v>4000000</v>
-      </c>
-      <c r="J27">
-        <v>2000</v>
-      </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-      <c r="L27">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2023-10-25
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="115">
   <si>
     <t>상장일</t>
   </si>
@@ -108,159 +108,150 @@
     <t>2023-09-04</t>
   </si>
   <si>
+    <t>에스엘에스바이오</t>
+  </si>
+  <si>
+    <t>신성에스티</t>
+  </si>
+  <si>
+    <t>퓨릿</t>
+  </si>
+  <si>
+    <t>에이치엠씨제6호스팩</t>
+  </si>
+  <si>
+    <t>두산로보틱스</t>
+  </si>
+  <si>
+    <t>신한제11호스팩</t>
+  </si>
+  <si>
+    <t>한싹</t>
+  </si>
+  <si>
+    <t>레뷰코퍼레이션</t>
+  </si>
+  <si>
+    <t>아이엠티</t>
+  </si>
+  <si>
+    <t>밀리의서재</t>
+  </si>
+  <si>
+    <t>인스웨이브시스템즈</t>
+  </si>
+  <si>
+    <t>상상인제4호스팩</t>
+  </si>
+  <si>
+    <t>한화플러스제4호스팩</t>
+  </si>
+  <si>
+    <t>대신밸런스제16호스팩</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>코스피</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>현대차</t>
+  </si>
+  <si>
+    <t>한국</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>키움</t>
+  </si>
+  <si>
+    <t>신영</t>
+  </si>
+  <si>
+    <t>유비에스</t>
+  </si>
+  <si>
+    <t>신한</t>
+  </si>
+  <si>
+    <t>삼성</t>
+  </si>
+  <si>
+    <t>유안타</t>
+  </si>
+  <si>
+    <t>유진</t>
+  </si>
+  <si>
+    <t>상상인</t>
+  </si>
+  <si>
+    <t>한화</t>
+  </si>
+  <si>
+    <t>대신</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>공동대표</t>
+  </si>
+  <si>
+    <t>공동</t>
+  </si>
+  <si>
+    <t>인수</t>
+  </si>
+  <si>
+    <t>2023-09-21</t>
+  </si>
+  <si>
+    <t>2023-09-19</t>
+  </si>
+  <si>
+    <t>2023-09-18</t>
+  </si>
+  <si>
+    <t>2023-08-29</t>
+  </si>
+  <si>
+    <t>2023-08-23</t>
+  </si>
+  <si>
+    <t>2023-10-11</t>
+  </si>
+  <si>
+    <t>2023-09-26</t>
+  </si>
+  <si>
+    <t>2023-09-22</t>
+  </si>
+  <si>
     <t>2023-09-01</t>
   </si>
   <si>
-    <t>에스엘에스바이오</t>
-  </si>
-  <si>
-    <t>신성에스티</t>
-  </si>
-  <si>
-    <t>퓨릿</t>
-  </si>
-  <si>
-    <t>에이치엠씨제6호스팩</t>
-  </si>
-  <si>
-    <t>두산로보틱스</t>
-  </si>
-  <si>
-    <t>신한제11호스팩</t>
-  </si>
-  <si>
-    <t>한싹</t>
-  </si>
-  <si>
-    <t>레뷰코퍼레이션</t>
-  </si>
-  <si>
-    <t>아이엠티</t>
-  </si>
-  <si>
-    <t>밀리의서재</t>
-  </si>
-  <si>
-    <t>인스웨이브시스템즈</t>
-  </si>
-  <si>
-    <t>상상인제4호스팩</t>
-  </si>
-  <si>
-    <t>한화플러스제4호스팩</t>
-  </si>
-  <si>
-    <t>대신밸런스제16호스팩</t>
-  </si>
-  <si>
-    <t>유안타제11호스팩</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>코스피</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>현대차</t>
-  </si>
-  <si>
-    <t>한국</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>KB</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t>키움</t>
-  </si>
-  <si>
-    <t>신영</t>
-  </si>
-  <si>
-    <t>유비에스</t>
-  </si>
-  <si>
-    <t>신한</t>
-  </si>
-  <si>
-    <t>삼성</t>
-  </si>
-  <si>
-    <t>유안타</t>
-  </si>
-  <si>
-    <t>유진</t>
-  </si>
-  <si>
-    <t>상상인</t>
-  </si>
-  <si>
-    <t>한화</t>
-  </si>
-  <si>
-    <t>대신</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>공동대표</t>
-  </si>
-  <si>
-    <t>공동</t>
-  </si>
-  <si>
-    <t>인수</t>
-  </si>
-  <si>
-    <t>2023-09-21</t>
-  </si>
-  <si>
-    <t>2023-09-19</t>
-  </si>
-  <si>
-    <t>2023-09-18</t>
-  </si>
-  <si>
-    <t>2023-08-29</t>
-  </si>
-  <si>
-    <t>2023-08-23</t>
-  </si>
-  <si>
-    <t>2023-08-22</t>
-  </si>
-  <si>
-    <t>2023-10-11</t>
-  </si>
-  <si>
-    <t>2023-09-26</t>
-  </si>
-  <si>
-    <t>2023-09-22</t>
-  </si>
-  <si>
     <t>2023-08-28</t>
   </si>
   <si>
-    <t>2023-08-25</t>
-  </si>
-  <si>
     <t>회사명</t>
   </si>
   <si>
@@ -355,9 +346,6 @@
   </si>
   <si>
     <t>527.68 : 1</t>
-  </si>
-  <si>
-    <t>296.2 : 1</t>
   </si>
   <si>
     <t>인수기관</t>
@@ -730,7 +718,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -794,37 +782,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D2">
         <v>53.9</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F2">
         <v>53.9</v>
       </c>
       <c r="G2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M2">
         <v>7000</v>
@@ -847,37 +835,37 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3">
         <v>520</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F3">
         <v>520</v>
       </c>
       <c r="G3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M3">
         <v>26000</v>
@@ -900,37 +888,37 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D4">
         <v>442.659</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F4">
         <v>442.659</v>
       </c>
       <c r="G4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M4">
         <v>10700</v>
@@ -942,7 +930,7 @@
         <v>21</v>
       </c>
       <c r="P4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="Q4">
         <v>3102750</v>
@@ -953,37 +941,37 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5">
         <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F5">
         <v>80</v>
       </c>
       <c r="G5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M5">
         <v>2000</v>
@@ -1006,37 +994,37 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D6">
         <v>4212</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F6">
         <v>1263.6</v>
       </c>
       <c r="G6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" t="s">
         <v>65</v>
       </c>
-      <c r="H6" t="s">
-        <v>65</v>
-      </c>
-      <c r="I6" t="s">
-        <v>65</v>
-      </c>
-      <c r="J6" t="s">
-        <v>65</v>
-      </c>
-      <c r="K6" t="s">
-        <v>67</v>
-      </c>
       <c r="L6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M6">
         <v>26000</v>
@@ -1045,10 +1033,10 @@
         <v>30</v>
       </c>
       <c r="O6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Q6">
         <v>87871545</v>
@@ -1059,37 +1047,37 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D7">
         <v>4212</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F7">
         <v>1263.6</v>
       </c>
       <c r="G7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" t="s">
         <v>65</v>
       </c>
-      <c r="H7" t="s">
-        <v>65</v>
-      </c>
-      <c r="I7" t="s">
-        <v>65</v>
-      </c>
-      <c r="J7" t="s">
-        <v>65</v>
-      </c>
-      <c r="K7" t="s">
-        <v>67</v>
-      </c>
       <c r="L7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M7">
         <v>26000</v>
@@ -1098,10 +1086,10 @@
         <v>30</v>
       </c>
       <c r="O7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Q7">
         <v>87871545</v>
@@ -1112,37 +1100,37 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D8">
         <v>4212</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F8">
         <v>421.2</v>
       </c>
       <c r="G8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M8">
         <v>26000</v>
@@ -1151,10 +1139,10 @@
         <v>10</v>
       </c>
       <c r="O8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Q8">
         <v>87871545</v>
@@ -1165,37 +1153,37 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D9">
         <v>4212</v>
       </c>
       <c r="E9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F9">
         <v>421.2</v>
       </c>
       <c r="G9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M9">
         <v>26000</v>
@@ -1204,10 +1192,10 @@
         <v>10</v>
       </c>
       <c r="O9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Q9">
         <v>87871545</v>
@@ -1218,37 +1206,37 @@
         <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D10">
         <v>4212</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F10">
         <v>421.2</v>
       </c>
       <c r="G10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M10">
         <v>26000</v>
@@ -1257,10 +1245,10 @@
         <v>10</v>
       </c>
       <c r="O10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P10" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Q10">
         <v>87871545</v>
@@ -1271,37 +1259,37 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D11">
         <v>4212</v>
       </c>
       <c r="E11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F11">
         <v>126.36</v>
       </c>
       <c r="G11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M11">
         <v>26000</v>
@@ -1310,10 +1298,10 @@
         <v>3</v>
       </c>
       <c r="O11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Q11">
         <v>87871545</v>
@@ -1324,37 +1312,37 @@
         <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D12">
         <v>4212</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F12">
         <v>126.36</v>
       </c>
       <c r="G12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M12">
         <v>26000</v>
@@ -1363,10 +1351,10 @@
         <v>3</v>
       </c>
       <c r="O12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Q12">
         <v>87871545</v>
@@ -1377,37 +1365,37 @@
         <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D13">
         <v>4212</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F13">
         <v>126.36</v>
       </c>
       <c r="G13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M13">
         <v>26000</v>
@@ -1416,10 +1404,10 @@
         <v>3</v>
       </c>
       <c r="O13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Q13">
         <v>87871545</v>
@@ -1430,37 +1418,37 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D14">
         <v>4212</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F14">
         <v>42.12</v>
       </c>
       <c r="G14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M14">
         <v>26000</v>
@@ -1469,10 +1457,10 @@
         <v>1</v>
       </c>
       <c r="O14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="Q14">
         <v>87871545</v>
@@ -1483,37 +1471,37 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D15">
         <v>360</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F15">
         <v>360</v>
       </c>
       <c r="G15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M15">
         <v>2000</v>
@@ -1522,10 +1510,10 @@
         <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="Q15">
         <v>13500000</v>
@@ -1536,37 +1524,37 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D16">
         <v>187.5</v>
       </c>
       <c r="E16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F16">
         <v>187.5</v>
       </c>
       <c r="G16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M16">
         <v>12500</v>
@@ -1575,10 +1563,10 @@
         <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="Q16">
         <v>1020000</v>
@@ -1589,37 +1577,37 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D17">
         <v>336</v>
       </c>
       <c r="E17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F17">
         <v>336</v>
       </c>
       <c r="G17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M17">
         <v>15000</v>
@@ -1628,10 +1616,10 @@
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="Q17">
         <v>1619200</v>
@@ -1642,37 +1630,37 @@
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D18">
         <v>221.2</v>
       </c>
       <c r="E18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F18">
         <v>154.84</v>
       </c>
       <c r="G18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M18">
         <v>14000</v>
@@ -1681,10 +1669,10 @@
         <v>70</v>
       </c>
       <c r="O18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Q18">
         <v>2370000</v>
@@ -1695,37 +1683,37 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D19">
         <v>221.2</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F19">
         <v>66.36</v>
       </c>
       <c r="G19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M19">
         <v>14000</v>
@@ -1734,10 +1722,10 @@
         <v>30</v>
       </c>
       <c r="O19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Q19">
         <v>2370000</v>
@@ -1748,37 +1736,37 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D20">
         <v>345</v>
       </c>
       <c r="E20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F20">
         <v>345</v>
       </c>
       <c r="G20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M20">
         <v>23000</v>
@@ -1787,10 +1775,10 @@
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Q20">
         <v>1125000</v>
@@ -1801,37 +1789,37 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D21">
         <v>264</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F21">
         <v>264</v>
       </c>
       <c r="G21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M21">
         <v>24000</v>
@@ -1843,7 +1831,7 @@
         <v>27</v>
       </c>
       <c r="P21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Q21">
         <v>825000</v>
@@ -1854,37 +1842,37 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D22">
         <v>90</v>
       </c>
       <c r="E22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F22">
         <v>90</v>
       </c>
       <c r="G22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M22">
         <v>2000</v>
@@ -1907,37 +1895,37 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D23">
         <v>95</v>
       </c>
       <c r="E23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F23">
         <v>95</v>
       </c>
       <c r="G23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M23">
         <v>2000</v>
@@ -1946,10 +1934,10 @@
         <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="P23" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="Q23">
         <v>3562500</v>
@@ -1960,37 +1948,37 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" t="s">
         <v>44</v>
-      </c>
-      <c r="C24" t="s">
-        <v>46</v>
       </c>
       <c r="D24">
         <v>130</v>
       </c>
       <c r="E24" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F24">
         <v>130</v>
       </c>
       <c r="G24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M24">
         <v>2000</v>
@@ -1999,66 +1987,13 @@
         <v>100</v>
       </c>
       <c r="O24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="P24" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q24">
         <v>4875000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17">
-      <c r="A25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25">
-        <v>100</v>
-      </c>
-      <c r="E25" t="s">
-        <v>60</v>
-      </c>
-      <c r="F25">
-        <v>100</v>
-      </c>
-      <c r="G25" t="s">
-        <v>65</v>
-      </c>
-      <c r="H25" t="s">
-        <v>65</v>
-      </c>
-      <c r="I25" t="s">
-        <v>65</v>
-      </c>
-      <c r="J25" t="s">
-        <v>65</v>
-      </c>
-      <c r="K25" t="s">
-        <v>66</v>
-      </c>
-      <c r="L25" t="s">
-        <v>65</v>
-      </c>
-      <c r="M25">
-        <v>2000</v>
-      </c>
-      <c r="N25">
-        <v>100</v>
-      </c>
-      <c r="O25" t="s">
-        <v>75</v>
-      </c>
-      <c r="P25" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q25">
-        <v>3750000</v>
       </c>
     </row>
   </sheetData>
@@ -2068,7 +2003,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2079,10 +2014,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -2091,49 +2026,49 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -2141,10 +2076,10 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>
@@ -2159,7 +2094,7 @@
         <v>770000</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I2">
         <v>8200</v>
@@ -2168,34 +2103,34 @@
         <v>9400</v>
       </c>
       <c r="K2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L2">
         <v>7000</v>
       </c>
       <c r="M2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="S2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -2203,10 +2138,10 @@
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
@@ -2221,7 +2156,7 @@
         <v>2000000</v>
       </c>
       <c r="H3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I3">
         <v>22000</v>
@@ -2230,34 +2165,34 @@
         <v>25000</v>
       </c>
       <c r="K3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L3">
         <v>26000</v>
       </c>
       <c r="M3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="S3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -2265,13 +2200,13 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
@@ -2283,7 +2218,7 @@
         <v>4137000</v>
       </c>
       <c r="H4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I4">
         <v>8800</v>
@@ -2292,34 +2227,34 @@
         <v>10700</v>
       </c>
       <c r="K4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L4">
         <v>10700</v>
       </c>
       <c r="M4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O4">
         <v>30.21513173797438</v>
       </c>
       <c r="P4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="S4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -2327,10 +2262,10 @@
         <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
         <v>22</v>
@@ -2345,7 +2280,7 @@
         <v>4000000</v>
       </c>
       <c r="H5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I5">
         <v>2000</v>
@@ -2354,48 +2289,48 @@
         <v>2000</v>
       </c>
       <c r="K5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L5">
         <v>2000</v>
       </c>
       <c r="M5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="S5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
@@ -2407,7 +2342,7 @@
         <v>16200000</v>
       </c>
       <c r="H6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I6">
         <v>21000</v>
@@ -2416,48 +2351,48 @@
         <v>26000</v>
       </c>
       <c r="K6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L6">
         <v>26000</v>
       </c>
       <c r="M6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="S6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E7" t="s">
         <v>22</v>
@@ -2469,7 +2404,7 @@
         <v>18000000</v>
       </c>
       <c r="H7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I7">
         <v>2000</v>
@@ -2478,48 +2413,48 @@
         <v>2000</v>
       </c>
       <c r="K7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L7">
         <v>2000</v>
       </c>
       <c r="M7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="S7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E8" t="s">
         <v>22</v>
@@ -2531,7 +2466,7 @@
         <v>1500000</v>
       </c>
       <c r="H8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I8">
         <v>8900</v>
@@ -2540,48 +2475,48 @@
         <v>11000</v>
       </c>
       <c r="K8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L8">
         <v>12500</v>
       </c>
       <c r="M8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="S8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E9" t="s">
         <v>23</v>
@@ -2593,7 +2528,7 @@
         <v>2240000</v>
       </c>
       <c r="H9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I9">
         <v>11500</v>
@@ -2602,48 +2537,48 @@
         <v>13200</v>
       </c>
       <c r="K9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L9">
         <v>15000</v>
       </c>
       <c r="M9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O9">
         <v>26.78571428571428</v>
       </c>
       <c r="P9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="S9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E10" t="s">
         <v>24</v>
@@ -2655,7 +2590,7 @@
         <v>1580000</v>
       </c>
       <c r="H10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I10">
         <v>10500</v>
@@ -2664,48 +2599,48 @@
         <v>12000</v>
       </c>
       <c r="K10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L10">
         <v>14000</v>
       </c>
       <c r="M10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R10" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="S10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E11" t="s">
         <v>25</v>
@@ -2717,7 +2652,7 @@
         <v>1500000</v>
       </c>
       <c r="H11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I11">
         <v>20000</v>
@@ -2726,34 +2661,34 @@
         <v>23000</v>
       </c>
       <c r="K11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L11">
         <v>23000</v>
       </c>
       <c r="M11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="S11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -2761,13 +2696,13 @@
         <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E12" t="s">
         <v>26</v>
@@ -2779,7 +2714,7 @@
         <v>1100000</v>
       </c>
       <c r="H12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I12">
         <v>20000</v>
@@ -2788,34 +2723,34 @@
         <v>24000</v>
       </c>
       <c r="K12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L12">
         <v>24000</v>
       </c>
       <c r="M12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O12">
         <v>18.18181818181818</v>
       </c>
       <c r="P12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R12" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="S12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -2823,10 +2758,10 @@
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D13" t="s">
         <v>28</v>
@@ -2841,7 +2776,7 @@
         <v>4500000</v>
       </c>
       <c r="H13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I13">
         <v>2000</v>
@@ -2850,48 +2785,48 @@
         <v>2000</v>
       </c>
       <c r="K13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L13">
         <v>2000</v>
       </c>
       <c r="M13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="S13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="E14" t="s">
         <v>28</v>
@@ -2903,7 +2838,7 @@
         <v>4750000</v>
       </c>
       <c r="H14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I14">
         <v>2000</v>
@@ -2912,48 +2847,48 @@
         <v>2000</v>
       </c>
       <c r="K14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L14">
         <v>2000</v>
       </c>
       <c r="M14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R14" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="S14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E15" t="s">
         <v>29</v>
@@ -2965,7 +2900,7 @@
         <v>6500000</v>
       </c>
       <c r="H15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I15">
         <v>2000</v>
@@ -2974,96 +2909,34 @@
         <v>2000</v>
       </c>
       <c r="K15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L15">
         <v>2000</v>
       </c>
       <c r="M15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R15" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="S15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20">
-      <c r="A16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16">
-        <v>10000000</v>
-      </c>
-      <c r="G16">
-        <v>5000000</v>
-      </c>
-      <c r="H16" t="s">
-        <v>65</v>
-      </c>
-      <c r="I16">
-        <v>2000</v>
-      </c>
-      <c r="J16">
-        <v>2000</v>
-      </c>
-      <c r="K16" t="s">
-        <v>65</v>
-      </c>
-      <c r="L16">
-        <v>2000</v>
-      </c>
-      <c r="M16" t="s">
-        <v>65</v>
-      </c>
-      <c r="N16" t="s">
-        <v>65</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>65</v>
-      </c>
-      <c r="R16" t="s">
-        <v>113</v>
-      </c>
-      <c r="S16" t="s">
-        <v>65</v>
-      </c>
-      <c r="T16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -3073,7 +2946,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3081,16 +2954,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -3102,10 +2975,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -3114,27 +2987,27 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G2" t="s">
         <v>21</v>
@@ -3157,98 +3030,98 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s">
-        <v>117</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H3">
-        <v>42120</v>
+        <v>18750</v>
       </c>
       <c r="I3">
-        <v>16200000</v>
+        <v>1500000</v>
       </c>
       <c r="J3">
-        <v>26000</v>
+        <v>12500</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>95</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>113</v>
       </c>
       <c r="F4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4">
-        <v>18750</v>
+        <v>42120</v>
       </c>
       <c r="I4">
-        <v>1500000</v>
+        <v>16200000</v>
       </c>
       <c r="J4">
-        <v>12500</v>
+        <v>26000</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G5" t="s">
         <v>21</v>
@@ -3271,22 +3144,22 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G6" t="s">
         <v>29</v>
@@ -3309,72 +3182,72 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>113</v>
       </c>
       <c r="F7" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="G7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H7">
-        <v>34500</v>
+        <v>126360</v>
       </c>
       <c r="I7">
-        <v>1500000</v>
+        <v>16200000</v>
       </c>
       <c r="J7">
-        <v>23000</v>
+        <v>26000</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
         <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H8">
-        <v>52000</v>
+        <v>44265.9</v>
       </c>
       <c r="I8">
-        <v>2000000</v>
+        <v>4137000</v>
       </c>
       <c r="J8">
-        <v>26000</v>
+        <v>10700</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -3385,34 +3258,34 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F9" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="G9" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H9">
-        <v>44265.9</v>
+        <v>34500</v>
       </c>
       <c r="I9">
-        <v>4137000</v>
+        <v>1500000</v>
       </c>
       <c r="J9">
-        <v>10700</v>
+        <v>23000</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -3423,31 +3296,31 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>98</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>117</v>
+        <v>47</v>
       </c>
       <c r="F10" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="G10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H10">
-        <v>126360</v>
+        <v>52000</v>
       </c>
       <c r="I10">
-        <v>16200000</v>
+        <v>2000000</v>
       </c>
       <c r="J10">
         <v>26000</v>
@@ -3456,27 +3329,27 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G11" t="s">
         <v>23</v>
@@ -3499,19 +3372,19 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
         <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F12" t="s">
         <v>28</v>
@@ -3537,98 +3410,98 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
       <c r="E13" t="s">
-        <v>56</v>
+        <v>113</v>
       </c>
       <c r="F13" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G13" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="H13">
-        <v>26400</v>
+        <v>12636</v>
       </c>
       <c r="I13">
-        <v>1100000</v>
+        <v>16200000</v>
       </c>
       <c r="J13">
-        <v>24000</v>
+        <v>26000</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="L13">
-        <v>100</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>98</v>
+        <v>54</v>
       </c>
       <c r="E14" t="s">
-        <v>117</v>
+        <v>54</v>
       </c>
       <c r="F14" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="G14" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="H14">
-        <v>12636</v>
+        <v>26400</v>
       </c>
       <c r="I14">
-        <v>16200000</v>
+        <v>1100000</v>
       </c>
       <c r="J14">
-        <v>26000</v>
+        <v>24000</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14">
-        <v>3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G15" t="s">
         <v>22</v>
@@ -3651,22 +3524,22 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E16" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F16" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G16" t="s">
         <v>21</v>
@@ -3689,22 +3562,22 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G17" t="s">
         <v>24</v>
@@ -3727,180 +3600,180 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E18" t="s">
-        <v>60</v>
+        <v>114</v>
       </c>
       <c r="F18" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="G18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H18">
-        <v>10000</v>
+        <v>6636</v>
       </c>
       <c r="I18">
-        <v>5000000</v>
+        <v>1580000</v>
       </c>
       <c r="J18">
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="E19" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="F19" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="G19" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H19">
-        <v>6636</v>
+        <v>12636</v>
       </c>
       <c r="I19">
-        <v>1580000</v>
+        <v>16200000</v>
       </c>
       <c r="J19">
-        <v>14000</v>
+        <v>26000</v>
       </c>
       <c r="K19">
         <v>0</v>
       </c>
       <c r="L19">
-        <v>30</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>98</v>
+        <v>46</v>
       </c>
       <c r="E20" t="s">
-        <v>117</v>
+        <v>46</v>
       </c>
       <c r="F20" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="G20" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H20">
-        <v>12636</v>
+        <v>5390</v>
       </c>
       <c r="I20">
-        <v>16200000</v>
+        <v>770000</v>
       </c>
       <c r="J20">
-        <v>26000</v>
+        <v>7000</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
       <c r="L20">
-        <v>3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>48</v>
+        <v>95</v>
       </c>
       <c r="E21" t="s">
-        <v>48</v>
+        <v>113</v>
       </c>
       <c r="F21" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="G21" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H21">
-        <v>5390</v>
+        <v>12636</v>
       </c>
       <c r="I21">
-        <v>770000</v>
+        <v>16200000</v>
       </c>
       <c r="J21">
-        <v>7000</v>
+        <v>26000</v>
       </c>
       <c r="K21">
         <v>0</v>
       </c>
       <c r="L21">
-        <v>100</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E22" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F22" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G22" t="s">
         <v>21</v>
       </c>
       <c r="H22">
-        <v>12636</v>
+        <v>126360</v>
       </c>
       <c r="I22">
         <v>16200000</v>
@@ -3912,74 +3785,74 @@
         <v>0</v>
       </c>
       <c r="L22">
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D23" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="E23" t="s">
-        <v>117</v>
+        <v>61</v>
       </c>
       <c r="F23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G23" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="H23">
-        <v>126360</v>
+        <v>9500</v>
       </c>
       <c r="I23">
-        <v>16200000</v>
+        <v>4750000</v>
       </c>
       <c r="J23">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="K23">
         <v>0</v>
       </c>
       <c r="L23">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D24" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="E24" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="F24" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G24" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="H24">
-        <v>9500</v>
+        <v>8000</v>
       </c>
       <c r="I24">
-        <v>4750000</v>
+        <v>4000000</v>
       </c>
       <c r="J24">
         <v>2000</v>
@@ -3988,44 +3861,6 @@
         <v>0</v>
       </c>
       <c r="L24">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" t="s">
-        <v>50</v>
-      </c>
-      <c r="F25" t="s">
-        <v>22</v>
-      </c>
-      <c r="G25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H25">
-        <v>8000</v>
-      </c>
-      <c r="I25">
-        <v>4000000</v>
-      </c>
-      <c r="J25">
-        <v>2000</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-      <c r="L25">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2023-11-04
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="122">
   <si>
     <t>상장일</t>
   </si>
@@ -69,6 +69,18 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2023-11-03</t>
+  </si>
+  <si>
+    <t>2023-11-02</t>
+  </si>
+  <si>
+    <t>2023-10-27</t>
+  </si>
+  <si>
+    <t>2023-10-26</t>
+  </si>
+  <si>
     <t>2023-10-20</t>
   </si>
   <si>
@@ -102,156 +114,156 @@
     <t>2023-09-14</t>
   </si>
   <si>
+    <t>KB제27호스팩</t>
+  </si>
+  <si>
+    <t>유진테크놀로지</t>
+  </si>
+  <si>
+    <t>유투바이오</t>
+  </si>
+  <si>
+    <t>퀄리타스반도체</t>
+  </si>
+  <si>
+    <t>워트</t>
+  </si>
+  <si>
+    <t>에스엘에스바이오</t>
+  </si>
+  <si>
+    <t>신성에스티</t>
+  </si>
+  <si>
+    <t>퓨릿</t>
+  </si>
+  <si>
+    <t>에이치엠씨제6호스팩</t>
+  </si>
+  <si>
+    <t>두산로보틱스</t>
+  </si>
+  <si>
+    <t>신한제11호스팩</t>
+  </si>
+  <si>
+    <t>한싹</t>
+  </si>
+  <si>
+    <t>레뷰코퍼레이션</t>
+  </si>
+  <si>
+    <t>아이엠티</t>
+  </si>
+  <si>
+    <t>밀리의서재</t>
+  </si>
+  <si>
+    <t>인스웨이브시스템즈</t>
+  </si>
+  <si>
+    <t>상상인제4호스팩</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>코스피</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>신한</t>
+  </si>
+  <si>
+    <t>한국</t>
+  </si>
+  <si>
+    <t>키움</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>현대차</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>신영</t>
+  </si>
+  <si>
+    <t>유비에스</t>
+  </si>
+  <si>
+    <t>삼성</t>
+  </si>
+  <si>
+    <t>유안타</t>
+  </si>
+  <si>
+    <t>유진</t>
+  </si>
+  <si>
+    <t>상상인</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>공동대표</t>
+  </si>
+  <si>
+    <t>공동</t>
+  </si>
+  <si>
+    <t>인수</t>
+  </si>
+  <si>
+    <t>2023-10-24</t>
+  </si>
+  <si>
+    <t>2023-10-23</t>
+  </si>
+  <si>
+    <t>2023-10-16</t>
+  </si>
+  <si>
+    <t>2023-09-21</t>
+  </si>
+  <si>
+    <t>2023-09-19</t>
+  </si>
+  <si>
+    <t>2023-09-18</t>
+  </si>
+  <si>
+    <t>2023-09-04</t>
+  </si>
+  <si>
+    <t>2023-10-11</t>
+  </si>
+  <si>
+    <t>2023-09-26</t>
+  </si>
+  <si>
+    <t>2023-09-22</t>
+  </si>
+  <si>
     <t>2023-09-07</t>
   </si>
   <si>
-    <t>2023-09-04</t>
-  </si>
-  <si>
-    <t>에스엘에스바이오</t>
-  </si>
-  <si>
-    <t>신성에스티</t>
-  </si>
-  <si>
-    <t>퓨릿</t>
-  </si>
-  <si>
-    <t>에이치엠씨제6호스팩</t>
-  </si>
-  <si>
-    <t>두산로보틱스</t>
-  </si>
-  <si>
-    <t>신한제11호스팩</t>
-  </si>
-  <si>
-    <t>한싹</t>
-  </si>
-  <si>
-    <t>레뷰코퍼레이션</t>
-  </si>
-  <si>
-    <t>아이엠티</t>
-  </si>
-  <si>
-    <t>밀리의서재</t>
-  </si>
-  <si>
-    <t>인스웨이브시스템즈</t>
-  </si>
-  <si>
-    <t>상상인제4호스팩</t>
-  </si>
-  <si>
-    <t>한화플러스제4호스팩</t>
-  </si>
-  <si>
-    <t>대신밸런스제16호스팩</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>코스피</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>현대차</t>
-  </si>
-  <si>
-    <t>한국</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>KB</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t>키움</t>
-  </si>
-  <si>
-    <t>신영</t>
-  </si>
-  <si>
-    <t>유비에스</t>
-  </si>
-  <si>
-    <t>신한</t>
-  </si>
-  <si>
-    <t>삼성</t>
-  </si>
-  <si>
-    <t>유안타</t>
-  </si>
-  <si>
-    <t>유진</t>
-  </si>
-  <si>
-    <t>상상인</t>
-  </si>
-  <si>
-    <t>한화</t>
-  </si>
-  <si>
-    <t>대신</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>공동대표</t>
-  </si>
-  <si>
-    <t>공동</t>
-  </si>
-  <si>
-    <t>인수</t>
-  </si>
-  <si>
-    <t>2023-09-21</t>
-  </si>
-  <si>
-    <t>2023-09-19</t>
-  </si>
-  <si>
-    <t>2023-09-18</t>
-  </si>
-  <si>
-    <t>2023-08-29</t>
-  </si>
-  <si>
-    <t>2023-08-23</t>
-  </si>
-  <si>
-    <t>2023-10-11</t>
-  </si>
-  <si>
-    <t>2023-09-26</t>
-  </si>
-  <si>
-    <t>2023-09-22</t>
-  </si>
-  <si>
-    <t>2023-09-01</t>
-  </si>
-  <si>
-    <t>2023-08-28</t>
-  </si>
-  <si>
     <t>회사명</t>
   </si>
   <si>
@@ -306,6 +318,21 @@
     <t>한국, 미래</t>
   </si>
   <si>
+    <t>8.1 : 1</t>
+  </si>
+  <si>
+    <t>1506.58 : 1</t>
+  </si>
+  <si>
+    <t>1286.85 : 1</t>
+  </si>
+  <si>
+    <t>1632.34 : 1</t>
+  </si>
+  <si>
+    <t>1781.78 : 1</t>
+  </si>
+  <si>
     <t>345.96 : 1</t>
   </si>
   <si>
@@ -340,12 +367,6 @@
   </si>
   <si>
     <t>1010.2 : 1</t>
-  </si>
-  <si>
-    <t>753.02 : 1</t>
-  </si>
-  <si>
-    <t>527.68 : 1</t>
   </si>
   <si>
     <t>인수기관</t>
@@ -718,7 +739,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q24"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -782,52 +803,52 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D2">
-        <v>53.9</v>
+        <v>250</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F2">
-        <v>53.9</v>
+        <v>250</v>
       </c>
       <c r="G2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="L2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M2">
-        <v>7000</v>
+        <v>2000</v>
       </c>
       <c r="N2">
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="P2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q2">
-        <v>577500</v>
+        <v>9375000</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -835,211 +856,211 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D3">
-        <v>520</v>
+        <v>178.41194</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="F3">
-        <v>520</v>
+        <v>178.41194</v>
       </c>
       <c r="G3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="L3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M3">
-        <v>26000</v>
+        <v>17000</v>
       </c>
       <c r="N3">
         <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="P3" t="s">
         <v>20</v>
       </c>
       <c r="Q3">
-        <v>1300000</v>
+        <v>787111</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D4">
-        <v>442.659</v>
+        <v>49.66368</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="F4">
-        <v>442.659</v>
+        <v>49.66368</v>
       </c>
       <c r="G4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="L4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M4">
-        <v>10700</v>
+        <v>4400</v>
       </c>
       <c r="N4">
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="P4" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="Q4">
-        <v>3102750</v>
+        <v>846540</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D5">
-        <v>80</v>
+        <v>306</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="F5">
-        <v>80</v>
+        <v>306</v>
       </c>
       <c r="G5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="L5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M5">
-        <v>2000</v>
+        <v>17000</v>
       </c>
       <c r="N5">
         <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="P5" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="Q5">
-        <v>3000000</v>
+        <v>1119600</v>
       </c>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D6">
-        <v>4212</v>
+        <v>260</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="F6">
-        <v>1263.6</v>
+        <v>260</v>
       </c>
       <c r="G6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M6">
-        <v>26000</v>
+        <v>6500</v>
       </c>
       <c r="N6">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="P6" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="Q6">
-        <v>87871545</v>
+        <v>2880000</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1047,261 +1068,261 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D7">
-        <v>4212</v>
+        <v>53.9</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F7">
-        <v>1263.6</v>
+        <v>53.9</v>
       </c>
       <c r="G7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M7">
-        <v>26000</v>
+        <v>7000</v>
       </c>
       <c r="N7">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="O7" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="P7" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="Q7">
-        <v>87871545</v>
+        <v>577500</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D8">
-        <v>4212</v>
+        <v>520</v>
       </c>
       <c r="E8" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F8">
-        <v>421.2</v>
+        <v>520</v>
       </c>
       <c r="G8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M8">
         <v>26000</v>
       </c>
       <c r="N8">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="P8" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="Q8">
-        <v>87871545</v>
+        <v>1300000</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D9">
-        <v>4212</v>
+        <v>442.659</v>
       </c>
       <c r="E9" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="F9">
-        <v>421.2</v>
+        <v>442.659</v>
       </c>
       <c r="G9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M9">
-        <v>26000</v>
+        <v>10700</v>
       </c>
       <c r="N9">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="P9" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="Q9">
-        <v>87871545</v>
+        <v>3102750</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D10">
-        <v>4212</v>
+        <v>80</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="F10">
-        <v>421.2</v>
+        <v>80</v>
       </c>
       <c r="G10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M10">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="N10">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="O10" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="P10" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="Q10">
-        <v>87871545</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D11">
         <v>4212</v>
       </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F11">
-        <v>126.36</v>
+        <v>1263.6</v>
       </c>
       <c r="G11" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H11" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I11" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J11" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L11" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M11">
         <v>26000</v>
       </c>
       <c r="N11">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="O11" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="P11" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="Q11">
         <v>87871545</v>
@@ -1309,52 +1330,52 @@
     </row>
     <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D12">
         <v>4212</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F12">
-        <v>126.36</v>
+        <v>1263.6</v>
       </c>
       <c r="G12" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H12" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I12" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J12" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L12" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M12">
         <v>26000</v>
       </c>
       <c r="N12">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="O12" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="P12" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="Q12">
         <v>87871545</v>
@@ -1362,52 +1383,52 @@
     </row>
     <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D13">
         <v>4212</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="F13">
-        <v>126.36</v>
+        <v>421.2</v>
       </c>
       <c r="G13" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H13" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I13" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J13" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K13" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L13" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M13">
         <v>26000</v>
       </c>
       <c r="N13">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="O13" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="P13" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="Q13">
         <v>87871545</v>
@@ -1415,52 +1436,52 @@
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D14">
         <v>4212</v>
       </c>
       <c r="E14" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F14">
-        <v>42.12</v>
+        <v>421.2</v>
       </c>
       <c r="G14" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H14" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I14" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J14" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L14" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M14">
         <v>26000</v>
       </c>
       <c r="N14">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="O14" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="P14" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="Q14">
         <v>87871545</v>
@@ -1468,320 +1489,320 @@
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D15">
-        <v>360</v>
+        <v>4212</v>
       </c>
       <c r="E15" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F15">
-        <v>360</v>
+        <v>421.2</v>
       </c>
       <c r="G15" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H15" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I15" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J15" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K15" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="L15" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M15">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="N15">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="O15" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="P15" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="Q15">
-        <v>13500000</v>
+        <v>87871545</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D16">
-        <v>187.5</v>
+        <v>4212</v>
       </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F16">
-        <v>187.5</v>
+        <v>126.36</v>
       </c>
       <c r="G16" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H16" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I16" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J16" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K16" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="L16" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M16">
-        <v>12500</v>
+        <v>26000</v>
       </c>
       <c r="N16">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="O16" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="P16" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="Q16">
-        <v>1020000</v>
+        <v>87871545</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D17">
-        <v>336</v>
+        <v>4212</v>
       </c>
       <c r="E17" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F17">
-        <v>336</v>
+        <v>126.36</v>
       </c>
       <c r="G17" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H17" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I17" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J17" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K17" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="L17" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M17">
-        <v>15000</v>
+        <v>26000</v>
       </c>
       <c r="N17">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="O17" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="P17" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="Q17">
-        <v>1619200</v>
+        <v>87871545</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D18">
-        <v>221.2</v>
+        <v>4212</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F18">
-        <v>154.84</v>
+        <v>126.36</v>
       </c>
       <c r="G18" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H18" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I18" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J18" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K18" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="L18" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M18">
-        <v>14000</v>
+        <v>26000</v>
       </c>
       <c r="N18">
-        <v>70</v>
+        <v>3</v>
       </c>
       <c r="O18" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="P18" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="Q18">
-        <v>2370000</v>
+        <v>87871545</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D19">
-        <v>221.2</v>
+        <v>4212</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F19">
-        <v>66.36</v>
+        <v>42.12</v>
       </c>
       <c r="G19" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H19" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I19" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J19" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K19" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="L19" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M19">
-        <v>14000</v>
+        <v>26000</v>
       </c>
       <c r="N19">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="O19" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="P19" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="Q19">
-        <v>2370000</v>
+        <v>87871545</v>
       </c>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D20">
-        <v>345</v>
+        <v>360</v>
       </c>
       <c r="E20" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="F20">
-        <v>345</v>
+        <v>360</v>
       </c>
       <c r="G20" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H20" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I20" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J20" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K20" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="L20" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M20">
-        <v>23000</v>
+        <v>2000</v>
       </c>
       <c r="N20">
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="P20" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="Q20">
-        <v>1125000</v>
+        <v>13500000</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1789,52 +1810,52 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D21">
-        <v>264</v>
+        <v>187.5</v>
       </c>
       <c r="E21" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F21">
-        <v>264</v>
+        <v>187.5</v>
       </c>
       <c r="G21" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H21" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I21" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J21" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K21" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="L21" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M21">
-        <v>24000</v>
+        <v>12500</v>
       </c>
       <c r="N21">
         <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="P21" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="Q21">
-        <v>825000</v>
+        <v>1020000</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1842,52 +1863,52 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D22">
-        <v>90</v>
+        <v>336</v>
       </c>
       <c r="E22" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F22">
-        <v>90</v>
+        <v>336</v>
       </c>
       <c r="G22" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H22" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I22" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J22" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K22" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="L22" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M22">
-        <v>2000</v>
+        <v>15000</v>
       </c>
       <c r="N22">
         <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="P22" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="Q22">
-        <v>3375000</v>
+        <v>1619200</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1895,105 +1916,264 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D23">
-        <v>95</v>
+        <v>221.2</v>
       </c>
       <c r="E23" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F23">
-        <v>95</v>
+        <v>154.84</v>
       </c>
       <c r="G23" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H23" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I23" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J23" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K23" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="L23" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M23">
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="N23">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="O23" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="P23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="Q23">
-        <v>3562500</v>
+        <v>2370000</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24">
+        <v>221.2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24">
+        <v>66.36</v>
+      </c>
+      <c r="G24" t="s">
+        <v>66</v>
+      </c>
+      <c r="H24" t="s">
+        <v>66</v>
+      </c>
+      <c r="I24" t="s">
+        <v>66</v>
+      </c>
+      <c r="J24" t="s">
+        <v>66</v>
+      </c>
+      <c r="K24" t="s">
+        <v>70</v>
+      </c>
+      <c r="L24" t="s">
+        <v>66</v>
+      </c>
+      <c r="M24">
+        <v>14000</v>
+      </c>
+      <c r="N24">
+        <v>30</v>
+      </c>
+      <c r="O24" t="s">
+        <v>76</v>
+      </c>
+      <c r="P24" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q24">
+        <v>2370000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" t="s">
         <v>29</v>
       </c>
-      <c r="B24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24">
-        <v>130</v>
-      </c>
-      <c r="E24" t="s">
-        <v>62</v>
-      </c>
-      <c r="F24">
-        <v>130</v>
-      </c>
-      <c r="G24" t="s">
-        <v>63</v>
-      </c>
-      <c r="H24" t="s">
-        <v>63</v>
-      </c>
-      <c r="I24" t="s">
-        <v>63</v>
-      </c>
-      <c r="J24" t="s">
-        <v>63</v>
-      </c>
-      <c r="K24" t="s">
-        <v>64</v>
-      </c>
-      <c r="L24" t="s">
-        <v>63</v>
-      </c>
-      <c r="M24">
+      <c r="B25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25">
+        <v>345</v>
+      </c>
+      <c r="E25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25">
+        <v>345</v>
+      </c>
+      <c r="G25" t="s">
+        <v>66</v>
+      </c>
+      <c r="H25" t="s">
+        <v>66</v>
+      </c>
+      <c r="I25" t="s">
+        <v>66</v>
+      </c>
+      <c r="J25" t="s">
+        <v>66</v>
+      </c>
+      <c r="K25" t="s">
+        <v>67</v>
+      </c>
+      <c r="L25" t="s">
+        <v>66</v>
+      </c>
+      <c r="M25">
+        <v>23000</v>
+      </c>
+      <c r="N25">
+        <v>100</v>
+      </c>
+      <c r="O25" t="s">
+        <v>76</v>
+      </c>
+      <c r="P25" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q25">
+        <v>1125000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26">
+        <v>264</v>
+      </c>
+      <c r="E26" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26">
+        <v>264</v>
+      </c>
+      <c r="G26" t="s">
+        <v>66</v>
+      </c>
+      <c r="H26" t="s">
+        <v>66</v>
+      </c>
+      <c r="I26" t="s">
+        <v>66</v>
+      </c>
+      <c r="J26" t="s">
+        <v>66</v>
+      </c>
+      <c r="K26" t="s">
+        <v>67</v>
+      </c>
+      <c r="L26" t="s">
+        <v>66</v>
+      </c>
+      <c r="M26">
+        <v>24000</v>
+      </c>
+      <c r="N26">
+        <v>100</v>
+      </c>
+      <c r="O26" t="s">
+        <v>31</v>
+      </c>
+      <c r="P26" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q26">
+        <v>825000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27">
+        <v>90</v>
+      </c>
+      <c r="E27" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27">
+        <v>90</v>
+      </c>
+      <c r="G27" t="s">
+        <v>66</v>
+      </c>
+      <c r="H27" t="s">
+        <v>66</v>
+      </c>
+      <c r="I27" t="s">
+        <v>66</v>
+      </c>
+      <c r="J27" t="s">
+        <v>66</v>
+      </c>
+      <c r="K27" t="s">
+        <v>67</v>
+      </c>
+      <c r="L27" t="s">
+        <v>66</v>
+      </c>
+      <c r="M27">
         <v>2000</v>
       </c>
-      <c r="N24">
+      <c r="N27">
         <v>100</v>
       </c>
-      <c r="O24" t="s">
-        <v>72</v>
-      </c>
-      <c r="P24" t="s">
+      <c r="O27" t="s">
         <v>77</v>
       </c>
-      <c r="Q24">
-        <v>4875000</v>
+      <c r="P27" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q27">
+        <v>3375000</v>
       </c>
     </row>
   </sheetData>
@@ -2003,7 +2183,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T15"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2014,10 +2194,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -2026,122 +2206,122 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
       </c>
       <c r="F2">
-        <v>5390000</v>
+        <v>25000000</v>
       </c>
       <c r="G2">
-        <v>770000</v>
+        <v>12500000</v>
       </c>
       <c r="H2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I2">
-        <v>8200</v>
+        <v>2000</v>
       </c>
       <c r="J2">
-        <v>9400</v>
+        <v>2000</v>
       </c>
       <c r="K2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="L2">
-        <v>7000</v>
+        <v>2000</v>
       </c>
       <c r="M2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="N2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="Q2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="R2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="S2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="T2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
@@ -2150,793 +2330,979 @@
         <v>18</v>
       </c>
       <c r="F3">
-        <v>52000000</v>
+        <v>17841194</v>
       </c>
       <c r="G3">
-        <v>2000000</v>
+        <v>1049482</v>
       </c>
       <c r="H3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I3">
-        <v>22000</v>
+        <v>12800</v>
       </c>
       <c r="J3">
-        <v>25000</v>
+        <v>14500</v>
       </c>
       <c r="K3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="L3">
-        <v>26000</v>
+        <v>17000</v>
       </c>
       <c r="M3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="N3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>9.999980942979489</v>
       </c>
       <c r="P3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="Q3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="R3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="S3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="T3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4">
-        <v>44265900</v>
+        <v>4966368</v>
       </c>
       <c r="G4">
-        <v>4137000</v>
+        <v>1128720</v>
       </c>
       <c r="H4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I4">
-        <v>8800</v>
+        <v>3300</v>
       </c>
       <c r="J4">
-        <v>10700</v>
+        <v>3900</v>
       </c>
       <c r="K4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="L4">
-        <v>10700</v>
+        <v>4400</v>
       </c>
       <c r="M4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="N4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="O4">
-        <v>30.21513173797438</v>
+        <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="Q4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="R4" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="S4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="T4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5">
-        <v>8000000</v>
+        <v>30600000</v>
       </c>
       <c r="G5">
-        <v>4000000</v>
+        <v>1800000</v>
       </c>
       <c r="H5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I5">
-        <v>2000</v>
+        <v>13000</v>
       </c>
       <c r="J5">
-        <v>2000</v>
+        <v>15000</v>
       </c>
       <c r="K5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="L5">
-        <v>2000</v>
+        <v>17000</v>
       </c>
       <c r="M5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="N5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="Q5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="R5" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="S5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="T5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F6">
-        <v>421200000</v>
+        <v>26000000</v>
       </c>
       <c r="G6">
-        <v>16200000</v>
+        <v>4000000</v>
       </c>
       <c r="H6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I6">
-        <v>21000</v>
+        <v>5000</v>
       </c>
       <c r="J6">
-        <v>26000</v>
+        <v>5600</v>
       </c>
       <c r="K6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="L6">
-        <v>26000</v>
+        <v>6500</v>
       </c>
       <c r="M6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="N6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="Q6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="R6" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="S6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="T6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
         <v>56</v>
       </c>
       <c r="D7" t="s">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7">
-        <v>36000000</v>
+        <v>5390000</v>
       </c>
       <c r="G7">
-        <v>18000000</v>
+        <v>770000</v>
       </c>
       <c r="H7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I7">
-        <v>2000</v>
+        <v>8200</v>
       </c>
       <c r="J7">
-        <v>2000</v>
+        <v>9400</v>
       </c>
       <c r="K7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="L7">
-        <v>2000</v>
+        <v>7000</v>
       </c>
       <c r="M7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="N7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="Q7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="R7" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="S7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="T7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
         <v>22</v>
       </c>
       <c r="F8">
-        <v>18750000</v>
+        <v>52000000</v>
       </c>
       <c r="G8">
-        <v>1500000</v>
+        <v>2000000</v>
       </c>
       <c r="H8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I8">
-        <v>8900</v>
+        <v>22000</v>
       </c>
       <c r="J8">
-        <v>11000</v>
+        <v>25000</v>
       </c>
       <c r="K8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="L8">
-        <v>12500</v>
+        <v>26000</v>
       </c>
       <c r="M8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="N8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="Q8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="R8" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="S8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="T8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
         <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E9" t="s">
         <v>23</v>
       </c>
       <c r="F9">
-        <v>33600000</v>
+        <v>44265900</v>
       </c>
       <c r="G9">
-        <v>2240000</v>
+        <v>4137000</v>
       </c>
       <c r="H9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I9">
-        <v>11500</v>
+        <v>8800</v>
       </c>
       <c r="J9">
-        <v>13200</v>
+        <v>10700</v>
       </c>
       <c r="K9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="L9">
-        <v>15000</v>
+        <v>10700</v>
       </c>
       <c r="M9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="N9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="O9">
-        <v>26.78571428571428</v>
+        <v>30.21513173797438</v>
       </c>
       <c r="P9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="Q9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="R9" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="S9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="T9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
         <v>58</v>
       </c>
       <c r="D10" t="s">
-        <v>68</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
         <v>24</v>
       </c>
       <c r="F10">
-        <v>22120000</v>
+        <v>8000000</v>
       </c>
       <c r="G10">
-        <v>1580000</v>
+        <v>4000000</v>
       </c>
       <c r="H10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I10">
-        <v>10500</v>
+        <v>2000</v>
       </c>
       <c r="J10">
-        <v>12000</v>
+        <v>2000</v>
       </c>
       <c r="K10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="L10">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="M10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="N10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="Q10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="R10" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="S10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="T10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
       <c r="D11" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="E11" t="s">
         <v>25</v>
       </c>
       <c r="F11">
-        <v>34500000</v>
+        <v>421200000</v>
       </c>
       <c r="G11">
-        <v>1500000</v>
+        <v>16200000</v>
       </c>
       <c r="H11" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I11">
-        <v>20000</v>
+        <v>21000</v>
       </c>
       <c r="J11">
-        <v>23000</v>
+        <v>26000</v>
       </c>
       <c r="K11" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="L11">
-        <v>23000</v>
+        <v>26000</v>
       </c>
       <c r="M11" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="N11" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="Q11" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="R11" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="S11" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="T11" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D12" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E12" t="s">
         <v>26</v>
       </c>
       <c r="F12">
-        <v>26400000</v>
+        <v>36000000</v>
       </c>
       <c r="G12">
-        <v>1100000</v>
+        <v>18000000</v>
       </c>
       <c r="H12" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I12">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="J12">
-        <v>24000</v>
+        <v>2000</v>
       </c>
       <c r="K12" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="L12">
-        <v>24000</v>
+        <v>2000</v>
       </c>
       <c r="M12" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="N12" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="O12">
-        <v>18.18181818181818</v>
+        <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="Q12" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="R12" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="S12" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="T12" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F13">
-        <v>9000000</v>
+        <v>18750000</v>
       </c>
       <c r="G13">
-        <v>4500000</v>
+        <v>1500000</v>
       </c>
       <c r="H13" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I13">
-        <v>2000</v>
+        <v>8900</v>
       </c>
       <c r="J13">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="K13" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="L13">
-        <v>2000</v>
+        <v>12500</v>
       </c>
       <c r="M13" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="N13" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="Q13" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="R13" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="S13" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="T13" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D14" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14">
-        <v>9500000</v>
+        <v>33600000</v>
       </c>
       <c r="G14">
-        <v>4750000</v>
+        <v>2240000</v>
       </c>
       <c r="H14" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I14">
-        <v>2000</v>
+        <v>11500</v>
       </c>
       <c r="J14">
-        <v>2000</v>
+        <v>13200</v>
       </c>
       <c r="K14" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="L14">
-        <v>2000</v>
+        <v>15000</v>
       </c>
       <c r="M14" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="N14" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="O14">
-        <v>0</v>
+        <v>26.78571428571428</v>
       </c>
       <c r="P14" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="Q14" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="R14" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="S14" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="T14" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15">
-        <v>13000000</v>
+        <v>22120000</v>
       </c>
       <c r="G15">
-        <v>6500000</v>
+        <v>1580000</v>
       </c>
       <c r="H15" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I15">
-        <v>2000</v>
+        <v>10500</v>
       </c>
       <c r="J15">
-        <v>2000</v>
+        <v>12000</v>
       </c>
       <c r="K15" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="L15">
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="M15" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="N15" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="Q15" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="R15" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="S15" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="T15" t="s">
-        <v>63</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16">
+        <v>34500000</v>
+      </c>
+      <c r="G16">
+        <v>1500000</v>
+      </c>
+      <c r="H16" t="s">
+        <v>66</v>
+      </c>
+      <c r="I16">
+        <v>20000</v>
+      </c>
+      <c r="J16">
+        <v>23000</v>
+      </c>
+      <c r="K16" t="s">
+        <v>66</v>
+      </c>
+      <c r="L16">
+        <v>23000</v>
+      </c>
+      <c r="M16" t="s">
+        <v>66</v>
+      </c>
+      <c r="N16" t="s">
+        <v>66</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>66</v>
+      </c>
+      <c r="R16" t="s">
+        <v>114</v>
+      </c>
+      <c r="S16" t="s">
+        <v>66</v>
+      </c>
+      <c r="T16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17">
+        <v>26400000</v>
+      </c>
+      <c r="G17">
+        <v>1100000</v>
+      </c>
+      <c r="H17" t="s">
+        <v>66</v>
+      </c>
+      <c r="I17">
+        <v>20000</v>
+      </c>
+      <c r="J17">
+        <v>24000</v>
+      </c>
+      <c r="K17" t="s">
+        <v>66</v>
+      </c>
+      <c r="L17">
+        <v>24000</v>
+      </c>
+      <c r="M17" t="s">
+        <v>66</v>
+      </c>
+      <c r="N17" t="s">
+        <v>66</v>
+      </c>
+      <c r="O17">
+        <v>18.18181818181818</v>
+      </c>
+      <c r="P17" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>66</v>
+      </c>
+      <c r="R17" t="s">
+        <v>115</v>
+      </c>
+      <c r="S17" t="s">
+        <v>66</v>
+      </c>
+      <c r="T17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18">
+        <v>9000000</v>
+      </c>
+      <c r="G18">
+        <v>4500000</v>
+      </c>
+      <c r="H18" t="s">
+        <v>66</v>
+      </c>
+      <c r="I18">
+        <v>2000</v>
+      </c>
+      <c r="J18">
+        <v>2000</v>
+      </c>
+      <c r="K18" t="s">
+        <v>66</v>
+      </c>
+      <c r="L18">
+        <v>2000</v>
+      </c>
+      <c r="M18" t="s">
+        <v>66</v>
+      </c>
+      <c r="N18" t="s">
+        <v>66</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>66</v>
+      </c>
+      <c r="R18" t="s">
+        <v>116</v>
+      </c>
+      <c r="S18" t="s">
+        <v>66</v>
+      </c>
+      <c r="T18" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2946,7 +3312,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2954,16 +3320,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -2975,10 +3341,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -2987,30 +3353,30 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E2" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="F2" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H2">
         <v>42120</v>
@@ -3033,10 +3399,10 @@
         <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
         <v>51</v>
@@ -3045,19 +3411,19 @@
         <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="H3">
-        <v>18750</v>
+        <v>25000</v>
       </c>
       <c r="I3">
-        <v>1500000</v>
+        <v>12500000</v>
       </c>
       <c r="J3">
-        <v>12500</v>
+        <v>2000</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -3071,60 +3437,60 @@
         <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>113</v>
+        <v>51</v>
       </c>
       <c r="F4" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="H4">
-        <v>42120</v>
+        <v>18750</v>
       </c>
       <c r="I4">
-        <v>16200000</v>
+        <v>1500000</v>
       </c>
       <c r="J4">
-        <v>26000</v>
+        <v>12500</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E5" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="F5" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H5">
         <v>42120</v>
@@ -3144,110 +3510,110 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>99</v>
       </c>
       <c r="E6" t="s">
-        <v>62</v>
+        <v>120</v>
       </c>
       <c r="F6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H6">
-        <v>13000</v>
+        <v>42120</v>
       </c>
       <c r="I6">
-        <v>6500000</v>
+        <v>16200000</v>
       </c>
       <c r="J6">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>95</v>
+        <v>52</v>
       </c>
       <c r="E7" t="s">
-        <v>113</v>
+        <v>52</v>
       </c>
       <c r="F7" t="s">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H7">
-        <v>126360</v>
+        <v>17841.194</v>
       </c>
       <c r="I7">
-        <v>16200000</v>
+        <v>1049482</v>
       </c>
       <c r="J7">
-        <v>26000</v>
+        <v>17000</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="F8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G8" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="H8">
-        <v>44265.9</v>
+        <v>34500</v>
       </c>
       <c r="I8">
-        <v>4137000</v>
+        <v>1500000</v>
       </c>
       <c r="J8">
-        <v>10700</v>
+        <v>23000</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -3258,34 +3624,34 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="F9" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="G9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H9">
-        <v>34500</v>
+        <v>52000</v>
       </c>
       <c r="I9">
-        <v>1500000</v>
+        <v>2000000</v>
       </c>
       <c r="J9">
-        <v>23000</v>
+        <v>26000</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -3296,34 +3662,34 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="G10" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H10">
-        <v>52000</v>
+        <v>44265.9</v>
       </c>
       <c r="I10">
-        <v>2000000</v>
+        <v>4137000</v>
       </c>
       <c r="J10">
-        <v>26000</v>
+        <v>10700</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -3337,69 +3703,69 @@
         <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
       <c r="E11" t="s">
-        <v>57</v>
+        <v>120</v>
       </c>
       <c r="F11" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H11">
-        <v>33600</v>
+        <v>126360</v>
       </c>
       <c r="I11">
-        <v>2240000</v>
+        <v>16200000</v>
       </c>
       <c r="J11">
-        <v>15000</v>
+        <v>26000</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F12" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="G12" t="s">
         <v>27</v>
       </c>
       <c r="H12">
-        <v>9000</v>
+        <v>33600</v>
       </c>
       <c r="I12">
-        <v>4500000</v>
+        <v>2240000</v>
       </c>
       <c r="J12">
-        <v>2000</v>
+        <v>15000</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -3410,63 +3776,63 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="E13" t="s">
-        <v>113</v>
+        <v>65</v>
       </c>
       <c r="F13" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="G13" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="H13">
-        <v>12636</v>
+        <v>9000</v>
       </c>
       <c r="I13">
-        <v>16200000</v>
+        <v>4500000</v>
       </c>
       <c r="J13">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="L13">
-        <v>3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F14" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="G14" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="H14">
         <v>26400</v>
@@ -3486,294 +3852,294 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="E15" t="s">
-        <v>56</v>
+        <v>120</v>
       </c>
       <c r="F15" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G15" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H15">
-        <v>36000</v>
+        <v>12636</v>
       </c>
       <c r="I15">
-        <v>18000000</v>
+        <v>16200000</v>
       </c>
       <c r="J15">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15">
-        <v>100</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
         <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>95</v>
+        <v>53</v>
       </c>
       <c r="E16" t="s">
-        <v>113</v>
+        <v>53</v>
       </c>
       <c r="F16" t="s">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="G16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H16">
-        <v>4212</v>
+        <v>4966.368</v>
       </c>
       <c r="I16">
-        <v>16200000</v>
+        <v>1128720</v>
       </c>
       <c r="J16">
-        <v>26000</v>
+        <v>4400</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E17" t="s">
-        <v>114</v>
+        <v>53</v>
       </c>
       <c r="F17" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="G17" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H17">
-        <v>15484</v>
+        <v>36000</v>
       </c>
       <c r="I17">
-        <v>1580000</v>
+        <v>18000000</v>
       </c>
       <c r="J17">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
-        <v>70</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>99</v>
       </c>
       <c r="E18" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="F18" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="G18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H18">
-        <v>6636</v>
+        <v>4212</v>
       </c>
       <c r="I18">
-        <v>1580000</v>
+        <v>16200000</v>
       </c>
       <c r="J18">
-        <v>14000</v>
+        <v>26000</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18">
-        <v>30</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D19" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="E19" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="F19" t="s">
         <v>74</v>
       </c>
       <c r="G19" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="H19">
-        <v>12636</v>
+        <v>15484</v>
       </c>
       <c r="I19">
-        <v>16200000</v>
+        <v>1580000</v>
       </c>
       <c r="J19">
-        <v>26000</v>
+        <v>14000</v>
       </c>
       <c r="K19">
         <v>0</v>
       </c>
       <c r="L19">
-        <v>3</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="E20" t="s">
-        <v>46</v>
+        <v>121</v>
       </c>
       <c r="F20" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="G20" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="H20">
-        <v>5390</v>
+        <v>6636</v>
       </c>
       <c r="I20">
-        <v>770000</v>
+        <v>1580000</v>
       </c>
       <c r="J20">
-        <v>7000</v>
+        <v>14000</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
       <c r="L20">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D21" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="E21" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
       <c r="F21" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="G21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H21">
-        <v>12636</v>
+        <v>26000</v>
       </c>
       <c r="I21">
-        <v>16200000</v>
+        <v>4000000</v>
       </c>
       <c r="J21">
-        <v>26000</v>
+        <v>6500</v>
       </c>
       <c r="K21">
         <v>0</v>
       </c>
       <c r="L21">
-        <v>3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D22" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E22" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="F22" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="G22" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H22">
-        <v>126360</v>
+        <v>12636</v>
       </c>
       <c r="I22">
         <v>16200000</v>
@@ -3785,39 +4151,39 @@
         <v>0</v>
       </c>
       <c r="L22">
-        <v>30</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F23" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="G23" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H23">
-        <v>9500</v>
+        <v>5390</v>
       </c>
       <c r="I23">
-        <v>4750000</v>
+        <v>770000</v>
       </c>
       <c r="J23">
-        <v>2000</v>
+        <v>7000</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -3828,39 +4194,153 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D24" t="s">
-        <v>48</v>
+        <v>99</v>
       </c>
       <c r="E24" t="s">
-        <v>48</v>
+        <v>120</v>
       </c>
       <c r="F24" t="s">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="G24" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H24">
-        <v>8000</v>
+        <v>12636</v>
       </c>
       <c r="I24">
-        <v>4000000</v>
+        <v>16200000</v>
       </c>
       <c r="J24">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="K24">
         <v>0</v>
       </c>
       <c r="L24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" t="s">
+        <v>72</v>
+      </c>
+      <c r="G25" t="s">
+        <v>19</v>
+      </c>
+      <c r="H25">
+        <v>30600</v>
+      </c>
+      <c r="I25">
+        <v>1800000</v>
+      </c>
+      <c r="J25">
+        <v>17000</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" t="s">
+        <v>120</v>
+      </c>
+      <c r="F26" t="s">
+        <v>79</v>
+      </c>
+      <c r="G26" t="s">
+        <v>25</v>
+      </c>
+      <c r="H26">
+        <v>126360</v>
+      </c>
+      <c r="I26">
+        <v>16200000</v>
+      </c>
+      <c r="J26">
+        <v>26000</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" t="s">
+        <v>24</v>
+      </c>
+      <c r="H27">
+        <v>8000</v>
+      </c>
+      <c r="I27">
+        <v>4000000</v>
+      </c>
+      <c r="J27">
+        <v>2000</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2023-11-07
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="117">
   <si>
     <t>상장일</t>
   </si>
@@ -111,147 +111,138 @@
     <t>2023-09-25</t>
   </si>
   <si>
+    <t>KB제27호스팩</t>
+  </si>
+  <si>
+    <t>유진테크놀로지</t>
+  </si>
+  <si>
+    <t>유투바이오</t>
+  </si>
+  <si>
+    <t>퀄리타스반도체</t>
+  </si>
+  <si>
+    <t>워트</t>
+  </si>
+  <si>
+    <t>에스엘에스바이오</t>
+  </si>
+  <si>
+    <t>신성에스티</t>
+  </si>
+  <si>
+    <t>퓨릿</t>
+  </si>
+  <si>
+    <t>에이치엠씨제6호스팩</t>
+  </si>
+  <si>
+    <t>두산로보틱스</t>
+  </si>
+  <si>
+    <t>신한제11호스팩</t>
+  </si>
+  <si>
+    <t>한싹</t>
+  </si>
+  <si>
+    <t>레뷰코퍼레이션</t>
+  </si>
+  <si>
+    <t>아이엠티</t>
+  </si>
+  <si>
+    <t>밀리의서재</t>
+  </si>
+  <si>
+    <t>인스웨이브시스템즈</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>코스피</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>신한</t>
+  </si>
+  <si>
+    <t>한국</t>
+  </si>
+  <si>
+    <t>키움</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>현대차</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>신영</t>
+  </si>
+  <si>
+    <t>유비에스</t>
+  </si>
+  <si>
+    <t>삼성</t>
+  </si>
+  <si>
+    <t>유안타</t>
+  </si>
+  <si>
+    <t>유진</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>공동대표</t>
+  </si>
+  <si>
+    <t>공동</t>
+  </si>
+  <si>
+    <t>인수</t>
+  </si>
+  <si>
+    <t>2023-10-24</t>
+  </si>
+  <si>
+    <t>2023-10-23</t>
+  </si>
+  <si>
+    <t>2023-10-16</t>
+  </si>
+  <si>
+    <t>2023-09-21</t>
+  </si>
+  <si>
+    <t>2023-09-19</t>
+  </si>
+  <si>
+    <t>2023-09-18</t>
+  </si>
+  <si>
     <t>2023-09-14</t>
   </si>
   <si>
-    <t>KB제27호스팩</t>
-  </si>
-  <si>
-    <t>유진테크놀로지</t>
-  </si>
-  <si>
-    <t>유투바이오</t>
-  </si>
-  <si>
-    <t>퀄리타스반도체</t>
-  </si>
-  <si>
-    <t>워트</t>
-  </si>
-  <si>
-    <t>에스엘에스바이오</t>
-  </si>
-  <si>
-    <t>신성에스티</t>
-  </si>
-  <si>
-    <t>퓨릿</t>
-  </si>
-  <si>
-    <t>에이치엠씨제6호스팩</t>
-  </si>
-  <si>
-    <t>두산로보틱스</t>
-  </si>
-  <si>
-    <t>신한제11호스팩</t>
-  </si>
-  <si>
-    <t>한싹</t>
-  </si>
-  <si>
-    <t>레뷰코퍼레이션</t>
-  </si>
-  <si>
-    <t>아이엠티</t>
-  </si>
-  <si>
-    <t>밀리의서재</t>
-  </si>
-  <si>
-    <t>인스웨이브시스템즈</t>
-  </si>
-  <si>
-    <t>상상인제4호스팩</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>코스피</t>
-  </si>
-  <si>
-    <t>KB</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>신한</t>
-  </si>
-  <si>
-    <t>한국</t>
-  </si>
-  <si>
-    <t>키움</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>현대차</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t>신영</t>
-  </si>
-  <si>
-    <t>유비에스</t>
-  </si>
-  <si>
-    <t>삼성</t>
-  </si>
-  <si>
-    <t>유안타</t>
-  </si>
-  <si>
-    <t>유진</t>
-  </si>
-  <si>
-    <t>상상인</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>공동대표</t>
-  </si>
-  <si>
-    <t>공동</t>
-  </si>
-  <si>
-    <t>인수</t>
-  </si>
-  <si>
-    <t>2023-10-24</t>
-  </si>
-  <si>
-    <t>2023-10-23</t>
-  </si>
-  <si>
-    <t>2023-10-16</t>
-  </si>
-  <si>
-    <t>2023-09-21</t>
-  </si>
-  <si>
-    <t>2023-09-19</t>
-  </si>
-  <si>
-    <t>2023-09-18</t>
-  </si>
-  <si>
-    <t>2023-09-04</t>
-  </si>
-  <si>
     <t>2023-10-11</t>
   </si>
   <si>
@@ -261,9 +252,6 @@
     <t>2023-09-22</t>
   </si>
   <si>
-    <t>2023-09-07</t>
-  </si>
-  <si>
     <t>회사명</t>
   </si>
   <si>
@@ -364,9 +352,6 @@
   </si>
   <si>
     <t>619 : 1</t>
-  </si>
-  <si>
-    <t>1010.2 : 1</t>
   </si>
   <si>
     <t>인수기관</t>
@@ -739,7 +724,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -803,37 +788,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D2">
         <v>250</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F2">
         <v>250</v>
       </c>
       <c r="G2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M2">
         <v>2000</v>
@@ -842,7 +827,7 @@
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P2" t="s">
         <v>19</v>
@@ -856,37 +841,37 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D3">
         <v>178.41194</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F3">
         <v>178.41194</v>
       </c>
       <c r="G3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M3">
         <v>17000</v>
@@ -895,7 +880,7 @@
         <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="P3" t="s">
         <v>20</v>
@@ -909,37 +894,37 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D4">
         <v>49.66368</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F4">
         <v>49.66368</v>
       </c>
       <c r="G4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M4">
         <v>4400</v>
@@ -948,7 +933,7 @@
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="P4" t="s">
         <v>20</v>
@@ -962,37 +947,37 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D5">
         <v>306</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F5">
         <v>306</v>
       </c>
       <c r="G5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M5">
         <v>17000</v>
@@ -1004,7 +989,7 @@
         <v>23</v>
       </c>
       <c r="P5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="Q5">
         <v>1119600</v>
@@ -1015,37 +1000,37 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D6">
         <v>260</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F6">
         <v>260</v>
       </c>
       <c r="G6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M6">
         <v>6500</v>
@@ -1054,7 +1039,7 @@
         <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="P6" t="s">
         <v>22</v>
@@ -1068,37 +1053,37 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D7">
         <v>53.9</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F7">
         <v>53.9</v>
       </c>
       <c r="G7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M7">
         <v>7000</v>
@@ -1121,37 +1106,37 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D8">
         <v>520</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F8">
         <v>520</v>
       </c>
       <c r="G8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M8">
         <v>26000</v>
@@ -1174,37 +1159,37 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D9">
         <v>442.659</v>
       </c>
       <c r="E9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F9">
         <v>442.659</v>
       </c>
       <c r="G9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M9">
         <v>10700</v>
@@ -1216,7 +1201,7 @@
         <v>25</v>
       </c>
       <c r="P9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="Q9">
         <v>3102750</v>
@@ -1227,37 +1212,37 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D10">
         <v>80</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F10">
         <v>80</v>
       </c>
       <c r="G10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M10">
         <v>2000</v>
@@ -1280,37 +1265,37 @@
         <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D11">
         <v>4212</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F11">
         <v>1263.6</v>
       </c>
       <c r="G11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M11">
         <v>26000</v>
@@ -1319,10 +1304,10 @@
         <v>30</v>
       </c>
       <c r="O11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="P11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="Q11">
         <v>87871545</v>
@@ -1333,37 +1318,37 @@
         <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D12">
         <v>4212</v>
       </c>
       <c r="E12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F12">
         <v>1263.6</v>
       </c>
       <c r="G12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M12">
         <v>26000</v>
@@ -1372,10 +1357,10 @@
         <v>30</v>
       </c>
       <c r="O12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="P12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="Q12">
         <v>87871545</v>
@@ -1386,37 +1371,37 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D13">
         <v>4212</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F13">
         <v>421.2</v>
       </c>
       <c r="G13" t="s">
+        <v>63</v>
+      </c>
+      <c r="H13" t="s">
+        <v>63</v>
+      </c>
+      <c r="I13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" t="s">
+        <v>63</v>
+      </c>
+      <c r="K13" t="s">
         <v>66</v>
       </c>
-      <c r="H13" t="s">
-        <v>66</v>
-      </c>
-      <c r="I13" t="s">
-        <v>66</v>
-      </c>
-      <c r="J13" t="s">
-        <v>66</v>
-      </c>
-      <c r="K13" t="s">
-        <v>69</v>
-      </c>
       <c r="L13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M13">
         <v>26000</v>
@@ -1425,10 +1410,10 @@
         <v>10</v>
       </c>
       <c r="O13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="P13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="Q13">
         <v>87871545</v>
@@ -1439,37 +1424,37 @@
         <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D14">
         <v>4212</v>
       </c>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F14">
         <v>421.2</v>
       </c>
       <c r="G14" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" t="s">
+        <v>63</v>
+      </c>
+      <c r="I14" t="s">
+        <v>63</v>
+      </c>
+      <c r="J14" t="s">
+        <v>63</v>
+      </c>
+      <c r="K14" t="s">
         <v>66</v>
       </c>
-      <c r="H14" t="s">
-        <v>66</v>
-      </c>
-      <c r="I14" t="s">
-        <v>66</v>
-      </c>
-      <c r="J14" t="s">
-        <v>66</v>
-      </c>
-      <c r="K14" t="s">
-        <v>69</v>
-      </c>
       <c r="L14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M14">
         <v>26000</v>
@@ -1478,10 +1463,10 @@
         <v>10</v>
       </c>
       <c r="O14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="P14" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="Q14">
         <v>87871545</v>
@@ -1492,37 +1477,37 @@
         <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D15">
         <v>4212</v>
       </c>
       <c r="E15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F15">
         <v>421.2</v>
       </c>
       <c r="G15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H15" t="s">
+        <v>63</v>
+      </c>
+      <c r="I15" t="s">
+        <v>63</v>
+      </c>
+      <c r="J15" t="s">
+        <v>63</v>
+      </c>
+      <c r="K15" t="s">
         <v>66</v>
       </c>
-      <c r="H15" t="s">
-        <v>66</v>
-      </c>
-      <c r="I15" t="s">
-        <v>66</v>
-      </c>
-      <c r="J15" t="s">
-        <v>66</v>
-      </c>
-      <c r="K15" t="s">
-        <v>69</v>
-      </c>
       <c r="L15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M15">
         <v>26000</v>
@@ -1531,10 +1516,10 @@
         <v>10</v>
       </c>
       <c r="O15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="P15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="Q15">
         <v>87871545</v>
@@ -1545,37 +1530,37 @@
         <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D16">
         <v>4212</v>
       </c>
       <c r="E16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F16">
         <v>126.36</v>
       </c>
       <c r="G16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K16" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="L16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M16">
         <v>26000</v>
@@ -1584,10 +1569,10 @@
         <v>3</v>
       </c>
       <c r="O16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="P16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="Q16">
         <v>87871545</v>
@@ -1598,37 +1583,37 @@
         <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D17">
         <v>4212</v>
       </c>
       <c r="E17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F17">
         <v>126.36</v>
       </c>
       <c r="G17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="L17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M17">
         <v>26000</v>
@@ -1637,10 +1622,10 @@
         <v>3</v>
       </c>
       <c r="O17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="P17" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="Q17">
         <v>87871545</v>
@@ -1651,37 +1636,37 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D18">
         <v>4212</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F18">
         <v>126.36</v>
       </c>
       <c r="G18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K18" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="L18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M18">
         <v>26000</v>
@@ -1690,10 +1675,10 @@
         <v>3</v>
       </c>
       <c r="O18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="P18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="Q18">
         <v>87871545</v>
@@ -1704,37 +1689,37 @@
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D19">
         <v>4212</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F19">
         <v>42.12</v>
       </c>
       <c r="G19" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H19" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I19" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J19" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K19" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="L19" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M19">
         <v>26000</v>
@@ -1743,10 +1728,10 @@
         <v>1</v>
       </c>
       <c r="O19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="P19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="Q19">
         <v>87871545</v>
@@ -1757,37 +1742,37 @@
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D20">
         <v>360</v>
       </c>
       <c r="E20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F20">
         <v>360</v>
       </c>
       <c r="G20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K20" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M20">
         <v>2000</v>
@@ -1796,10 +1781,10 @@
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="P20" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="Q20">
         <v>13500000</v>
@@ -1810,37 +1795,37 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D21">
         <v>187.5</v>
       </c>
       <c r="E21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F21">
         <v>187.5</v>
       </c>
       <c r="G21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M21">
         <v>12500</v>
@@ -1849,10 +1834,10 @@
         <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="P21" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="Q21">
         <v>1020000</v>
@@ -1863,37 +1848,37 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D22">
         <v>336</v>
       </c>
       <c r="E22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F22">
         <v>336</v>
       </c>
       <c r="G22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K22" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M22">
         <v>15000</v>
@@ -1902,10 +1887,10 @@
         <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="P22" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="Q22">
         <v>1619200</v>
@@ -1916,37 +1901,37 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D23">
         <v>221.2</v>
       </c>
       <c r="E23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F23">
         <v>154.84</v>
       </c>
       <c r="G23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K23" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M23">
         <v>14000</v>
@@ -1955,10 +1940,10 @@
         <v>70</v>
       </c>
       <c r="O23" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P23" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="Q23">
         <v>2370000</v>
@@ -1969,37 +1954,37 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D24">
         <v>221.2</v>
       </c>
       <c r="E24" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F24">
         <v>66.36</v>
       </c>
       <c r="G24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="L24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M24">
         <v>14000</v>
@@ -2008,10 +1993,10 @@
         <v>30</v>
       </c>
       <c r="O24" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P24" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="Q24">
         <v>2370000</v>
@@ -2022,37 +2007,37 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D25">
         <v>345</v>
       </c>
       <c r="E25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F25">
         <v>345</v>
       </c>
       <c r="G25" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H25" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I25" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J25" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K25" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L25" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M25">
         <v>23000</v>
@@ -2061,10 +2046,10 @@
         <v>100</v>
       </c>
       <c r="O25" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="Q25">
         <v>1125000</v>
@@ -2075,37 +2060,37 @@
         <v>30</v>
       </c>
       <c r="B26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" t="s">
         <v>47</v>
-      </c>
-      <c r="C26" t="s">
-        <v>49</v>
       </c>
       <c r="D26">
         <v>264</v>
       </c>
       <c r="E26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F26">
         <v>264</v>
       </c>
       <c r="G26" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H26" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I26" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J26" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L26" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M26">
         <v>24000</v>
@@ -2114,66 +2099,13 @@
         <v>100</v>
       </c>
       <c r="O26" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="P26" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="Q26">
         <v>825000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17">
-      <c r="A27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" t="s">
-        <v>49</v>
-      </c>
-      <c r="D27">
-        <v>90</v>
-      </c>
-      <c r="E27" t="s">
-        <v>65</v>
-      </c>
-      <c r="F27">
-        <v>90</v>
-      </c>
-      <c r="G27" t="s">
-        <v>66</v>
-      </c>
-      <c r="H27" t="s">
-        <v>66</v>
-      </c>
-      <c r="I27" t="s">
-        <v>66</v>
-      </c>
-      <c r="J27" t="s">
-        <v>66</v>
-      </c>
-      <c r="K27" t="s">
-        <v>67</v>
-      </c>
-      <c r="L27" t="s">
-        <v>66</v>
-      </c>
-      <c r="M27">
-        <v>2000</v>
-      </c>
-      <c r="N27">
-        <v>100</v>
-      </c>
-      <c r="O27" t="s">
-        <v>77</v>
-      </c>
-      <c r="P27" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q27">
-        <v>3375000</v>
       </c>
     </row>
   </sheetData>
@@ -2183,7 +2115,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T18"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2194,10 +2126,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -2206,60 +2138,60 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -2274,7 +2206,7 @@
         <v>12500000</v>
       </c>
       <c r="H2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I2">
         <v>2000</v>
@@ -2283,45 +2215,45 @@
         <v>2000</v>
       </c>
       <c r="K2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L2">
         <v>2000</v>
       </c>
       <c r="M2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="R2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="S2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="T2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
@@ -2336,7 +2268,7 @@
         <v>1049482</v>
       </c>
       <c r="H3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I3">
         <v>12800</v>
@@ -2345,45 +2277,45 @@
         <v>14500</v>
       </c>
       <c r="K3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L3">
         <v>17000</v>
       </c>
       <c r="M3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O3">
         <v>9.999980942979489</v>
       </c>
       <c r="P3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="R3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="S3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="T3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
@@ -2398,7 +2330,7 @@
         <v>1128720</v>
       </c>
       <c r="H4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I4">
         <v>3300</v>
@@ -2407,34 +2339,34 @@
         <v>3900</v>
       </c>
       <c r="K4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L4">
         <v>4400</v>
       </c>
       <c r="M4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="R4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="S4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="T4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -2442,13 +2374,13 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
@@ -2460,7 +2392,7 @@
         <v>1800000</v>
       </c>
       <c r="H5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I5">
         <v>13000</v>
@@ -2469,45 +2401,45 @@
         <v>15000</v>
       </c>
       <c r="K5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L5">
         <v>17000</v>
       </c>
       <c r="M5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="R5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="S5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="T5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
         <v>22</v>
@@ -2522,7 +2454,7 @@
         <v>4000000</v>
       </c>
       <c r="H6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I6">
         <v>5000</v>
@@ -2531,34 +2463,34 @@
         <v>5600</v>
       </c>
       <c r="K6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L6">
         <v>6500</v>
       </c>
       <c r="M6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="R6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="S6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="T6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -2566,10 +2498,10 @@
         <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
         <v>24</v>
@@ -2584,7 +2516,7 @@
         <v>770000</v>
       </c>
       <c r="H7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I7">
         <v>8200</v>
@@ -2593,34 +2525,34 @@
         <v>9400</v>
       </c>
       <c r="K7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L7">
         <v>7000</v>
       </c>
       <c r="M7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="R7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="S7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="T7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -2628,10 +2560,10 @@
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D8" t="s">
         <v>24</v>
@@ -2646,7 +2578,7 @@
         <v>2000000</v>
       </c>
       <c r="H8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I8">
         <v>22000</v>
@@ -2655,34 +2587,34 @@
         <v>25000</v>
       </c>
       <c r="K8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L8">
         <v>26000</v>
       </c>
       <c r="M8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="R8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="S8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="T8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -2690,13 +2622,13 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E9" t="s">
         <v>23</v>
@@ -2708,7 +2640,7 @@
         <v>4137000</v>
       </c>
       <c r="H9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I9">
         <v>8800</v>
@@ -2717,34 +2649,34 @@
         <v>10700</v>
       </c>
       <c r="K9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L9">
         <v>10700</v>
       </c>
       <c r="M9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O9">
         <v>30.21513173797438</v>
       </c>
       <c r="P9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="R9" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="S9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="T9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -2752,10 +2684,10 @@
         <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D10" t="s">
         <v>26</v>
@@ -2770,7 +2702,7 @@
         <v>4000000</v>
       </c>
       <c r="H10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I10">
         <v>2000</v>
@@ -2779,48 +2711,48 @@
         <v>2000</v>
       </c>
       <c r="K10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L10">
         <v>2000</v>
       </c>
       <c r="M10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="R10" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="S10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="T10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E11" t="s">
         <v>25</v>
@@ -2832,7 +2764,7 @@
         <v>16200000</v>
       </c>
       <c r="H11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I11">
         <v>21000</v>
@@ -2841,48 +2773,48 @@
         <v>26000</v>
       </c>
       <c r="K11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L11">
         <v>26000</v>
       </c>
       <c r="M11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="R11" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="S11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="T11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E12" t="s">
         <v>26</v>
@@ -2894,7 +2826,7 @@
         <v>18000000</v>
       </c>
       <c r="H12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I12">
         <v>2000</v>
@@ -2903,48 +2835,48 @@
         <v>2000</v>
       </c>
       <c r="K12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L12">
         <v>2000</v>
       </c>
       <c r="M12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="R12" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="S12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="T12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E13" t="s">
         <v>26</v>
@@ -2956,7 +2888,7 @@
         <v>1500000</v>
       </c>
       <c r="H13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I13">
         <v>8900</v>
@@ -2965,48 +2897,48 @@
         <v>11000</v>
       </c>
       <c r="K13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L13">
         <v>12500</v>
       </c>
       <c r="M13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="R13" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="S13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="T13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D14" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E14" t="s">
         <v>27</v>
@@ -3018,7 +2950,7 @@
         <v>2240000</v>
       </c>
       <c r="H14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I14">
         <v>11500</v>
@@ -3027,48 +2959,48 @@
         <v>13200</v>
       </c>
       <c r="K14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L14">
         <v>15000</v>
       </c>
       <c r="M14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O14">
         <v>26.78571428571428</v>
       </c>
       <c r="P14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="R14" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="S14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="T14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E15" t="s">
         <v>28</v>
@@ -3080,7 +3012,7 @@
         <v>1580000</v>
       </c>
       <c r="H15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I15">
         <v>10500</v>
@@ -3089,48 +3021,48 @@
         <v>12000</v>
       </c>
       <c r="K15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L15">
         <v>14000</v>
       </c>
       <c r="M15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="R15" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="S15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="T15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E16" t="s">
         <v>29</v>
@@ -3142,7 +3074,7 @@
         <v>1500000</v>
       </c>
       <c r="H16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I16">
         <v>20000</v>
@@ -3151,48 +3083,48 @@
         <v>23000</v>
       </c>
       <c r="K16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L16">
         <v>23000</v>
       </c>
       <c r="M16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="R16" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="S16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="T16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E17" t="s">
         <v>30</v>
@@ -3204,7 +3136,7 @@
         <v>1100000</v>
       </c>
       <c r="H17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I17">
         <v>20000</v>
@@ -3213,96 +3145,34 @@
         <v>24000</v>
       </c>
       <c r="K17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L17">
         <v>24000</v>
       </c>
       <c r="M17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O17">
         <v>18.18181818181818</v>
       </c>
       <c r="P17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="R17" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="S17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="T17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20">
-      <c r="A18" t="s">
-        <v>77</v>
-      </c>
-      <c r="B18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18">
-        <v>9000000</v>
-      </c>
-      <c r="G18">
-        <v>4500000</v>
-      </c>
-      <c r="H18" t="s">
-        <v>66</v>
-      </c>
-      <c r="I18">
-        <v>2000</v>
-      </c>
-      <c r="J18">
-        <v>2000</v>
-      </c>
-      <c r="K18" t="s">
-        <v>66</v>
-      </c>
-      <c r="L18">
-        <v>2000</v>
-      </c>
-      <c r="M18" t="s">
-        <v>66</v>
-      </c>
-      <c r="N18" t="s">
-        <v>66</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>66</v>
-      </c>
-      <c r="R18" t="s">
-        <v>116</v>
-      </c>
-      <c r="S18" t="s">
-        <v>66</v>
-      </c>
-      <c r="T18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -3312,7 +3182,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3320,16 +3190,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -3341,10 +3211,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -3353,27 +3223,27 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G2" t="s">
         <v>25</v>
@@ -3396,19 +3266,19 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F3" t="s">
         <v>19</v>
@@ -3434,22 +3304,22 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G4" t="s">
         <v>26</v>
@@ -3472,22 +3342,22 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E5" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G5" t="s">
         <v>25</v>
@@ -3510,22 +3380,22 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E6" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G6" t="s">
         <v>25</v>
@@ -3548,19 +3418,19 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F7" t="s">
         <v>20</v>
@@ -3586,34 +3456,34 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F8" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="H8">
-        <v>34500</v>
+        <v>52000</v>
       </c>
       <c r="I8">
-        <v>1500000</v>
+        <v>2000000</v>
       </c>
       <c r="J8">
-        <v>23000</v>
+        <v>26000</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -3624,34 +3494,34 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
         <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="G9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H9">
-        <v>52000</v>
+        <v>44265.9</v>
       </c>
       <c r="I9">
-        <v>2000000</v>
+        <v>4137000</v>
       </c>
       <c r="J9">
-        <v>26000</v>
+        <v>10700</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -3662,98 +3532,98 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" t="s">
         <v>25</v>
       </c>
-      <c r="C10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F10" t="s">
-        <v>78</v>
-      </c>
-      <c r="G10" t="s">
-        <v>23</v>
-      </c>
       <c r="H10">
-        <v>44265.9</v>
+        <v>126360</v>
       </c>
       <c r="I10">
-        <v>4137000</v>
+        <v>16200000</v>
       </c>
       <c r="J10">
-        <v>10700</v>
+        <v>26000</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
-        <v>120</v>
+        <v>55</v>
       </c>
       <c r="F11" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G11" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="H11">
-        <v>126360</v>
+        <v>34500</v>
       </c>
       <c r="I11">
-        <v>16200000</v>
+        <v>1500000</v>
       </c>
       <c r="J11">
-        <v>26000</v>
+        <v>23000</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G12" t="s">
         <v>27</v>
@@ -3776,34 +3646,34 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E13" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="F13" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H13">
-        <v>9000</v>
+        <v>26400</v>
       </c>
       <c r="I13">
-        <v>4500000</v>
+        <v>1100000</v>
       </c>
       <c r="J13">
-        <v>2000</v>
+        <v>24000</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -3814,110 +3684,110 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="F14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G14" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H14">
-        <v>26400</v>
+        <v>12636</v>
       </c>
       <c r="I14">
-        <v>1100000</v>
+        <v>16200000</v>
       </c>
       <c r="J14">
-        <v>24000</v>
+        <v>26000</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14">
-        <v>100</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>99</v>
+        <v>51</v>
       </c>
       <c r="E15" t="s">
-        <v>120</v>
+        <v>51</v>
       </c>
       <c r="F15" t="s">
-        <v>79</v>
+        <v>20</v>
       </c>
       <c r="G15" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H15">
-        <v>12636</v>
+        <v>4966.368</v>
       </c>
       <c r="I15">
-        <v>16200000</v>
+        <v>1128720</v>
       </c>
       <c r="J15">
-        <v>26000</v>
+        <v>4400</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15">
-        <v>3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
         <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F16" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="G16" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="H16">
-        <v>4966.368</v>
+        <v>36000</v>
       </c>
       <c r="I16">
-        <v>1128720</v>
+        <v>18000000</v>
       </c>
       <c r="J16">
-        <v>4400</v>
+        <v>2000</v>
       </c>
       <c r="K16">
         <v>0</v>
@@ -3928,40 +3798,40 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>95</v>
       </c>
       <c r="E17" t="s">
-        <v>53</v>
+        <v>115</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H17">
-        <v>36000</v>
+        <v>4212</v>
       </c>
       <c r="I17">
-        <v>18000000</v>
+        <v>16200000</v>
       </c>
       <c r="J17">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -3969,63 +3839,63 @@
         <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D18" t="s">
-        <v>99</v>
+        <v>61</v>
       </c>
       <c r="E18" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F18" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G18" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H18">
-        <v>4212</v>
+        <v>15484</v>
       </c>
       <c r="I18">
-        <v>16200000</v>
+        <v>1580000</v>
       </c>
       <c r="J18">
-        <v>26000</v>
+        <v>14000</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18">
-        <v>1</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E19" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G19" t="s">
         <v>28</v>
       </c>
       <c r="H19">
-        <v>15484</v>
+        <v>6636</v>
       </c>
       <c r="I19">
         <v>1580000</v>
@@ -4037,310 +3907,272 @@
         <v>0</v>
       </c>
       <c r="L19">
-        <v>70</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E20" t="s">
-        <v>121</v>
+        <v>53</v>
       </c>
       <c r="F20" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="G20" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="H20">
-        <v>6636</v>
+        <v>26000</v>
       </c>
       <c r="I20">
-        <v>1580000</v>
+        <v>4000000</v>
       </c>
       <c r="J20">
-        <v>14000</v>
+        <v>6500</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
       <c r="L20">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="E21" t="s">
-        <v>55</v>
+        <v>115</v>
       </c>
       <c r="F21" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="G21" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H21">
+        <v>12636</v>
+      </c>
+      <c r="I21">
+        <v>16200000</v>
+      </c>
+      <c r="J21">
         <v>26000</v>
-      </c>
-      <c r="I21">
-        <v>4000000</v>
-      </c>
-      <c r="J21">
-        <v>6500</v>
       </c>
       <c r="K21">
         <v>0</v>
       </c>
       <c r="L21">
-        <v>100</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>99</v>
+        <v>54</v>
       </c>
       <c r="E22" t="s">
-        <v>120</v>
+        <v>54</v>
       </c>
       <c r="F22" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="G22" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H22">
-        <v>12636</v>
+        <v>5390</v>
       </c>
       <c r="I22">
-        <v>16200000</v>
+        <v>770000</v>
       </c>
       <c r="J22">
-        <v>26000</v>
+        <v>7000</v>
       </c>
       <c r="K22">
         <v>0</v>
       </c>
       <c r="L22">
-        <v>3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D23" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
       <c r="E23" t="s">
-        <v>56</v>
+        <v>115</v>
       </c>
       <c r="F23" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="G23" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H23">
-        <v>5390</v>
+        <v>12636</v>
       </c>
       <c r="I23">
-        <v>770000</v>
+        <v>16200000</v>
       </c>
       <c r="J23">
-        <v>7000</v>
+        <v>26000</v>
       </c>
       <c r="K23">
         <v>0</v>
       </c>
       <c r="L23">
-        <v>100</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D24" t="s">
-        <v>99</v>
+        <v>52</v>
       </c>
       <c r="E24" t="s">
-        <v>120</v>
+        <v>52</v>
       </c>
       <c r="F24" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G24" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H24">
-        <v>12636</v>
+        <v>30600</v>
       </c>
       <c r="I24">
-        <v>16200000</v>
+        <v>1800000</v>
       </c>
       <c r="J24">
-        <v>26000</v>
+        <v>17000</v>
       </c>
       <c r="K24">
         <v>0</v>
       </c>
       <c r="L24">
-        <v>3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D25" t="s">
-        <v>54</v>
+        <v>95</v>
       </c>
       <c r="E25" t="s">
-        <v>54</v>
+        <v>115</v>
       </c>
       <c r="F25" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="G25" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H25">
-        <v>30600</v>
+        <v>126360</v>
       </c>
       <c r="I25">
-        <v>1800000</v>
+        <v>16200000</v>
       </c>
       <c r="J25">
-        <v>17000</v>
+        <v>26000</v>
       </c>
       <c r="K25">
         <v>0</v>
       </c>
       <c r="L25">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D26" t="s">
-        <v>99</v>
+        <v>56</v>
       </c>
       <c r="E26" t="s">
-        <v>120</v>
+        <v>56</v>
       </c>
       <c r="F26" t="s">
-        <v>79</v>
+        <v>26</v>
       </c>
       <c r="G26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H26">
-        <v>126360</v>
+        <v>8000</v>
       </c>
       <c r="I26">
-        <v>16200000</v>
+        <v>4000000</v>
       </c>
       <c r="J26">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="K26">
         <v>0</v>
       </c>
       <c r="L26">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" t="s">
-        <v>58</v>
-      </c>
-      <c r="E27" t="s">
-        <v>58</v>
-      </c>
-      <c r="F27" t="s">
-        <v>26</v>
-      </c>
-      <c r="G27" t="s">
-        <v>24</v>
-      </c>
-      <c r="H27">
-        <v>8000</v>
-      </c>
-      <c r="I27">
-        <v>4000000</v>
-      </c>
-      <c r="J27">
-        <v>2000</v>
-      </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-      <c r="L27">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2023-11-08
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="121">
   <si>
     <t>상장일</t>
   </si>
@@ -69,6 +69,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2023-11-07</t>
+  </si>
+  <si>
     <t>2023-11-03</t>
   </si>
   <si>
@@ -111,6 +114,9 @@
     <t>2023-09-25</t>
   </si>
   <si>
+    <t>쏘닉스</t>
+  </si>
+  <si>
     <t>KB제27호스팩</t>
   </si>
   <si>
@@ -243,6 +249,9 @@
     <t>2023-09-14</t>
   </si>
   <si>
+    <t>2023-10-31</t>
+  </si>
+  <si>
     <t>2023-10-11</t>
   </si>
   <si>
@@ -304,6 +313,9 @@
   </si>
   <si>
     <t>한국, 미래</t>
+  </si>
+  <si>
+    <t>773.94 : 1</t>
   </si>
   <si>
     <t>8.1 : 1</t>
@@ -724,7 +736,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -788,52 +800,52 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D2">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F2">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="G2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M2">
-        <v>2000</v>
+        <v>7500</v>
       </c>
       <c r="N2">
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="P2" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="Q2">
-        <v>9375000</v>
+        <v>2600000</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -841,105 +853,105 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D3">
-        <v>178.41194</v>
+        <v>250</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F3">
-        <v>178.41194</v>
+        <v>250</v>
       </c>
       <c r="G3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M3">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="N3">
         <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="P3" t="s">
         <v>20</v>
       </c>
       <c r="Q3">
-        <v>787111</v>
+        <v>9375000</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D4">
-        <v>49.66368</v>
+        <v>178.41194</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F4">
-        <v>49.66368</v>
+        <v>178.41194</v>
       </c>
       <c r="G4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M4">
-        <v>4400</v>
+        <v>17000</v>
       </c>
       <c r="N4">
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="P4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q4">
-        <v>846540</v>
+        <v>787111</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -947,52 +959,52 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D5">
-        <v>306</v>
+        <v>49.66368</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F5">
-        <v>306</v>
+        <v>49.66368</v>
       </c>
       <c r="G5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M5">
-        <v>17000</v>
+        <v>4400</v>
       </c>
       <c r="N5">
         <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="P5" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="Q5">
-        <v>1119600</v>
+        <v>846540</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1000,52 +1012,52 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D6">
-        <v>260</v>
+        <v>306</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F6">
-        <v>260</v>
+        <v>306</v>
       </c>
       <c r="G6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M6">
-        <v>6500</v>
+        <v>17000</v>
       </c>
       <c r="N6">
         <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="P6" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="Q6">
-        <v>2880000</v>
+        <v>1119600</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1053,52 +1065,52 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D7">
-        <v>53.9</v>
+        <v>260</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F7">
-        <v>53.9</v>
+        <v>260</v>
       </c>
       <c r="G7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M7">
-        <v>7000</v>
+        <v>6500</v>
       </c>
       <c r="N7">
         <v>100</v>
       </c>
       <c r="O7" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="P7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q7">
-        <v>577500</v>
+        <v>2880000</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1106,52 +1118,52 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D8">
-        <v>520</v>
+        <v>53.9</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F8">
-        <v>520</v>
+        <v>53.9</v>
       </c>
       <c r="G8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M8">
-        <v>26000</v>
+        <v>7000</v>
       </c>
       <c r="N8">
         <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q8">
-        <v>1300000</v>
+        <v>577500</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1159,52 +1171,52 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D9">
-        <v>442.659</v>
+        <v>520</v>
       </c>
       <c r="E9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F9">
-        <v>442.659</v>
+        <v>520</v>
       </c>
       <c r="G9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M9">
-        <v>10700</v>
+        <v>26000</v>
       </c>
       <c r="N9">
         <v>100</v>
       </c>
       <c r="O9" t="s">
+        <v>29</v>
+      </c>
+      <c r="P9" t="s">
         <v>25</v>
       </c>
-      <c r="P9" t="s">
-        <v>75</v>
-      </c>
       <c r="Q9">
-        <v>3102750</v>
+        <v>1300000</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1212,52 +1224,52 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D10">
-        <v>80</v>
+        <v>442.659</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F10">
-        <v>80</v>
+        <v>442.659</v>
       </c>
       <c r="G10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M10">
-        <v>2000</v>
+        <v>10700</v>
       </c>
       <c r="N10">
         <v>100</v>
       </c>
       <c r="O10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="P10" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="Q10">
-        <v>3000000</v>
+        <v>3102750</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1265,90 +1277,90 @@
         <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D11">
-        <v>4212</v>
+        <v>80</v>
       </c>
       <c r="E11" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="F11">
-        <v>1263.6</v>
+        <v>80</v>
       </c>
       <c r="G11" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H11" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I11" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J11" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L11" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M11">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="N11">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="P11" t="s">
-        <v>76</v>
+        <v>27</v>
       </c>
       <c r="Q11">
-        <v>87871545</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D12">
         <v>4212</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F12">
         <v>1263.6</v>
       </c>
       <c r="G12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K12" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M12">
         <v>26000</v>
@@ -1357,10 +1369,10 @@
         <v>30</v>
       </c>
       <c r="O12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="P12" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="Q12">
         <v>87871545</v>
@@ -1368,52 +1380,52 @@
     </row>
     <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D13">
         <v>4212</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F13">
-        <v>421.2</v>
+        <v>1263.6</v>
       </c>
       <c r="G13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M13">
         <v>26000</v>
       </c>
       <c r="N13">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="O13" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="P13" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="Q13">
         <v>87871545</v>
@@ -1421,40 +1433,40 @@
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D14">
         <v>4212</v>
       </c>
       <c r="E14" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F14">
         <v>421.2</v>
       </c>
       <c r="G14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M14">
         <v>26000</v>
@@ -1463,10 +1475,10 @@
         <v>10</v>
       </c>
       <c r="O14" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="P14" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="Q14">
         <v>87871545</v>
@@ -1474,40 +1486,40 @@
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D15">
         <v>4212</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F15">
         <v>421.2</v>
       </c>
       <c r="G15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M15">
         <v>26000</v>
@@ -1516,10 +1528,10 @@
         <v>10</v>
       </c>
       <c r="O15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="P15" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="Q15">
         <v>87871545</v>
@@ -1527,52 +1539,52 @@
     </row>
     <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D16">
         <v>4212</v>
       </c>
       <c r="E16" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F16">
-        <v>126.36</v>
+        <v>421.2</v>
       </c>
       <c r="G16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M16">
         <v>26000</v>
       </c>
       <c r="N16">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="O16" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="P16" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="Q16">
         <v>87871545</v>
@@ -1580,40 +1592,40 @@
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D17">
         <v>4212</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F17">
         <v>126.36</v>
       </c>
       <c r="G17" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H17" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I17" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J17" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L17" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M17">
         <v>26000</v>
@@ -1622,10 +1634,10 @@
         <v>3</v>
       </c>
       <c r="O17" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="P17" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="Q17">
         <v>87871545</v>
@@ -1633,40 +1645,40 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D18">
         <v>4212</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F18">
         <v>126.36</v>
       </c>
       <c r="G18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M18">
         <v>26000</v>
@@ -1675,10 +1687,10 @@
         <v>3</v>
       </c>
       <c r="O18" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="P18" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="Q18">
         <v>87871545</v>
@@ -1686,52 +1698,52 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D19">
         <v>4212</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F19">
-        <v>42.12</v>
+        <v>126.36</v>
       </c>
       <c r="G19" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H19" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I19" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J19" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K19" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L19" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M19">
         <v>26000</v>
       </c>
       <c r="N19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O19" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="P19" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="Q19">
         <v>87871545</v>
@@ -1742,105 +1754,105 @@
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D20">
-        <v>360</v>
+        <v>4212</v>
       </c>
       <c r="E20" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="F20">
-        <v>360</v>
+        <v>42.12</v>
       </c>
       <c r="G20" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H20" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I20" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J20" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K20" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="L20" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M20">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="N20">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="O20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="P20" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="Q20">
-        <v>13500000</v>
+        <v>87871545</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D21">
-        <v>187.5</v>
+        <v>360</v>
       </c>
       <c r="E21" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="F21">
-        <v>187.5</v>
+        <v>360</v>
       </c>
       <c r="G21" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H21" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I21" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J21" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K21" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L21" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M21">
-        <v>12500</v>
+        <v>2000</v>
       </c>
       <c r="N21">
         <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="P21" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="Q21">
-        <v>1020000</v>
+        <v>13500000</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1848,52 +1860,52 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D22">
-        <v>336</v>
+        <v>187.5</v>
       </c>
       <c r="E22" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F22">
-        <v>336</v>
+        <v>187.5</v>
       </c>
       <c r="G22" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H22" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I22" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J22" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K22" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L22" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M22">
-        <v>15000</v>
+        <v>12500</v>
       </c>
       <c r="N22">
         <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="P22" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="Q22">
-        <v>1619200</v>
+        <v>1020000</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1901,102 +1913,102 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D23">
-        <v>221.2</v>
+        <v>336</v>
       </c>
       <c r="E23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F23">
-        <v>154.84</v>
+        <v>336</v>
       </c>
       <c r="G23" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H23" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I23" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J23" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K23" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L23" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M23">
-        <v>14000</v>
+        <v>15000</v>
       </c>
       <c r="N23">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="P23" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="Q23">
-        <v>2370000</v>
+        <v>1619200</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D24">
         <v>221.2</v>
       </c>
       <c r="E24" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F24">
-        <v>66.36</v>
+        <v>154.84</v>
       </c>
       <c r="G24" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H24" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I24" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J24" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L24" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M24">
         <v>14000</v>
       </c>
       <c r="N24">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="O24" t="s">
+        <v>75</v>
+      </c>
+      <c r="P24" t="s">
         <v>73</v>
-      </c>
-      <c r="P24" t="s">
-        <v>71</v>
       </c>
       <c r="Q24">
         <v>2370000</v>
@@ -2007,52 +2019,52 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D25">
-        <v>345</v>
+        <v>221.2</v>
       </c>
       <c r="E25" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F25">
-        <v>345</v>
+        <v>66.36</v>
       </c>
       <c r="G25" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H25" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I25" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J25" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K25" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="L25" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M25">
-        <v>23000</v>
+        <v>14000</v>
       </c>
       <c r="N25">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="O25" t="s">
+        <v>75</v>
+      </c>
+      <c r="P25" t="s">
         <v>73</v>
       </c>
-      <c r="P25" t="s">
-        <v>71</v>
-      </c>
       <c r="Q25">
-        <v>1125000</v>
+        <v>2370000</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -2060,51 +2072,104 @@
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C26" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D26">
-        <v>264</v>
+        <v>345</v>
       </c>
       <c r="E26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F26">
-        <v>264</v>
+        <v>345</v>
       </c>
       <c r="G26" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H26" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I26" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J26" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K26" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L26" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M26">
-        <v>24000</v>
+        <v>23000</v>
       </c>
       <c r="N26">
         <v>100</v>
       </c>
       <c r="O26" t="s">
+        <v>75</v>
+      </c>
+      <c r="P26" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q26">
+        <v>1125000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27">
+        <v>264</v>
+      </c>
+      <c r="E27" t="s">
+        <v>60</v>
+      </c>
+      <c r="F27">
+        <v>264</v>
+      </c>
+      <c r="G27" t="s">
+        <v>65</v>
+      </c>
+      <c r="H27" t="s">
+        <v>65</v>
+      </c>
+      <c r="I27" t="s">
+        <v>65</v>
+      </c>
+      <c r="J27" t="s">
+        <v>65</v>
+      </c>
+      <c r="K27" t="s">
+        <v>66</v>
+      </c>
+      <c r="L27" t="s">
+        <v>65</v>
+      </c>
+      <c r="M27">
+        <v>24000</v>
+      </c>
+      <c r="N27">
+        <v>100</v>
+      </c>
+      <c r="O27" t="s">
+        <v>76</v>
+      </c>
+      <c r="P27" t="s">
         <v>74</v>
       </c>
-      <c r="P26" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q26">
+      <c r="Q27">
         <v>825000</v>
       </c>
     </row>
@@ -2115,7 +2180,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2126,10 +2191,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -2138,122 +2203,122 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
       </c>
       <c r="F2">
-        <v>25000000</v>
+        <v>27000000</v>
       </c>
       <c r="G2">
-        <v>12500000</v>
+        <v>3600000</v>
       </c>
       <c r="H2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I2">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="J2">
-        <v>2000</v>
+        <v>7000</v>
       </c>
       <c r="K2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L2">
-        <v>2000</v>
+        <v>7500</v>
       </c>
       <c r="M2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="N2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="Q2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="R2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="S2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="T2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
@@ -2262,917 +2327,979 @@
         <v>18</v>
       </c>
       <c r="F3">
-        <v>17841194</v>
+        <v>25000000</v>
       </c>
       <c r="G3">
-        <v>1049482</v>
+        <v>12500000</v>
       </c>
       <c r="H3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I3">
-        <v>12800</v>
+        <v>2000</v>
       </c>
       <c r="J3">
-        <v>14500</v>
+        <v>2000</v>
       </c>
       <c r="K3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L3">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="M3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="N3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="O3">
-        <v>9.999980942979489</v>
+        <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="Q3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="R3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="T3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4">
-        <v>4966368</v>
+        <v>17841194</v>
       </c>
       <c r="G4">
-        <v>1128720</v>
+        <v>1049482</v>
       </c>
       <c r="H4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I4">
-        <v>3300</v>
+        <v>12800</v>
       </c>
       <c r="J4">
-        <v>3900</v>
+        <v>14500</v>
       </c>
       <c r="K4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L4">
-        <v>4400</v>
+        <v>17000</v>
       </c>
       <c r="M4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="N4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>9.999980942979489</v>
       </c>
       <c r="P4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="Q4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="R4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="S4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="T4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
       </c>
       <c r="F5">
-        <v>30600000</v>
+        <v>4966368</v>
       </c>
       <c r="G5">
-        <v>1800000</v>
+        <v>1128720</v>
       </c>
       <c r="H5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I5">
-        <v>13000</v>
+        <v>3300</v>
       </c>
       <c r="J5">
-        <v>15000</v>
+        <v>3900</v>
       </c>
       <c r="K5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L5">
-        <v>17000</v>
+        <v>4400</v>
       </c>
       <c r="M5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="N5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="Q5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="R5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="S5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="T5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="E6" t="s">
         <v>20</v>
       </c>
       <c r="F6">
-        <v>26000000</v>
+        <v>30600000</v>
       </c>
       <c r="G6">
-        <v>4000000</v>
+        <v>1800000</v>
       </c>
       <c r="H6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I6">
-        <v>5000</v>
+        <v>13000</v>
       </c>
       <c r="J6">
-        <v>5600</v>
+        <v>15000</v>
       </c>
       <c r="K6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L6">
-        <v>6500</v>
+        <v>17000</v>
       </c>
       <c r="M6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="N6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="Q6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="R6" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="S6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="T6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
         <v>21</v>
       </c>
       <c r="F7">
-        <v>5390000</v>
+        <v>26000000</v>
       </c>
       <c r="G7">
-        <v>770000</v>
+        <v>4000000</v>
       </c>
       <c r="H7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I7">
-        <v>8200</v>
+        <v>5000</v>
       </c>
       <c r="J7">
-        <v>9400</v>
+        <v>5600</v>
       </c>
       <c r="K7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L7">
-        <v>7000</v>
+        <v>6500</v>
       </c>
       <c r="M7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="N7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="Q7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="R7" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="S7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="T7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
         <v>22</v>
       </c>
       <c r="F8">
-        <v>52000000</v>
+        <v>5390000</v>
       </c>
       <c r="G8">
-        <v>2000000</v>
+        <v>770000</v>
       </c>
       <c r="H8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I8">
-        <v>22000</v>
+        <v>8200</v>
       </c>
       <c r="J8">
-        <v>25000</v>
+        <v>9400</v>
       </c>
       <c r="K8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L8">
-        <v>26000</v>
+        <v>7000</v>
       </c>
       <c r="M8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="N8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="Q8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="R8" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="S8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="T8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" t="s">
         <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" t="s">
-        <v>75</v>
       </c>
       <c r="E9" t="s">
         <v>23</v>
       </c>
       <c r="F9">
-        <v>44265900</v>
+        <v>52000000</v>
       </c>
       <c r="G9">
-        <v>4137000</v>
+        <v>2000000</v>
       </c>
       <c r="H9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I9">
-        <v>8800</v>
+        <v>22000</v>
       </c>
       <c r="J9">
-        <v>10700</v>
+        <v>25000</v>
       </c>
       <c r="K9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L9">
-        <v>10700</v>
+        <v>26000</v>
       </c>
       <c r="M9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="N9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="O9">
-        <v>30.21513173797438</v>
+        <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="Q9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="R9" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="S9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="T9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="E10" t="s">
         <v>24</v>
       </c>
       <c r="F10">
-        <v>8000000</v>
+        <v>44265900</v>
       </c>
       <c r="G10">
-        <v>4000000</v>
+        <v>4137000</v>
       </c>
       <c r="H10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I10">
-        <v>2000</v>
+        <v>8800</v>
       </c>
       <c r="J10">
-        <v>2000</v>
+        <v>10700</v>
       </c>
       <c r="K10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L10">
-        <v>2000</v>
+        <v>10700</v>
       </c>
       <c r="M10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="N10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="O10">
-        <v>0</v>
+        <v>30.21513173797438</v>
       </c>
       <c r="P10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="Q10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="R10" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="S10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="T10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="D11" t="s">
-        <v>76</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
         <v>25</v>
       </c>
       <c r="F11">
-        <v>421200000</v>
+        <v>8000000</v>
       </c>
       <c r="G11">
-        <v>16200000</v>
+        <v>4000000</v>
       </c>
       <c r="H11" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I11">
-        <v>21000</v>
+        <v>2000</v>
       </c>
       <c r="J11">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="K11" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L11">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="M11" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="N11" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="Q11" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="R11" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="S11" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="T11" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>98</v>
       </c>
       <c r="D12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E12" t="s">
         <v>26</v>
       </c>
       <c r="F12">
-        <v>36000000</v>
+        <v>421200000</v>
       </c>
       <c r="G12">
-        <v>18000000</v>
+        <v>16200000</v>
       </c>
       <c r="H12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I12">
-        <v>2000</v>
+        <v>21000</v>
       </c>
       <c r="J12">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="K12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L12">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="M12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="N12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="Q12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="R12" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="S12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="T12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D13" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F13">
-        <v>18750000</v>
+        <v>36000000</v>
       </c>
       <c r="G13">
-        <v>1500000</v>
+        <v>18000000</v>
       </c>
       <c r="H13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I13">
-        <v>8900</v>
+        <v>2000</v>
       </c>
       <c r="J13">
-        <v>11000</v>
+        <v>2000</v>
       </c>
       <c r="K13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L13">
-        <v>12500</v>
+        <v>2000</v>
       </c>
       <c r="M13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="N13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="Q13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="R13" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="S13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="T13" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E14" t="s">
         <v>27</v>
       </c>
       <c r="F14">
-        <v>33600000</v>
+        <v>18750000</v>
       </c>
       <c r="G14">
-        <v>2240000</v>
+        <v>1500000</v>
       </c>
       <c r="H14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I14">
-        <v>11500</v>
+        <v>8900</v>
       </c>
       <c r="J14">
-        <v>13200</v>
+        <v>11000</v>
       </c>
       <c r="K14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L14">
-        <v>15000</v>
+        <v>12500</v>
       </c>
       <c r="M14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="N14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="O14">
-        <v>26.78571428571428</v>
+        <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="Q14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="R14" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="S14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="T14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D15" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E15" t="s">
         <v>28</v>
       </c>
       <c r="F15">
-        <v>22120000</v>
+        <v>33600000</v>
       </c>
       <c r="G15">
-        <v>1580000</v>
+        <v>2240000</v>
       </c>
       <c r="H15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I15">
-        <v>10500</v>
+        <v>11500</v>
       </c>
       <c r="J15">
-        <v>12000</v>
+        <v>13200</v>
       </c>
       <c r="K15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L15">
-        <v>14000</v>
+        <v>15000</v>
       </c>
       <c r="M15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="N15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="O15">
-        <v>0</v>
+        <v>26.78571428571428</v>
       </c>
       <c r="P15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="Q15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="R15" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="S15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="T15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" t="s">
         <v>73</v>
-      </c>
-      <c r="B16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" t="s">
-        <v>71</v>
       </c>
       <c r="E16" t="s">
         <v>29</v>
       </c>
       <c r="F16">
-        <v>34500000</v>
+        <v>22120000</v>
       </c>
       <c r="G16">
-        <v>1500000</v>
+        <v>1580000</v>
       </c>
       <c r="H16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I16">
-        <v>20000</v>
+        <v>10500</v>
       </c>
       <c r="J16">
-        <v>23000</v>
+        <v>12000</v>
       </c>
       <c r="K16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L16">
-        <v>23000</v>
+        <v>14000</v>
       </c>
       <c r="M16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="N16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="Q16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="R16" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="S16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="T16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E17" t="s">
         <v>30</v>
       </c>
       <c r="F17">
-        <v>26400000</v>
+        <v>34500000</v>
       </c>
       <c r="G17">
-        <v>1100000</v>
+        <v>1500000</v>
       </c>
       <c r="H17" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I17">
         <v>20000</v>
       </c>
       <c r="J17">
+        <v>23000</v>
+      </c>
+      <c r="K17" t="s">
+        <v>65</v>
+      </c>
+      <c r="L17">
+        <v>23000</v>
+      </c>
+      <c r="M17" t="s">
+        <v>65</v>
+      </c>
+      <c r="N17" t="s">
+        <v>65</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>65</v>
+      </c>
+      <c r="R17" t="s">
+        <v>114</v>
+      </c>
+      <c r="S17" t="s">
+        <v>65</v>
+      </c>
+      <c r="T17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18">
+        <v>26400000</v>
+      </c>
+      <c r="G18">
+        <v>1100000</v>
+      </c>
+      <c r="H18" t="s">
+        <v>65</v>
+      </c>
+      <c r="I18">
+        <v>20000</v>
+      </c>
+      <c r="J18">
         <v>24000</v>
       </c>
-      <c r="K17" t="s">
-        <v>63</v>
-      </c>
-      <c r="L17">
+      <c r="K18" t="s">
+        <v>65</v>
+      </c>
+      <c r="L18">
         <v>24000</v>
       </c>
-      <c r="M17" t="s">
-        <v>63</v>
-      </c>
-      <c r="N17" t="s">
-        <v>63</v>
-      </c>
-      <c r="O17">
+      <c r="M18" t="s">
+        <v>65</v>
+      </c>
+      <c r="N18" t="s">
+        <v>65</v>
+      </c>
+      <c r="O18">
         <v>18.18181818181818</v>
       </c>
-      <c r="P17" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>63</v>
-      </c>
-      <c r="R17" t="s">
-        <v>111</v>
-      </c>
-      <c r="S17" t="s">
-        <v>63</v>
-      </c>
-      <c r="T17" t="s">
-        <v>63</v>
+      <c r="P18" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>65</v>
+      </c>
+      <c r="R18" t="s">
+        <v>115</v>
+      </c>
+      <c r="S18" t="s">
+        <v>65</v>
+      </c>
+      <c r="T18" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -3182,7 +3309,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3190,16 +3317,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -3211,10 +3338,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -3223,30 +3350,30 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="F2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H2">
         <v>42120</v>
@@ -3266,34 +3393,34 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="G3" t="s">
         <v>17</v>
       </c>
       <c r="H3">
-        <v>25000</v>
+        <v>27000</v>
       </c>
       <c r="I3">
-        <v>12500000</v>
+        <v>3600000</v>
       </c>
       <c r="J3">
-        <v>2000</v>
+        <v>7500</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -3304,34 +3431,34 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F4" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="H4">
-        <v>18750</v>
+        <v>25000</v>
       </c>
       <c r="I4">
-        <v>1500000</v>
+        <v>12500000</v>
       </c>
       <c r="J4">
-        <v>12500</v>
+        <v>2000</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -3342,63 +3469,63 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>95</v>
+        <v>51</v>
       </c>
       <c r="E5" t="s">
-        <v>115</v>
+        <v>51</v>
       </c>
       <c r="F5" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H5">
-        <v>42120</v>
+        <v>18750</v>
       </c>
       <c r="I5">
-        <v>16200000</v>
+        <v>1500000</v>
       </c>
       <c r="J5">
-        <v>26000</v>
+        <v>12500</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E6" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="F6" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H6">
         <v>42120</v>
@@ -3418,72 +3545,72 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>119</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="H7">
-        <v>17841.194</v>
+        <v>42120</v>
       </c>
       <c r="I7">
-        <v>1049482</v>
+        <v>16200000</v>
       </c>
       <c r="J7">
-        <v>17000</v>
+        <v>26000</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H8">
-        <v>52000</v>
+        <v>17841.194</v>
       </c>
       <c r="I8">
-        <v>2000000</v>
+        <v>1049482</v>
       </c>
       <c r="J8">
-        <v>26000</v>
+        <v>17000</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -3494,34 +3621,34 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" t="s">
         <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" t="s">
-        <v>75</v>
       </c>
       <c r="G9" t="s">
         <v>23</v>
       </c>
       <c r="H9">
-        <v>44265.9</v>
+        <v>52000</v>
       </c>
       <c r="I9">
-        <v>4137000</v>
+        <v>2000000</v>
       </c>
       <c r="J9">
-        <v>10700</v>
+        <v>26000</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -3532,110 +3659,110 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
         <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>95</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F10" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H10">
-        <v>126360</v>
+        <v>44265.9</v>
       </c>
       <c r="I10">
-        <v>16200000</v>
+        <v>4137000</v>
       </c>
       <c r="J10">
-        <v>26000</v>
+        <v>10700</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
         <v>73</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="E11" t="s">
-        <v>55</v>
+        <v>119</v>
       </c>
       <c r="F11" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="G11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H11">
-        <v>34500</v>
+        <v>126360</v>
       </c>
       <c r="I11">
-        <v>1500000</v>
+        <v>16200000</v>
       </c>
       <c r="J11">
-        <v>23000</v>
+        <v>26000</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H12">
-        <v>33600</v>
+        <v>34500</v>
       </c>
       <c r="I12">
-        <v>2240000</v>
+        <v>1500000</v>
       </c>
       <c r="J12">
-        <v>15000</v>
+        <v>23000</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -3646,34 +3773,34 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
         <v>74</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F13" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="G13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H13">
-        <v>26400</v>
+        <v>33600</v>
       </c>
       <c r="I13">
-        <v>1100000</v>
+        <v>2240000</v>
       </c>
       <c r="J13">
-        <v>24000</v>
+        <v>15000</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -3684,110 +3811,110 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D14" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="E14" t="s">
-        <v>115</v>
+        <v>60</v>
       </c>
       <c r="F14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G14" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="H14">
-        <v>12636</v>
+        <v>26400</v>
       </c>
       <c r="I14">
-        <v>16200000</v>
+        <v>1100000</v>
       </c>
       <c r="J14">
-        <v>26000</v>
+        <v>24000</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14">
-        <v>3</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>98</v>
       </c>
       <c r="E15" t="s">
-        <v>51</v>
+        <v>119</v>
       </c>
       <c r="F15" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="G15" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="H15">
-        <v>4966.368</v>
+        <v>12636</v>
       </c>
       <c r="I15">
-        <v>1128720</v>
+        <v>16200000</v>
       </c>
       <c r="J15">
-        <v>4400</v>
+        <v>26000</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15">
-        <v>100</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F16" t="s">
-        <v>77</v>
+        <v>21</v>
       </c>
       <c r="G16" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H16">
-        <v>36000</v>
+        <v>4966.368</v>
       </c>
       <c r="I16">
-        <v>18000000</v>
+        <v>1128720</v>
       </c>
       <c r="J16">
-        <v>2000</v>
+        <v>4400</v>
       </c>
       <c r="K16">
         <v>0</v>
@@ -3798,40 +3925,40 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>95</v>
+        <v>53</v>
       </c>
       <c r="E17" t="s">
-        <v>115</v>
+        <v>53</v>
       </c>
       <c r="F17" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="G17" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H17">
-        <v>4212</v>
+        <v>36000</v>
       </c>
       <c r="I17">
-        <v>16200000</v>
+        <v>18000000</v>
       </c>
       <c r="J17">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -3842,60 +3969,60 @@
         <v>73</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>98</v>
       </c>
       <c r="E18" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F18" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="G18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H18">
-        <v>15484</v>
+        <v>4212</v>
       </c>
       <c r="I18">
-        <v>1580000</v>
+        <v>16200000</v>
       </c>
       <c r="J18">
-        <v>14000</v>
+        <v>26000</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18">
-        <v>70</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" t="s">
+        <v>120</v>
+      </c>
+      <c r="F19" t="s">
         <v>73</v>
       </c>
-      <c r="C19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" t="s">
-        <v>116</v>
-      </c>
-      <c r="F19" t="s">
-        <v>71</v>
-      </c>
       <c r="G19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H19">
-        <v>6636</v>
+        <v>15484</v>
       </c>
       <c r="I19">
         <v>1580000</v>
@@ -3907,68 +4034,68 @@
         <v>0</v>
       </c>
       <c r="L19">
-        <v>30</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="D20" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="E20" t="s">
-        <v>53</v>
+        <v>120</v>
       </c>
       <c r="F20" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="G20" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="H20">
-        <v>26000</v>
+        <v>6636</v>
       </c>
       <c r="I20">
-        <v>4000000</v>
+        <v>1580000</v>
       </c>
       <c r="J20">
-        <v>6500</v>
+        <v>14000</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
       <c r="L20">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E21" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="F21" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H21">
         <v>12636</v>
@@ -3988,34 +4115,34 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E22" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G22" t="s">
         <v>21</v>
       </c>
       <c r="H22">
-        <v>5390</v>
+        <v>26000</v>
       </c>
       <c r="I22">
-        <v>770000</v>
+        <v>4000000</v>
       </c>
       <c r="J22">
-        <v>7000</v>
+        <v>6500</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -4026,25 +4153,25 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D23" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E23" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="F23" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G23" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H23">
         <v>12636</v>
@@ -4064,34 +4191,34 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E24" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F24" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="G24" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H24">
-        <v>30600</v>
+        <v>5390</v>
       </c>
       <c r="I24">
-        <v>1800000</v>
+        <v>770000</v>
       </c>
       <c r="J24">
-        <v>17000</v>
+        <v>7000</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -4102,77 +4229,115 @@
     </row>
     <row r="25" spans="1:12">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" t="s">
         <v>71</v>
       </c>
-      <c r="C25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" t="s">
-        <v>95</v>
-      </c>
-      <c r="E25" t="s">
-        <v>115</v>
-      </c>
-      <c r="F25" t="s">
-        <v>76</v>
-      </c>
       <c r="G25" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H25">
-        <v>126360</v>
+        <v>30600</v>
       </c>
       <c r="I25">
-        <v>16200000</v>
+        <v>1800000</v>
       </c>
       <c r="J25">
-        <v>26000</v>
+        <v>17000</v>
       </c>
       <c r="K25">
         <v>0</v>
       </c>
       <c r="L25">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="C26" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D26" t="s">
-        <v>56</v>
+        <v>98</v>
       </c>
       <c r="E26" t="s">
-        <v>56</v>
+        <v>119</v>
       </c>
       <c r="F26" t="s">
+        <v>79</v>
+      </c>
+      <c r="G26" t="s">
         <v>26</v>
       </c>
-      <c r="G26" t="s">
-        <v>24</v>
-      </c>
       <c r="H26">
-        <v>8000</v>
+        <v>126360</v>
       </c>
       <c r="I26">
-        <v>4000000</v>
+        <v>16200000</v>
       </c>
       <c r="J26">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="K26">
         <v>0</v>
       </c>
       <c r="L26">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H27">
+        <v>8000</v>
+      </c>
+      <c r="I27">
+        <v>4000000</v>
+      </c>
+      <c r="J27">
+        <v>2000</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2024-01-07
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="134">
   <si>
     <t>상장일</t>
   </si>
@@ -114,144 +114,141 @@
     <t>2023-11-09</t>
   </si>
   <si>
+    <t>DS단석</t>
+  </si>
+  <si>
+    <t>하나30호스팩</t>
+  </si>
+  <si>
+    <t>IBKS제23호스팩</t>
+  </si>
+  <si>
+    <t>LS머트리얼즈</t>
+  </si>
+  <si>
+    <t>블루엠텍</t>
+  </si>
+  <si>
+    <t>교보15호스팩</t>
+  </si>
+  <si>
+    <t>케이엔에스</t>
+  </si>
+  <si>
+    <t>와이바이오로직스</t>
+  </si>
+  <si>
+    <t>삼성스팩9호</t>
+  </si>
+  <si>
+    <t>에이텀</t>
+  </si>
+  <si>
+    <t>엔에이치스팩30호</t>
+  </si>
+  <si>
+    <t>에이에스텍</t>
+  </si>
+  <si>
+    <t>그린리소스</t>
+  </si>
+  <si>
+    <t>스톰테크</t>
+  </si>
+  <si>
+    <t>한선엔지니어링</t>
+  </si>
+  <si>
+    <t>에코아이</t>
+  </si>
+  <si>
+    <t>동인기연</t>
+  </si>
+  <si>
+    <t>에코프로머티</t>
+  </si>
+  <si>
+    <t>캡스톤파트너스</t>
+  </si>
+  <si>
+    <t>큐로셀</t>
+  </si>
+  <si>
+    <t>코스피</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>IBK</t>
+  </si>
+  <si>
+    <t>키움</t>
+  </si>
+  <si>
+    <t>이베스트</t>
+  </si>
+  <si>
+    <t>하이</t>
+  </si>
+  <si>
+    <t>교보</t>
+  </si>
+  <si>
+    <t>신영</t>
+  </si>
+  <si>
+    <t>유안타</t>
+  </si>
+  <si>
+    <t>삼성</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>대신</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>공동대표</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>인수</t>
+  </si>
+  <si>
+    <t>공동</t>
+  </si>
+  <si>
+    <t>2023-12-14</t>
+  </si>
+  <si>
+    <t>2023-11-23</t>
+  </si>
+  <si>
+    <t>2023-11-27</t>
+  </si>
+  <si>
+    <t>2023-11-16</t>
+  </si>
+  <si>
     <t>2023-11-13</t>
   </si>
   <si>
-    <t>DS단석</t>
-  </si>
-  <si>
-    <t>하나30호스팩</t>
-  </si>
-  <si>
-    <t>IBKS제23호스팩</t>
-  </si>
-  <si>
-    <t>LS머트리얼즈</t>
-  </si>
-  <si>
-    <t>블루엠텍</t>
-  </si>
-  <si>
-    <t>교보15호스팩</t>
-  </si>
-  <si>
-    <t>케이엔에스</t>
-  </si>
-  <si>
-    <t>와이바이오로직스</t>
-  </si>
-  <si>
-    <t>삼성스팩9호</t>
-  </si>
-  <si>
-    <t>에이텀</t>
-  </si>
-  <si>
-    <t>엔에이치스팩30호</t>
-  </si>
-  <si>
-    <t>에이에스텍</t>
-  </si>
-  <si>
-    <t>그린리소스</t>
-  </si>
-  <si>
-    <t>스톰테크</t>
-  </si>
-  <si>
-    <t>한선엔지니어링</t>
-  </si>
-  <si>
-    <t>에코아이</t>
-  </si>
-  <si>
-    <t>동인기연</t>
-  </si>
-  <si>
-    <t>에코프로머티</t>
-  </si>
-  <si>
-    <t>캡스톤파트너스</t>
-  </si>
-  <si>
-    <t>큐로셀</t>
-  </si>
-  <si>
-    <t>에이직랜드</t>
-  </si>
-  <si>
-    <t>코스피</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>KB</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>IBK</t>
-  </si>
-  <si>
-    <t>키움</t>
-  </si>
-  <si>
-    <t>이베스트</t>
-  </si>
-  <si>
-    <t>하이</t>
-  </si>
-  <si>
-    <t>교보</t>
-  </si>
-  <si>
-    <t>신영</t>
-  </si>
-  <si>
-    <t>유안타</t>
-  </si>
-  <si>
-    <t>삼성</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>대신</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>공동대표</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>인수</t>
-  </si>
-  <si>
-    <t>공동</t>
-  </si>
-  <si>
-    <t>2023-12-14</t>
-  </si>
-  <si>
-    <t>2023-11-23</t>
-  </si>
-  <si>
-    <t>2023-11-27</t>
-  </si>
-  <si>
-    <t>2023-11-16</t>
-  </si>
-  <si>
     <t>2023-11-10</t>
   </si>
   <si>
@@ -264,9 +261,6 @@
     <t>2023-10-31</t>
   </si>
   <si>
-    <t>2023-11-02</t>
-  </si>
-  <si>
     <t>2023-12-19</t>
   </si>
   <si>
@@ -288,9 +282,6 @@
     <t>2023-11-03</t>
   </si>
   <si>
-    <t>2023-11-07</t>
-  </si>
-  <si>
     <t>회사명</t>
   </si>
   <si>
@@ -409,9 +400,6 @@
   </si>
   <si>
     <t>169.95 : 1</t>
-  </si>
-  <si>
-    <t>759.88 : 1</t>
   </si>
   <si>
     <t>인수기관</t>
@@ -787,7 +775,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -851,37 +839,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D2">
         <v>1220</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F2">
         <v>793</v>
       </c>
       <c r="G2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M2">
         <v>100000</v>
@@ -890,10 +878,10 @@
         <v>65</v>
       </c>
       <c r="O2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="P2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q2">
         <v>1830000</v>
@@ -904,37 +892,37 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D3">
         <v>1220</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F3">
         <v>427</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M3">
         <v>100000</v>
@@ -943,10 +931,10 @@
         <v>35</v>
       </c>
       <c r="O3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="P3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q3">
         <v>1830000</v>
@@ -957,37 +945,37 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D4">
         <v>140</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F4">
         <v>140</v>
       </c>
       <c r="G4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K4" t="s">
         <v>69</v>
       </c>
-      <c r="H4" t="s">
-        <v>69</v>
-      </c>
-      <c r="I4" t="s">
-        <v>69</v>
-      </c>
-      <c r="J4" t="s">
-        <v>69</v>
-      </c>
-      <c r="K4" t="s">
-        <v>71</v>
-      </c>
       <c r="L4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M4">
         <v>2000</v>
@@ -999,7 +987,7 @@
         <v>19</v>
       </c>
       <c r="P4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Q4">
         <v>5250000</v>
@@ -1010,37 +998,37 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D5">
         <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F5">
         <v>80</v>
       </c>
       <c r="G5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J5" t="s">
+        <v>67</v>
+      </c>
+      <c r="K5" t="s">
         <v>69</v>
       </c>
-      <c r="H5" t="s">
-        <v>69</v>
-      </c>
-      <c r="I5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J5" t="s">
-        <v>69</v>
-      </c>
-      <c r="K5" t="s">
-        <v>71</v>
-      </c>
       <c r="L5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M5">
         <v>2000</v>
@@ -1052,7 +1040,7 @@
         <v>18</v>
       </c>
       <c r="P5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q5">
         <v>3000000</v>
@@ -1063,37 +1051,37 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D6">
         <v>877.5</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F6">
         <v>361.96872</v>
       </c>
       <c r="G6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M6">
         <v>6000</v>
@@ -1116,37 +1104,37 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D7">
         <v>877.5</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F7">
         <v>361.96872</v>
       </c>
       <c r="G7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M7">
         <v>6000</v>
@@ -1169,37 +1157,37 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D8">
         <v>877.5</v>
       </c>
       <c r="E8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F8">
         <v>65.81256</v>
       </c>
       <c r="G8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M8">
         <v>6000</v>
@@ -1222,37 +1210,37 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D9">
         <v>877.5</v>
       </c>
       <c r="E9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F9">
         <v>43.875</v>
       </c>
       <c r="G9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M9">
         <v>6000</v>
@@ -1275,37 +1263,37 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D10">
         <v>877.5</v>
       </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F10">
         <v>43.875</v>
       </c>
       <c r="G10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M10">
         <v>6000</v>
@@ -1328,37 +1316,37 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D11">
         <v>266</v>
       </c>
       <c r="E11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F11">
         <v>186.2</v>
       </c>
       <c r="G11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" t="s">
+        <v>67</v>
+      </c>
+      <c r="I11" t="s">
+        <v>67</v>
+      </c>
+      <c r="J11" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11" t="s">
         <v>69</v>
       </c>
-      <c r="H11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I11" t="s">
-        <v>69</v>
-      </c>
-      <c r="J11" t="s">
-        <v>69</v>
-      </c>
-      <c r="K11" t="s">
-        <v>71</v>
-      </c>
       <c r="L11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M11">
         <v>19000</v>
@@ -1370,7 +1358,7 @@
         <v>22</v>
       </c>
       <c r="P11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="Q11">
         <v>2100000</v>
@@ -1381,37 +1369,37 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D12">
         <v>266</v>
       </c>
       <c r="E12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F12">
         <v>79.8</v>
       </c>
       <c r="G12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M12">
         <v>19000</v>
@@ -1423,7 +1411,7 @@
         <v>22</v>
       </c>
       <c r="P12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="Q12">
         <v>2100000</v>
@@ -1434,37 +1422,37 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D13">
         <v>70</v>
       </c>
       <c r="E13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F13">
         <v>70</v>
       </c>
       <c r="G13" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" t="s">
+        <v>67</v>
+      </c>
+      <c r="J13" t="s">
+        <v>67</v>
+      </c>
+      <c r="K13" t="s">
         <v>69</v>
       </c>
-      <c r="H13" t="s">
-        <v>69</v>
-      </c>
-      <c r="I13" t="s">
-        <v>69</v>
-      </c>
-      <c r="J13" t="s">
-        <v>69</v>
-      </c>
-      <c r="K13" t="s">
-        <v>71</v>
-      </c>
       <c r="L13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M13">
         <v>2000</v>
@@ -1473,7 +1461,7 @@
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P13" t="s">
         <v>24</v>
@@ -1487,37 +1475,37 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D14">
         <v>172.5</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F14">
         <v>172.5</v>
       </c>
       <c r="G14" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" t="s">
+        <v>67</v>
+      </c>
+      <c r="I14" t="s">
+        <v>67</v>
+      </c>
+      <c r="J14" t="s">
+        <v>67</v>
+      </c>
+      <c r="K14" t="s">
         <v>69</v>
       </c>
-      <c r="H14" t="s">
-        <v>69</v>
-      </c>
-      <c r="I14" t="s">
-        <v>69</v>
-      </c>
-      <c r="J14" t="s">
-        <v>69</v>
-      </c>
-      <c r="K14" t="s">
-        <v>71</v>
-      </c>
       <c r="L14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M14">
         <v>23000</v>
@@ -1526,10 +1514,10 @@
         <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Q14">
         <v>475800</v>
@@ -1540,37 +1528,37 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D15">
         <v>135</v>
       </c>
       <c r="E15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F15">
         <v>135</v>
       </c>
       <c r="G15" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" t="s">
+        <v>67</v>
+      </c>
+      <c r="I15" t="s">
+        <v>67</v>
+      </c>
+      <c r="J15" t="s">
+        <v>67</v>
+      </c>
+      <c r="K15" t="s">
         <v>69</v>
       </c>
-      <c r="H15" t="s">
-        <v>69</v>
-      </c>
-      <c r="I15" t="s">
-        <v>69</v>
-      </c>
-      <c r="J15" t="s">
-        <v>69</v>
-      </c>
-      <c r="K15" t="s">
-        <v>71</v>
-      </c>
       <c r="L15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M15">
         <v>9000</v>
@@ -1579,7 +1567,7 @@
         <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P15" t="s">
         <v>24</v>
@@ -1593,37 +1581,37 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D16">
         <v>200</v>
       </c>
       <c r="E16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F16">
         <v>200</v>
       </c>
       <c r="G16" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" t="s">
+        <v>67</v>
+      </c>
+      <c r="I16" t="s">
+        <v>67</v>
+      </c>
+      <c r="J16" t="s">
+        <v>67</v>
+      </c>
+      <c r="K16" t="s">
         <v>69</v>
       </c>
-      <c r="H16" t="s">
-        <v>69</v>
-      </c>
-      <c r="I16" t="s">
-        <v>69</v>
-      </c>
-      <c r="J16" t="s">
-        <v>69</v>
-      </c>
-      <c r="K16" t="s">
-        <v>71</v>
-      </c>
       <c r="L16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M16">
         <v>2000</v>
@@ -1632,7 +1620,7 @@
         <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P16" t="s">
         <v>24</v>
@@ -1646,37 +1634,37 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D17">
         <v>117</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F17">
         <v>117</v>
       </c>
       <c r="G17" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" t="s">
+        <v>67</v>
+      </c>
+      <c r="I17" t="s">
+        <v>67</v>
+      </c>
+      <c r="J17" t="s">
+        <v>67</v>
+      </c>
+      <c r="K17" t="s">
         <v>69</v>
       </c>
-      <c r="H17" t="s">
-        <v>69</v>
-      </c>
-      <c r="I17" t="s">
-        <v>69</v>
-      </c>
-      <c r="J17" t="s">
-        <v>69</v>
-      </c>
-      <c r="K17" t="s">
-        <v>71</v>
-      </c>
       <c r="L17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M17">
         <v>18000</v>
@@ -1699,37 +1687,37 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D18">
         <v>160</v>
       </c>
       <c r="E18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F18">
         <v>160</v>
       </c>
       <c r="G18" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18" t="s">
+        <v>67</v>
+      </c>
+      <c r="I18" t="s">
+        <v>67</v>
+      </c>
+      <c r="J18" t="s">
+        <v>67</v>
+      </c>
+      <c r="K18" t="s">
         <v>69</v>
       </c>
-      <c r="H18" t="s">
-        <v>69</v>
-      </c>
-      <c r="I18" t="s">
-        <v>69</v>
-      </c>
-      <c r="J18" t="s">
-        <v>69</v>
-      </c>
-      <c r="K18" t="s">
-        <v>71</v>
-      </c>
       <c r="L18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M18">
         <v>2000</v>
@@ -1752,37 +1740,37 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D19">
         <v>393.96</v>
       </c>
       <c r="E19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F19">
         <v>393.96</v>
       </c>
       <c r="G19" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" t="s">
+        <v>67</v>
+      </c>
+      <c r="I19" t="s">
+        <v>67</v>
+      </c>
+      <c r="J19" t="s">
+        <v>67</v>
+      </c>
+      <c r="K19" t="s">
         <v>69</v>
       </c>
-      <c r="H19" t="s">
-        <v>69</v>
-      </c>
-      <c r="I19" t="s">
-        <v>69</v>
-      </c>
-      <c r="J19" t="s">
-        <v>69</v>
-      </c>
-      <c r="K19" t="s">
-        <v>71</v>
-      </c>
       <c r="L19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M19">
         <v>28000</v>
@@ -1791,7 +1779,7 @@
         <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P19" t="s">
         <v>27</v>
@@ -1805,37 +1793,37 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D20">
         <v>278.8</v>
       </c>
       <c r="E20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F20">
         <v>278.8</v>
       </c>
       <c r="G20" t="s">
+        <v>67</v>
+      </c>
+      <c r="H20" t="s">
+        <v>67</v>
+      </c>
+      <c r="I20" t="s">
+        <v>67</v>
+      </c>
+      <c r="J20" t="s">
+        <v>67</v>
+      </c>
+      <c r="K20" t="s">
         <v>69</v>
       </c>
-      <c r="H20" t="s">
-        <v>69</v>
-      </c>
-      <c r="I20" t="s">
-        <v>69</v>
-      </c>
-      <c r="J20" t="s">
-        <v>69</v>
-      </c>
-      <c r="K20" t="s">
-        <v>71</v>
-      </c>
       <c r="L20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M20">
         <v>17000</v>
@@ -1844,10 +1832,10 @@
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="P20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Q20">
         <v>1221420</v>
@@ -1858,37 +1846,37 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D21">
         <v>368.5</v>
       </c>
       <c r="E21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F21">
         <v>368.5</v>
       </c>
       <c r="G21" t="s">
+        <v>67</v>
+      </c>
+      <c r="H21" t="s">
+        <v>67</v>
+      </c>
+      <c r="I21" t="s">
+        <v>67</v>
+      </c>
+      <c r="J21" t="s">
+        <v>67</v>
+      </c>
+      <c r="K21" t="s">
         <v>69</v>
       </c>
-      <c r="H21" t="s">
-        <v>69</v>
-      </c>
-      <c r="I21" t="s">
-        <v>69</v>
-      </c>
-      <c r="J21" t="s">
-        <v>69</v>
-      </c>
-      <c r="K21" t="s">
-        <v>71</v>
-      </c>
       <c r="L21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M21">
         <v>11000</v>
@@ -1900,7 +1888,7 @@
         <v>31</v>
       </c>
       <c r="P21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Q21">
         <v>2374500</v>
@@ -1911,37 +1899,37 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D22">
         <v>297.5</v>
       </c>
       <c r="E22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F22">
         <v>297.5</v>
       </c>
       <c r="G22" t="s">
+        <v>67</v>
+      </c>
+      <c r="H22" t="s">
+        <v>67</v>
+      </c>
+      <c r="I22" t="s">
+        <v>67</v>
+      </c>
+      <c r="J22" t="s">
+        <v>67</v>
+      </c>
+      <c r="K22" t="s">
         <v>69</v>
       </c>
-      <c r="H22" t="s">
-        <v>69</v>
-      </c>
-      <c r="I22" t="s">
-        <v>69</v>
-      </c>
-      <c r="J22" t="s">
-        <v>69</v>
-      </c>
-      <c r="K22" t="s">
-        <v>71</v>
-      </c>
       <c r="L22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M22">
         <v>7000</v>
@@ -1950,10 +1938,10 @@
         <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="P22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Q22">
         <v>3187500</v>
@@ -1964,37 +1952,37 @@
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D23">
         <v>721.413</v>
       </c>
       <c r="E23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F23">
         <v>721.413</v>
       </c>
       <c r="G23" t="s">
+        <v>67</v>
+      </c>
+      <c r="H23" t="s">
+        <v>67</v>
+      </c>
+      <c r="I23" t="s">
+        <v>67</v>
+      </c>
+      <c r="J23" t="s">
+        <v>67</v>
+      </c>
+      <c r="K23" t="s">
         <v>69</v>
       </c>
-      <c r="H23" t="s">
-        <v>69</v>
-      </c>
-      <c r="I23" t="s">
-        <v>69</v>
-      </c>
-      <c r="J23" t="s">
-        <v>69</v>
-      </c>
-      <c r="K23" t="s">
-        <v>71</v>
-      </c>
       <c r="L23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M23">
         <v>34700</v>
@@ -2003,7 +1991,7 @@
         <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P23" t="s">
         <v>30</v>
@@ -2017,37 +2005,37 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D24">
         <v>441.12</v>
       </c>
       <c r="E24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F24">
         <v>441.12</v>
       </c>
       <c r="G24" t="s">
+        <v>67</v>
+      </c>
+      <c r="H24" t="s">
+        <v>67</v>
+      </c>
+      <c r="I24" t="s">
+        <v>67</v>
+      </c>
+      <c r="J24" t="s">
+        <v>67</v>
+      </c>
+      <c r="K24" t="s">
         <v>69</v>
       </c>
-      <c r="H24" t="s">
-        <v>69</v>
-      </c>
-      <c r="I24" t="s">
-        <v>69</v>
-      </c>
-      <c r="J24" t="s">
-        <v>69</v>
-      </c>
-      <c r="K24" t="s">
-        <v>71</v>
-      </c>
       <c r="L24" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M24">
         <v>30000</v>
@@ -2059,7 +2047,7 @@
         <v>31</v>
       </c>
       <c r="P24" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Q24">
         <v>1072999</v>
@@ -2070,37 +2058,37 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D25">
         <v>4192.2496</v>
       </c>
       <c r="E25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F25">
         <v>2846.537406</v>
       </c>
       <c r="G25" t="s">
+        <v>67</v>
+      </c>
+      <c r="H25" t="s">
+        <v>67</v>
+      </c>
+      <c r="I25" t="s">
+        <v>67</v>
+      </c>
+      <c r="J25" t="s">
+        <v>67</v>
+      </c>
+      <c r="K25" t="s">
         <v>69</v>
       </c>
-      <c r="H25" t="s">
-        <v>69</v>
-      </c>
-      <c r="I25" t="s">
-        <v>69</v>
-      </c>
-      <c r="J25" t="s">
-        <v>69</v>
-      </c>
-      <c r="K25" t="s">
-        <v>71</v>
-      </c>
       <c r="L25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M25">
         <v>36200</v>
@@ -2109,10 +2097,10 @@
         <v>67.90000000000001</v>
       </c>
       <c r="O25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P25" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="Q25">
         <v>19108320</v>
@@ -2123,37 +2111,37 @@
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D26">
         <v>4192.2496</v>
       </c>
       <c r="E26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F26">
         <v>1219.944706</v>
       </c>
       <c r="G26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M26">
         <v>36200</v>
@@ -2162,10 +2150,10 @@
         <v>29.1</v>
       </c>
       <c r="O26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P26" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="Q26">
         <v>19108320</v>
@@ -2176,37 +2164,37 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D27">
         <v>4192.2496</v>
       </c>
       <c r="E27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F27">
         <v>125.767488</v>
       </c>
       <c r="G27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M27">
         <v>36200</v>
@@ -2215,10 +2203,10 @@
         <v>3</v>
       </c>
       <c r="O27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P27" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="Q27">
         <v>19108320</v>
@@ -2229,37 +2217,37 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D28">
         <v>63.84</v>
       </c>
       <c r="E28" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F28">
         <v>63.84</v>
       </c>
       <c r="G28" t="s">
+        <v>67</v>
+      </c>
+      <c r="H28" t="s">
+        <v>67</v>
+      </c>
+      <c r="I28" t="s">
+        <v>67</v>
+      </c>
+      <c r="J28" t="s">
+        <v>67</v>
+      </c>
+      <c r="K28" t="s">
         <v>69</v>
       </c>
-      <c r="H28" t="s">
-        <v>69</v>
-      </c>
-      <c r="I28" t="s">
-        <v>69</v>
-      </c>
-      <c r="J28" t="s">
-        <v>69</v>
-      </c>
-      <c r="K28" t="s">
-        <v>71</v>
-      </c>
       <c r="L28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M28">
         <v>4000</v>
@@ -2268,7 +2256,7 @@
         <v>100</v>
       </c>
       <c r="O28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P28" t="s">
         <v>31</v>
@@ -2282,37 +2270,37 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D29">
         <v>320</v>
       </c>
       <c r="E29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F29">
         <v>160</v>
       </c>
       <c r="G29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M29">
         <v>20000</v>
@@ -2321,10 +2309,10 @@
         <v>50</v>
       </c>
       <c r="O29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P29" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Q29">
         <v>2254770</v>
@@ -2335,37 +2323,37 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D30">
         <v>320</v>
       </c>
       <c r="E30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F30">
         <v>160</v>
       </c>
       <c r="G30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K30" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M30">
         <v>20000</v>
@@ -2374,66 +2362,13 @@
         <v>50</v>
       </c>
       <c r="O30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Q30">
         <v>2254770</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="A31" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" t="s">
-        <v>53</v>
-      </c>
-      <c r="C31" t="s">
-        <v>55</v>
-      </c>
-      <c r="D31">
-        <v>659.0825</v>
-      </c>
-      <c r="E31" t="s">
-        <v>66</v>
-      </c>
-      <c r="F31">
-        <v>659.0825</v>
-      </c>
-      <c r="G31" t="s">
-        <v>69</v>
-      </c>
-      <c r="H31" t="s">
-        <v>69</v>
-      </c>
-      <c r="I31" t="s">
-        <v>69</v>
-      </c>
-      <c r="J31" t="s">
-        <v>69</v>
-      </c>
-      <c r="K31" t="s">
-        <v>71</v>
-      </c>
-      <c r="L31" t="s">
-        <v>69</v>
-      </c>
-      <c r="M31">
-        <v>25000</v>
-      </c>
-      <c r="N31">
-        <v>100</v>
-      </c>
-      <c r="O31" t="s">
-        <v>82</v>
-      </c>
-      <c r="P31" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q31">
-        <v>1827247</v>
       </c>
     </row>
   </sheetData>
@@ -2443,7 +2378,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T22"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2454,10 +2389,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -2466,63 +2401,63 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
@@ -2534,7 +2469,7 @@
         <v>1220000</v>
       </c>
       <c r="H2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I2">
         <v>79000</v>
@@ -2543,34 +2478,34 @@
         <v>89000</v>
       </c>
       <c r="K2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L2">
         <v>100000</v>
       </c>
       <c r="M2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O2">
         <v>34.42622950819672</v>
       </c>
       <c r="P2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="S2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -2578,13 +2513,13 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E3" t="s">
         <v>17</v>
@@ -2596,7 +2531,7 @@
         <v>7000000</v>
       </c>
       <c r="H3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I3">
         <v>2000</v>
@@ -2605,34 +2540,34 @@
         <v>2000</v>
       </c>
       <c r="K3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L3">
         <v>2000</v>
       </c>
       <c r="M3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="S3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -2640,13 +2575,13 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
@@ -2658,7 +2593,7 @@
         <v>4000000</v>
       </c>
       <c r="H4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I4">
         <v>2000</v>
@@ -2667,34 +2602,34 @@
         <v>2000</v>
       </c>
       <c r="K4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L4">
         <v>2000</v>
       </c>
       <c r="M4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="S4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -2702,10 +2637,10 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -2720,7 +2655,7 @@
         <v>14625000</v>
       </c>
       <c r="H5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I5">
         <v>4400</v>
@@ -2729,34 +2664,34 @@
         <v>5500</v>
       </c>
       <c r="K5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L5">
         <v>6000</v>
       </c>
       <c r="M5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O5">
         <v>40</v>
       </c>
       <c r="P5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="S5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -2764,13 +2699,13 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -2782,7 +2717,7 @@
         <v>1400000</v>
       </c>
       <c r="H6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I6">
         <v>15000</v>
@@ -2791,45 +2726,45 @@
         <v>19000</v>
       </c>
       <c r="K6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L6">
         <v>19000</v>
       </c>
       <c r="M6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="S6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D7" t="s">
         <v>24</v>
@@ -2844,7 +2779,7 @@
         <v>3500000</v>
       </c>
       <c r="H7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I7">
         <v>2000</v>
@@ -2853,48 +2788,48 @@
         <v>2000</v>
       </c>
       <c r="K7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L7">
         <v>2000</v>
       </c>
       <c r="M7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="S7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E8" t="s">
         <v>21</v>
@@ -2906,7 +2841,7 @@
         <v>750000</v>
       </c>
       <c r="H8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I8">
         <v>19000</v>
@@ -2915,45 +2850,45 @@
         <v>22000</v>
       </c>
       <c r="K8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L8">
         <v>23000</v>
       </c>
       <c r="M8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="S8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D9" t="s">
         <v>24</v>
@@ -2968,7 +2903,7 @@
         <v>1500000</v>
       </c>
       <c r="H9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I9">
         <v>9000</v>
@@ -2977,45 +2912,45 @@
         <v>11000</v>
       </c>
       <c r="K9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L9">
         <v>9000</v>
       </c>
       <c r="M9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="S9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s">
         <v>24</v>
@@ -3030,7 +2965,7 @@
         <v>10000000</v>
       </c>
       <c r="H10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I10">
         <v>2000</v>
@@ -3039,34 +2974,34 @@
         <v>2000</v>
       </c>
       <c r="K10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L10">
         <v>2000</v>
       </c>
       <c r="M10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R10" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="S10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -3074,10 +3009,10 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
         <v>25</v>
@@ -3092,7 +3027,7 @@
         <v>650000</v>
       </c>
       <c r="H11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I11">
         <v>23000</v>
@@ -3101,34 +3036,34 @@
         <v>30000</v>
       </c>
       <c r="K11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L11">
         <v>18000</v>
       </c>
       <c r="M11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R11" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="S11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -3136,10 +3071,10 @@
         <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
         <v>25</v>
@@ -3154,7 +3089,7 @@
         <v>8000000</v>
       </c>
       <c r="H12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I12">
         <v>2000</v>
@@ -3163,45 +3098,45 @@
         <v>2000</v>
       </c>
       <c r="K12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L12">
         <v>2000</v>
       </c>
       <c r="M12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="S12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D13" t="s">
         <v>27</v>
@@ -3216,7 +3151,7 @@
         <v>1407000</v>
       </c>
       <c r="H13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I13">
         <v>21000</v>
@@ -3225,48 +3160,48 @@
         <v>25000</v>
       </c>
       <c r="K13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L13">
         <v>28000</v>
       </c>
       <c r="M13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O13">
         <v>40.01421464108032</v>
       </c>
       <c r="P13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R13" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="S13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E14" t="s">
         <v>25</v>
@@ -3278,7 +3213,7 @@
         <v>1640000</v>
       </c>
       <c r="H14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I14">
         <v>11000</v>
@@ -3287,34 +3222,34 @@
         <v>14000</v>
       </c>
       <c r="K14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L14">
         <v>17000</v>
       </c>
       <c r="M14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R14" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -3322,13 +3257,13 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E15" t="s">
         <v>26</v>
@@ -3340,7 +3275,7 @@
         <v>3350000</v>
       </c>
       <c r="H15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I15">
         <v>8000</v>
@@ -3349,48 +3284,48 @@
         <v>9500</v>
       </c>
       <c r="K15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L15">
         <v>11000</v>
       </c>
       <c r="M15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R15" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="S15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E16" t="s">
         <v>25</v>
@@ -3402,7 +3337,7 @@
         <v>4250000</v>
       </c>
       <c r="H16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I16">
         <v>5200</v>
@@ -3411,45 +3346,45 @@
         <v>6000</v>
       </c>
       <c r="K16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L16">
         <v>7000</v>
       </c>
       <c r="M16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R16" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="S16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
         <v>30</v>
@@ -3464,7 +3399,7 @@
         <v>2079000</v>
       </c>
       <c r="H17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I17">
         <v>28500</v>
@@ -3473,34 +3408,34 @@
         <v>34700</v>
       </c>
       <c r="K17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L17">
         <v>34700</v>
       </c>
       <c r="M17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O17">
         <v>0</v>
       </c>
       <c r="P17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R17" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="S17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:20">
@@ -3508,13 +3443,13 @@
         <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E18" t="s">
         <v>28</v>
@@ -3526,7 +3461,7 @@
         <v>1470400</v>
       </c>
       <c r="H18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I18">
         <v>33000</v>
@@ -3535,48 +3470,48 @@
         <v>37000</v>
       </c>
       <c r="K18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L18">
         <v>30000</v>
       </c>
       <c r="M18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O18">
         <v>23.28618063112079</v>
       </c>
       <c r="P18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R18" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="S18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:20">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="E19" t="s">
         <v>29</v>
@@ -3588,7 +3523,7 @@
         <v>11580800</v>
       </c>
       <c r="H19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I19">
         <v>36200</v>
@@ -3597,45 +3532,45 @@
         <v>44000</v>
       </c>
       <c r="K19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L19">
         <v>36200</v>
       </c>
       <c r="M19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O19">
         <v>0</v>
       </c>
       <c r="P19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R19" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="S19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D20" t="s">
         <v>31</v>
@@ -3650,7 +3585,7 @@
         <v>1596000</v>
       </c>
       <c r="H20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I20">
         <v>3200</v>
@@ -3659,48 +3594,48 @@
         <v>3600</v>
       </c>
       <c r="K20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L20">
         <v>4000</v>
       </c>
       <c r="M20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O20">
         <v>0</v>
       </c>
       <c r="P20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R20" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="S20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:20">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E21" t="s">
         <v>31</v>
@@ -3712,7 +3647,7 @@
         <v>1600000</v>
       </c>
       <c r="H21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I21">
         <v>29800</v>
@@ -3721,96 +3656,34 @@
         <v>33500</v>
       </c>
       <c r="K21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L21">
         <v>20000</v>
       </c>
       <c r="M21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O21">
         <v>0</v>
       </c>
       <c r="P21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R21" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="S21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20">
-      <c r="A22" t="s">
-        <v>82</v>
-      </c>
-      <c r="B22" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" t="s">
-        <v>90</v>
-      </c>
-      <c r="E22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F22">
-        <v>65908250</v>
-      </c>
-      <c r="G22">
-        <v>2636330</v>
-      </c>
-      <c r="H22" t="s">
-        <v>69</v>
-      </c>
-      <c r="I22">
-        <v>19100</v>
-      </c>
-      <c r="J22">
-        <v>21400</v>
-      </c>
-      <c r="K22" t="s">
-        <v>69</v>
-      </c>
-      <c r="L22">
-        <v>25000</v>
-      </c>
-      <c r="M22" t="s">
-        <v>69</v>
-      </c>
-      <c r="N22" t="s">
-        <v>69</v>
-      </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-      <c r="P22" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>69</v>
-      </c>
-      <c r="R22" t="s">
-        <v>131</v>
-      </c>
-      <c r="S22" t="s">
-        <v>69</v>
-      </c>
-      <c r="T22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -3820,7 +3693,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3828,16 +3701,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -3849,10 +3722,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -3861,27 +3734,27 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G2" t="s">
         <v>17</v>
@@ -3904,22 +3777,22 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G3" t="s">
         <v>17</v>
@@ -3942,19 +3815,19 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F4" t="s">
         <v>21</v>
@@ -3980,19 +3853,19 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
         <v>30</v>
@@ -4018,22 +3891,22 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G6" t="s">
         <v>17</v>
@@ -4056,19 +3929,19 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F7" t="s">
         <v>31</v>
@@ -4094,22 +3967,22 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="G8" t="s">
         <v>29</v>
@@ -4132,98 +4005,98 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>109</v>
+        <v>55</v>
       </c>
       <c r="E9" t="s">
-        <v>135</v>
+        <v>55</v>
       </c>
       <c r="F9" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="H9">
-        <v>4387.5</v>
+        <v>44112</v>
       </c>
       <c r="I9">
-        <v>14625000</v>
+        <v>1470400</v>
       </c>
       <c r="J9">
-        <v>6000</v>
+        <v>30000</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9">
-        <v>5</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>106</v>
       </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>131</v>
       </c>
       <c r="F10" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="G10" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="H10">
-        <v>44112</v>
+        <v>4387.5</v>
       </c>
       <c r="I10">
-        <v>1470400</v>
+        <v>14625000</v>
       </c>
       <c r="J10">
-        <v>30000</v>
+        <v>6000</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
-        <v>100</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G11" t="s">
         <v>25</v>
@@ -4246,19 +4119,19 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
         <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F12" t="s">
         <v>25</v>
@@ -4284,19 +4157,19 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F13" t="s">
         <v>24</v>
@@ -4322,22 +4195,22 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G14" t="s">
         <v>25</v>
@@ -4360,133 +4233,133 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>110</v>
+        <v>65</v>
       </c>
       <c r="E15" t="s">
-        <v>110</v>
+        <v>132</v>
       </c>
       <c r="F15" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="G15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H15">
-        <v>16000</v>
+        <v>284653.7406</v>
       </c>
       <c r="I15">
-        <v>1600000</v>
+        <v>11580800</v>
       </c>
       <c r="J15">
-        <v>20000</v>
+        <v>36200</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15">
-        <v>50</v>
+        <v>67.90000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E16" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="F16" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G16" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H16">
-        <v>284653.7406</v>
+        <v>39396</v>
       </c>
       <c r="I16">
-        <v>11580800</v>
+        <v>1407000</v>
       </c>
       <c r="J16">
-        <v>36200</v>
+        <v>28000</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16">
-        <v>67.90000000000001</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
       <c r="E17" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
       <c r="F17" t="s">
-        <v>27</v>
+        <v>87</v>
       </c>
       <c r="G17" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="H17">
-        <v>39396</v>
+        <v>16000</v>
       </c>
       <c r="I17">
-        <v>1407000</v>
+        <v>1600000</v>
       </c>
       <c r="J17">
-        <v>28000</v>
+        <v>20000</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F18" t="s">
         <v>24</v>
@@ -4512,22 +4385,22 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D19" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E19" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G19" t="s">
         <v>31</v>
@@ -4550,34 +4423,34 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F20" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G20" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="H20">
-        <v>65908.25</v>
+        <v>17250</v>
       </c>
       <c r="I20">
-        <v>2636330</v>
+        <v>750000</v>
       </c>
       <c r="J20">
-        <v>25000</v>
+        <v>23000</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -4588,34 +4461,34 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C21" t="s">
         <v>39</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F21" t="s">
-        <v>87</v>
+        <v>24</v>
       </c>
       <c r="G21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H21">
-        <v>17250</v>
+        <v>13500</v>
       </c>
       <c r="I21">
-        <v>750000</v>
+        <v>1500000</v>
       </c>
       <c r="J21">
-        <v>23000</v>
+        <v>9000</v>
       </c>
       <c r="K21">
         <v>0</v>
@@ -4626,224 +4499,224 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D22" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
       <c r="E22" t="s">
-        <v>65</v>
+        <v>131</v>
       </c>
       <c r="F22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H22">
-        <v>13500</v>
+        <v>6581.256</v>
       </c>
       <c r="I22">
-        <v>1500000</v>
+        <v>14625000</v>
       </c>
       <c r="J22">
-        <v>9000</v>
+        <v>6000</v>
       </c>
       <c r="K22">
         <v>0</v>
       </c>
       <c r="L22">
-        <v>100</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
         <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>109</v>
+        <v>56</v>
       </c>
       <c r="E23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F23" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="G23" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H23">
-        <v>6581.256</v>
+        <v>7980</v>
       </c>
       <c r="I23">
-        <v>14625000</v>
+        <v>1400000</v>
       </c>
       <c r="J23">
-        <v>6000</v>
+        <v>19000</v>
       </c>
       <c r="K23">
         <v>0</v>
       </c>
       <c r="L23">
-        <v>7.5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="E24" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="F24" t="s">
-        <v>86</v>
+        <v>21</v>
       </c>
       <c r="G24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H24">
-        <v>7980</v>
+        <v>36196.872</v>
       </c>
       <c r="I24">
-        <v>1400000</v>
+        <v>14625000</v>
       </c>
       <c r="J24">
-        <v>19000</v>
+        <v>6000</v>
       </c>
       <c r="K24">
         <v>0</v>
       </c>
       <c r="L24">
-        <v>30</v>
+        <v>41.25</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" t="s">
         <v>36</v>
       </c>
       <c r="D25" t="s">
-        <v>109</v>
+        <v>56</v>
       </c>
       <c r="E25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F25" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="G25" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H25">
-        <v>36196.872</v>
+        <v>18620</v>
       </c>
       <c r="I25">
-        <v>14625000</v>
+        <v>1400000</v>
       </c>
       <c r="J25">
-        <v>6000</v>
+        <v>19000</v>
       </c>
       <c r="K25">
         <v>0</v>
       </c>
       <c r="L25">
-        <v>41.25</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E26" t="s">
-        <v>137</v>
+        <v>56</v>
       </c>
       <c r="F26" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G26" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H26">
-        <v>18620</v>
+        <v>14000</v>
       </c>
       <c r="I26">
-        <v>1400000</v>
+        <v>7000000</v>
       </c>
       <c r="J26">
-        <v>19000</v>
+        <v>2000</v>
       </c>
       <c r="K26">
         <v>0</v>
       </c>
       <c r="L26">
-        <v>70</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F27" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="G27" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H27">
-        <v>14000</v>
+        <v>11700</v>
       </c>
       <c r="I27">
-        <v>7000000</v>
+        <v>650000</v>
       </c>
       <c r="J27">
-        <v>2000</v>
+        <v>18000</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -4854,34 +4727,34 @@
     </row>
     <row r="28" spans="1:12">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F28" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="G28" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H28">
-        <v>11700</v>
+        <v>36850</v>
       </c>
       <c r="I28">
-        <v>650000</v>
+        <v>3350000</v>
       </c>
       <c r="J28">
-        <v>18000</v>
+        <v>11000</v>
       </c>
       <c r="K28">
         <v>0</v>
@@ -4892,115 +4765,77 @@
     </row>
     <row r="29" spans="1:12">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D29" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="E29" t="s">
-        <v>62</v>
+        <v>131</v>
       </c>
       <c r="F29" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="G29" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="H29">
-        <v>36850</v>
+        <v>4387.5</v>
       </c>
       <c r="I29">
-        <v>3350000</v>
+        <v>14625000</v>
       </c>
       <c r="J29">
-        <v>11000</v>
+        <v>6000</v>
       </c>
       <c r="K29">
         <v>0</v>
       </c>
       <c r="L29">
-        <v>100</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B30" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="C30" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="D30" t="s">
-        <v>109</v>
+        <v>65</v>
       </c>
       <c r="E30" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F30" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
       <c r="G30" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H30">
-        <v>4387.5</v>
+        <v>12576.7488</v>
       </c>
       <c r="I30">
-        <v>14625000</v>
+        <v>11580800</v>
       </c>
       <c r="J30">
-        <v>6000</v>
+        <v>36200</v>
       </c>
       <c r="K30">
         <v>0</v>
       </c>
       <c r="L30">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31" t="s">
-        <v>62</v>
-      </c>
-      <c r="B31" t="s">
-        <v>79</v>
-      </c>
-      <c r="C31" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" t="s">
-        <v>67</v>
-      </c>
-      <c r="E31" t="s">
-        <v>136</v>
-      </c>
-      <c r="F31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G31" t="s">
-        <v>29</v>
-      </c>
-      <c r="H31">
-        <v>12576.7488</v>
-      </c>
-      <c r="I31">
-        <v>11580800</v>
-      </c>
-      <c r="J31">
-        <v>36200</v>
-      </c>
-      <c r="K31">
-        <v>0</v>
-      </c>
-      <c r="L31">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2024-01-08
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="129">
   <si>
     <t>상장일</t>
   </si>
@@ -111,144 +111,141 @@
     <t>2023-11-15</t>
   </si>
   <si>
+    <t>DS단석</t>
+  </si>
+  <si>
+    <t>하나30호스팩</t>
+  </si>
+  <si>
+    <t>IBKS제23호스팩</t>
+  </si>
+  <si>
+    <t>LS머트리얼즈</t>
+  </si>
+  <si>
+    <t>블루엠텍</t>
+  </si>
+  <si>
+    <t>교보15호스팩</t>
+  </si>
+  <si>
+    <t>케이엔에스</t>
+  </si>
+  <si>
+    <t>와이바이오로직스</t>
+  </si>
+  <si>
+    <t>삼성스팩9호</t>
+  </si>
+  <si>
+    <t>에이텀</t>
+  </si>
+  <si>
+    <t>엔에이치스팩30호</t>
+  </si>
+  <si>
+    <t>에이에스텍</t>
+  </si>
+  <si>
+    <t>그린리소스</t>
+  </si>
+  <si>
+    <t>스톰테크</t>
+  </si>
+  <si>
+    <t>한선엔지니어링</t>
+  </si>
+  <si>
+    <t>에코아이</t>
+  </si>
+  <si>
+    <t>동인기연</t>
+  </si>
+  <si>
+    <t>에코프로머티</t>
+  </si>
+  <si>
+    <t>캡스톤파트너스</t>
+  </si>
+  <si>
+    <t>코스피</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>IBK</t>
+  </si>
+  <si>
+    <t>키움</t>
+  </si>
+  <si>
+    <t>이베스트</t>
+  </si>
+  <si>
+    <t>하이</t>
+  </si>
+  <si>
+    <t>교보</t>
+  </si>
+  <si>
+    <t>신영</t>
+  </si>
+  <si>
+    <t>유안타</t>
+  </si>
+  <si>
+    <t>삼성</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>대신</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>공동대표</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>인수</t>
+  </si>
+  <si>
+    <t>공동</t>
+  </si>
+  <si>
+    <t>2023-12-14</t>
+  </si>
+  <si>
+    <t>2023-11-23</t>
+  </si>
+  <si>
+    <t>2023-11-27</t>
+  </si>
+  <si>
+    <t>2023-11-16</t>
+  </si>
+  <si>
+    <t>2023-11-13</t>
+  </si>
+  <si>
     <t>2023-11-09</t>
   </si>
   <si>
-    <t>DS단석</t>
-  </si>
-  <si>
-    <t>하나30호스팩</t>
-  </si>
-  <si>
-    <t>IBKS제23호스팩</t>
-  </si>
-  <si>
-    <t>LS머트리얼즈</t>
-  </si>
-  <si>
-    <t>블루엠텍</t>
-  </si>
-  <si>
-    <t>교보15호스팩</t>
-  </si>
-  <si>
-    <t>케이엔에스</t>
-  </si>
-  <si>
-    <t>와이바이오로직스</t>
-  </si>
-  <si>
-    <t>삼성스팩9호</t>
-  </si>
-  <si>
-    <t>에이텀</t>
-  </si>
-  <si>
-    <t>엔에이치스팩30호</t>
-  </si>
-  <si>
-    <t>에이에스텍</t>
-  </si>
-  <si>
-    <t>그린리소스</t>
-  </si>
-  <si>
-    <t>스톰테크</t>
-  </si>
-  <si>
-    <t>한선엔지니어링</t>
-  </si>
-  <si>
-    <t>에코아이</t>
-  </si>
-  <si>
-    <t>동인기연</t>
-  </si>
-  <si>
-    <t>에코프로머티</t>
-  </si>
-  <si>
-    <t>캡스톤파트너스</t>
-  </si>
-  <si>
-    <t>큐로셀</t>
-  </si>
-  <si>
-    <t>코스피</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>KB</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>IBK</t>
-  </si>
-  <si>
-    <t>키움</t>
-  </si>
-  <si>
-    <t>이베스트</t>
-  </si>
-  <si>
-    <t>하이</t>
-  </si>
-  <si>
-    <t>교보</t>
-  </si>
-  <si>
-    <t>신영</t>
-  </si>
-  <si>
-    <t>유안타</t>
-  </si>
-  <si>
-    <t>삼성</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>대신</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>공동대표</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>인수</t>
-  </si>
-  <si>
-    <t>공동</t>
-  </si>
-  <si>
-    <t>2023-12-14</t>
-  </si>
-  <si>
-    <t>2023-11-23</t>
-  </si>
-  <si>
-    <t>2023-11-27</t>
-  </si>
-  <si>
-    <t>2023-11-16</t>
-  </si>
-  <si>
-    <t>2023-11-13</t>
-  </si>
-  <si>
     <t>2023-11-10</t>
   </si>
   <si>
@@ -258,9 +255,6 @@
     <t>2023-11-06</t>
   </si>
   <si>
-    <t>2023-10-31</t>
-  </si>
-  <si>
     <t>2023-12-19</t>
   </si>
   <si>
@@ -279,9 +273,6 @@
     <t>2023-11-14</t>
   </si>
   <si>
-    <t>2023-11-03</t>
-  </si>
-  <si>
     <t>회사명</t>
   </si>
   <si>
@@ -339,9 +330,6 @@
     <t>키움, KB</t>
   </si>
   <si>
-    <t>미래, 삼성</t>
-  </si>
-  <si>
     <t>982.9 : 1</t>
   </si>
   <si>
@@ -397,9 +385,6 @@
   </si>
   <si>
     <t>1345.6 : 1</t>
-  </si>
-  <si>
-    <t>169.95 : 1</t>
   </si>
   <si>
     <t>인수기관</t>
@@ -775,7 +760,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -839,37 +824,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D2">
         <v>1220</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F2">
         <v>793</v>
       </c>
       <c r="G2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M2">
         <v>100000</v>
@@ -878,10 +863,10 @@
         <v>65</v>
       </c>
       <c r="O2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q2">
         <v>1830000</v>
@@ -892,37 +877,37 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D3">
         <v>1220</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F3">
         <v>427</v>
       </c>
       <c r="G3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M3">
         <v>100000</v>
@@ -931,10 +916,10 @@
         <v>35</v>
       </c>
       <c r="O3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q3">
         <v>1830000</v>
@@ -945,37 +930,37 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D4">
         <v>140</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F4">
         <v>140</v>
       </c>
       <c r="G4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" t="s">
         <v>67</v>
       </c>
-      <c r="H4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I4" t="s">
-        <v>67</v>
-      </c>
-      <c r="J4" t="s">
-        <v>67</v>
-      </c>
-      <c r="K4" t="s">
-        <v>69</v>
-      </c>
       <c r="L4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M4">
         <v>2000</v>
@@ -987,7 +972,7 @@
         <v>19</v>
       </c>
       <c r="P4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q4">
         <v>5250000</v>
@@ -998,37 +983,37 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D5">
         <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F5">
         <v>80</v>
       </c>
       <c r="G5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J5" t="s">
+        <v>65</v>
+      </c>
+      <c r="K5" t="s">
         <v>67</v>
       </c>
-      <c r="H5" t="s">
-        <v>67</v>
-      </c>
-      <c r="I5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J5" t="s">
-        <v>67</v>
-      </c>
-      <c r="K5" t="s">
-        <v>69</v>
-      </c>
       <c r="L5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M5">
         <v>2000</v>
@@ -1040,7 +1025,7 @@
         <v>18</v>
       </c>
       <c r="P5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q5">
         <v>3000000</v>
@@ -1051,37 +1036,37 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D6">
         <v>877.5</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F6">
         <v>361.96872</v>
       </c>
       <c r="G6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M6">
         <v>6000</v>
@@ -1104,37 +1089,37 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D7">
         <v>877.5</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F7">
         <v>361.96872</v>
       </c>
       <c r="G7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M7">
         <v>6000</v>
@@ -1157,37 +1142,37 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D8">
         <v>877.5</v>
       </c>
       <c r="E8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F8">
         <v>65.81256</v>
       </c>
       <c r="G8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M8">
         <v>6000</v>
@@ -1210,37 +1195,37 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D9">
         <v>877.5</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F9">
         <v>43.875</v>
       </c>
       <c r="G9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M9">
         <v>6000</v>
@@ -1263,37 +1248,37 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D10">
         <v>877.5</v>
       </c>
       <c r="E10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F10">
         <v>43.875</v>
       </c>
       <c r="G10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M10">
         <v>6000</v>
@@ -1316,37 +1301,37 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D11">
         <v>266</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F11">
         <v>186.2</v>
       </c>
       <c r="G11" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" t="s">
+        <v>65</v>
+      </c>
+      <c r="J11" t="s">
+        <v>65</v>
+      </c>
+      <c r="K11" t="s">
         <v>67</v>
       </c>
-      <c r="H11" t="s">
-        <v>67</v>
-      </c>
-      <c r="I11" t="s">
-        <v>67</v>
-      </c>
-      <c r="J11" t="s">
-        <v>67</v>
-      </c>
-      <c r="K11" t="s">
-        <v>69</v>
-      </c>
       <c r="L11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M11">
         <v>19000</v>
@@ -1358,7 +1343,7 @@
         <v>22</v>
       </c>
       <c r="P11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Q11">
         <v>2100000</v>
@@ -1369,37 +1354,37 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D12">
         <v>266</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F12">
         <v>79.8</v>
       </c>
       <c r="G12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M12">
         <v>19000</v>
@@ -1411,7 +1396,7 @@
         <v>22</v>
       </c>
       <c r="P12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Q12">
         <v>2100000</v>
@@ -1422,37 +1407,37 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D13">
         <v>70</v>
       </c>
       <c r="E13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F13">
         <v>70</v>
       </c>
       <c r="G13" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" t="s">
+        <v>65</v>
+      </c>
+      <c r="I13" t="s">
+        <v>65</v>
+      </c>
+      <c r="J13" t="s">
+        <v>65</v>
+      </c>
+      <c r="K13" t="s">
         <v>67</v>
       </c>
-      <c r="H13" t="s">
-        <v>67</v>
-      </c>
-      <c r="I13" t="s">
-        <v>67</v>
-      </c>
-      <c r="J13" t="s">
-        <v>67</v>
-      </c>
-      <c r="K13" t="s">
-        <v>69</v>
-      </c>
       <c r="L13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M13">
         <v>2000</v>
@@ -1461,7 +1446,7 @@
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="P13" t="s">
         <v>24</v>
@@ -1475,37 +1460,37 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D14">
         <v>172.5</v>
       </c>
       <c r="E14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F14">
         <v>172.5</v>
       </c>
       <c r="G14" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14" t="s">
+        <v>65</v>
+      </c>
+      <c r="I14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K14" t="s">
         <v>67</v>
       </c>
-      <c r="H14" t="s">
-        <v>67</v>
-      </c>
-      <c r="I14" t="s">
-        <v>67</v>
-      </c>
-      <c r="J14" t="s">
-        <v>67</v>
-      </c>
-      <c r="K14" t="s">
-        <v>69</v>
-      </c>
       <c r="L14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M14">
         <v>23000</v>
@@ -1514,10 +1499,10 @@
         <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="P14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q14">
         <v>475800</v>
@@ -1528,37 +1513,37 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D15">
         <v>135</v>
       </c>
       <c r="E15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F15">
         <v>135</v>
       </c>
       <c r="G15" t="s">
+        <v>65</v>
+      </c>
+      <c r="H15" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" t="s">
+        <v>65</v>
+      </c>
+      <c r="J15" t="s">
+        <v>65</v>
+      </c>
+      <c r="K15" t="s">
         <v>67</v>
       </c>
-      <c r="H15" t="s">
-        <v>67</v>
-      </c>
-      <c r="I15" t="s">
-        <v>67</v>
-      </c>
-      <c r="J15" t="s">
-        <v>67</v>
-      </c>
-      <c r="K15" t="s">
-        <v>69</v>
-      </c>
       <c r="L15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M15">
         <v>9000</v>
@@ -1567,7 +1552,7 @@
         <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="P15" t="s">
         <v>24</v>
@@ -1581,37 +1566,37 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D16">
         <v>200</v>
       </c>
       <c r="E16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F16">
         <v>200</v>
       </c>
       <c r="G16" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16" t="s">
+        <v>65</v>
+      </c>
+      <c r="I16" t="s">
+        <v>65</v>
+      </c>
+      <c r="J16" t="s">
+        <v>65</v>
+      </c>
+      <c r="K16" t="s">
         <v>67</v>
       </c>
-      <c r="H16" t="s">
-        <v>67</v>
-      </c>
-      <c r="I16" t="s">
-        <v>67</v>
-      </c>
-      <c r="J16" t="s">
-        <v>67</v>
-      </c>
-      <c r="K16" t="s">
-        <v>69</v>
-      </c>
       <c r="L16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M16">
         <v>2000</v>
@@ -1620,7 +1605,7 @@
         <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="P16" t="s">
         <v>24</v>
@@ -1634,37 +1619,37 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D17">
         <v>117</v>
       </c>
       <c r="E17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F17">
         <v>117</v>
       </c>
       <c r="G17" t="s">
+        <v>65</v>
+      </c>
+      <c r="H17" t="s">
+        <v>65</v>
+      </c>
+      <c r="I17" t="s">
+        <v>65</v>
+      </c>
+      <c r="J17" t="s">
+        <v>65</v>
+      </c>
+      <c r="K17" t="s">
         <v>67</v>
       </c>
-      <c r="H17" t="s">
-        <v>67</v>
-      </c>
-      <c r="I17" t="s">
-        <v>67</v>
-      </c>
-      <c r="J17" t="s">
-        <v>67</v>
-      </c>
-      <c r="K17" t="s">
-        <v>69</v>
-      </c>
       <c r="L17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M17">
         <v>18000</v>
@@ -1687,37 +1672,37 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D18">
         <v>160</v>
       </c>
       <c r="E18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F18">
         <v>160</v>
       </c>
       <c r="G18" t="s">
+        <v>65</v>
+      </c>
+      <c r="H18" t="s">
+        <v>65</v>
+      </c>
+      <c r="I18" t="s">
+        <v>65</v>
+      </c>
+      <c r="J18" t="s">
+        <v>65</v>
+      </c>
+      <c r="K18" t="s">
         <v>67</v>
       </c>
-      <c r="H18" t="s">
-        <v>67</v>
-      </c>
-      <c r="I18" t="s">
-        <v>67</v>
-      </c>
-      <c r="J18" t="s">
-        <v>67</v>
-      </c>
-      <c r="K18" t="s">
-        <v>69</v>
-      </c>
       <c r="L18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M18">
         <v>2000</v>
@@ -1740,37 +1725,37 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D19">
         <v>393.96</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F19">
         <v>393.96</v>
       </c>
       <c r="G19" t="s">
+        <v>65</v>
+      </c>
+      <c r="H19" t="s">
+        <v>65</v>
+      </c>
+      <c r="I19" t="s">
+        <v>65</v>
+      </c>
+      <c r="J19" t="s">
+        <v>65</v>
+      </c>
+      <c r="K19" t="s">
         <v>67</v>
       </c>
-      <c r="H19" t="s">
-        <v>67</v>
-      </c>
-      <c r="I19" t="s">
-        <v>67</v>
-      </c>
-      <c r="J19" t="s">
-        <v>67</v>
-      </c>
-      <c r="K19" t="s">
-        <v>69</v>
-      </c>
       <c r="L19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M19">
         <v>28000</v>
@@ -1779,7 +1764,7 @@
         <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P19" t="s">
         <v>27</v>
@@ -1793,37 +1778,37 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D20">
         <v>278.8</v>
       </c>
       <c r="E20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F20">
         <v>278.8</v>
       </c>
       <c r="G20" t="s">
+        <v>65</v>
+      </c>
+      <c r="H20" t="s">
+        <v>65</v>
+      </c>
+      <c r="I20" t="s">
+        <v>65</v>
+      </c>
+      <c r="J20" t="s">
+        <v>65</v>
+      </c>
+      <c r="K20" t="s">
         <v>67</v>
       </c>
-      <c r="H20" t="s">
-        <v>67</v>
-      </c>
-      <c r="I20" t="s">
-        <v>67</v>
-      </c>
-      <c r="J20" t="s">
-        <v>67</v>
-      </c>
-      <c r="K20" t="s">
-        <v>69</v>
-      </c>
       <c r="L20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M20">
         <v>17000</v>
@@ -1832,10 +1817,10 @@
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P20" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Q20">
         <v>1221420</v>
@@ -1846,37 +1831,37 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D21">
         <v>368.5</v>
       </c>
       <c r="E21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F21">
         <v>368.5</v>
       </c>
       <c r="G21" t="s">
+        <v>65</v>
+      </c>
+      <c r="H21" t="s">
+        <v>65</v>
+      </c>
+      <c r="I21" t="s">
+        <v>65</v>
+      </c>
+      <c r="J21" t="s">
+        <v>65</v>
+      </c>
+      <c r="K21" t="s">
         <v>67</v>
       </c>
-      <c r="H21" t="s">
-        <v>67</v>
-      </c>
-      <c r="I21" t="s">
-        <v>67</v>
-      </c>
-      <c r="J21" t="s">
-        <v>67</v>
-      </c>
-      <c r="K21" t="s">
-        <v>69</v>
-      </c>
       <c r="L21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M21">
         <v>11000</v>
@@ -1885,10 +1870,10 @@
         <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="P21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="Q21">
         <v>2374500</v>
@@ -1899,37 +1884,37 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D22">
         <v>297.5</v>
       </c>
       <c r="E22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F22">
         <v>297.5</v>
       </c>
       <c r="G22" t="s">
+        <v>65</v>
+      </c>
+      <c r="H22" t="s">
+        <v>65</v>
+      </c>
+      <c r="I22" t="s">
+        <v>65</v>
+      </c>
+      <c r="J22" t="s">
+        <v>65</v>
+      </c>
+      <c r="K22" t="s">
         <v>67</v>
       </c>
-      <c r="H22" t="s">
-        <v>67</v>
-      </c>
-      <c r="I22" t="s">
-        <v>67</v>
-      </c>
-      <c r="J22" t="s">
-        <v>67</v>
-      </c>
-      <c r="K22" t="s">
-        <v>69</v>
-      </c>
       <c r="L22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M22">
         <v>7000</v>
@@ -1938,10 +1923,10 @@
         <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Q22">
         <v>3187500</v>
@@ -1952,37 +1937,37 @@
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D23">
         <v>721.413</v>
       </c>
       <c r="E23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F23">
         <v>721.413</v>
       </c>
       <c r="G23" t="s">
+        <v>65</v>
+      </c>
+      <c r="H23" t="s">
+        <v>65</v>
+      </c>
+      <c r="I23" t="s">
+        <v>65</v>
+      </c>
+      <c r="J23" t="s">
+        <v>65</v>
+      </c>
+      <c r="K23" t="s">
         <v>67</v>
       </c>
-      <c r="H23" t="s">
-        <v>67</v>
-      </c>
-      <c r="I23" t="s">
-        <v>67</v>
-      </c>
-      <c r="J23" t="s">
-        <v>67</v>
-      </c>
-      <c r="K23" t="s">
-        <v>69</v>
-      </c>
       <c r="L23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M23">
         <v>34700</v>
@@ -1991,7 +1976,7 @@
         <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P23" t="s">
         <v>30</v>
@@ -2005,37 +1990,37 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D24">
         <v>441.12</v>
       </c>
       <c r="E24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F24">
         <v>441.12</v>
       </c>
       <c r="G24" t="s">
+        <v>65</v>
+      </c>
+      <c r="H24" t="s">
+        <v>65</v>
+      </c>
+      <c r="I24" t="s">
+        <v>65</v>
+      </c>
+      <c r="J24" t="s">
+        <v>65</v>
+      </c>
+      <c r="K24" t="s">
         <v>67</v>
       </c>
-      <c r="H24" t="s">
-        <v>67</v>
-      </c>
-      <c r="I24" t="s">
-        <v>67</v>
-      </c>
-      <c r="J24" t="s">
-        <v>67</v>
-      </c>
-      <c r="K24" t="s">
-        <v>69</v>
-      </c>
       <c r="L24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M24">
         <v>30000</v>
@@ -2044,10 +2029,10 @@
         <v>100</v>
       </c>
       <c r="O24" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="P24" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="Q24">
         <v>1072999</v>
@@ -2058,37 +2043,37 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D25">
         <v>4192.2496</v>
       </c>
       <c r="E25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F25">
         <v>2846.537406</v>
       </c>
       <c r="G25" t="s">
+        <v>65</v>
+      </c>
+      <c r="H25" t="s">
+        <v>65</v>
+      </c>
+      <c r="I25" t="s">
+        <v>65</v>
+      </c>
+      <c r="J25" t="s">
+        <v>65</v>
+      </c>
+      <c r="K25" t="s">
         <v>67</v>
       </c>
-      <c r="H25" t="s">
-        <v>67</v>
-      </c>
-      <c r="I25" t="s">
-        <v>67</v>
-      </c>
-      <c r="J25" t="s">
-        <v>67</v>
-      </c>
-      <c r="K25" t="s">
-        <v>69</v>
-      </c>
       <c r="L25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M25">
         <v>36200</v>
@@ -2097,10 +2082,10 @@
         <v>67.90000000000001</v>
       </c>
       <c r="O25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="Q25">
         <v>19108320</v>
@@ -2111,37 +2096,37 @@
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D26">
         <v>4192.2496</v>
       </c>
       <c r="E26" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F26">
         <v>1219.944706</v>
       </c>
       <c r="G26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M26">
         <v>36200</v>
@@ -2150,10 +2135,10 @@
         <v>29.1</v>
       </c>
       <c r="O26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="Q26">
         <v>19108320</v>
@@ -2164,37 +2149,37 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D27">
         <v>4192.2496</v>
       </c>
       <c r="E27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F27">
         <v>125.767488</v>
       </c>
       <c r="G27" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H27" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I27" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J27" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L27" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M27">
         <v>36200</v>
@@ -2203,10 +2188,10 @@
         <v>3</v>
       </c>
       <c r="O27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P27" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="Q27">
         <v>19108320</v>
@@ -2217,37 +2202,37 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D28">
         <v>63.84</v>
       </c>
       <c r="E28" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F28">
         <v>63.84</v>
       </c>
       <c r="G28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H28" t="s">
+        <v>65</v>
+      </c>
+      <c r="I28" t="s">
+        <v>65</v>
+      </c>
+      <c r="J28" t="s">
+        <v>65</v>
+      </c>
+      <c r="K28" t="s">
         <v>67</v>
       </c>
-      <c r="H28" t="s">
-        <v>67</v>
-      </c>
-      <c r="I28" t="s">
-        <v>67</v>
-      </c>
-      <c r="J28" t="s">
-        <v>67</v>
-      </c>
-      <c r="K28" t="s">
-        <v>69</v>
-      </c>
       <c r="L28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M28">
         <v>4000</v>
@@ -2256,119 +2241,13 @@
         <v>100</v>
       </c>
       <c r="O28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P28" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="Q28">
         <v>1197000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17">
-      <c r="A29" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" t="s">
-        <v>53</v>
-      </c>
-      <c r="D29">
-        <v>320</v>
-      </c>
-      <c r="E29" t="s">
-        <v>65</v>
-      </c>
-      <c r="F29">
-        <v>160</v>
-      </c>
-      <c r="G29" t="s">
-        <v>67</v>
-      </c>
-      <c r="H29" t="s">
-        <v>67</v>
-      </c>
-      <c r="I29" t="s">
-        <v>67</v>
-      </c>
-      <c r="J29" t="s">
-        <v>67</v>
-      </c>
-      <c r="K29" t="s">
-        <v>68</v>
-      </c>
-      <c r="L29" t="s">
-        <v>67</v>
-      </c>
-      <c r="M29">
-        <v>20000</v>
-      </c>
-      <c r="N29">
-        <v>50</v>
-      </c>
-      <c r="O29" t="s">
-        <v>80</v>
-      </c>
-      <c r="P29" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q29">
-        <v>2254770</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17">
-      <c r="A30" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" t="s">
-        <v>51</v>
-      </c>
-      <c r="C30" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30">
-        <v>320</v>
-      </c>
-      <c r="E30" t="s">
-        <v>64</v>
-      </c>
-      <c r="F30">
-        <v>160</v>
-      </c>
-      <c r="G30" t="s">
-        <v>67</v>
-      </c>
-      <c r="H30" t="s">
-        <v>67</v>
-      </c>
-      <c r="I30" t="s">
-        <v>67</v>
-      </c>
-      <c r="J30" t="s">
-        <v>67</v>
-      </c>
-      <c r="K30" t="s">
-        <v>68</v>
-      </c>
-      <c r="L30" t="s">
-        <v>67</v>
-      </c>
-      <c r="M30">
-        <v>20000</v>
-      </c>
-      <c r="N30">
-        <v>50</v>
-      </c>
-      <c r="O30" t="s">
-        <v>80</v>
-      </c>
-      <c r="P30" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q30">
-        <v>2254770</v>
       </c>
     </row>
   </sheetData>
@@ -2378,7 +2257,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T21"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2389,10 +2268,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -2401,63 +2280,63 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
@@ -2469,7 +2348,7 @@
         <v>1220000</v>
       </c>
       <c r="H2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I2">
         <v>79000</v>
@@ -2478,34 +2357,34 @@
         <v>89000</v>
       </c>
       <c r="K2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L2">
         <v>100000</v>
       </c>
       <c r="M2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O2">
         <v>34.42622950819672</v>
       </c>
       <c r="P2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="R2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="S2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -2513,13 +2392,13 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E3" t="s">
         <v>17</v>
@@ -2531,7 +2410,7 @@
         <v>7000000</v>
       </c>
       <c r="H3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I3">
         <v>2000</v>
@@ -2540,34 +2419,34 @@
         <v>2000</v>
       </c>
       <c r="K3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L3">
         <v>2000</v>
       </c>
       <c r="M3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="R3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="S3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -2575,13 +2454,13 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
@@ -2593,7 +2472,7 @@
         <v>4000000</v>
       </c>
       <c r="H4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I4">
         <v>2000</v>
@@ -2602,34 +2481,34 @@
         <v>2000</v>
       </c>
       <c r="K4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L4">
         <v>2000</v>
       </c>
       <c r="M4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="R4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="S4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -2637,10 +2516,10 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -2655,7 +2534,7 @@
         <v>14625000</v>
       </c>
       <c r="H5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I5">
         <v>4400</v>
@@ -2664,34 +2543,34 @@
         <v>5500</v>
       </c>
       <c r="K5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L5">
         <v>6000</v>
       </c>
       <c r="M5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O5">
         <v>40</v>
       </c>
       <c r="P5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="R5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="S5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -2699,13 +2578,13 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -2717,7 +2596,7 @@
         <v>1400000</v>
       </c>
       <c r="H6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I6">
         <v>15000</v>
@@ -2726,45 +2605,45 @@
         <v>19000</v>
       </c>
       <c r="K6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L6">
         <v>19000</v>
       </c>
       <c r="M6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="R6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="S6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
         <v>24</v>
@@ -2779,7 +2658,7 @@
         <v>3500000</v>
       </c>
       <c r="H7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I7">
         <v>2000</v>
@@ -2788,48 +2667,48 @@
         <v>2000</v>
       </c>
       <c r="K7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L7">
         <v>2000</v>
       </c>
       <c r="M7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="R7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="S7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E8" t="s">
         <v>21</v>
@@ -2841,7 +2720,7 @@
         <v>750000</v>
       </c>
       <c r="H8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I8">
         <v>19000</v>
@@ -2850,45 +2729,45 @@
         <v>22000</v>
       </c>
       <c r="K8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L8">
         <v>23000</v>
       </c>
       <c r="M8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="R8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="S8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s">
         <v>24</v>
@@ -2903,7 +2782,7 @@
         <v>1500000</v>
       </c>
       <c r="H9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I9">
         <v>9000</v>
@@ -2912,45 +2791,45 @@
         <v>11000</v>
       </c>
       <c r="K9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L9">
         <v>9000</v>
       </c>
       <c r="M9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="R9" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="S9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D10" t="s">
         <v>24</v>
@@ -2965,7 +2844,7 @@
         <v>10000000</v>
       </c>
       <c r="H10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I10">
         <v>2000</v>
@@ -2974,34 +2853,34 @@
         <v>2000</v>
       </c>
       <c r="K10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L10">
         <v>2000</v>
       </c>
       <c r="M10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="R10" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="S10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -3009,10 +2888,10 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
         <v>25</v>
@@ -3027,7 +2906,7 @@
         <v>650000</v>
       </c>
       <c r="H11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I11">
         <v>23000</v>
@@ -3036,34 +2915,34 @@
         <v>30000</v>
       </c>
       <c r="K11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L11">
         <v>18000</v>
       </c>
       <c r="M11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="R11" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="S11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -3071,10 +2950,10 @@
         <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D12" t="s">
         <v>25</v>
@@ -3089,7 +2968,7 @@
         <v>8000000</v>
       </c>
       <c r="H12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I12">
         <v>2000</v>
@@ -3098,45 +2977,45 @@
         <v>2000</v>
       </c>
       <c r="K12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L12">
         <v>2000</v>
       </c>
       <c r="M12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="R12" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="S12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D13" t="s">
         <v>27</v>
@@ -3151,7 +3030,7 @@
         <v>1407000</v>
       </c>
       <c r="H13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I13">
         <v>21000</v>
@@ -3160,48 +3039,48 @@
         <v>25000</v>
       </c>
       <c r="K13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L13">
         <v>28000</v>
       </c>
       <c r="M13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O13">
         <v>40.01421464108032</v>
       </c>
       <c r="P13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="R13" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="S13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E14" t="s">
         <v>25</v>
@@ -3213,7 +3092,7 @@
         <v>1640000</v>
       </c>
       <c r="H14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I14">
         <v>11000</v>
@@ -3222,48 +3101,48 @@
         <v>14000</v>
       </c>
       <c r="K14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L14">
         <v>17000</v>
       </c>
       <c r="M14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="R14" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="S14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E15" t="s">
         <v>26</v>
@@ -3275,7 +3154,7 @@
         <v>3350000</v>
       </c>
       <c r="H15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I15">
         <v>8000</v>
@@ -3284,48 +3163,48 @@
         <v>9500</v>
       </c>
       <c r="K15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L15">
         <v>11000</v>
       </c>
       <c r="M15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="R15" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="S15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E16" t="s">
         <v>25</v>
@@ -3337,7 +3216,7 @@
         <v>4250000</v>
       </c>
       <c r="H16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I16">
         <v>5200</v>
@@ -3346,45 +3225,45 @@
         <v>6000</v>
       </c>
       <c r="K16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L16">
         <v>7000</v>
       </c>
       <c r="M16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="R16" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="S16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
         <v>30</v>
@@ -3399,7 +3278,7 @@
         <v>2079000</v>
       </c>
       <c r="H17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I17">
         <v>28500</v>
@@ -3408,48 +3287,48 @@
         <v>34700</v>
       </c>
       <c r="K17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L17">
         <v>34700</v>
       </c>
       <c r="M17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O17">
         <v>0</v>
       </c>
       <c r="P17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="R17" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="S17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:20">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E18" t="s">
         <v>28</v>
@@ -3461,7 +3340,7 @@
         <v>1470400</v>
       </c>
       <c r="H18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I18">
         <v>33000</v>
@@ -3470,48 +3349,48 @@
         <v>37000</v>
       </c>
       <c r="K18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L18">
         <v>30000</v>
       </c>
       <c r="M18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O18">
         <v>23.28618063112079</v>
       </c>
       <c r="P18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="R18" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="S18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:20">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E19" t="s">
         <v>29</v>
@@ -3523,7 +3402,7 @@
         <v>11580800</v>
       </c>
       <c r="H19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I19">
         <v>36200</v>
@@ -3532,48 +3411,48 @@
         <v>44000</v>
       </c>
       <c r="K19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L19">
         <v>36200</v>
       </c>
       <c r="M19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O19">
         <v>0</v>
       </c>
       <c r="P19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="R19" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="S19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="E20" t="s">
         <v>30</v>
@@ -3585,7 +3464,7 @@
         <v>1596000</v>
       </c>
       <c r="H20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I20">
         <v>3200</v>
@@ -3594,96 +3473,34 @@
         <v>3600</v>
       </c>
       <c r="K20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L20">
         <v>4000</v>
       </c>
       <c r="M20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O20">
         <v>0</v>
       </c>
       <c r="P20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="R20" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="S20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T20" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20">
-      <c r="A21" t="s">
-        <v>80</v>
-      </c>
-      <c r="B21" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" t="s">
-        <v>107</v>
-      </c>
-      <c r="D21" t="s">
-        <v>87</v>
-      </c>
-      <c r="E21" t="s">
-        <v>31</v>
-      </c>
-      <c r="F21">
-        <v>32000000</v>
-      </c>
-      <c r="G21">
-        <v>1600000</v>
-      </c>
-      <c r="H21" t="s">
-        <v>67</v>
-      </c>
-      <c r="I21">
-        <v>29800</v>
-      </c>
-      <c r="J21">
-        <v>33500</v>
-      </c>
-      <c r="K21" t="s">
-        <v>67</v>
-      </c>
-      <c r="L21">
-        <v>20000</v>
-      </c>
-      <c r="M21" t="s">
-        <v>67</v>
-      </c>
-      <c r="N21" t="s">
-        <v>67</v>
-      </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>67</v>
-      </c>
-      <c r="R21" t="s">
-        <v>127</v>
-      </c>
-      <c r="S21" t="s">
-        <v>67</v>
-      </c>
-      <c r="T21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -3693,7 +3510,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3701,16 +3518,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -3722,10 +3539,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -3734,27 +3551,27 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G2" t="s">
         <v>17</v>
@@ -3777,22 +3594,22 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G3" t="s">
         <v>17</v>
@@ -3815,148 +3632,148 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>106</v>
+        <v>52</v>
       </c>
       <c r="E4" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="H4">
-        <v>36196.872</v>
+        <v>72141.3</v>
       </c>
       <c r="I4">
-        <v>14625000</v>
+        <v>2079000</v>
       </c>
       <c r="J4">
-        <v>6000</v>
+        <v>34700</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>41.25</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>103</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>126</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="H5">
-        <v>72141.3</v>
+        <v>36196.872</v>
       </c>
       <c r="I5">
-        <v>2079000</v>
+        <v>14625000</v>
       </c>
       <c r="J5">
-        <v>34700</v>
+        <v>6000</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
-        <v>100</v>
+        <v>41.25</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
-        <v>105</v>
+        <v>63</v>
       </c>
       <c r="E6" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="F6" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="H6">
-        <v>42700</v>
+        <v>121994.4706</v>
       </c>
       <c r="I6">
-        <v>1220000</v>
+        <v>11580800</v>
       </c>
       <c r="J6">
-        <v>100000</v>
+        <v>36200</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6">
-        <v>35</v>
+        <v>29.1</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H7">
-        <v>6384</v>
+        <v>44112</v>
       </c>
       <c r="I7">
-        <v>1596000</v>
+        <v>1470400</v>
       </c>
       <c r="J7">
-        <v>4000</v>
+        <v>30000</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -3967,72 +3784,72 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="E8" t="s">
-        <v>132</v>
+        <v>53</v>
       </c>
       <c r="F8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H8">
-        <v>121994.4706</v>
+        <v>27880</v>
       </c>
       <c r="I8">
-        <v>11580800</v>
+        <v>1640000</v>
       </c>
       <c r="J8">
-        <v>36200</v>
+        <v>17000</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8">
-        <v>29.1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F9" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="G9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="H9">
-        <v>44112</v>
+        <v>16000</v>
       </c>
       <c r="I9">
-        <v>1470400</v>
+        <v>8000000</v>
       </c>
       <c r="J9">
-        <v>30000</v>
+        <v>2000</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -4043,133 +3860,133 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
-        <v>106</v>
+        <v>53</v>
       </c>
       <c r="E10" t="s">
-        <v>131</v>
+        <v>53</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="G10" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="H10">
-        <v>4387.5</v>
+        <v>6384</v>
       </c>
       <c r="I10">
-        <v>14625000</v>
+        <v>1596000</v>
       </c>
       <c r="J10">
-        <v>6000</v>
+        <v>4000</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
-        <v>5</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>102</v>
       </c>
       <c r="E11" t="s">
-        <v>55</v>
+        <v>102</v>
       </c>
       <c r="F11" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G11" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="H11">
-        <v>27880</v>
+        <v>42700</v>
       </c>
       <c r="I11">
-        <v>1640000</v>
+        <v>1220000</v>
       </c>
       <c r="J11">
-        <v>17000</v>
+        <v>100000</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
-        <v>100</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
+        <v>126</v>
       </c>
       <c r="F12" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G12" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="H12">
-        <v>16000</v>
+        <v>4387.5</v>
       </c>
       <c r="I12">
-        <v>8000000</v>
+        <v>14625000</v>
       </c>
       <c r="J12">
-        <v>2000</v>
+        <v>6000</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12">
-        <v>100</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F13" t="s">
         <v>24</v>
@@ -4195,22 +4012,22 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G14" t="s">
         <v>25</v>
@@ -4233,148 +4050,148 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E15" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
       <c r="F15" t="s">
-        <v>76</v>
+        <v>27</v>
       </c>
       <c r="G15" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H15">
-        <v>284653.7406</v>
+        <v>39396</v>
       </c>
       <c r="I15">
-        <v>11580800</v>
+        <v>1407000</v>
       </c>
       <c r="J15">
-        <v>36200</v>
+        <v>28000</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15">
-        <v>67.90000000000001</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E16" t="s">
-        <v>65</v>
+        <v>127</v>
       </c>
       <c r="F16" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="G16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="H16">
-        <v>39396</v>
+        <v>284653.7406</v>
       </c>
       <c r="I16">
-        <v>1407000</v>
+        <v>11580800</v>
       </c>
       <c r="J16">
-        <v>28000</v>
+        <v>36200</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16">
-        <v>100</v>
+        <v>67.90000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>107</v>
+        <v>62</v>
       </c>
       <c r="E17" t="s">
-        <v>107</v>
+        <v>62</v>
       </c>
       <c r="F17" t="s">
-        <v>87</v>
+        <v>24</v>
       </c>
       <c r="G17" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="H17">
-        <v>16000</v>
+        <v>20000</v>
       </c>
       <c r="I17">
-        <v>1600000</v>
+        <v>10000000</v>
       </c>
       <c r="J17">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F18" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="G18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H18">
-        <v>20000</v>
+        <v>17250</v>
       </c>
       <c r="I18">
-        <v>10000000</v>
+        <v>750000</v>
       </c>
       <c r="J18">
-        <v>2000</v>
+        <v>23000</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -4385,250 +4202,250 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>107</v>
+        <v>61</v>
       </c>
       <c r="E19" t="s">
-        <v>107</v>
+        <v>61</v>
       </c>
       <c r="F19" t="s">
-        <v>87</v>
+        <v>24</v>
       </c>
       <c r="G19" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="H19">
-        <v>16000</v>
+        <v>13500</v>
       </c>
       <c r="I19">
-        <v>1600000</v>
+        <v>1500000</v>
       </c>
       <c r="J19">
-        <v>20000</v>
+        <v>9000</v>
       </c>
       <c r="K19">
         <v>0</v>
       </c>
       <c r="L19">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>103</v>
       </c>
       <c r="E20" t="s">
-        <v>62</v>
+        <v>126</v>
       </c>
       <c r="F20" t="s">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="G20" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H20">
-        <v>17250</v>
+        <v>6581.256</v>
       </c>
       <c r="I20">
-        <v>750000</v>
+        <v>14625000</v>
       </c>
       <c r="J20">
-        <v>23000</v>
+        <v>6000</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
       <c r="L20">
-        <v>100</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="E21" t="s">
-        <v>63</v>
+        <v>126</v>
       </c>
       <c r="F21" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H21">
-        <v>13500</v>
+        <v>36196.872</v>
       </c>
       <c r="I21">
-        <v>1500000</v>
+        <v>14625000</v>
       </c>
       <c r="J21">
-        <v>9000</v>
+        <v>6000</v>
       </c>
       <c r="K21">
         <v>0</v>
       </c>
       <c r="L21">
-        <v>100</v>
+        <v>41.25</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
         <v>35</v>
       </c>
       <c r="D22" t="s">
-        <v>106</v>
+        <v>54</v>
       </c>
       <c r="E22" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F22" t="s">
-        <v>21</v>
+        <v>82</v>
       </c>
       <c r="G22" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H22">
-        <v>6581.256</v>
+        <v>7980</v>
       </c>
       <c r="I22">
-        <v>14625000</v>
+        <v>1400000</v>
       </c>
       <c r="J22">
-        <v>6000</v>
+        <v>19000</v>
       </c>
       <c r="K22">
         <v>0</v>
       </c>
       <c r="L22">
-        <v>7.5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E23" t="s">
-        <v>133</v>
+        <v>54</v>
       </c>
       <c r="F23" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="G23" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H23">
-        <v>7980</v>
+        <v>11700</v>
       </c>
       <c r="I23">
-        <v>1400000</v>
+        <v>650000</v>
       </c>
       <c r="J23">
-        <v>19000</v>
+        <v>18000</v>
       </c>
       <c r="K23">
         <v>0</v>
       </c>
       <c r="L23">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D24" t="s">
-        <v>106</v>
+        <v>54</v>
       </c>
       <c r="E24" t="s">
-        <v>131</v>
+        <v>54</v>
       </c>
       <c r="F24" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="G24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H24">
-        <v>36196.872</v>
+        <v>14000</v>
       </c>
       <c r="I24">
-        <v>14625000</v>
+        <v>7000000</v>
       </c>
       <c r="J24">
-        <v>6000</v>
+        <v>2000</v>
       </c>
       <c r="K24">
         <v>0</v>
       </c>
       <c r="L24">
-        <v>41.25</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
         <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E25" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F25" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G25" t="s">
         <v>19</v>
@@ -4651,34 +4468,34 @@
     </row>
     <row r="26" spans="1:12">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="C26" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D26" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E26" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F26" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G26" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="H26">
-        <v>14000</v>
+        <v>36850</v>
       </c>
       <c r="I26">
-        <v>7000000</v>
+        <v>3350000</v>
       </c>
       <c r="J26">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="K26">
         <v>0</v>
@@ -4689,154 +4506,78 @@
     </row>
     <row r="27" spans="1:12">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="C27" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D27" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="E27" t="s">
-        <v>56</v>
+        <v>127</v>
       </c>
       <c r="F27" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="G27" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="H27">
-        <v>11700</v>
+        <v>12576.7488</v>
       </c>
       <c r="I27">
-        <v>650000</v>
+        <v>11580800</v>
       </c>
       <c r="J27">
-        <v>18000</v>
+        <v>36200</v>
       </c>
       <c r="K27">
         <v>0</v>
       </c>
       <c r="L27">
-        <v>100</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="D28" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="E28" t="s">
-        <v>60</v>
+        <v>126</v>
       </c>
       <c r="F28" t="s">
-        <v>86</v>
+        <v>21</v>
       </c>
       <c r="G28" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="H28">
-        <v>36850</v>
+        <v>4387.5</v>
       </c>
       <c r="I28">
-        <v>3350000</v>
+        <v>14625000</v>
       </c>
       <c r="J28">
-        <v>11000</v>
+        <v>6000</v>
       </c>
       <c r="K28">
         <v>0</v>
       </c>
       <c r="L28">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" t="s">
-        <v>106</v>
-      </c>
-      <c r="E29" t="s">
-        <v>131</v>
-      </c>
-      <c r="F29" t="s">
-        <v>21</v>
-      </c>
-      <c r="G29" t="s">
-        <v>18</v>
-      </c>
-      <c r="H29">
-        <v>4387.5</v>
-      </c>
-      <c r="I29">
-        <v>14625000</v>
-      </c>
-      <c r="J29">
-        <v>6000</v>
-      </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
-      <c r="L29">
         <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" t="s">
-        <v>78</v>
-      </c>
-      <c r="C30" t="s">
-        <v>49</v>
-      </c>
-      <c r="D30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E30" t="s">
-        <v>132</v>
-      </c>
-      <c r="F30" t="s">
-        <v>76</v>
-      </c>
-      <c r="G30" t="s">
-        <v>29</v>
-      </c>
-      <c r="H30">
-        <v>12576.7488</v>
-      </c>
-      <c r="I30">
-        <v>11580800</v>
-      </c>
-      <c r="J30">
-        <v>36200</v>
-      </c>
-      <c r="K30">
-        <v>0</v>
-      </c>
-      <c r="L30">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-01-09
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="126">
   <si>
     <t>상장일</t>
   </si>
@@ -108,171 +108,165 @@
     <t>2023-11-17</t>
   </si>
   <si>
+    <t>DS단석</t>
+  </si>
+  <si>
+    <t>하나30호스팩</t>
+  </si>
+  <si>
+    <t>IBKS제23호스팩</t>
+  </si>
+  <si>
+    <t>LS머트리얼즈</t>
+  </si>
+  <si>
+    <t>블루엠텍</t>
+  </si>
+  <si>
+    <t>교보15호스팩</t>
+  </si>
+  <si>
+    <t>케이엔에스</t>
+  </si>
+  <si>
+    <t>와이바이오로직스</t>
+  </si>
+  <si>
+    <t>삼성스팩9호</t>
+  </si>
+  <si>
+    <t>에이텀</t>
+  </si>
+  <si>
+    <t>엔에이치스팩30호</t>
+  </si>
+  <si>
+    <t>에이에스텍</t>
+  </si>
+  <si>
+    <t>그린리소스</t>
+  </si>
+  <si>
+    <t>스톰테크</t>
+  </si>
+  <si>
+    <t>한선엔지니어링</t>
+  </si>
+  <si>
+    <t>에코아이</t>
+  </si>
+  <si>
+    <t>동인기연</t>
+  </si>
+  <si>
+    <t>에코프로머티</t>
+  </si>
+  <si>
+    <t>코스피</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>IBK</t>
+  </si>
+  <si>
+    <t>키움</t>
+  </si>
+  <si>
+    <t>이베스트</t>
+  </si>
+  <si>
+    <t>하이</t>
+  </si>
+  <si>
+    <t>교보</t>
+  </si>
+  <si>
+    <t>신영</t>
+  </si>
+  <si>
+    <t>유안타</t>
+  </si>
+  <si>
+    <t>삼성</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>대신</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>공동대표</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>인수</t>
+  </si>
+  <si>
+    <t>공동</t>
+  </si>
+  <si>
+    <t>2023-12-14</t>
+  </si>
+  <si>
+    <t>2023-11-23</t>
+  </si>
+  <si>
+    <t>2023-11-27</t>
+  </si>
+  <si>
+    <t>2023-11-16</t>
+  </si>
+  <si>
+    <t>2023-11-13</t>
+  </si>
+  <si>
+    <t>2023-11-09</t>
+  </si>
+  <si>
+    <t>2023-11-10</t>
+  </si>
+  <si>
+    <t>2023-11-08</t>
+  </si>
+  <si>
+    <t>2023-12-19</t>
+  </si>
+  <si>
+    <t>2023-12-18</t>
+  </si>
+  <si>
+    <t>2023-12-15</t>
+  </si>
+  <si>
+    <t>2023-12-07</t>
+  </si>
+  <si>
+    <t>2023-11-30</t>
+  </si>
+  <si>
+    <t>2023-11-14</t>
+  </si>
+  <si>
     <t>2023-11-15</t>
   </si>
   <si>
-    <t>DS단석</t>
-  </si>
-  <si>
-    <t>하나30호스팩</t>
-  </si>
-  <si>
-    <t>IBKS제23호스팩</t>
-  </si>
-  <si>
-    <t>LS머트리얼즈</t>
-  </si>
-  <si>
-    <t>블루엠텍</t>
-  </si>
-  <si>
-    <t>교보15호스팩</t>
-  </si>
-  <si>
-    <t>케이엔에스</t>
-  </si>
-  <si>
-    <t>와이바이오로직스</t>
-  </si>
-  <si>
-    <t>삼성스팩9호</t>
-  </si>
-  <si>
-    <t>에이텀</t>
-  </si>
-  <si>
-    <t>엔에이치스팩30호</t>
-  </si>
-  <si>
-    <t>에이에스텍</t>
-  </si>
-  <si>
-    <t>그린리소스</t>
-  </si>
-  <si>
-    <t>스톰테크</t>
-  </si>
-  <si>
-    <t>한선엔지니어링</t>
-  </si>
-  <si>
-    <t>에코아이</t>
-  </si>
-  <si>
-    <t>동인기연</t>
-  </si>
-  <si>
-    <t>에코프로머티</t>
-  </si>
-  <si>
-    <t>캡스톤파트너스</t>
-  </si>
-  <si>
-    <t>코스피</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>KB</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>IBK</t>
-  </si>
-  <si>
-    <t>키움</t>
-  </si>
-  <si>
-    <t>이베스트</t>
-  </si>
-  <si>
-    <t>하이</t>
-  </si>
-  <si>
-    <t>교보</t>
-  </si>
-  <si>
-    <t>신영</t>
-  </si>
-  <si>
-    <t>유안타</t>
-  </si>
-  <si>
-    <t>삼성</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>대신</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>공동대표</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>인수</t>
-  </si>
-  <si>
-    <t>공동</t>
-  </si>
-  <si>
-    <t>2023-12-14</t>
-  </si>
-  <si>
-    <t>2023-11-23</t>
-  </si>
-  <si>
-    <t>2023-11-27</t>
-  </si>
-  <si>
-    <t>2023-11-16</t>
-  </si>
-  <si>
-    <t>2023-11-13</t>
-  </si>
-  <si>
-    <t>2023-11-09</t>
-  </si>
-  <si>
-    <t>2023-11-10</t>
-  </si>
-  <si>
-    <t>2023-11-08</t>
-  </si>
-  <si>
-    <t>2023-11-06</t>
-  </si>
-  <si>
-    <t>2023-12-19</t>
-  </si>
-  <si>
-    <t>2023-12-18</t>
-  </si>
-  <si>
-    <t>2023-12-15</t>
-  </si>
-  <si>
-    <t>2023-12-07</t>
-  </si>
-  <si>
-    <t>2023-11-30</t>
-  </si>
-  <si>
-    <t>2023-11-14</t>
-  </si>
-  <si>
     <t>회사명</t>
   </si>
   <si>
@@ -382,9 +376,6 @@
   </si>
   <si>
     <t>70.04 : 1</t>
-  </si>
-  <si>
-    <t>1345.6 : 1</t>
   </si>
   <si>
     <t>인수기관</t>
@@ -760,7 +751,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -824,37 +815,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D2">
         <v>1220</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F2">
         <v>793</v>
       </c>
       <c r="G2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M2">
         <v>100000</v>
@@ -863,10 +854,10 @@
         <v>65</v>
       </c>
       <c r="O2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="Q2">
         <v>1830000</v>
@@ -877,37 +868,37 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D3">
         <v>1220</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F3">
         <v>427</v>
       </c>
       <c r="G3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M3">
         <v>100000</v>
@@ -916,10 +907,10 @@
         <v>35</v>
       </c>
       <c r="O3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="Q3">
         <v>1830000</v>
@@ -930,37 +921,37 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D4">
         <v>140</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F4">
         <v>140</v>
       </c>
       <c r="G4" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K4" t="s">
         <v>65</v>
       </c>
-      <c r="H4" t="s">
-        <v>65</v>
-      </c>
-      <c r="I4" t="s">
-        <v>65</v>
-      </c>
-      <c r="J4" t="s">
-        <v>65</v>
-      </c>
-      <c r="K4" t="s">
-        <v>67</v>
-      </c>
       <c r="L4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M4">
         <v>2000</v>
@@ -972,7 +963,7 @@
         <v>19</v>
       </c>
       <c r="P4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="Q4">
         <v>5250000</v>
@@ -983,37 +974,37 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D5">
         <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F5">
         <v>80</v>
       </c>
       <c r="G5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" t="s">
+        <v>63</v>
+      </c>
+      <c r="I5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" t="s">
         <v>65</v>
       </c>
-      <c r="H5" t="s">
-        <v>65</v>
-      </c>
-      <c r="I5" t="s">
-        <v>65</v>
-      </c>
-      <c r="J5" t="s">
-        <v>65</v>
-      </c>
-      <c r="K5" t="s">
-        <v>67</v>
-      </c>
       <c r="L5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M5">
         <v>2000</v>
@@ -1025,7 +1016,7 @@
         <v>18</v>
       </c>
       <c r="P5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q5">
         <v>3000000</v>
@@ -1036,37 +1027,37 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D6">
         <v>877.5</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F6">
         <v>361.96872</v>
       </c>
       <c r="G6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M6">
         <v>6000</v>
@@ -1089,37 +1080,37 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D7">
         <v>877.5</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F7">
         <v>361.96872</v>
       </c>
       <c r="G7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M7">
         <v>6000</v>
@@ -1142,37 +1133,37 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D8">
         <v>877.5</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F8">
         <v>65.81256</v>
       </c>
       <c r="G8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M8">
         <v>6000</v>
@@ -1195,37 +1186,37 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D9">
         <v>877.5</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F9">
         <v>43.875</v>
       </c>
       <c r="G9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M9">
         <v>6000</v>
@@ -1248,37 +1239,37 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D10">
         <v>877.5</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F10">
         <v>43.875</v>
       </c>
       <c r="G10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M10">
         <v>6000</v>
@@ -1301,37 +1292,37 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D11">
         <v>266</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F11">
         <v>186.2</v>
       </c>
       <c r="G11" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11" t="s">
+        <v>63</v>
+      </c>
+      <c r="I11" t="s">
+        <v>63</v>
+      </c>
+      <c r="J11" t="s">
+        <v>63</v>
+      </c>
+      <c r="K11" t="s">
         <v>65</v>
       </c>
-      <c r="H11" t="s">
-        <v>65</v>
-      </c>
-      <c r="I11" t="s">
-        <v>65</v>
-      </c>
-      <c r="J11" t="s">
-        <v>65</v>
-      </c>
-      <c r="K11" t="s">
-        <v>67</v>
-      </c>
       <c r="L11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M11">
         <v>19000</v>
@@ -1343,7 +1334,7 @@
         <v>22</v>
       </c>
       <c r="P11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="Q11">
         <v>2100000</v>
@@ -1354,37 +1345,37 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D12">
         <v>266</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F12">
         <v>79.8</v>
       </c>
       <c r="G12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M12">
         <v>19000</v>
@@ -1396,7 +1387,7 @@
         <v>22</v>
       </c>
       <c r="P12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="Q12">
         <v>2100000</v>
@@ -1407,37 +1398,37 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D13">
         <v>70</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F13">
         <v>70</v>
       </c>
       <c r="G13" t="s">
+        <v>63</v>
+      </c>
+      <c r="H13" t="s">
+        <v>63</v>
+      </c>
+      <c r="I13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" t="s">
+        <v>63</v>
+      </c>
+      <c r="K13" t="s">
         <v>65</v>
       </c>
-      <c r="H13" t="s">
-        <v>65</v>
-      </c>
-      <c r="I13" t="s">
-        <v>65</v>
-      </c>
-      <c r="J13" t="s">
-        <v>65</v>
-      </c>
-      <c r="K13" t="s">
-        <v>67</v>
-      </c>
       <c r="L13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M13">
         <v>2000</v>
@@ -1446,7 +1437,7 @@
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P13" t="s">
         <v>24</v>
@@ -1460,37 +1451,37 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D14">
         <v>172.5</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F14">
         <v>172.5</v>
       </c>
       <c r="G14" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" t="s">
+        <v>63</v>
+      </c>
+      <c r="I14" t="s">
+        <v>63</v>
+      </c>
+      <c r="J14" t="s">
+        <v>63</v>
+      </c>
+      <c r="K14" t="s">
         <v>65</v>
       </c>
-      <c r="H14" t="s">
-        <v>65</v>
-      </c>
-      <c r="I14" t="s">
-        <v>65</v>
-      </c>
-      <c r="J14" t="s">
-        <v>65</v>
-      </c>
-      <c r="K14" t="s">
-        <v>67</v>
-      </c>
       <c r="L14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M14">
         <v>23000</v>
@@ -1499,10 +1490,10 @@
         <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="Q14">
         <v>475800</v>
@@ -1513,37 +1504,37 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D15">
         <v>135</v>
       </c>
       <c r="E15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F15">
         <v>135</v>
       </c>
       <c r="G15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H15" t="s">
+        <v>63</v>
+      </c>
+      <c r="I15" t="s">
+        <v>63</v>
+      </c>
+      <c r="J15" t="s">
+        <v>63</v>
+      </c>
+      <c r="K15" t="s">
         <v>65</v>
       </c>
-      <c r="H15" t="s">
-        <v>65</v>
-      </c>
-      <c r="I15" t="s">
-        <v>65</v>
-      </c>
-      <c r="J15" t="s">
-        <v>65</v>
-      </c>
-      <c r="K15" t="s">
-        <v>67</v>
-      </c>
       <c r="L15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M15">
         <v>9000</v>
@@ -1552,7 +1543,7 @@
         <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P15" t="s">
         <v>24</v>
@@ -1566,37 +1557,37 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D16">
         <v>200</v>
       </c>
       <c r="E16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F16">
         <v>200</v>
       </c>
       <c r="G16" t="s">
+        <v>63</v>
+      </c>
+      <c r="H16" t="s">
+        <v>63</v>
+      </c>
+      <c r="I16" t="s">
+        <v>63</v>
+      </c>
+      <c r="J16" t="s">
+        <v>63</v>
+      </c>
+      <c r="K16" t="s">
         <v>65</v>
       </c>
-      <c r="H16" t="s">
-        <v>65</v>
-      </c>
-      <c r="I16" t="s">
-        <v>65</v>
-      </c>
-      <c r="J16" t="s">
-        <v>65</v>
-      </c>
-      <c r="K16" t="s">
-        <v>67</v>
-      </c>
       <c r="L16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M16">
         <v>2000</v>
@@ -1605,7 +1596,7 @@
         <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P16" t="s">
         <v>24</v>
@@ -1619,37 +1610,37 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D17">
         <v>117</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F17">
         <v>117</v>
       </c>
       <c r="G17" t="s">
+        <v>63</v>
+      </c>
+      <c r="H17" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" t="s">
+        <v>63</v>
+      </c>
+      <c r="J17" t="s">
+        <v>63</v>
+      </c>
+      <c r="K17" t="s">
         <v>65</v>
       </c>
-      <c r="H17" t="s">
-        <v>65</v>
-      </c>
-      <c r="I17" t="s">
-        <v>65</v>
-      </c>
-      <c r="J17" t="s">
-        <v>65</v>
-      </c>
-      <c r="K17" t="s">
-        <v>67</v>
-      </c>
       <c r="L17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M17">
         <v>18000</v>
@@ -1672,37 +1663,37 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D18">
         <v>160</v>
       </c>
       <c r="E18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F18">
         <v>160</v>
       </c>
       <c r="G18" t="s">
+        <v>63</v>
+      </c>
+      <c r="H18" t="s">
+        <v>63</v>
+      </c>
+      <c r="I18" t="s">
+        <v>63</v>
+      </c>
+      <c r="J18" t="s">
+        <v>63</v>
+      </c>
+      <c r="K18" t="s">
         <v>65</v>
       </c>
-      <c r="H18" t="s">
-        <v>65</v>
-      </c>
-      <c r="I18" t="s">
-        <v>65</v>
-      </c>
-      <c r="J18" t="s">
-        <v>65</v>
-      </c>
-      <c r="K18" t="s">
-        <v>67</v>
-      </c>
       <c r="L18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M18">
         <v>2000</v>
@@ -1725,37 +1716,37 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D19">
         <v>393.96</v>
       </c>
       <c r="E19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F19">
         <v>393.96</v>
       </c>
       <c r="G19" t="s">
+        <v>63</v>
+      </c>
+      <c r="H19" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" t="s">
+        <v>63</v>
+      </c>
+      <c r="J19" t="s">
+        <v>63</v>
+      </c>
+      <c r="K19" t="s">
         <v>65</v>
       </c>
-      <c r="H19" t="s">
-        <v>65</v>
-      </c>
-      <c r="I19" t="s">
-        <v>65</v>
-      </c>
-      <c r="J19" t="s">
-        <v>65</v>
-      </c>
-      <c r="K19" t="s">
-        <v>67</v>
-      </c>
       <c r="L19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M19">
         <v>28000</v>
@@ -1764,7 +1755,7 @@
         <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="P19" t="s">
         <v>27</v>
@@ -1778,37 +1769,37 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D20">
         <v>278.8</v>
       </c>
       <c r="E20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F20">
         <v>278.8</v>
       </c>
       <c r="G20" t="s">
+        <v>63</v>
+      </c>
+      <c r="H20" t="s">
+        <v>63</v>
+      </c>
+      <c r="I20" t="s">
+        <v>63</v>
+      </c>
+      <c r="J20" t="s">
+        <v>63</v>
+      </c>
+      <c r="K20" t="s">
         <v>65</v>
       </c>
-      <c r="H20" t="s">
-        <v>65</v>
-      </c>
-      <c r="I20" t="s">
-        <v>65</v>
-      </c>
-      <c r="J20" t="s">
-        <v>65</v>
-      </c>
-      <c r="K20" t="s">
-        <v>67</v>
-      </c>
       <c r="L20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M20">
         <v>17000</v>
@@ -1817,10 +1808,10 @@
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="P20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="Q20">
         <v>1221420</v>
@@ -1831,37 +1822,37 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D21">
         <v>368.5</v>
       </c>
       <c r="E21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F21">
         <v>368.5</v>
       </c>
       <c r="G21" t="s">
+        <v>63</v>
+      </c>
+      <c r="H21" t="s">
+        <v>63</v>
+      </c>
+      <c r="I21" t="s">
+        <v>63</v>
+      </c>
+      <c r="J21" t="s">
+        <v>63</v>
+      </c>
+      <c r="K21" t="s">
         <v>65</v>
       </c>
-      <c r="H21" t="s">
-        <v>65</v>
-      </c>
-      <c r="I21" t="s">
-        <v>65</v>
-      </c>
-      <c r="J21" t="s">
-        <v>65</v>
-      </c>
-      <c r="K21" t="s">
-        <v>67</v>
-      </c>
       <c r="L21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M21">
         <v>11000</v>
@@ -1870,10 +1861,10 @@
         <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P21" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="Q21">
         <v>2374500</v>
@@ -1884,37 +1875,37 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D22">
         <v>297.5</v>
       </c>
       <c r="E22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F22">
         <v>297.5</v>
       </c>
       <c r="G22" t="s">
+        <v>63</v>
+      </c>
+      <c r="H22" t="s">
+        <v>63</v>
+      </c>
+      <c r="I22" t="s">
+        <v>63</v>
+      </c>
+      <c r="J22" t="s">
+        <v>63</v>
+      </c>
+      <c r="K22" t="s">
         <v>65</v>
       </c>
-      <c r="H22" t="s">
-        <v>65</v>
-      </c>
-      <c r="I22" t="s">
-        <v>65</v>
-      </c>
-      <c r="J22" t="s">
-        <v>65</v>
-      </c>
-      <c r="K22" t="s">
-        <v>67</v>
-      </c>
       <c r="L22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M22">
         <v>7000</v>
@@ -1923,10 +1914,10 @@
         <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="P22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="Q22">
         <v>3187500</v>
@@ -1937,37 +1928,37 @@
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D23">
         <v>721.413</v>
       </c>
       <c r="E23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F23">
         <v>721.413</v>
       </c>
       <c r="G23" t="s">
+        <v>63</v>
+      </c>
+      <c r="H23" t="s">
+        <v>63</v>
+      </c>
+      <c r="I23" t="s">
+        <v>63</v>
+      </c>
+      <c r="J23" t="s">
+        <v>63</v>
+      </c>
+      <c r="K23" t="s">
         <v>65</v>
       </c>
-      <c r="H23" t="s">
-        <v>65</v>
-      </c>
-      <c r="I23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J23" t="s">
-        <v>65</v>
-      </c>
-      <c r="K23" t="s">
-        <v>67</v>
-      </c>
       <c r="L23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M23">
         <v>34700</v>
@@ -1976,10 +1967,10 @@
         <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P23" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="Q23">
         <v>1537150</v>
@@ -1990,37 +1981,37 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D24">
         <v>441.12</v>
       </c>
       <c r="E24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F24">
         <v>441.12</v>
       </c>
       <c r="G24" t="s">
+        <v>63</v>
+      </c>
+      <c r="H24" t="s">
+        <v>63</v>
+      </c>
+      <c r="I24" t="s">
+        <v>63</v>
+      </c>
+      <c r="J24" t="s">
+        <v>63</v>
+      </c>
+      <c r="K24" t="s">
         <v>65</v>
       </c>
-      <c r="H24" t="s">
-        <v>65</v>
-      </c>
-      <c r="I24" t="s">
-        <v>65</v>
-      </c>
-      <c r="J24" t="s">
-        <v>65</v>
-      </c>
-      <c r="K24" t="s">
-        <v>67</v>
-      </c>
       <c r="L24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M24">
         <v>30000</v>
@@ -2029,10 +2020,10 @@
         <v>100</v>
       </c>
       <c r="O24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P24" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="Q24">
         <v>1072999</v>
@@ -2043,37 +2034,37 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" t="s">
         <v>48</v>
-      </c>
-      <c r="C25" t="s">
-        <v>50</v>
       </c>
       <c r="D25">
         <v>4192.2496</v>
       </c>
       <c r="E25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F25">
         <v>2846.537406</v>
       </c>
       <c r="G25" t="s">
+        <v>63</v>
+      </c>
+      <c r="H25" t="s">
+        <v>63</v>
+      </c>
+      <c r="I25" t="s">
+        <v>63</v>
+      </c>
+      <c r="J25" t="s">
+        <v>63</v>
+      </c>
+      <c r="K25" t="s">
         <v>65</v>
       </c>
-      <c r="H25" t="s">
-        <v>65</v>
-      </c>
-      <c r="I25" t="s">
-        <v>65</v>
-      </c>
-      <c r="J25" t="s">
-        <v>65</v>
-      </c>
-      <c r="K25" t="s">
-        <v>67</v>
-      </c>
       <c r="L25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M25">
         <v>36200</v>
@@ -2082,10 +2073,10 @@
         <v>67.90000000000001</v>
       </c>
       <c r="O25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Q25">
         <v>19108320</v>
@@ -2096,37 +2087,37 @@
         <v>29</v>
       </c>
       <c r="B26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" t="s">
         <v>48</v>
-      </c>
-      <c r="C26" t="s">
-        <v>50</v>
       </c>
       <c r="D26">
         <v>4192.2496</v>
       </c>
       <c r="E26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F26">
         <v>1219.944706</v>
       </c>
       <c r="G26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M26">
         <v>36200</v>
@@ -2135,10 +2126,10 @@
         <v>29.1</v>
       </c>
       <c r="O26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P26" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Q26">
         <v>19108320</v>
@@ -2149,37 +2140,37 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" t="s">
         <v>48</v>
-      </c>
-      <c r="C27" t="s">
-        <v>50</v>
       </c>
       <c r="D27">
         <v>4192.2496</v>
       </c>
       <c r="E27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F27">
         <v>125.767488</v>
       </c>
       <c r="G27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K27" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M27">
         <v>36200</v>
@@ -2188,66 +2179,13 @@
         <v>3</v>
       </c>
       <c r="O27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Q27">
         <v>19108320</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17">
-      <c r="A28" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28">
-        <v>63.84</v>
-      </c>
-      <c r="E28" t="s">
-        <v>53</v>
-      </c>
-      <c r="F28">
-        <v>63.84</v>
-      </c>
-      <c r="G28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H28" t="s">
-        <v>65</v>
-      </c>
-      <c r="I28" t="s">
-        <v>65</v>
-      </c>
-      <c r="J28" t="s">
-        <v>65</v>
-      </c>
-      <c r="K28" t="s">
-        <v>67</v>
-      </c>
-      <c r="L28" t="s">
-        <v>65</v>
-      </c>
-      <c r="M28">
-        <v>4000</v>
-      </c>
-      <c r="N28">
-        <v>100</v>
-      </c>
-      <c r="O28" t="s">
-        <v>78</v>
-      </c>
-      <c r="P28" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q28">
-        <v>1197000</v>
       </c>
     </row>
   </sheetData>
@@ -2257,7 +2195,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2268,10 +2206,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -2280,63 +2218,63 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
@@ -2348,7 +2286,7 @@
         <v>1220000</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I2">
         <v>79000</v>
@@ -2357,34 +2295,34 @@
         <v>89000</v>
       </c>
       <c r="K2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L2">
         <v>100000</v>
       </c>
       <c r="M2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O2">
         <v>34.42622950819672</v>
       </c>
       <c r="P2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="S2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -2392,13 +2330,13 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E3" t="s">
         <v>17</v>
@@ -2410,7 +2348,7 @@
         <v>7000000</v>
       </c>
       <c r="H3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I3">
         <v>2000</v>
@@ -2419,34 +2357,34 @@
         <v>2000</v>
       </c>
       <c r="K3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L3">
         <v>2000</v>
       </c>
       <c r="M3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="S3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -2454,13 +2392,13 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
@@ -2472,7 +2410,7 @@
         <v>4000000</v>
       </c>
       <c r="H4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I4">
         <v>2000</v>
@@ -2481,34 +2419,34 @@
         <v>2000</v>
       </c>
       <c r="K4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L4">
         <v>2000</v>
       </c>
       <c r="M4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="S4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -2516,10 +2454,10 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -2534,7 +2472,7 @@
         <v>14625000</v>
       </c>
       <c r="H5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I5">
         <v>4400</v>
@@ -2543,34 +2481,34 @@
         <v>5500</v>
       </c>
       <c r="K5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L5">
         <v>6000</v>
       </c>
       <c r="M5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O5">
         <v>40</v>
       </c>
       <c r="P5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="S5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -2578,13 +2516,13 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -2596,7 +2534,7 @@
         <v>1400000</v>
       </c>
       <c r="H6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I6">
         <v>15000</v>
@@ -2605,45 +2543,45 @@
         <v>19000</v>
       </c>
       <c r="K6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L6">
         <v>19000</v>
       </c>
       <c r="M6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="S6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D7" t="s">
         <v>24</v>
@@ -2658,7 +2596,7 @@
         <v>3500000</v>
       </c>
       <c r="H7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I7">
         <v>2000</v>
@@ -2667,48 +2605,48 @@
         <v>2000</v>
       </c>
       <c r="K7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L7">
         <v>2000</v>
       </c>
       <c r="M7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="S7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E8" t="s">
         <v>21</v>
@@ -2720,7 +2658,7 @@
         <v>750000</v>
       </c>
       <c r="H8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I8">
         <v>19000</v>
@@ -2729,45 +2667,45 @@
         <v>22000</v>
       </c>
       <c r="K8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L8">
         <v>23000</v>
       </c>
       <c r="M8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="S8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
         <v>24</v>
@@ -2782,7 +2720,7 @@
         <v>1500000</v>
       </c>
       <c r="H9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I9">
         <v>9000</v>
@@ -2791,45 +2729,45 @@
         <v>11000</v>
       </c>
       <c r="K9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L9">
         <v>9000</v>
       </c>
       <c r="M9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="S9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
         <v>24</v>
@@ -2844,7 +2782,7 @@
         <v>10000000</v>
       </c>
       <c r="H10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I10">
         <v>2000</v>
@@ -2853,34 +2791,34 @@
         <v>2000</v>
       </c>
       <c r="K10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L10">
         <v>2000</v>
       </c>
       <c r="M10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="S10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -2888,10 +2826,10 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
         <v>25</v>
@@ -2906,7 +2844,7 @@
         <v>650000</v>
       </c>
       <c r="H11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I11">
         <v>23000</v>
@@ -2915,34 +2853,34 @@
         <v>30000</v>
       </c>
       <c r="K11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L11">
         <v>18000</v>
       </c>
       <c r="M11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="S11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -2950,10 +2888,10 @@
         <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
         <v>25</v>
@@ -2968,7 +2906,7 @@
         <v>8000000</v>
       </c>
       <c r="H12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I12">
         <v>2000</v>
@@ -2977,45 +2915,45 @@
         <v>2000</v>
       </c>
       <c r="K12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L12">
         <v>2000</v>
       </c>
       <c r="M12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="S12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D13" t="s">
         <v>27</v>
@@ -3030,7 +2968,7 @@
         <v>1407000</v>
       </c>
       <c r="H13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I13">
         <v>21000</v>
@@ -3039,48 +2977,48 @@
         <v>25000</v>
       </c>
       <c r="K13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L13">
         <v>28000</v>
       </c>
       <c r="M13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O13">
         <v>40.01421464108032</v>
       </c>
       <c r="P13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="S13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E14" t="s">
         <v>25</v>
@@ -3092,7 +3030,7 @@
         <v>1640000</v>
       </c>
       <c r="H14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I14">
         <v>11000</v>
@@ -3101,48 +3039,48 @@
         <v>14000</v>
       </c>
       <c r="K14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L14">
         <v>17000</v>
       </c>
       <c r="M14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="S14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D15" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E15" t="s">
         <v>26</v>
@@ -3154,7 +3092,7 @@
         <v>3350000</v>
       </c>
       <c r="H15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I15">
         <v>8000</v>
@@ -3163,48 +3101,48 @@
         <v>9500</v>
       </c>
       <c r="K15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L15">
         <v>11000</v>
       </c>
       <c r="M15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="S15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E16" t="s">
         <v>25</v>
@@ -3216,7 +3154,7 @@
         <v>4250000</v>
       </c>
       <c r="H16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I16">
         <v>5200</v>
@@ -3225,48 +3163,48 @@
         <v>6000</v>
       </c>
       <c r="K16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L16">
         <v>7000</v>
       </c>
       <c r="M16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="S16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="E17" t="s">
         <v>27</v>
@@ -3278,7 +3216,7 @@
         <v>2079000</v>
       </c>
       <c r="H17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I17">
         <v>28500</v>
@@ -3287,48 +3225,48 @@
         <v>34700</v>
       </c>
       <c r="K17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L17">
         <v>34700</v>
       </c>
       <c r="M17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O17">
         <v>0</v>
       </c>
       <c r="P17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R17" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="S17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:20">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D18" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E18" t="s">
         <v>28</v>
@@ -3340,7 +3278,7 @@
         <v>1470400</v>
       </c>
       <c r="H18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I18">
         <v>33000</v>
@@ -3349,48 +3287,48 @@
         <v>37000</v>
       </c>
       <c r="K18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L18">
         <v>30000</v>
       </c>
       <c r="M18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O18">
         <v>23.28618063112079</v>
       </c>
       <c r="P18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="S18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:20">
       <c r="A19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E19" t="s">
         <v>29</v>
@@ -3402,7 +3340,7 @@
         <v>11580800</v>
       </c>
       <c r="H19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I19">
         <v>36200</v>
@@ -3411,96 +3349,34 @@
         <v>44000</v>
       </c>
       <c r="K19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L19">
         <v>36200</v>
       </c>
       <c r="M19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O19">
         <v>0</v>
       </c>
       <c r="P19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="S19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20">
-      <c r="A20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" t="s">
-        <v>75</v>
-      </c>
-      <c r="E20" t="s">
-        <v>30</v>
-      </c>
-      <c r="F20">
-        <v>6384000</v>
-      </c>
-      <c r="G20">
-        <v>1596000</v>
-      </c>
-      <c r="H20" t="s">
-        <v>65</v>
-      </c>
-      <c r="I20">
-        <v>3200</v>
-      </c>
-      <c r="J20">
-        <v>3600</v>
-      </c>
-      <c r="K20" t="s">
-        <v>65</v>
-      </c>
-      <c r="L20">
-        <v>4000</v>
-      </c>
-      <c r="M20" t="s">
-        <v>65</v>
-      </c>
-      <c r="N20" t="s">
-        <v>65</v>
-      </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>65</v>
-      </c>
-      <c r="R20" t="s">
-        <v>122</v>
-      </c>
-      <c r="S20" t="s">
-        <v>65</v>
-      </c>
-      <c r="T20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -3510,7 +3386,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3518,16 +3394,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -3539,10 +3415,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -3551,27 +3427,27 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G2" t="s">
         <v>17</v>
@@ -3594,22 +3470,22 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G3" t="s">
         <v>17</v>
@@ -3632,136 +3508,136 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>101</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>123</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="H4">
-        <v>72141.3</v>
+        <v>36196.872</v>
       </c>
       <c r="I4">
-        <v>2079000</v>
+        <v>14625000</v>
       </c>
       <c r="J4">
-        <v>34700</v>
+        <v>6000</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>100</v>
+        <v>41.25</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>103</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>126</v>
+        <v>50</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>82</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="H5">
-        <v>36196.872</v>
+        <v>72141.3</v>
       </c>
       <c r="I5">
-        <v>14625000</v>
+        <v>2079000</v>
       </c>
       <c r="J5">
-        <v>6000</v>
+        <v>34700</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
-        <v>41.25</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="E6" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="F6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="H6">
-        <v>121994.4706</v>
+        <v>42700</v>
       </c>
       <c r="I6">
-        <v>11580800</v>
+        <v>1220000</v>
       </c>
       <c r="J6">
-        <v>36200</v>
+        <v>100000</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6">
-        <v>29.1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G7" t="s">
         <v>28</v>
@@ -3784,72 +3660,72 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>101</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>123</v>
       </c>
       <c r="F8" t="s">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="G8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H8">
-        <v>27880</v>
+        <v>4387.5</v>
       </c>
       <c r="I8">
-        <v>1640000</v>
+        <v>14625000</v>
       </c>
       <c r="J8">
-        <v>17000</v>
+        <v>6000</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8">
-        <v>100</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" t="s">
         <v>25</v>
       </c>
-      <c r="G9" t="s">
-        <v>23</v>
-      </c>
       <c r="H9">
-        <v>16000</v>
+        <v>27880</v>
       </c>
       <c r="I9">
-        <v>8000000</v>
+        <v>1640000</v>
       </c>
       <c r="J9">
-        <v>2000</v>
+        <v>17000</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -3860,148 +3736,148 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>124</v>
       </c>
       <c r="F10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H10">
-        <v>6384</v>
+        <v>121994.4706</v>
       </c>
       <c r="I10">
-        <v>1596000</v>
+        <v>11580800</v>
       </c>
       <c r="J10">
-        <v>4000</v>
+        <v>36200</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
-        <v>100</v>
+        <v>29.1</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
       <c r="E11" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>79</v>
+        <v>25</v>
       </c>
       <c r="G11" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H11">
-        <v>42700</v>
+        <v>16000</v>
       </c>
       <c r="I11">
-        <v>1220000</v>
+        <v>8000000</v>
       </c>
       <c r="J11">
-        <v>100000</v>
+        <v>2000</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
-        <v>35</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>103</v>
+        <v>57</v>
       </c>
       <c r="E12" t="s">
-        <v>126</v>
+        <v>57</v>
       </c>
       <c r="F12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H12">
-        <v>4387.5</v>
+        <v>7000</v>
       </c>
       <c r="I12">
-        <v>14625000</v>
+        <v>3500000</v>
       </c>
       <c r="J12">
-        <v>6000</v>
+        <v>2000</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12">
-        <v>5</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" t="s">
         <v>71</v>
       </c>
-      <c r="C13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" t="s">
-        <v>24</v>
-      </c>
       <c r="G13" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H13">
+        <v>29750</v>
+      </c>
+      <c r="I13">
+        <v>4250000</v>
+      </c>
+      <c r="J13">
         <v>7000</v>
-      </c>
-      <c r="I13">
-        <v>3500000</v>
-      </c>
-      <c r="J13">
-        <v>2000</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -4012,57 +3888,57 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>124</v>
       </c>
       <c r="F14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G14" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="H14">
-        <v>29750</v>
+        <v>284653.7406</v>
       </c>
       <c r="I14">
-        <v>4250000</v>
+        <v>11580800</v>
       </c>
       <c r="J14">
-        <v>7000</v>
+        <v>36200</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14">
-        <v>100</v>
+        <v>67.90000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F15" t="s">
         <v>27</v>
@@ -4088,72 +3964,72 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E16" t="s">
-        <v>127</v>
+        <v>60</v>
       </c>
       <c r="F16" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="G16" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="H16">
-        <v>284653.7406</v>
+        <v>20000</v>
       </c>
       <c r="I16">
-        <v>11580800</v>
+        <v>10000000</v>
       </c>
       <c r="J16">
-        <v>36200</v>
+        <v>2000</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16">
-        <v>67.90000000000001</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F17" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="G17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H17">
-        <v>20000</v>
+        <v>17250</v>
       </c>
       <c r="I17">
-        <v>10000000</v>
+        <v>750000</v>
       </c>
       <c r="J17">
-        <v>2000</v>
+        <v>23000</v>
       </c>
       <c r="K17">
         <v>0</v>
@@ -4164,34 +4040,34 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C18" t="s">
         <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F18" t="s">
-        <v>83</v>
+        <v>24</v>
       </c>
       <c r="G18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H18">
-        <v>17250</v>
+        <v>13500</v>
       </c>
       <c r="I18">
-        <v>750000</v>
+        <v>1500000</v>
       </c>
       <c r="J18">
-        <v>23000</v>
+        <v>9000</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -4202,95 +4078,95 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>123</v>
       </c>
       <c r="F19" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H19">
-        <v>13500</v>
+        <v>6581.256</v>
       </c>
       <c r="I19">
-        <v>1500000</v>
+        <v>14625000</v>
       </c>
       <c r="J19">
-        <v>9000</v>
+        <v>6000</v>
       </c>
       <c r="K19">
         <v>0</v>
       </c>
       <c r="L19">
-        <v>100</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s">
         <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="E20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F20" t="s">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="G20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H20">
-        <v>6581.256</v>
+        <v>7980</v>
       </c>
       <c r="I20">
-        <v>14625000</v>
+        <v>1400000</v>
       </c>
       <c r="J20">
-        <v>6000</v>
+        <v>19000</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
       <c r="L20">
-        <v>7.5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B21" t="s">
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E21" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F21" t="s">
         <v>21</v>
@@ -4316,28 +4192,28 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E22" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F22" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G22" t="s">
         <v>19</v>
       </c>
       <c r="H22">
-        <v>7980</v>
+        <v>18620</v>
       </c>
       <c r="I22">
         <v>1400000</v>
@@ -4349,39 +4225,39 @@
         <v>0</v>
       </c>
       <c r="L22">
-        <v>30</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F23" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="G23" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H23">
-        <v>11700</v>
+        <v>14000</v>
       </c>
       <c r="I23">
-        <v>650000</v>
+        <v>7000000</v>
       </c>
       <c r="J23">
-        <v>18000</v>
+        <v>2000</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -4392,34 +4268,34 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D24" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E24" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F24" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="G24" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H24">
-        <v>14000</v>
+        <v>11700</v>
       </c>
       <c r="I24">
-        <v>7000000</v>
+        <v>650000</v>
       </c>
       <c r="J24">
-        <v>2000</v>
+        <v>18000</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -4430,98 +4306,98 @@
     </row>
     <row r="25" spans="1:12">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D25" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E25" t="s">
-        <v>128</v>
+        <v>56</v>
       </c>
       <c r="F25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G25" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="H25">
-        <v>18620</v>
+        <v>36850</v>
       </c>
       <c r="I25">
-        <v>1400000</v>
+        <v>3350000</v>
       </c>
       <c r="J25">
-        <v>19000</v>
+        <v>11000</v>
       </c>
       <c r="K25">
         <v>0</v>
       </c>
       <c r="L25">
-        <v>70</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D26" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
       <c r="E26" t="s">
-        <v>58</v>
+        <v>123</v>
       </c>
       <c r="F26" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="G26" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="H26">
-        <v>36850</v>
+        <v>4387.5</v>
       </c>
       <c r="I26">
-        <v>3350000</v>
+        <v>14625000</v>
       </c>
       <c r="J26">
-        <v>11000</v>
+        <v>6000</v>
       </c>
       <c r="K26">
         <v>0</v>
       </c>
       <c r="L26">
-        <v>100</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D27" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E27" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G27" t="s">
         <v>29</v>
@@ -4540,44 +4416,6 @@
       </c>
       <c r="L27">
         <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28" t="s">
-        <v>103</v>
-      </c>
-      <c r="E28" t="s">
-        <v>126</v>
-      </c>
-      <c r="F28" t="s">
-        <v>21</v>
-      </c>
-      <c r="G28" t="s">
-        <v>18</v>
-      </c>
-      <c r="H28">
-        <v>4387.5</v>
-      </c>
-      <c r="I28">
-        <v>14625000</v>
-      </c>
-      <c r="J28">
-        <v>6000</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="L28">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-03-14
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="128">
   <si>
     <t>상장일</t>
   </si>
@@ -69,6 +69,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2024-03-13</t>
+  </si>
+  <si>
     <t>2024-03-07</t>
   </si>
   <si>
@@ -108,6 +111,9 @@
     <t>2024-01-24</t>
   </si>
   <si>
+    <t>오상헬스케어</t>
+  </si>
+  <si>
     <t>케이엔알시스템</t>
   </si>
   <si>
@@ -322,6 +328,9 @@
   </si>
   <si>
     <t>DB, NH</t>
+  </si>
+  <si>
+    <t>2126.13 : 1</t>
   </si>
   <si>
     <t>2266.72 : 1</t>
@@ -748,7 +757,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -812,90 +821,90 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D2">
-        <v>284.04</v>
+        <v>198</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F2">
-        <v>142.02</v>
+        <v>198</v>
       </c>
       <c r="G2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="L2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M2">
-        <v>13500</v>
+        <v>20000</v>
       </c>
       <c r="N2">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>70</v>
+        <v>21</v>
       </c>
       <c r="P2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q2">
-        <v>2916000</v>
+        <v>742500</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D3">
         <v>284.04</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F3">
         <v>142.02</v>
       </c>
       <c r="G3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M3">
         <v>13500</v>
@@ -904,10 +913,10 @@
         <v>50</v>
       </c>
       <c r="O3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="P3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q3">
         <v>2916000</v>
@@ -918,52 +927,52 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D4">
-        <v>100</v>
+        <v>284.04</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F4">
-        <v>100</v>
+        <v>142.02</v>
       </c>
       <c r="G4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="L4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M4">
-        <v>2000</v>
+        <v>13500</v>
       </c>
       <c r="N4">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O4" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="P4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Q4">
-        <v>3750000</v>
+        <v>2916000</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -971,37 +980,37 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D5">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F5">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M5">
         <v>2000</v>
@@ -1010,13 +1019,13 @@
         <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="P5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="Q5">
-        <v>4875000</v>
+        <v>3750000</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1024,37 +1033,37 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D6">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F6">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="G6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M6">
         <v>2000</v>
@@ -1063,51 +1072,51 @@
         <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="P6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q6">
-        <v>3000000</v>
+        <v>4875000</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D7">
         <v>80</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F7">
         <v>80</v>
       </c>
       <c r="G7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M7">
         <v>2000</v>
@@ -1116,10 +1125,10 @@
         <v>100</v>
       </c>
       <c r="O7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="P7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q7">
         <v>3000000</v>
@@ -1130,37 +1139,37 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D8">
         <v>80</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F8">
         <v>80</v>
       </c>
       <c r="G8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K8" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M8">
         <v>2000</v>
@@ -1169,10 +1178,10 @@
         <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="P8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q8">
         <v>3000000</v>
@@ -1180,55 +1189,55 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D9">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F9">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="G9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K9" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M9">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="N9">
         <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="P9" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="Q9">
-        <v>420000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1236,102 +1245,102 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D10">
-        <v>947.5</v>
+        <v>96</v>
       </c>
       <c r="E10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F10">
-        <v>758</v>
+        <v>96</v>
       </c>
       <c r="G10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K10" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M10">
-        <v>250000</v>
+        <v>16000</v>
       </c>
       <c r="N10">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="O10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="P10" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="Q10">
-        <v>416900</v>
+        <v>420000</v>
       </c>
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D11">
         <v>947.5</v>
       </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="F11">
-        <v>189.5</v>
+        <v>758</v>
       </c>
       <c r="G11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M11">
         <v>250000</v>
       </c>
       <c r="N11">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="O11" t="s">
+        <v>76</v>
+      </c>
+      <c r="P11" t="s">
         <v>74</v>
-      </c>
-      <c r="P11" t="s">
-        <v>72</v>
       </c>
       <c r="Q11">
         <v>416900</v>
@@ -1342,211 +1351,211 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D12">
-        <v>70</v>
+        <v>947.5</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F12">
-        <v>70</v>
+        <v>189.5</v>
       </c>
       <c r="G12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K12" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="L12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M12">
-        <v>7000</v>
+        <v>250000</v>
       </c>
       <c r="N12">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="O12" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="P12" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="Q12">
-        <v>750000</v>
+        <v>416900</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D13">
-        <v>226</v>
+        <v>70</v>
       </c>
       <c r="E13" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F13">
-        <v>226</v>
+        <v>70</v>
       </c>
       <c r="G13" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H13" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I13" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J13" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K13" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L13" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M13">
-        <v>20000</v>
+        <v>7000</v>
       </c>
       <c r="N13">
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="P13" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="Q13">
-        <v>827500</v>
+        <v>750000</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D14">
-        <v>91.5</v>
+        <v>226</v>
       </c>
       <c r="E14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F14">
-        <v>91.5</v>
+        <v>226</v>
       </c>
       <c r="G14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K14" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M14">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="N14">
         <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="P14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Q14">
-        <v>3431250</v>
+        <v>827500</v>
       </c>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D15">
-        <v>153</v>
+        <v>91.5</v>
       </c>
       <c r="E15" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="F15">
-        <v>153</v>
+        <v>91.5</v>
       </c>
       <c r="G15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K15" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M15">
-        <v>18000</v>
+        <v>2000</v>
       </c>
       <c r="N15">
         <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P15" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="Q15">
-        <v>637500</v>
+        <v>3431250</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1554,105 +1563,105 @@
         <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D16">
-        <v>420</v>
+        <v>153</v>
       </c>
       <c r="E16" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F16">
-        <v>420</v>
+        <v>153</v>
       </c>
       <c r="G16" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H16" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I16" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J16" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K16" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L16" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M16">
-        <v>14000</v>
+        <v>18000</v>
       </c>
       <c r="N16">
         <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="P16" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="Q16">
-        <v>2100000</v>
+        <v>637500</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D17">
-        <v>80</v>
+        <v>420</v>
       </c>
       <c r="E17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F17">
-        <v>80</v>
+        <v>420</v>
       </c>
       <c r="G17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K17" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M17">
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="N17">
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="P17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q17">
-        <v>3000000</v>
+        <v>2100000</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -1660,52 +1669,52 @@
         <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D18">
-        <v>270</v>
+        <v>80</v>
       </c>
       <c r="E18" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="F18">
-        <v>270</v>
+        <v>80</v>
       </c>
       <c r="G18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K18" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M18">
-        <v>18000</v>
+        <v>2000</v>
       </c>
       <c r="N18">
         <v>100</v>
       </c>
       <c r="O18" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="P18" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="Q18">
-        <v>1112478</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1713,52 +1722,52 @@
         <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D19">
-        <v>635.611</v>
+        <v>270</v>
       </c>
       <c r="E19" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="F19">
-        <v>635.611</v>
+        <v>270</v>
       </c>
       <c r="G19" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H19" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I19" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J19" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K19" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L19" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M19">
-        <v>7300</v>
+        <v>18000</v>
       </c>
       <c r="N19">
         <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="P19" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="Q19">
-        <v>5513403</v>
+        <v>1112478</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -1766,52 +1775,52 @@
         <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D20">
-        <v>226.678</v>
+        <v>635.611</v>
       </c>
       <c r="E20" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="F20">
-        <v>226.678</v>
+        <v>635.611</v>
       </c>
       <c r="G20" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H20" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I20" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J20" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K20" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L20" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M20">
-        <v>3400</v>
+        <v>7300</v>
       </c>
       <c r="N20">
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="P20" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="Q20">
-        <v>5000250</v>
+        <v>5513403</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1819,104 +1828,157 @@
         <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D21">
-        <v>109.18</v>
+        <v>226.678</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="F21">
-        <v>109.18</v>
+        <v>226.678</v>
       </c>
       <c r="G21" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H21" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I21" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J21" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K21" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L21" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M21">
-        <v>5300</v>
+        <v>3400</v>
       </c>
       <c r="N21">
         <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="P21" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q21">
-        <v>1133000</v>
+        <v>5000250</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D22">
-        <v>110</v>
+        <v>109.18</v>
       </c>
       <c r="E22" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F22">
-        <v>110</v>
+        <v>109.18</v>
       </c>
       <c r="G22" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H22" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I22" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J22" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K22" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L22" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M22">
-        <v>2000</v>
+        <v>5300</v>
       </c>
       <c r="N22">
         <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="P22" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="Q22">
+        <v>1133000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23">
+        <v>110</v>
+      </c>
+      <c r="E23" t="s">
+        <v>68</v>
+      </c>
+      <c r="F23">
+        <v>110</v>
+      </c>
+      <c r="G23" t="s">
+        <v>69</v>
+      </c>
+      <c r="H23" t="s">
+        <v>69</v>
+      </c>
+      <c r="I23" t="s">
+        <v>69</v>
+      </c>
+      <c r="J23" t="s">
+        <v>69</v>
+      </c>
+      <c r="K23" t="s">
+        <v>70</v>
+      </c>
+      <c r="L23" t="s">
+        <v>69</v>
+      </c>
+      <c r="M23">
+        <v>2000</v>
+      </c>
+      <c r="N23">
+        <v>100</v>
+      </c>
+      <c r="O23" t="s">
+        <v>80</v>
+      </c>
+      <c r="P23" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q23">
         <v>4125000</v>
       </c>
     </row>
@@ -1927,7 +1989,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1938,10 +2000,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -1950,199 +2012,199 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
       </c>
       <c r="F2">
-        <v>28404000</v>
+        <v>19800000</v>
       </c>
       <c r="G2">
-        <v>2104000</v>
+        <v>990000</v>
       </c>
       <c r="H2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I2">
-        <v>9000</v>
+        <v>13000</v>
       </c>
       <c r="J2">
-        <v>11000</v>
+        <v>15000</v>
       </c>
       <c r="K2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L2">
-        <v>13500</v>
+        <v>20000</v>
       </c>
       <c r="M2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="S2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="T2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>103</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
       </c>
       <c r="F3">
-        <v>10000000</v>
+        <v>28404000</v>
       </c>
       <c r="G3">
-        <v>5000000</v>
+        <v>2104000</v>
       </c>
       <c r="H3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I3">
-        <v>2000</v>
+        <v>9000</v>
       </c>
       <c r="J3">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="K3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L3">
-        <v>2000</v>
+        <v>13500</v>
       </c>
       <c r="M3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="S3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="T3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
       </c>
       <c r="F4">
-        <v>13000000</v>
+        <v>10000000</v>
       </c>
       <c r="G4">
-        <v>6500000</v>
+        <v>5000000</v>
       </c>
       <c r="H4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I4">
         <v>2000</v>
@@ -2151,60 +2213,60 @@
         <v>2000</v>
       </c>
       <c r="K4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L4">
         <v>2000</v>
       </c>
       <c r="M4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="S4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="T4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
       </c>
       <c r="F5">
-        <v>8000000</v>
+        <v>13000000</v>
       </c>
       <c r="G5">
-        <v>4000000</v>
+        <v>6500000</v>
       </c>
       <c r="H5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I5">
         <v>2000</v>
@@ -2213,51 +2275,51 @@
         <v>2000</v>
       </c>
       <c r="K5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L5">
         <v>2000</v>
       </c>
       <c r="M5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="S5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="T5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F6">
         <v>8000000</v>
@@ -2266,7 +2328,7 @@
         <v>4000000</v>
       </c>
       <c r="H6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I6">
         <v>2000</v>
@@ -2275,48 +2337,48 @@
         <v>2000</v>
       </c>
       <c r="K6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L6">
         <v>2000</v>
       </c>
       <c r="M6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R6" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="S6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="T6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
@@ -2328,7 +2390,7 @@
         <v>4000000</v>
       </c>
       <c r="H7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I7">
         <v>2000</v>
@@ -2337,840 +2399,902 @@
         <v>2000</v>
       </c>
       <c r="K7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L7">
         <v>2000</v>
       </c>
       <c r="M7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R7" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="S7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="T7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8">
-        <v>9600000</v>
+        <v>8000000</v>
       </c>
       <c r="G8">
-        <v>600000</v>
+        <v>4000000</v>
       </c>
       <c r="H8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I8">
-        <v>12000</v>
+        <v>2000</v>
       </c>
       <c r="J8">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="K8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L8">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="M8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="S8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="T8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="E9" t="s">
         <v>22</v>
       </c>
       <c r="F9">
-        <v>94750000</v>
+        <v>9600000</v>
       </c>
       <c r="G9">
-        <v>379000</v>
+        <v>600000</v>
       </c>
       <c r="H9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I9">
-        <v>147000</v>
+        <v>12000</v>
       </c>
       <c r="J9">
-        <v>200000</v>
+        <v>14000</v>
       </c>
       <c r="K9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L9">
-        <v>250000</v>
+        <v>16000</v>
       </c>
       <c r="M9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O9">
-        <v>18.46965699208443</v>
+        <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R9" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="S9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="T9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E10" t="s">
         <v>23</v>
       </c>
       <c r="F10">
-        <v>7000000</v>
+        <v>94750000</v>
       </c>
       <c r="G10">
-        <v>1000000</v>
+        <v>379000</v>
       </c>
       <c r="H10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I10">
-        <v>4800</v>
+        <v>147000</v>
       </c>
       <c r="J10">
-        <v>5800</v>
+        <v>200000</v>
       </c>
       <c r="K10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L10">
-        <v>7000</v>
+        <v>250000</v>
       </c>
       <c r="M10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O10">
-        <v>0</v>
+        <v>18.46965699208443</v>
       </c>
       <c r="P10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="S10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="T10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E11" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F11">
-        <v>22600000</v>
+        <v>7000000</v>
       </c>
       <c r="G11">
-        <v>1130000</v>
+        <v>1000000</v>
       </c>
       <c r="H11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I11">
-        <v>14500</v>
+        <v>4800</v>
       </c>
       <c r="J11">
-        <v>18500</v>
+        <v>5800</v>
       </c>
       <c r="K11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L11">
-        <v>20000</v>
+        <v>7000</v>
       </c>
       <c r="M11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R11" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="S11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="T11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F12">
-        <v>9150000</v>
+        <v>22600000</v>
       </c>
       <c r="G12">
-        <v>4575000</v>
+        <v>1130000</v>
       </c>
       <c r="H12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I12">
-        <v>2000</v>
+        <v>14500</v>
       </c>
       <c r="J12">
-        <v>2000</v>
+        <v>18500</v>
       </c>
       <c r="K12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L12">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="M12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R12" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="S12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="T12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="D13" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F13">
-        <v>15300000</v>
+        <v>9150000</v>
       </c>
       <c r="G13">
-        <v>850000</v>
+        <v>4575000</v>
       </c>
       <c r="H13" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I13">
-        <v>14500</v>
+        <v>2000</v>
       </c>
       <c r="J13">
-        <v>16500</v>
+        <v>2000</v>
       </c>
       <c r="K13" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L13">
-        <v>18000</v>
+        <v>2000</v>
       </c>
       <c r="M13" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N13" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q13" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R13" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="S13" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="T13" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="E14" t="s">
         <v>25</v>
       </c>
       <c r="F14">
-        <v>42000000</v>
+        <v>15300000</v>
       </c>
       <c r="G14">
-        <v>3000000</v>
+        <v>850000</v>
       </c>
       <c r="H14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I14">
-        <v>9200</v>
+        <v>14500</v>
       </c>
       <c r="J14">
-        <v>11000</v>
+        <v>16500</v>
       </c>
       <c r="K14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L14">
-        <v>14000</v>
+        <v>18000</v>
       </c>
       <c r="M14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R14" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="S14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="T14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F15">
-        <v>8000000</v>
+        <v>42000000</v>
       </c>
       <c r="G15">
-        <v>4000000</v>
+        <v>3000000</v>
       </c>
       <c r="H15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I15">
-        <v>2000</v>
+        <v>9200</v>
       </c>
       <c r="J15">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="K15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L15">
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="M15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R15" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="S15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="T15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="D16" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="E16" t="s">
         <v>26</v>
       </c>
       <c r="F16">
-        <v>27000000</v>
+        <v>8000000</v>
       </c>
       <c r="G16">
-        <v>1500000</v>
+        <v>4000000</v>
       </c>
       <c r="H16" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I16">
-        <v>13000</v>
+        <v>2000</v>
       </c>
       <c r="J16">
-        <v>15000</v>
+        <v>2000</v>
       </c>
       <c r="K16" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L16">
-        <v>18000</v>
+        <v>2000</v>
       </c>
       <c r="M16" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N16" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q16" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R16" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="S16" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="T16" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D17" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E17" t="s">
         <v>27</v>
       </c>
       <c r="F17">
-        <v>63561100</v>
+        <v>27000000</v>
       </c>
       <c r="G17">
-        <v>8707000</v>
+        <v>1500000</v>
       </c>
       <c r="H17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I17">
-        <v>5000</v>
+        <v>13000</v>
       </c>
       <c r="J17">
-        <v>6300</v>
+        <v>15000</v>
       </c>
       <c r="K17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L17">
-        <v>7300</v>
+        <v>18000</v>
       </c>
       <c r="M17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O17">
-        <v>40.00229700241185</v>
+        <v>0</v>
       </c>
       <c r="P17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R17" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="S17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="T17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:20">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E18" t="s">
         <v>28</v>
       </c>
       <c r="F18">
-        <v>22667800</v>
+        <v>63561100</v>
       </c>
       <c r="G18">
-        <v>6667000</v>
+        <v>8707000</v>
       </c>
       <c r="H18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I18">
-        <v>2400</v>
+        <v>5000</v>
       </c>
       <c r="J18">
-        <v>2800</v>
+        <v>6300</v>
       </c>
       <c r="K18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L18">
-        <v>3400</v>
+        <v>7300</v>
       </c>
       <c r="M18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O18">
-        <v>0</v>
+        <v>40.00229700241185</v>
       </c>
       <c r="P18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R18" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="S18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="T18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:20">
       <c r="A19" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E19" t="s">
         <v>29</v>
       </c>
       <c r="F19">
-        <v>10918000</v>
+        <v>22667800</v>
       </c>
       <c r="G19">
-        <v>2060000</v>
+        <v>6667000</v>
       </c>
       <c r="H19" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I19">
-        <v>4300</v>
+        <v>2400</v>
       </c>
       <c r="J19">
-        <v>4900</v>
+        <v>2800</v>
       </c>
       <c r="K19" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L19">
-        <v>5300</v>
+        <v>3400</v>
       </c>
       <c r="M19" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N19" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O19">
         <v>0</v>
       </c>
       <c r="P19" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q19" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R19" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="S19" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="T19" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D20" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F20">
+        <v>10918000</v>
+      </c>
+      <c r="G20">
+        <v>2060000</v>
+      </c>
+      <c r="H20" t="s">
+        <v>69</v>
+      </c>
+      <c r="I20">
+        <v>4300</v>
+      </c>
+      <c r="J20">
+        <v>4900</v>
+      </c>
+      <c r="K20" t="s">
+        <v>69</v>
+      </c>
+      <c r="L20">
+        <v>5300</v>
+      </c>
+      <c r="M20" t="s">
+        <v>69</v>
+      </c>
+      <c r="N20" t="s">
+        <v>69</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>69</v>
+      </c>
+      <c r="R20" t="s">
+        <v>122</v>
+      </c>
+      <c r="S20" t="s">
+        <v>69</v>
+      </c>
+      <c r="T20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21">
         <v>11000000</v>
       </c>
-      <c r="G20">
+      <c r="G21">
         <v>5500000</v>
       </c>
-      <c r="H20" t="s">
-        <v>67</v>
-      </c>
-      <c r="I20">
+      <c r="H21" t="s">
+        <v>69</v>
+      </c>
+      <c r="I21">
         <v>2000</v>
       </c>
-      <c r="J20">
+      <c r="J21">
         <v>2000</v>
       </c>
-      <c r="K20" t="s">
-        <v>67</v>
-      </c>
-      <c r="L20">
+      <c r="K21" t="s">
+        <v>69</v>
+      </c>
+      <c r="L21">
         <v>2000</v>
       </c>
-      <c r="M20" t="s">
-        <v>67</v>
-      </c>
-      <c r="N20" t="s">
-        <v>67</v>
-      </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>67</v>
-      </c>
-      <c r="R20" t="s">
-        <v>120</v>
-      </c>
-      <c r="S20" t="s">
-        <v>67</v>
-      </c>
-      <c r="T20" t="s">
-        <v>67</v>
+      <c r="M21" t="s">
+        <v>69</v>
+      </c>
+      <c r="N21" t="s">
+        <v>69</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>69</v>
+      </c>
+      <c r="R21" t="s">
+        <v>123</v>
+      </c>
+      <c r="S21" t="s">
+        <v>69</v>
+      </c>
+      <c r="T21" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -3180,7 +3304,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3188,16 +3312,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -3209,10 +3333,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -3221,30 +3345,30 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H2">
         <v>8000</v>
@@ -3264,25 +3388,25 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H3">
         <v>14202</v>
@@ -3302,25 +3426,25 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H4">
         <v>15300</v>
@@ -3340,25 +3464,25 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H5">
         <v>8000</v>
@@ -3378,25 +3502,25 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H6">
         <v>10918</v>
@@ -3416,110 +3540,110 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>101</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>101</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G7" t="s">
         <v>17</v>
       </c>
       <c r="H7">
-        <v>14202</v>
+        <v>19800</v>
       </c>
       <c r="I7">
-        <v>2104000</v>
+        <v>990000</v>
       </c>
       <c r="J7">
-        <v>13500</v>
+        <v>20000</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
       <c r="E8" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
       <c r="F8" t="s">
-        <v>82</v>
+        <v>20</v>
       </c>
       <c r="G8" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="H8">
-        <v>22667.8</v>
+        <v>14202</v>
       </c>
       <c r="I8">
-        <v>6667000</v>
+        <v>2104000</v>
       </c>
       <c r="J8">
-        <v>3400</v>
+        <v>13500</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F9" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="G9" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="H9">
-        <v>7000</v>
+        <v>22667.8</v>
       </c>
       <c r="I9">
-        <v>1000000</v>
+        <v>6667000</v>
       </c>
       <c r="J9">
-        <v>7000</v>
+        <v>3400</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -3530,34 +3654,34 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="G10" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H10">
-        <v>8000</v>
+        <v>7000</v>
       </c>
       <c r="I10">
-        <v>4000000</v>
+        <v>1000000</v>
       </c>
       <c r="J10">
-        <v>2000</v>
+        <v>7000</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -3568,31 +3692,31 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="F11" t="s">
-        <v>83</v>
+        <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H11">
-        <v>11000</v>
+        <v>8000</v>
       </c>
       <c r="I11">
-        <v>5500000</v>
+        <v>4000000</v>
       </c>
       <c r="J11">
         <v>2000</v>
@@ -3606,34 +3730,34 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E12" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="F12" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H12">
-        <v>63561.1</v>
+        <v>11000</v>
       </c>
       <c r="I12">
-        <v>8707000</v>
+        <v>5500000</v>
       </c>
       <c r="J12">
-        <v>7300</v>
+        <v>2000</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -3644,34 +3768,34 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E13" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F13" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="G13" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H13">
-        <v>42000</v>
+        <v>63561.1</v>
       </c>
       <c r="I13">
-        <v>3000000</v>
+        <v>8707000</v>
       </c>
       <c r="J13">
-        <v>14000</v>
+        <v>7300</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -3682,34 +3806,34 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" t="s">
         <v>28</v>
       </c>
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" t="s">
-        <v>61</v>
-      </c>
-      <c r="F14" t="s">
-        <v>80</v>
-      </c>
       <c r="G14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H14">
-        <v>9150</v>
+        <v>42000</v>
       </c>
       <c r="I14">
-        <v>4575000</v>
+        <v>3000000</v>
       </c>
       <c r="J14">
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -3720,107 +3844,107 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E15" t="s">
-        <v>124</v>
+        <v>63</v>
       </c>
       <c r="F15" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="G15" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H15">
-        <v>75800</v>
+        <v>9150</v>
       </c>
       <c r="I15">
-        <v>379000</v>
+        <v>4575000</v>
       </c>
       <c r="J15">
-        <v>250000</v>
+        <v>2000</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>127</v>
       </c>
       <c r="F16" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="G16" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H16">
-        <v>13000</v>
+        <v>75800</v>
       </c>
       <c r="I16">
-        <v>6500000</v>
+        <v>379000</v>
       </c>
       <c r="J16">
-        <v>2000</v>
+        <v>250000</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H17">
-        <v>8000</v>
+        <v>13000</v>
       </c>
       <c r="I17">
-        <v>4000000</v>
+        <v>6500000</v>
       </c>
       <c r="J17">
         <v>2000</v>
@@ -3834,34 +3958,34 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F18" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="G18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H18">
-        <v>9600</v>
+        <v>8000</v>
       </c>
       <c r="I18">
-        <v>600000</v>
+        <v>4000000</v>
       </c>
       <c r="J18">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -3872,63 +3996,63 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E19" t="s">
-        <v>124</v>
+        <v>60</v>
       </c>
       <c r="F19" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="G19" t="s">
         <v>22</v>
       </c>
       <c r="H19">
-        <v>18950</v>
+        <v>9600</v>
       </c>
       <c r="I19">
-        <v>379000</v>
+        <v>600000</v>
       </c>
       <c r="J19">
-        <v>250000</v>
+        <v>16000</v>
       </c>
       <c r="K19">
         <v>0</v>
       </c>
       <c r="L19">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D20" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E20" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F20" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H20">
         <v>27000</v>
@@ -3948,25 +4072,25 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" t="s">
         <v>23</v>
       </c>
-      <c r="C21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" t="s">
-        <v>22</v>
-      </c>
       <c r="G21" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H21">
         <v>10000</v>
@@ -3986,39 +4110,77 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C22" t="s">
         <v>39</v>
       </c>
       <c r="D22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E22" t="s">
-        <v>60</v>
+        <v>127</v>
       </c>
       <c r="F22" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G22" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H22">
+        <v>18950</v>
+      </c>
+      <c r="I22">
+        <v>379000</v>
+      </c>
+      <c r="J22">
+        <v>250000</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" t="s">
+        <v>81</v>
+      </c>
+      <c r="G23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23">
         <v>22600</v>
       </c>
-      <c r="I22">
+      <c r="I23">
         <v>1130000</v>
       </c>
-      <c r="J22">
+      <c r="J23">
         <v>20000</v>
       </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2024-03-19
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="123">
   <si>
     <t>상장일</t>
   </si>
@@ -168,9 +168,6 @@
     <t>우진엔텍</t>
   </si>
   <si>
-    <t>대신밸런스제17호스팩</t>
-  </si>
-  <si>
     <t>코스닥</t>
   </si>
   <si>
@@ -222,9 +219,6 @@
     <t>KB</t>
   </si>
   <si>
-    <t>대신</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -258,9 +252,6 @@
     <t>2024-01-16</t>
   </si>
   <si>
-    <t>2024-01-15</t>
-  </si>
-  <si>
     <t>2024-02-16</t>
   </si>
   <si>
@@ -273,9 +264,6 @@
     <t>2024-01-19</t>
   </si>
   <si>
-    <t>2024-01-18</t>
-  </si>
-  <si>
     <t>회사명</t>
   </si>
   <si>
@@ -385,9 +373,6 @@
   </si>
   <si>
     <t>2707.18 : 1</t>
-  </si>
-  <si>
-    <t>1240.15 : 1</t>
   </si>
   <si>
     <t>인수기관</t>
@@ -757,7 +742,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -824,34 +809,34 @@
         <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2">
         <v>198</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F2">
         <v>198</v>
       </c>
       <c r="G2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M2">
         <v>20000</v>
@@ -877,34 +862,34 @@
         <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3">
         <v>284.04</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F3">
         <v>142.02</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M3">
         <v>13500</v>
@@ -913,7 +898,7 @@
         <v>50</v>
       </c>
       <c r="O3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P3" t="s">
         <v>20</v>
@@ -930,34 +915,34 @@
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4">
         <v>284.04</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F4">
         <v>142.02</v>
       </c>
       <c r="G4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M4">
         <v>13500</v>
@@ -966,7 +951,7 @@
         <v>50</v>
       </c>
       <c r="O4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P4" t="s">
         <v>20</v>
@@ -983,34 +968,34 @@
         <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5">
         <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F5">
         <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M5">
         <v>2000</v>
@@ -1036,34 +1021,34 @@
         <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6">
         <v>130</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F6">
         <v>130</v>
       </c>
       <c r="G6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M6">
         <v>2000</v>
@@ -1072,7 +1057,7 @@
         <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="P6" t="s">
         <v>22</v>
@@ -1089,34 +1074,34 @@
         <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7">
         <v>80</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F7">
         <v>80</v>
       </c>
       <c r="G7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M7">
         <v>2000</v>
@@ -1125,7 +1110,7 @@
         <v>100</v>
       </c>
       <c r="O7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="P7" t="s">
         <v>22</v>
@@ -1142,34 +1127,34 @@
         <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8">
         <v>80</v>
       </c>
       <c r="E8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F8">
         <v>80</v>
       </c>
       <c r="G8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M8">
         <v>2000</v>
@@ -1178,7 +1163,7 @@
         <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="P8" t="s">
         <v>24</v>
@@ -1195,34 +1180,34 @@
         <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D9">
         <v>80</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F9">
         <v>80</v>
       </c>
       <c r="G9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M9">
         <v>2000</v>
@@ -1231,7 +1216,7 @@
         <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="P9" t="s">
         <v>24</v>
@@ -1248,34 +1233,34 @@
         <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10">
         <v>96</v>
       </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F10">
         <v>96</v>
       </c>
       <c r="G10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M10">
         <v>16000</v>
@@ -1284,10 +1269,10 @@
         <v>100</v>
       </c>
       <c r="O10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q10">
         <v>420000</v>
@@ -1301,34 +1286,34 @@
         <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D11">
         <v>947.5</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F11">
         <v>758</v>
       </c>
       <c r="G11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M11">
         <v>250000</v>
@@ -1337,10 +1322,10 @@
         <v>80</v>
       </c>
       <c r="O11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Q11">
         <v>416900</v>
@@ -1354,34 +1339,34 @@
         <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D12">
         <v>947.5</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F12">
         <v>189.5</v>
       </c>
       <c r="G12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J12" t="s">
+        <v>67</v>
+      </c>
+      <c r="K12" t="s">
         <v>69</v>
       </c>
-      <c r="H12" t="s">
-        <v>69</v>
-      </c>
-      <c r="I12" t="s">
-        <v>69</v>
-      </c>
-      <c r="J12" t="s">
-        <v>69</v>
-      </c>
-      <c r="K12" t="s">
-        <v>71</v>
-      </c>
       <c r="L12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M12">
         <v>250000</v>
@@ -1390,10 +1375,10 @@
         <v>20</v>
       </c>
       <c r="O12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Q12">
         <v>416900</v>
@@ -1407,34 +1392,34 @@
         <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D13">
         <v>70</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F13">
         <v>70</v>
       </c>
       <c r="G13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M13">
         <v>7000</v>
@@ -1443,10 +1428,10 @@
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q13">
         <v>750000</v>
@@ -1460,34 +1445,34 @@
         <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14">
         <v>226</v>
       </c>
       <c r="E14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F14">
         <v>226</v>
       </c>
       <c r="G14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M14">
         <v>20000</v>
@@ -1496,10 +1481,10 @@
         <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q14">
         <v>827500</v>
@@ -1513,34 +1498,34 @@
         <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15">
         <v>91.5</v>
       </c>
       <c r="E15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F15">
         <v>91.5</v>
       </c>
       <c r="G15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M15">
         <v>2000</v>
@@ -1552,7 +1537,7 @@
         <v>29</v>
       </c>
       <c r="P15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="Q15">
         <v>3431250</v>
@@ -1566,34 +1551,34 @@
         <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D16">
         <v>153</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F16">
         <v>153</v>
       </c>
       <c r="G16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M16">
         <v>18000</v>
@@ -1605,7 +1590,7 @@
         <v>29</v>
       </c>
       <c r="P16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="Q16">
         <v>637500</v>
@@ -1619,34 +1604,34 @@
         <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D17">
         <v>420</v>
       </c>
       <c r="E17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F17">
         <v>420</v>
       </c>
       <c r="G17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M17">
         <v>14000</v>
@@ -1655,7 +1640,7 @@
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P17" t="s">
         <v>28</v>
@@ -1672,34 +1657,34 @@
         <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D18">
         <v>80</v>
       </c>
       <c r="E18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F18">
         <v>80</v>
       </c>
       <c r="G18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M18">
         <v>2000</v>
@@ -1708,7 +1693,7 @@
         <v>100</v>
       </c>
       <c r="O18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P18" t="s">
         <v>28</v>
@@ -1725,34 +1710,34 @@
         <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D19">
         <v>270</v>
       </c>
       <c r="E19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F19">
         <v>270</v>
       </c>
       <c r="G19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M19">
         <v>18000</v>
@@ -1761,10 +1746,10 @@
         <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="P19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="Q19">
         <v>1112478</v>
@@ -1778,34 +1763,34 @@
         <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D20">
         <v>635.611</v>
       </c>
       <c r="E20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F20">
         <v>635.611</v>
       </c>
       <c r="G20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M20">
         <v>7300</v>
@@ -1814,10 +1799,10 @@
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="P20" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="Q20">
         <v>5513403</v>
@@ -1831,34 +1816,34 @@
         <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D21">
         <v>226.678</v>
       </c>
       <c r="E21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F21">
         <v>226.678</v>
       </c>
       <c r="G21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M21">
         <v>3400</v>
@@ -1867,10 +1852,10 @@
         <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P21" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="Q21">
         <v>5000250</v>
@@ -1884,34 +1869,34 @@
         <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D22">
         <v>109.18</v>
       </c>
       <c r="E22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F22">
         <v>109.18</v>
       </c>
       <c r="G22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M22">
         <v>5300</v>
@@ -1920,66 +1905,13 @@
         <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P22" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="Q22">
         <v>1133000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17">
-      <c r="A23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23">
-        <v>110</v>
-      </c>
-      <c r="E23" t="s">
-        <v>68</v>
-      </c>
-      <c r="F23">
-        <v>110</v>
-      </c>
-      <c r="G23" t="s">
-        <v>69</v>
-      </c>
-      <c r="H23" t="s">
-        <v>69</v>
-      </c>
-      <c r="I23" t="s">
-        <v>69</v>
-      </c>
-      <c r="J23" t="s">
-        <v>69</v>
-      </c>
-      <c r="K23" t="s">
-        <v>70</v>
-      </c>
-      <c r="L23" t="s">
-        <v>69</v>
-      </c>
-      <c r="M23">
-        <v>2000</v>
-      </c>
-      <c r="N23">
-        <v>100</v>
-      </c>
-      <c r="O23" t="s">
-        <v>80</v>
-      </c>
-      <c r="P23" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q23">
-        <v>4125000</v>
       </c>
     </row>
   </sheetData>
@@ -1989,7 +1921,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T21"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2000,10 +1932,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -2012,49 +1944,49 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -2065,7 +1997,7 @@
         <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -2080,7 +2012,7 @@
         <v>990000</v>
       </c>
       <c r="H2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I2">
         <v>13000</v>
@@ -2089,45 +2021,45 @@
         <v>15000</v>
       </c>
       <c r="K2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L2">
         <v>20000</v>
       </c>
       <c r="M2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="S2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
@@ -2142,7 +2074,7 @@
         <v>2104000</v>
       </c>
       <c r="H3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I3">
         <v>9000</v>
@@ -2151,34 +2083,34 @@
         <v>11000</v>
       </c>
       <c r="K3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L3">
         <v>13500</v>
       </c>
       <c r="M3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="S3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -2189,7 +2121,7 @@
         <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>
@@ -2204,7 +2136,7 @@
         <v>5000000</v>
       </c>
       <c r="H4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I4">
         <v>2000</v>
@@ -2213,45 +2145,45 @@
         <v>2000</v>
       </c>
       <c r="K4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L4">
         <v>2000</v>
       </c>
       <c r="M4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="S4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
         <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" t="s">
         <v>22</v>
@@ -2266,7 +2198,7 @@
         <v>6500000</v>
       </c>
       <c r="H5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I5">
         <v>2000</v>
@@ -2275,45 +2207,45 @@
         <v>2000</v>
       </c>
       <c r="K5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L5">
         <v>2000</v>
       </c>
       <c r="M5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="S5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
         <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" t="s">
         <v>22</v>
@@ -2328,7 +2260,7 @@
         <v>4000000</v>
       </c>
       <c r="H6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I6">
         <v>2000</v>
@@ -2337,45 +2269,45 @@
         <v>2000</v>
       </c>
       <c r="K6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L6">
         <v>2000</v>
       </c>
       <c r="M6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="S6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
         <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7" t="s">
         <v>24</v>
@@ -2390,7 +2322,7 @@
         <v>4000000</v>
       </c>
       <c r="H7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I7">
         <v>2000</v>
@@ -2399,45 +2331,45 @@
         <v>2000</v>
       </c>
       <c r="K7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L7">
         <v>2000</v>
       </c>
       <c r="M7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="S7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
         <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
         <v>24</v>
@@ -2452,7 +2384,7 @@
         <v>4000000</v>
       </c>
       <c r="H8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I8">
         <v>2000</v>
@@ -2461,48 +2393,48 @@
         <v>2000</v>
       </c>
       <c r="K8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L8">
         <v>2000</v>
       </c>
       <c r="M8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="S8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s">
         <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E9" t="s">
         <v>22</v>
@@ -2514,7 +2446,7 @@
         <v>600000</v>
       </c>
       <c r="H9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I9">
         <v>12000</v>
@@ -2523,48 +2455,48 @@
         <v>14000</v>
       </c>
       <c r="K9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L9">
         <v>16000</v>
       </c>
       <c r="M9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R9" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="S9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s">
         <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E10" t="s">
         <v>23</v>
@@ -2576,7 +2508,7 @@
         <v>379000</v>
       </c>
       <c r="H10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I10">
         <v>147000</v>
@@ -2585,48 +2517,48 @@
         <v>200000</v>
       </c>
       <c r="K10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L10">
         <v>250000</v>
       </c>
       <c r="M10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O10">
         <v>18.46965699208443</v>
       </c>
       <c r="P10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R10" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="S10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
         <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E11" t="s">
         <v>24</v>
@@ -2638,7 +2570,7 @@
         <v>1000000</v>
       </c>
       <c r="H11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I11">
         <v>4800</v>
@@ -2647,48 +2579,48 @@
         <v>5800</v>
       </c>
       <c r="K11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L11">
         <v>7000</v>
       </c>
       <c r="M11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="S11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B12" t="s">
         <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E12" t="s">
         <v>22</v>
@@ -2700,7 +2632,7 @@
         <v>1130000</v>
       </c>
       <c r="H12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I12">
         <v>14500</v>
@@ -2709,34 +2641,34 @@
         <v>18500</v>
       </c>
       <c r="K12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L12">
         <v>20000</v>
       </c>
       <c r="M12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R12" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="S12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -2747,10 +2679,10 @@
         <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E13" t="s">
         <v>25</v>
@@ -2762,7 +2694,7 @@
         <v>4575000</v>
       </c>
       <c r="H13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I13">
         <v>2000</v>
@@ -2771,34 +2703,34 @@
         <v>2000</v>
       </c>
       <c r="K13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L13">
         <v>2000</v>
       </c>
       <c r="M13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R13" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="S13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -2809,10 +2741,10 @@
         <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E14" t="s">
         <v>25</v>
@@ -2824,7 +2756,7 @@
         <v>850000</v>
       </c>
       <c r="H14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I14">
         <v>14500</v>
@@ -2833,45 +2765,45 @@
         <v>16500</v>
       </c>
       <c r="K14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L14">
         <v>18000</v>
       </c>
       <c r="M14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R14" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="S14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
         <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D15" t="s">
         <v>28</v>
@@ -2886,7 +2818,7 @@
         <v>3000000</v>
       </c>
       <c r="H15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I15">
         <v>9200</v>
@@ -2895,45 +2827,45 @@
         <v>11000</v>
       </c>
       <c r="K15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L15">
         <v>14000</v>
       </c>
       <c r="M15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R15" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="S15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B16" t="s">
         <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D16" t="s">
         <v>28</v>
@@ -2948,7 +2880,7 @@
         <v>4000000</v>
       </c>
       <c r="H16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I16">
         <v>2000</v>
@@ -2957,48 +2889,48 @@
         <v>2000</v>
       </c>
       <c r="K16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L16">
         <v>2000</v>
       </c>
       <c r="M16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R16" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="S16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B17" t="s">
         <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E17" t="s">
         <v>27</v>
@@ -3010,7 +2942,7 @@
         <v>1500000</v>
       </c>
       <c r="H17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I17">
         <v>13000</v>
@@ -3019,48 +2951,48 @@
         <v>15000</v>
       </c>
       <c r="K17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L17">
         <v>18000</v>
       </c>
       <c r="M17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O17">
         <v>0</v>
       </c>
       <c r="P17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R17" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="S17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:20">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
         <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D18" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E18" t="s">
         <v>28</v>
@@ -3072,7 +3004,7 @@
         <v>8707000</v>
       </c>
       <c r="H18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I18">
         <v>5000</v>
@@ -3081,48 +3013,48 @@
         <v>6300</v>
       </c>
       <c r="K18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L18">
         <v>7300</v>
       </c>
       <c r="M18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O18">
         <v>40.00229700241185</v>
       </c>
       <c r="P18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R18" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="S18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:20">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
         <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D19" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E19" t="s">
         <v>29</v>
@@ -3134,7 +3066,7 @@
         <v>6667000</v>
       </c>
       <c r="H19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I19">
         <v>2400</v>
@@ -3143,48 +3075,48 @@
         <v>2800</v>
       </c>
       <c r="K19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L19">
         <v>3400</v>
       </c>
       <c r="M19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O19">
         <v>0</v>
       </c>
       <c r="P19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R19" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="S19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B20" t="s">
         <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D20" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E20" t="s">
         <v>30</v>
@@ -3196,7 +3128,7 @@
         <v>2060000</v>
       </c>
       <c r="H20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I20">
         <v>4300</v>
@@ -3205,96 +3137,34 @@
         <v>4900</v>
       </c>
       <c r="K20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L20">
         <v>5300</v>
       </c>
       <c r="M20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O20">
         <v>0</v>
       </c>
       <c r="P20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R20" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="S20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T20" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20">
-      <c r="A21" t="s">
-        <v>80</v>
-      </c>
-      <c r="B21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" t="s">
-        <v>85</v>
-      </c>
-      <c r="E21" t="s">
-        <v>30</v>
-      </c>
-      <c r="F21">
-        <v>11000000</v>
-      </c>
-      <c r="G21">
-        <v>5500000</v>
-      </c>
-      <c r="H21" t="s">
-        <v>69</v>
-      </c>
-      <c r="I21">
-        <v>2000</v>
-      </c>
-      <c r="J21">
-        <v>2000</v>
-      </c>
-      <c r="K21" t="s">
-        <v>69</v>
-      </c>
-      <c r="L21">
-        <v>2000</v>
-      </c>
-      <c r="M21" t="s">
-        <v>69</v>
-      </c>
-      <c r="N21" t="s">
-        <v>69</v>
-      </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>69</v>
-      </c>
-      <c r="R21" t="s">
-        <v>123</v>
-      </c>
-      <c r="S21" t="s">
-        <v>69</v>
-      </c>
-      <c r="T21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -3304,7 +3174,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3312,16 +3182,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -3333,10 +3203,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -3345,24 +3215,24 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
         <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
         <v>24</v>
@@ -3388,19 +3258,19 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
         <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
@@ -3426,7 +3296,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
         <v>29</v>
@@ -3435,13 +3305,13 @@
         <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G4" t="s">
         <v>25</v>
@@ -3464,19 +3334,19 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C5" t="s">
         <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F5" t="s">
         <v>28</v>
@@ -3502,22 +3372,22 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
         <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G6" t="s">
         <v>30</v>
@@ -3540,34 +3410,34 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="G7" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="H7">
-        <v>19800</v>
+        <v>7000</v>
       </c>
       <c r="I7">
-        <v>990000</v>
+        <v>1000000</v>
       </c>
       <c r="J7">
-        <v>20000</v>
+        <v>7000</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -3578,72 +3448,72 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="E8" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>81</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H8">
-        <v>14202</v>
+        <v>22667.8</v>
       </c>
       <c r="I8">
-        <v>2104000</v>
+        <v>6667000</v>
       </c>
       <c r="J8">
-        <v>13500</v>
+        <v>3400</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>79</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F9" t="s">
-        <v>84</v>
+        <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="H9">
-        <v>22667.8</v>
+        <v>19800</v>
       </c>
       <c r="I9">
-        <v>6667000</v>
+        <v>990000</v>
       </c>
       <c r="J9">
-        <v>3400</v>
+        <v>20000</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -3654,57 +3524,57 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
       <c r="F10" t="s">
-        <v>81</v>
+        <v>20</v>
       </c>
       <c r="G10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H10">
-        <v>7000</v>
+        <v>14202</v>
       </c>
       <c r="I10">
-        <v>1000000</v>
+        <v>2104000</v>
       </c>
       <c r="J10">
-        <v>7000</v>
+        <v>13500</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
         <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F11" t="s">
         <v>22</v>
@@ -3730,34 +3600,34 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" t="s">
         <v>80</v>
       </c>
-      <c r="C12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F12" t="s">
-        <v>85</v>
-      </c>
       <c r="G12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H12">
-        <v>11000</v>
+        <v>63561.1</v>
       </c>
       <c r="I12">
-        <v>5500000</v>
+        <v>8707000</v>
       </c>
       <c r="J12">
-        <v>2000</v>
+        <v>7300</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -3768,34 +3638,34 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F13" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="G13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H13">
-        <v>63561.1</v>
+        <v>42000</v>
       </c>
       <c r="I13">
-        <v>8707000</v>
+        <v>3000000</v>
       </c>
       <c r="J13">
-        <v>7300</v>
+        <v>14000</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -3806,34 +3676,34 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F14" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="G14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H14">
-        <v>42000</v>
+        <v>9150</v>
       </c>
       <c r="I14">
-        <v>3000000</v>
+        <v>4575000</v>
       </c>
       <c r="J14">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -3844,107 +3714,107 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E15" t="s">
-        <v>63</v>
+        <v>122</v>
       </c>
       <c r="F15" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="G15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H15">
-        <v>9150</v>
+        <v>75800</v>
       </c>
       <c r="I15">
-        <v>4575000</v>
+        <v>379000</v>
       </c>
       <c r="J15">
-        <v>2000</v>
+        <v>250000</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E16" t="s">
-        <v>127</v>
+        <v>55</v>
       </c>
       <c r="F16" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="G16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H16">
-        <v>75800</v>
+        <v>13000</v>
       </c>
       <c r="I16">
-        <v>379000</v>
+        <v>6500000</v>
       </c>
       <c r="J16">
-        <v>250000</v>
+        <v>2000</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F17" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G17" t="s">
         <v>20</v>
       </c>
       <c r="H17">
-        <v>13000</v>
+        <v>8000</v>
       </c>
       <c r="I17">
-        <v>6500000</v>
+        <v>4000000</v>
       </c>
       <c r="J17">
         <v>2000</v>
@@ -3961,10 +3831,10 @@
         <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
         <v>59</v>
@@ -3973,19 +3843,19 @@
         <v>59</v>
       </c>
       <c r="F18" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="G18" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H18">
-        <v>8000</v>
+        <v>9600</v>
       </c>
       <c r="I18">
-        <v>4000000</v>
+        <v>600000</v>
       </c>
       <c r="J18">
-        <v>2000</v>
+        <v>16000</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -3996,34 +3866,34 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E19" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F19" t="s">
-        <v>81</v>
+        <v>23</v>
       </c>
       <c r="G19" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H19">
-        <v>9600</v>
+        <v>10000</v>
       </c>
       <c r="I19">
-        <v>600000</v>
+        <v>5000000</v>
       </c>
       <c r="J19">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -4034,22 +3904,22 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C20" t="s">
         <v>46</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F20" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G20" t="s">
         <v>27</v>
@@ -4072,115 +3942,77 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E21" t="s">
-        <v>55</v>
+        <v>122</v>
       </c>
       <c r="F21" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" t="s">
         <v>23</v>
       </c>
-      <c r="G21" t="s">
-        <v>19</v>
-      </c>
       <c r="H21">
-        <v>10000</v>
+        <v>18950</v>
       </c>
       <c r="I21">
-        <v>5000000</v>
+        <v>379000</v>
       </c>
       <c r="J21">
-        <v>2000</v>
+        <v>250000</v>
       </c>
       <c r="K21">
         <v>0</v>
       </c>
       <c r="L21">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D22" t="s">
         <v>61</v>
       </c>
       <c r="E22" t="s">
-        <v>127</v>
+        <v>61</v>
       </c>
       <c r="F22" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="G22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H22">
-        <v>18950</v>
+        <v>22600</v>
       </c>
       <c r="I22">
-        <v>379000</v>
+        <v>1130000</v>
       </c>
       <c r="J22">
-        <v>250000</v>
+        <v>20000</v>
       </c>
       <c r="K22">
         <v>0</v>
       </c>
       <c r="L22">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" t="s">
-        <v>75</v>
-      </c>
-      <c r="C23" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" t="s">
-        <v>62</v>
-      </c>
-      <c r="E23" t="s">
-        <v>62</v>
-      </c>
-      <c r="F23" t="s">
-        <v>81</v>
-      </c>
-      <c r="G23" t="s">
-        <v>22</v>
-      </c>
-      <c r="H23">
-        <v>22600</v>
-      </c>
-      <c r="I23">
-        <v>1130000</v>
-      </c>
-      <c r="J23">
-        <v>20000</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2024-03-20
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="115">
   <si>
     <t>상장일</t>
   </si>
@@ -105,153 +105,138 @@
     <t>2024-01-26</t>
   </si>
   <si>
+    <t>오상헬스케어</t>
+  </si>
+  <si>
+    <t>케이엔알시스템</t>
+  </si>
+  <si>
+    <t>하나31호스팩</t>
+  </si>
+  <si>
+    <t>유안타제15호스팩</t>
+  </si>
+  <si>
+    <t>SK증권제11호스팩</t>
+  </si>
+  <si>
+    <t>비엔케이제2호스팩</t>
+  </si>
+  <si>
+    <t>유진스팩10호</t>
+  </si>
+  <si>
+    <t>코셈</t>
+  </si>
+  <si>
+    <t>에이피알</t>
+  </si>
+  <si>
+    <t>케이웨더</t>
+  </si>
+  <si>
+    <t>이에이트</t>
+  </si>
+  <si>
+    <t>신영스팩10호</t>
+  </si>
+  <si>
+    <t>스튜디오삼익</t>
+  </si>
+  <si>
+    <t>이닉스</t>
+  </si>
+  <si>
+    <t>IBKS제24호스팩</t>
+  </si>
+  <si>
+    <t>포스뱅크</t>
+  </si>
+  <si>
+    <t>현대힘스</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>코스피</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>유안타</t>
+  </si>
+  <si>
+    <t>SK</t>
+  </si>
+  <si>
+    <t>BNK</t>
+  </si>
+  <si>
+    <t>유진</t>
+  </si>
+  <si>
+    <t>키움</t>
+  </si>
+  <si>
+    <t>신한</t>
+  </si>
+  <si>
+    <t>한화</t>
+  </si>
+  <si>
+    <t>신영</t>
+  </si>
+  <si>
+    <t>삼성</t>
+  </si>
+  <si>
+    <t>IBK</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>공동</t>
+  </si>
+  <si>
+    <t>2024-02-26</t>
+  </si>
+  <si>
+    <t>2024-02-20</t>
+  </si>
+  <si>
+    <t>2024-02-19</t>
+  </si>
+  <si>
+    <t>2024-02-13</t>
+  </si>
+  <si>
+    <t>2024-02-14</t>
+  </si>
+  <si>
     <t>2024-01-25</t>
   </si>
   <si>
-    <t>2024-01-24</t>
-  </si>
-  <si>
-    <t>오상헬스케어</t>
-  </si>
-  <si>
-    <t>케이엔알시스템</t>
-  </si>
-  <si>
-    <t>하나31호스팩</t>
-  </si>
-  <si>
-    <t>유안타제15호스팩</t>
-  </si>
-  <si>
-    <t>SK증권제11호스팩</t>
-  </si>
-  <si>
-    <t>비엔케이제2호스팩</t>
-  </si>
-  <si>
-    <t>유진스팩10호</t>
-  </si>
-  <si>
-    <t>코셈</t>
-  </si>
-  <si>
-    <t>에이피알</t>
-  </si>
-  <si>
-    <t>케이웨더</t>
-  </si>
-  <si>
-    <t>이에이트</t>
-  </si>
-  <si>
-    <t>신영스팩10호</t>
-  </si>
-  <si>
-    <t>스튜디오삼익</t>
-  </si>
-  <si>
-    <t>이닉스</t>
-  </si>
-  <si>
-    <t>IBKS제24호스팩</t>
-  </si>
-  <si>
-    <t>포스뱅크</t>
-  </si>
-  <si>
-    <t>현대힘스</t>
-  </si>
-  <si>
-    <t>HB인베스트먼트</t>
-  </si>
-  <si>
-    <t>우진엔텍</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>코스피</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>DB</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>유안타</t>
-  </si>
-  <si>
-    <t>SK</t>
-  </si>
-  <si>
-    <t>BNK</t>
-  </si>
-  <si>
-    <t>유진</t>
-  </si>
-  <si>
-    <t>키움</t>
-  </si>
-  <si>
-    <t>신한</t>
-  </si>
-  <si>
-    <t>한화</t>
-  </si>
-  <si>
-    <t>신영</t>
-  </si>
-  <si>
-    <t>삼성</t>
-  </si>
-  <si>
-    <t>IBK</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>KB</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>공동</t>
-  </si>
-  <si>
-    <t>2024-02-26</t>
-  </si>
-  <si>
-    <t>2024-02-20</t>
-  </si>
-  <si>
-    <t>2024-02-19</t>
-  </si>
-  <si>
-    <t>2024-02-13</t>
-  </si>
-  <si>
-    <t>2024-02-14</t>
-  </si>
-  <si>
     <t>2024-01-23</t>
   </si>
   <si>
     <t>2024-01-17</t>
   </si>
   <si>
-    <t>2024-01-16</t>
-  </si>
-  <si>
     <t>2024-02-16</t>
   </si>
   <si>
@@ -261,9 +246,6 @@
     <t>2024-01-22</t>
   </si>
   <si>
-    <t>2024-01-19</t>
-  </si>
-  <si>
     <t>회사명</t>
   </si>
   <si>
@@ -367,12 +349,6 @@
   </si>
   <si>
     <t>1231.2 : 1</t>
-  </si>
-  <si>
-    <t>892.559 : 1</t>
-  </si>
-  <si>
-    <t>2707.18 : 1</t>
   </si>
   <si>
     <t>인수기관</t>
@@ -742,7 +718,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -806,37 +782,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D2">
         <v>198</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F2">
         <v>198</v>
       </c>
       <c r="G2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="L2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="M2">
         <v>20000</v>
@@ -859,37 +835,37 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D3">
         <v>284.04</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F3">
         <v>142.02</v>
       </c>
       <c r="G3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="L3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="M3">
         <v>13500</v>
@@ -898,7 +874,7 @@
         <v>50</v>
       </c>
       <c r="O3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="P3" t="s">
         <v>20</v>
@@ -912,37 +888,37 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D4">
         <v>284.04</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F4">
         <v>142.02</v>
       </c>
       <c r="G4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="L4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="M4">
         <v>13500</v>
@@ -951,7 +927,7 @@
         <v>50</v>
       </c>
       <c r="O4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="P4" t="s">
         <v>20</v>
@@ -965,37 +941,37 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D5">
         <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F5">
         <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="L5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="M5">
         <v>2000</v>
@@ -1018,37 +994,37 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D6">
         <v>130</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F6">
         <v>130</v>
       </c>
       <c r="G6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="L6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="M6">
         <v>2000</v>
@@ -1057,7 +1033,7 @@
         <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="P6" t="s">
         <v>22</v>
@@ -1071,37 +1047,37 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D7">
         <v>80</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F7">
         <v>80</v>
       </c>
       <c r="G7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="L7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="M7">
         <v>2000</v>
@@ -1110,7 +1086,7 @@
         <v>100</v>
       </c>
       <c r="O7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="P7" t="s">
         <v>22</v>
@@ -1124,37 +1100,37 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D8">
         <v>80</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F8">
         <v>80</v>
       </c>
       <c r="G8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="L8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="M8">
         <v>2000</v>
@@ -1163,7 +1139,7 @@
         <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="P8" t="s">
         <v>24</v>
@@ -1177,37 +1153,37 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D9">
         <v>80</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F9">
         <v>80</v>
       </c>
       <c r="G9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K9" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="L9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="M9">
         <v>2000</v>
@@ -1216,7 +1192,7 @@
         <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="P9" t="s">
         <v>24</v>
@@ -1230,37 +1206,37 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D10">
         <v>96</v>
       </c>
       <c r="E10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F10">
         <v>96</v>
       </c>
       <c r="G10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="L10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="M10">
         <v>16000</v>
@@ -1269,10 +1245,10 @@
         <v>100</v>
       </c>
       <c r="O10" t="s">
+        <v>68</v>
+      </c>
+      <c r="P10" t="s">
         <v>73</v>
-      </c>
-      <c r="P10" t="s">
-        <v>78</v>
       </c>
       <c r="Q10">
         <v>420000</v>
@@ -1283,37 +1259,37 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D11">
         <v>947.5</v>
       </c>
       <c r="E11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F11">
         <v>758</v>
       </c>
       <c r="G11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K11" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="L11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="M11">
         <v>250000</v>
@@ -1322,10 +1298,10 @@
         <v>80</v>
       </c>
       <c r="O11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="P11" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="Q11">
         <v>416900</v>
@@ -1336,37 +1312,37 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D12">
         <v>947.5</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F12">
         <v>189.5</v>
       </c>
       <c r="G12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K12" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="L12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="M12">
         <v>250000</v>
@@ -1375,10 +1351,10 @@
         <v>20</v>
       </c>
       <c r="O12" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="P12" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="Q12">
         <v>416900</v>
@@ -1389,37 +1365,37 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D13">
         <v>70</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F13">
         <v>70</v>
       </c>
       <c r="G13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K13" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="L13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="M13">
         <v>7000</v>
@@ -1428,10 +1404,10 @@
         <v>100</v>
       </c>
       <c r="O13" t="s">
+        <v>68</v>
+      </c>
+      <c r="P13" t="s">
         <v>73</v>
-      </c>
-      <c r="P13" t="s">
-        <v>78</v>
       </c>
       <c r="Q13">
         <v>750000</v>
@@ -1442,37 +1418,37 @@
         <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D14">
         <v>226</v>
       </c>
       <c r="E14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F14">
         <v>226</v>
       </c>
       <c r="G14" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H14" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I14" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J14" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K14" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="L14" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="M14">
         <v>20000</v>
@@ -1481,10 +1457,10 @@
         <v>100</v>
       </c>
       <c r="O14" t="s">
+        <v>68</v>
+      </c>
+      <c r="P14" t="s">
         <v>73</v>
-      </c>
-      <c r="P14" t="s">
-        <v>78</v>
       </c>
       <c r="Q14">
         <v>827500</v>
@@ -1495,37 +1471,37 @@
         <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D15">
         <v>91.5</v>
       </c>
       <c r="E15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F15">
         <v>91.5</v>
       </c>
       <c r="G15" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H15" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I15" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J15" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K15" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="L15" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="M15">
         <v>2000</v>
@@ -1534,10 +1510,10 @@
         <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="P15" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="Q15">
         <v>3431250</v>
@@ -1548,37 +1524,37 @@
         <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D16">
         <v>153</v>
       </c>
       <c r="E16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F16">
         <v>153</v>
       </c>
       <c r="G16" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H16" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I16" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J16" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K16" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="L16" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="M16">
         <v>18000</v>
@@ -1587,10 +1563,10 @@
         <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="P16" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="Q16">
         <v>637500</v>
@@ -1601,37 +1577,37 @@
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D17">
         <v>420</v>
       </c>
       <c r="E17" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F17">
         <v>420</v>
       </c>
       <c r="G17" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H17" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I17" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J17" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K17" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="L17" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="M17">
         <v>14000</v>
@@ -1640,7 +1616,7 @@
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="P17" t="s">
         <v>28</v>
@@ -1654,37 +1630,37 @@
         <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D18">
         <v>80</v>
       </c>
       <c r="E18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F18">
         <v>80</v>
       </c>
       <c r="G18" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H18" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I18" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J18" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K18" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="L18" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="M18">
         <v>2000</v>
@@ -1693,7 +1669,7 @@
         <v>100</v>
       </c>
       <c r="O18" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="P18" t="s">
         <v>28</v>
@@ -1707,37 +1683,37 @@
         <v>27</v>
       </c>
       <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" t="s">
         <v>46</v>
-      </c>
-      <c r="C19" t="s">
-        <v>50</v>
       </c>
       <c r="D19">
         <v>270</v>
       </c>
       <c r="E19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F19">
         <v>270</v>
       </c>
       <c r="G19" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H19" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I19" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J19" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K19" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="L19" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="M19">
         <v>18000</v>
@@ -1746,10 +1722,10 @@
         <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="P19" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="Q19">
         <v>1112478</v>
@@ -1760,37 +1736,37 @@
         <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D20">
         <v>635.611</v>
       </c>
       <c r="E20" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F20">
         <v>635.611</v>
       </c>
       <c r="G20" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H20" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I20" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J20" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K20" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="L20" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="M20">
         <v>7300</v>
@@ -1799,119 +1775,13 @@
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="P20" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="Q20">
         <v>5513403</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17">
-      <c r="A21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21">
-        <v>226.678</v>
-      </c>
-      <c r="E21" t="s">
-        <v>52</v>
-      </c>
-      <c r="F21">
-        <v>226.678</v>
-      </c>
-      <c r="G21" t="s">
-        <v>67</v>
-      </c>
-      <c r="H21" t="s">
-        <v>67</v>
-      </c>
-      <c r="I21" t="s">
-        <v>67</v>
-      </c>
-      <c r="J21" t="s">
-        <v>67</v>
-      </c>
-      <c r="K21" t="s">
-        <v>68</v>
-      </c>
-      <c r="L21" t="s">
-        <v>67</v>
-      </c>
-      <c r="M21">
-        <v>3400</v>
-      </c>
-      <c r="N21">
-        <v>100</v>
-      </c>
-      <c r="O21" t="s">
-        <v>77</v>
-      </c>
-      <c r="P21" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q21">
-        <v>5000250</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17">
-      <c r="A22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22">
-        <v>109.18</v>
-      </c>
-      <c r="E22" t="s">
-        <v>66</v>
-      </c>
-      <c r="F22">
-        <v>109.18</v>
-      </c>
-      <c r="G22" t="s">
-        <v>67</v>
-      </c>
-      <c r="H22" t="s">
-        <v>67</v>
-      </c>
-      <c r="I22" t="s">
-        <v>67</v>
-      </c>
-      <c r="J22" t="s">
-        <v>67</v>
-      </c>
-      <c r="K22" t="s">
-        <v>68</v>
-      </c>
-      <c r="L22" t="s">
-        <v>67</v>
-      </c>
-      <c r="M22">
-        <v>5300</v>
-      </c>
-      <c r="N22">
-        <v>100</v>
-      </c>
-      <c r="O22" t="s">
-        <v>77</v>
-      </c>
-      <c r="P22" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q22">
-        <v>1133000</v>
       </c>
     </row>
   </sheetData>
@@ -1921,7 +1791,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1932,10 +1802,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -1944,49 +1814,49 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -1994,10 +1864,10 @@
         <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -2012,7 +1882,7 @@
         <v>990000</v>
       </c>
       <c r="H2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I2">
         <v>13000</v>
@@ -2021,45 +1891,45 @@
         <v>15000</v>
       </c>
       <c r="K2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="L2">
         <v>20000</v>
       </c>
       <c r="M2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="Q2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="R2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="S2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="T2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
@@ -2074,7 +1944,7 @@
         <v>2104000</v>
       </c>
       <c r="H3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I3">
         <v>9000</v>
@@ -2083,34 +1953,34 @@
         <v>11000</v>
       </c>
       <c r="K3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="L3">
         <v>13500</v>
       </c>
       <c r="M3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="Q3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="R3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="S3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="T3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -2118,10 +1988,10 @@
         <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>
@@ -2136,7 +2006,7 @@
         <v>5000000</v>
       </c>
       <c r="H4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I4">
         <v>2000</v>
@@ -2145,45 +2015,45 @@
         <v>2000</v>
       </c>
       <c r="K4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="L4">
         <v>2000</v>
       </c>
       <c r="M4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="Q4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="R4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="S4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="T4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
         <v>22</v>
@@ -2198,7 +2068,7 @@
         <v>6500000</v>
       </c>
       <c r="H5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I5">
         <v>2000</v>
@@ -2207,45 +2077,45 @@
         <v>2000</v>
       </c>
       <c r="K5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="L5">
         <v>2000</v>
       </c>
       <c r="M5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="Q5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="R5" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="S5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="T5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
         <v>22</v>
@@ -2260,7 +2130,7 @@
         <v>4000000</v>
       </c>
       <c r="H6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I6">
         <v>2000</v>
@@ -2269,45 +2139,45 @@
         <v>2000</v>
       </c>
       <c r="K6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="L6">
         <v>2000</v>
       </c>
       <c r="M6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="Q6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="R6" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="S6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="T6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
         <v>24</v>
@@ -2322,7 +2192,7 @@
         <v>4000000</v>
       </c>
       <c r="H7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I7">
         <v>2000</v>
@@ -2331,45 +2201,45 @@
         <v>2000</v>
       </c>
       <c r="K7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="L7">
         <v>2000</v>
       </c>
       <c r="M7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="Q7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="R7" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="S7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="T7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
         <v>24</v>
@@ -2384,7 +2254,7 @@
         <v>4000000</v>
       </c>
       <c r="H8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I8">
         <v>2000</v>
@@ -2393,48 +2263,48 @@
         <v>2000</v>
       </c>
       <c r="K8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="L8">
         <v>2000</v>
       </c>
       <c r="M8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="Q8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="R8" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="S8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="T8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" t="s">
         <v>73</v>
-      </c>
-      <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" t="s">
-        <v>78</v>
       </c>
       <c r="E9" t="s">
         <v>22</v>
@@ -2446,7 +2316,7 @@
         <v>600000</v>
       </c>
       <c r="H9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I9">
         <v>12000</v>
@@ -2455,48 +2325,48 @@
         <v>14000</v>
       </c>
       <c r="K9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="L9">
         <v>16000</v>
       </c>
       <c r="M9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="Q9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="R9" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="S9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="T9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E10" t="s">
         <v>23</v>
@@ -2508,7 +2378,7 @@
         <v>379000</v>
       </c>
       <c r="H10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I10">
         <v>147000</v>
@@ -2517,48 +2387,48 @@
         <v>200000</v>
       </c>
       <c r="K10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="L10">
         <v>250000</v>
       </c>
       <c r="M10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="O10">
         <v>18.46965699208443</v>
       </c>
       <c r="P10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="Q10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="R10" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="S10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="T10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" t="s">
         <v>73</v>
-      </c>
-      <c r="B11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" t="s">
-        <v>78</v>
       </c>
       <c r="E11" t="s">
         <v>24</v>
@@ -2570,7 +2440,7 @@
         <v>1000000</v>
       </c>
       <c r="H11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I11">
         <v>4800</v>
@@ -2579,48 +2449,48 @@
         <v>5800</v>
       </c>
       <c r="K11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="L11">
         <v>7000</v>
       </c>
       <c r="M11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="Q11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="R11" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="S11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="T11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" t="s">
         <v>73</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" t="s">
-        <v>78</v>
       </c>
       <c r="E12" t="s">
         <v>22</v>
@@ -2632,7 +2502,7 @@
         <v>1130000</v>
       </c>
       <c r="H12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I12">
         <v>14500</v>
@@ -2641,48 +2511,48 @@
         <v>18500</v>
       </c>
       <c r="K12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="L12">
         <v>20000</v>
       </c>
       <c r="M12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="Q12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="R12" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="S12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="T12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E13" t="s">
         <v>25</v>
@@ -2694,7 +2564,7 @@
         <v>4575000</v>
       </c>
       <c r="H13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I13">
         <v>2000</v>
@@ -2703,48 +2573,48 @@
         <v>2000</v>
       </c>
       <c r="K13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="L13">
         <v>2000</v>
       </c>
       <c r="M13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="Q13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="R13" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="S13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="T13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E14" t="s">
         <v>25</v>
@@ -2756,7 +2626,7 @@
         <v>850000</v>
       </c>
       <c r="H14" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I14">
         <v>14500</v>
@@ -2765,45 +2635,45 @@
         <v>16500</v>
       </c>
       <c r="K14" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="L14">
         <v>18000</v>
       </c>
       <c r="M14" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N14" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="Q14" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="R14" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="S14" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="T14" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
         <v>28</v>
@@ -2818,7 +2688,7 @@
         <v>3000000</v>
       </c>
       <c r="H15" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I15">
         <v>9200</v>
@@ -2827,45 +2697,45 @@
         <v>11000</v>
       </c>
       <c r="K15" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="L15">
         <v>14000</v>
       </c>
       <c r="M15" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N15" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="Q15" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="R15" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="S15" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="T15" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D16" t="s">
         <v>28</v>
@@ -2880,7 +2750,7 @@
         <v>4000000</v>
       </c>
       <c r="H16" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I16">
         <v>2000</v>
@@ -2889,48 +2759,48 @@
         <v>2000</v>
       </c>
       <c r="K16" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="L16">
         <v>2000</v>
       </c>
       <c r="M16" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N16" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="Q16" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="R16" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="S16" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="T16" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E17" t="s">
         <v>27</v>
@@ -2942,7 +2812,7 @@
         <v>1500000</v>
       </c>
       <c r="H17" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I17">
         <v>13000</v>
@@ -2951,48 +2821,48 @@
         <v>15000</v>
       </c>
       <c r="K17" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="L17">
         <v>18000</v>
       </c>
       <c r="M17" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N17" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="O17">
         <v>0</v>
       </c>
       <c r="P17" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="Q17" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="R17" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="S17" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="T17" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:20">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D18" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E18" t="s">
         <v>28</v>
@@ -3004,7 +2874,7 @@
         <v>8707000</v>
       </c>
       <c r="H18" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I18">
         <v>5000</v>
@@ -3013,158 +2883,34 @@
         <v>6300</v>
       </c>
       <c r="K18" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="L18">
         <v>7300</v>
       </c>
       <c r="M18" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N18" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="O18">
         <v>40.00229700241185</v>
       </c>
       <c r="P18" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="Q18" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="R18" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="S18" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="T18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20">
-      <c r="A19" t="s">
-        <v>77</v>
-      </c>
-      <c r="B19" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" t="s">
-        <v>81</v>
-      </c>
-      <c r="E19" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19">
-        <v>22667800</v>
-      </c>
-      <c r="G19">
-        <v>6667000</v>
-      </c>
-      <c r="H19" t="s">
-        <v>67</v>
-      </c>
-      <c r="I19">
-        <v>2400</v>
-      </c>
-      <c r="J19">
-        <v>2800</v>
-      </c>
-      <c r="K19" t="s">
-        <v>67</v>
-      </c>
-      <c r="L19">
-        <v>3400</v>
-      </c>
-      <c r="M19" t="s">
-        <v>67</v>
-      </c>
-      <c r="N19" t="s">
-        <v>67</v>
-      </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
-      <c r="P19" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>67</v>
-      </c>
-      <c r="R19" t="s">
-        <v>117</v>
-      </c>
-      <c r="S19" t="s">
-        <v>67</v>
-      </c>
-      <c r="T19" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20">
-      <c r="A20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" t="s">
-        <v>81</v>
-      </c>
-      <c r="E20" t="s">
-        <v>30</v>
-      </c>
-      <c r="F20">
-        <v>10918000</v>
-      </c>
-      <c r="G20">
-        <v>2060000</v>
-      </c>
-      <c r="H20" t="s">
-        <v>67</v>
-      </c>
-      <c r="I20">
-        <v>4300</v>
-      </c>
-      <c r="J20">
-        <v>4900</v>
-      </c>
-      <c r="K20" t="s">
-        <v>67</v>
-      </c>
-      <c r="L20">
-        <v>5300</v>
-      </c>
-      <c r="M20" t="s">
-        <v>67</v>
-      </c>
-      <c r="N20" t="s">
-        <v>67</v>
-      </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>67</v>
-      </c>
-      <c r="R20" t="s">
-        <v>118</v>
-      </c>
-      <c r="S20" t="s">
-        <v>67</v>
-      </c>
-      <c r="T20" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -3174,7 +2920,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3182,16 +2928,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -3203,10 +2949,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -3215,24 +2961,24 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
         <v>24</v>
@@ -3258,19 +3004,19 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
@@ -3296,22 +3042,22 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G4" t="s">
         <v>25</v>
@@ -3334,19 +3080,19 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F5" t="s">
         <v>28</v>
@@ -3372,34 +3118,34 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="F6" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="H6">
-        <v>10918</v>
+        <v>19800</v>
       </c>
       <c r="I6">
-        <v>2060000</v>
+        <v>990000</v>
       </c>
       <c r="J6">
-        <v>5300</v>
+        <v>20000</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -3410,72 +3156,72 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>93</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>93</v>
       </c>
       <c r="F7" t="s">
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H7">
-        <v>7000</v>
+        <v>14202</v>
       </c>
       <c r="I7">
-        <v>1000000</v>
+        <v>2104000</v>
       </c>
       <c r="J7">
-        <v>7000</v>
+        <v>13500</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
         <v>48</v>
       </c>
-      <c r="D8" t="s">
-        <v>52</v>
-      </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F8" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H8">
-        <v>22667.8</v>
+        <v>7000</v>
       </c>
       <c r="I8">
-        <v>6667000</v>
+        <v>1000000</v>
       </c>
       <c r="J8">
-        <v>3400</v>
+        <v>7000</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -3489,10 +3235,10 @@
         <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
         <v>52</v>
@@ -3501,19 +3247,19 @@
         <v>52</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H9">
-        <v>19800</v>
+        <v>8000</v>
       </c>
       <c r="I9">
-        <v>990000</v>
+        <v>4000000</v>
       </c>
       <c r="J9">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -3524,72 +3270,72 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="D10" t="s">
-        <v>99</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
-        <v>99</v>
+        <v>61</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="G10" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="H10">
-        <v>14202</v>
+        <v>63561.1</v>
       </c>
       <c r="I10">
-        <v>2104000</v>
+        <v>8707000</v>
       </c>
       <c r="J10">
-        <v>13500</v>
+        <v>7300</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
         <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F11" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G11" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="H11">
-        <v>8000</v>
+        <v>42000</v>
       </c>
       <c r="I11">
-        <v>4000000</v>
+        <v>3000000</v>
       </c>
       <c r="J11">
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -3600,34 +3346,34 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="F12" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H12">
-        <v>63561.1</v>
+        <v>9150</v>
       </c>
       <c r="I12">
-        <v>8707000</v>
+        <v>4575000</v>
       </c>
       <c r="J12">
-        <v>7300</v>
+        <v>2000</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -3638,69 +3384,69 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E13" t="s">
-        <v>63</v>
+        <v>114</v>
       </c>
       <c r="F13" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="G13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H13">
-        <v>42000</v>
+        <v>75800</v>
       </c>
       <c r="I13">
-        <v>3000000</v>
+        <v>379000</v>
       </c>
       <c r="J13">
-        <v>14000</v>
+        <v>250000</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="L13">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E14" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>79</v>
+        <v>22</v>
       </c>
       <c r="G14" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H14">
-        <v>9150</v>
+        <v>13000</v>
       </c>
       <c r="I14">
-        <v>4575000</v>
+        <v>6500000</v>
       </c>
       <c r="J14">
         <v>2000</v>
@@ -3714,40 +3460,40 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E15" t="s">
-        <v>122</v>
+        <v>54</v>
       </c>
       <c r="F15" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="G15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H15">
-        <v>75800</v>
+        <v>8000</v>
       </c>
       <c r="I15">
-        <v>379000</v>
+        <v>4000000</v>
       </c>
       <c r="J15">
-        <v>250000</v>
+        <v>2000</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -3755,10 +3501,10 @@
         <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
         <v>55</v>
@@ -3767,19 +3513,19 @@
         <v>55</v>
       </c>
       <c r="F16" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" t="s">
         <v>22</v>
       </c>
-      <c r="G16" t="s">
-        <v>20</v>
-      </c>
       <c r="H16">
-        <v>13000</v>
+        <v>9600</v>
       </c>
       <c r="I16">
-        <v>6500000</v>
+        <v>600000</v>
       </c>
       <c r="J16">
-        <v>2000</v>
+        <v>16000</v>
       </c>
       <c r="K16">
         <v>0</v>
@@ -3790,34 +3536,34 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
         <v>72</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="F17" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="G17" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H17">
-        <v>8000</v>
+        <v>27000</v>
       </c>
       <c r="I17">
-        <v>4000000</v>
+        <v>1500000</v>
       </c>
       <c r="J17">
-        <v>2000</v>
+        <v>18000</v>
       </c>
       <c r="K17">
         <v>0</v>
@@ -3828,57 +3574,57 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>114</v>
       </c>
       <c r="F18" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="G18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H18">
-        <v>9600</v>
+        <v>18950</v>
       </c>
       <c r="I18">
-        <v>600000</v>
+        <v>379000</v>
       </c>
       <c r="J18">
-        <v>16000</v>
+        <v>250000</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B19" t="s">
         <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F19" t="s">
         <v>23</v>
@@ -3904,115 +3650,39 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D20" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E20" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F20" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G20" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H20">
-        <v>27000</v>
+        <v>22600</v>
       </c>
       <c r="I20">
-        <v>1500000</v>
+        <v>1130000</v>
       </c>
       <c r="J20">
-        <v>18000</v>
+        <v>20000</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
       <c r="L20">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" t="s">
-        <v>74</v>
-      </c>
-      <c r="C21" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" t="s">
-        <v>60</v>
-      </c>
-      <c r="E21" t="s">
-        <v>122</v>
-      </c>
-      <c r="F21" t="s">
-        <v>72</v>
-      </c>
-      <c r="G21" t="s">
-        <v>23</v>
-      </c>
-      <c r="H21">
-        <v>18950</v>
-      </c>
-      <c r="I21">
-        <v>379000</v>
-      </c>
-      <c r="J21">
-        <v>250000</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" t="s">
-        <v>73</v>
-      </c>
-      <c r="C22" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" t="s">
-        <v>61</v>
-      </c>
-      <c r="E22" t="s">
-        <v>61</v>
-      </c>
-      <c r="F22" t="s">
-        <v>78</v>
-      </c>
-      <c r="G22" t="s">
-        <v>22</v>
-      </c>
-      <c r="H22">
-        <v>22600</v>
-      </c>
-      <c r="I22">
-        <v>1130000</v>
-      </c>
-      <c r="J22">
-        <v>20000</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2024-03-23
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="113">
   <si>
     <t>상장일</t>
   </si>
@@ -69,6 +69,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2024-03-21</t>
+  </si>
+  <si>
     <t>2024-03-13</t>
   </si>
   <si>
@@ -99,153 +102,147 @@
     <t>2024-02-01</t>
   </si>
   <si>
-    <t>2024-01-29</t>
+    <t>삼현</t>
+  </si>
+  <si>
+    <t>오상헬스케어</t>
+  </si>
+  <si>
+    <t>케이엔알시스템</t>
+  </si>
+  <si>
+    <t>하나31호스팩</t>
+  </si>
+  <si>
+    <t>유안타제15호스팩</t>
+  </si>
+  <si>
+    <t>SK증권제11호스팩</t>
+  </si>
+  <si>
+    <t>비엔케이제2호스팩</t>
+  </si>
+  <si>
+    <t>유진스팩10호</t>
+  </si>
+  <si>
+    <t>코셈</t>
+  </si>
+  <si>
+    <t>에이피알</t>
+  </si>
+  <si>
+    <t>케이웨더</t>
+  </si>
+  <si>
+    <t>이에이트</t>
+  </si>
+  <si>
+    <t>신영스팩10호</t>
+  </si>
+  <si>
+    <t>스튜디오삼익</t>
+  </si>
+  <si>
+    <t>이닉스</t>
+  </si>
+  <si>
+    <t>IBKS제24호스팩</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>코스피</t>
+  </si>
+  <si>
+    <t>한국</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>유안타</t>
+  </si>
+  <si>
+    <t>SK</t>
+  </si>
+  <si>
+    <t>BNK</t>
+  </si>
+  <si>
+    <t>유진</t>
+  </si>
+  <si>
+    <t>키움</t>
+  </si>
+  <si>
+    <t>신한</t>
+  </si>
+  <si>
+    <t>한화</t>
+  </si>
+  <si>
+    <t>신영</t>
+  </si>
+  <si>
+    <t>삼성</t>
+  </si>
+  <si>
+    <t>IBK</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>공동</t>
+  </si>
+  <si>
+    <t>2024-03-12</t>
+  </si>
+  <si>
+    <t>2024-02-26</t>
+  </si>
+  <si>
+    <t>2024-02-20</t>
+  </si>
+  <si>
+    <t>2024-02-19</t>
+  </si>
+  <si>
+    <t>2024-02-13</t>
+  </si>
+  <si>
+    <t>2024-02-14</t>
+  </si>
+  <si>
+    <t>2024-01-25</t>
+  </si>
+  <si>
+    <t>2024-01-23</t>
+  </si>
+  <si>
+    <t>2024-03-15</t>
+  </si>
+  <si>
+    <t>2024-02-16</t>
+  </si>
+  <si>
+    <t>2024-01-30</t>
   </si>
   <si>
     <t>2024-01-26</t>
   </si>
   <si>
-    <t>오상헬스케어</t>
-  </si>
-  <si>
-    <t>케이엔알시스템</t>
-  </si>
-  <si>
-    <t>하나31호스팩</t>
-  </si>
-  <si>
-    <t>유안타제15호스팩</t>
-  </si>
-  <si>
-    <t>SK증권제11호스팩</t>
-  </si>
-  <si>
-    <t>비엔케이제2호스팩</t>
-  </si>
-  <si>
-    <t>유진스팩10호</t>
-  </si>
-  <si>
-    <t>코셈</t>
-  </si>
-  <si>
-    <t>에이피알</t>
-  </si>
-  <si>
-    <t>케이웨더</t>
-  </si>
-  <si>
-    <t>이에이트</t>
-  </si>
-  <si>
-    <t>신영스팩10호</t>
-  </si>
-  <si>
-    <t>스튜디오삼익</t>
-  </si>
-  <si>
-    <t>이닉스</t>
-  </si>
-  <si>
-    <t>IBKS제24호스팩</t>
-  </si>
-  <si>
-    <t>포스뱅크</t>
-  </si>
-  <si>
-    <t>현대힘스</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>코스피</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>DB</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>유안타</t>
-  </si>
-  <si>
-    <t>SK</t>
-  </si>
-  <si>
-    <t>BNK</t>
-  </si>
-  <si>
-    <t>유진</t>
-  </si>
-  <si>
-    <t>키움</t>
-  </si>
-  <si>
-    <t>신한</t>
-  </si>
-  <si>
-    <t>한화</t>
-  </si>
-  <si>
-    <t>신영</t>
-  </si>
-  <si>
-    <t>삼성</t>
-  </si>
-  <si>
-    <t>IBK</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>공동</t>
-  </si>
-  <si>
-    <t>2024-02-26</t>
-  </si>
-  <si>
-    <t>2024-02-20</t>
-  </si>
-  <si>
-    <t>2024-02-19</t>
-  </si>
-  <si>
-    <t>2024-02-13</t>
-  </si>
-  <si>
-    <t>2024-02-14</t>
-  </si>
-  <si>
-    <t>2024-01-25</t>
-  </si>
-  <si>
-    <t>2024-01-23</t>
-  </si>
-  <si>
-    <t>2024-01-17</t>
-  </si>
-  <si>
-    <t>2024-02-16</t>
-  </si>
-  <si>
-    <t>2024-01-30</t>
-  </si>
-  <si>
-    <t>2024-01-22</t>
-  </si>
-  <si>
     <t>회사명</t>
   </si>
   <si>
@@ -300,6 +297,9 @@
     <t>DB, NH</t>
   </si>
   <si>
+    <t>1645.13 : 1</t>
+  </si>
+  <si>
     <t>2126.13 : 1</t>
   </si>
   <si>
@@ -343,12 +343,6 @@
   </si>
   <si>
     <t>940.84 : 1</t>
-  </si>
-  <si>
-    <t>1397.07 : 1</t>
-  </si>
-  <si>
-    <t>1231.2 : 1</t>
   </si>
   <si>
     <t>인수기관</t>
@@ -718,7 +712,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -782,52 +776,52 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2">
+        <v>600</v>
+      </c>
+      <c r="E2" t="s">
         <v>46</v>
       </c>
-      <c r="D2">
-        <v>198</v>
-      </c>
-      <c r="E2" t="s">
-        <v>48</v>
-      </c>
       <c r="F2">
-        <v>198</v>
+        <v>600</v>
       </c>
       <c r="G2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M2">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="N2">
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="P2" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="Q2">
-        <v>742500</v>
+        <v>1368000</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -835,90 +829,90 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3">
-        <v>284.04</v>
+        <v>198</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F3">
-        <v>142.02</v>
+        <v>198</v>
       </c>
       <c r="G3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M3">
-        <v>13500</v>
+        <v>20000</v>
       </c>
       <c r="N3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="P3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q3">
-        <v>2916000</v>
+        <v>742500</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D4">
         <v>284.04</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F4">
         <v>142.02</v>
       </c>
       <c r="G4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M4">
         <v>13500</v>
@@ -927,10 +921,10 @@
         <v>50</v>
       </c>
       <c r="O4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q4">
         <v>2916000</v>
@@ -941,52 +935,52 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5">
-        <v>100</v>
+        <v>284.04</v>
       </c>
       <c r="E5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5">
+        <v>142.02</v>
+      </c>
+      <c r="G5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L5" t="s">
+        <v>60</v>
+      </c>
+      <c r="M5">
+        <v>13500</v>
+      </c>
+      <c r="N5">
         <v>50</v>
       </c>
-      <c r="F5">
-        <v>100</v>
-      </c>
-      <c r="G5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H5" t="s">
-        <v>62</v>
-      </c>
-      <c r="I5" t="s">
-        <v>62</v>
-      </c>
-      <c r="J5" t="s">
-        <v>62</v>
-      </c>
-      <c r="K5" t="s">
-        <v>63</v>
-      </c>
-      <c r="L5" t="s">
-        <v>62</v>
-      </c>
-      <c r="M5">
-        <v>2000</v>
-      </c>
-      <c r="N5">
-        <v>100</v>
-      </c>
       <c r="O5" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="P5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Q5">
-        <v>3750000</v>
+        <v>2916000</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -994,37 +988,37 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D6">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F6">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="G6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M6">
         <v>2000</v>
@@ -1033,13 +1027,13 @@
         <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="P6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="Q6">
-        <v>4875000</v>
+        <v>3750000</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1047,37 +1041,37 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F7">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="G7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M7">
         <v>2000</v>
@@ -1086,51 +1080,51 @@
         <v>100</v>
       </c>
       <c r="O7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Q7">
-        <v>3000000</v>
+        <v>4875000</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D8">
         <v>80</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F8">
         <v>80</v>
       </c>
       <c r="G8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M8">
         <v>2000</v>
@@ -1139,10 +1133,10 @@
         <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="P8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q8">
         <v>3000000</v>
@@ -1153,37 +1147,37 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D9">
         <v>80</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F9">
         <v>80</v>
       </c>
       <c r="G9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M9">
         <v>2000</v>
@@ -1192,10 +1186,10 @@
         <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q9">
         <v>3000000</v>
@@ -1203,55 +1197,55 @@
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D10">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="E10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F10">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="G10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M10">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="N10">
         <v>100</v>
       </c>
       <c r="O10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="P10" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="Q10">
-        <v>420000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1259,102 +1253,102 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D11">
-        <v>947.5</v>
+        <v>96</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F11">
-        <v>758</v>
+        <v>96</v>
       </c>
       <c r="G11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M11">
-        <v>250000</v>
+        <v>16000</v>
       </c>
       <c r="N11">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P11" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="Q11">
-        <v>416900</v>
+        <v>420000</v>
       </c>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
         <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D12">
         <v>947.5</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="F12">
-        <v>189.5</v>
+        <v>758</v>
       </c>
       <c r="G12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M12">
         <v>250000</v>
       </c>
       <c r="N12">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="O12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q12">
         <v>416900</v>
@@ -1365,211 +1359,211 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13">
-        <v>70</v>
+        <v>947.5</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F13">
-        <v>70</v>
+        <v>189.5</v>
       </c>
       <c r="G13" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" t="s">
+        <v>60</v>
+      </c>
+      <c r="I13" t="s">
+        <v>60</v>
+      </c>
+      <c r="J13" t="s">
+        <v>60</v>
+      </c>
+      <c r="K13" t="s">
         <v>62</v>
       </c>
-      <c r="H13" t="s">
-        <v>62</v>
-      </c>
-      <c r="I13" t="s">
-        <v>62</v>
-      </c>
-      <c r="J13" t="s">
-        <v>62</v>
-      </c>
-      <c r="K13" t="s">
-        <v>63</v>
-      </c>
       <c r="L13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M13">
-        <v>7000</v>
+        <v>250000</v>
       </c>
       <c r="N13">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="O13" t="s">
         <v>68</v>
       </c>
       <c r="P13" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="Q13">
-        <v>750000</v>
+        <v>416900</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D14">
-        <v>226</v>
+        <v>70</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="F14">
-        <v>226</v>
+        <v>70</v>
       </c>
       <c r="G14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M14">
-        <v>20000</v>
+        <v>7000</v>
       </c>
       <c r="N14">
         <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q14">
-        <v>827500</v>
+        <v>750000</v>
       </c>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D15">
-        <v>91.5</v>
+        <v>226</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F15">
-        <v>91.5</v>
+        <v>226</v>
       </c>
       <c r="G15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M15">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="N15">
         <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="P15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Q15">
-        <v>3431250</v>
+        <v>827500</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D16">
-        <v>153</v>
+        <v>91.5</v>
       </c>
       <c r="E16" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="F16">
-        <v>153</v>
+        <v>91.5</v>
       </c>
       <c r="G16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M16">
-        <v>18000</v>
+        <v>2000</v>
       </c>
       <c r="N16">
         <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q16">
-        <v>637500</v>
+        <v>3431250</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1577,105 +1571,105 @@
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D17">
-        <v>420</v>
+        <v>153</v>
       </c>
       <c r="E17" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="F17">
-        <v>420</v>
+        <v>153</v>
       </c>
       <c r="G17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M17">
-        <v>14000</v>
+        <v>18000</v>
       </c>
       <c r="N17">
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P17" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="Q17">
-        <v>2100000</v>
+        <v>637500</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D18">
-        <v>80</v>
+        <v>420</v>
       </c>
       <c r="E18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F18">
-        <v>80</v>
+        <v>420</v>
       </c>
       <c r="G18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M18">
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="N18">
         <v>100</v>
       </c>
       <c r="O18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P18" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="Q18">
-        <v>3000000</v>
+        <v>2100000</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1683,105 +1677,52 @@
         <v>27</v>
       </c>
       <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
         <v>44</v>
       </c>
-      <c r="C19" t="s">
-        <v>46</v>
-      </c>
       <c r="D19">
-        <v>270</v>
+        <v>80</v>
       </c>
       <c r="E19" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="F19">
-        <v>270</v>
+        <v>80</v>
       </c>
       <c r="G19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M19">
-        <v>18000</v>
+        <v>2000</v>
       </c>
       <c r="N19">
         <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q19">
-        <v>1112478</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17">
-      <c r="A20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20">
-        <v>635.611</v>
-      </c>
-      <c r="E20" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20">
-        <v>635.611</v>
-      </c>
-      <c r="G20" t="s">
-        <v>62</v>
-      </c>
-      <c r="H20" t="s">
-        <v>62</v>
-      </c>
-      <c r="I20" t="s">
-        <v>62</v>
-      </c>
-      <c r="J20" t="s">
-        <v>62</v>
-      </c>
-      <c r="K20" t="s">
-        <v>63</v>
-      </c>
-      <c r="L20" t="s">
-        <v>62</v>
-      </c>
-      <c r="M20">
-        <v>7300</v>
-      </c>
-      <c r="N20">
-        <v>100</v>
-      </c>
-      <c r="O20" t="s">
-        <v>72</v>
-      </c>
-      <c r="P20" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q20">
-        <v>5513403</v>
+        <v>3000000</v>
       </c>
     </row>
   </sheetData>
@@ -1791,7 +1732,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T18"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1802,10 +1743,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -1814,261 +1755,261 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
       </c>
       <c r="F2">
-        <v>19800000</v>
+        <v>60000000</v>
       </c>
       <c r="G2">
-        <v>990000</v>
+        <v>2000000</v>
       </c>
       <c r="H2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I2">
-        <v>13000</v>
+        <v>20000</v>
       </c>
       <c r="J2">
-        <v>15000</v>
+        <v>25000</v>
       </c>
       <c r="K2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L2">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="M2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="N2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Q2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="S2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="T2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
       </c>
       <c r="F3">
-        <v>28404000</v>
+        <v>19800000</v>
       </c>
       <c r="G3">
-        <v>2104000</v>
+        <v>990000</v>
       </c>
       <c r="H3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I3">
-        <v>9000</v>
+        <v>13000</v>
       </c>
       <c r="J3">
-        <v>11000</v>
+        <v>15000</v>
       </c>
       <c r="K3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L3">
-        <v>13500</v>
+        <v>20000</v>
       </c>
       <c r="M3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="N3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Q3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="T3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
       </c>
       <c r="F4">
-        <v>10000000</v>
+        <v>28404000</v>
       </c>
       <c r="G4">
-        <v>5000000</v>
+        <v>2104000</v>
       </c>
       <c r="H4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I4">
-        <v>2000</v>
+        <v>9000</v>
       </c>
       <c r="J4">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="K4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L4">
-        <v>2000</v>
+        <v>13500</v>
       </c>
       <c r="M4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="N4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Q4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="T4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
       </c>
       <c r="F5">
-        <v>13000000</v>
+        <v>10000000</v>
       </c>
       <c r="G5">
-        <v>6500000</v>
+        <v>5000000</v>
       </c>
       <c r="H5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I5">
         <v>2000</v>
@@ -2077,60 +2018,60 @@
         <v>2000</v>
       </c>
       <c r="K5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L5">
         <v>2000</v>
       </c>
       <c r="M5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="N5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Q5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="T5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
       </c>
       <c r="F6">
-        <v>8000000</v>
+        <v>13000000</v>
       </c>
       <c r="G6">
-        <v>4000000</v>
+        <v>6500000</v>
       </c>
       <c r="H6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I6">
         <v>2000</v>
@@ -2139,51 +2080,51 @@
         <v>2000</v>
       </c>
       <c r="K6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L6">
         <v>2000</v>
       </c>
       <c r="M6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="N6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Q6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="S6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="T6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F7">
         <v>8000000</v>
@@ -2192,7 +2133,7 @@
         <v>4000000</v>
       </c>
       <c r="H7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I7">
         <v>2000</v>
@@ -2201,48 +2142,48 @@
         <v>2000</v>
       </c>
       <c r="K7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L7">
         <v>2000</v>
       </c>
       <c r="M7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="N7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Q7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="T7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
         <v>20</v>
@@ -2254,7 +2195,7 @@
         <v>4000000</v>
       </c>
       <c r="H8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I8">
         <v>2000</v>
@@ -2263,158 +2204,158 @@
         <v>2000</v>
       </c>
       <c r="K8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L8">
         <v>2000</v>
       </c>
       <c r="M8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="N8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Q8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="T8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F9">
-        <v>9600000</v>
+        <v>8000000</v>
       </c>
       <c r="G9">
-        <v>600000</v>
+        <v>4000000</v>
       </c>
       <c r="H9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I9">
-        <v>12000</v>
+        <v>2000</v>
       </c>
       <c r="J9">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="K9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L9">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="M9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="N9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Q9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="T9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E10" t="s">
         <v>23</v>
       </c>
       <c r="F10">
-        <v>94750000</v>
+        <v>9600000</v>
       </c>
       <c r="G10">
-        <v>379000</v>
+        <v>600000</v>
       </c>
       <c r="H10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I10">
-        <v>147000</v>
+        <v>12000</v>
       </c>
       <c r="J10">
-        <v>200000</v>
+        <v>14000</v>
       </c>
       <c r="K10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L10">
-        <v>250000</v>
+        <v>16000</v>
       </c>
       <c r="M10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="N10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O10">
-        <v>18.46965699208443</v>
+        <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Q10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="S10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="T10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -2422,495 +2363,433 @@
         <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E11" t="s">
         <v>24</v>
       </c>
       <c r="F11">
-        <v>7000000</v>
+        <v>94750000</v>
       </c>
       <c r="G11">
-        <v>1000000</v>
+        <v>379000</v>
       </c>
       <c r="H11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I11">
-        <v>4800</v>
+        <v>147000</v>
       </c>
       <c r="J11">
-        <v>5800</v>
+        <v>200000</v>
       </c>
       <c r="K11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L11">
-        <v>7000</v>
+        <v>250000</v>
       </c>
       <c r="M11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="N11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>18.46965699208443</v>
       </c>
       <c r="P11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Q11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="S11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="T11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E12" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F12">
-        <v>22600000</v>
+        <v>7000000</v>
       </c>
       <c r="G12">
-        <v>1130000</v>
+        <v>1000000</v>
       </c>
       <c r="H12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I12">
-        <v>14500</v>
+        <v>4800</v>
       </c>
       <c r="J12">
-        <v>18500</v>
+        <v>5800</v>
       </c>
       <c r="K12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L12">
-        <v>20000</v>
+        <v>7000</v>
       </c>
       <c r="M12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="N12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Q12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="S12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="T12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F13">
-        <v>9150000</v>
+        <v>22600000</v>
       </c>
       <c r="G13">
-        <v>4575000</v>
+        <v>1130000</v>
       </c>
       <c r="H13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I13">
-        <v>2000</v>
+        <v>14500</v>
       </c>
       <c r="J13">
-        <v>2000</v>
+        <v>18500</v>
       </c>
       <c r="K13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L13">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="M13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="N13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Q13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="S13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="T13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F14">
-        <v>15300000</v>
+        <v>9150000</v>
       </c>
       <c r="G14">
-        <v>850000</v>
+        <v>4575000</v>
       </c>
       <c r="H14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I14">
-        <v>14500</v>
+        <v>2000</v>
       </c>
       <c r="J14">
-        <v>16500</v>
+        <v>2000</v>
       </c>
       <c r="K14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L14">
-        <v>18000</v>
+        <v>2000</v>
       </c>
       <c r="M14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="N14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Q14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="S14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="T14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="E15" t="s">
         <v>26</v>
       </c>
       <c r="F15">
-        <v>42000000</v>
+        <v>15300000</v>
       </c>
       <c r="G15">
-        <v>3000000</v>
+        <v>850000</v>
       </c>
       <c r="H15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I15">
-        <v>9200</v>
+        <v>14500</v>
       </c>
       <c r="J15">
-        <v>11000</v>
+        <v>16500</v>
       </c>
       <c r="K15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L15">
-        <v>14000</v>
+        <v>18000</v>
       </c>
       <c r="M15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="N15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Q15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="T15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F16">
-        <v>8000000</v>
+        <v>42000000</v>
       </c>
       <c r="G16">
-        <v>4000000</v>
+        <v>3000000</v>
       </c>
       <c r="H16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I16">
-        <v>2000</v>
+        <v>9200</v>
       </c>
       <c r="J16">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="K16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L16">
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="M16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="N16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Q16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="T16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E17" t="s">
         <v>27</v>
       </c>
       <c r="F17">
-        <v>27000000</v>
+        <v>8000000</v>
       </c>
       <c r="G17">
-        <v>1500000</v>
+        <v>4000000</v>
       </c>
       <c r="H17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I17">
-        <v>13000</v>
+        <v>2000</v>
       </c>
       <c r="J17">
-        <v>15000</v>
+        <v>2000</v>
       </c>
       <c r="K17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L17">
-        <v>18000</v>
+        <v>2000</v>
       </c>
       <c r="M17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="N17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O17">
         <v>0</v>
       </c>
       <c r="P17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Q17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="T17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20">
-      <c r="A18" t="s">
-        <v>72</v>
-      </c>
-      <c r="B18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" t="s">
-        <v>75</v>
-      </c>
-      <c r="E18" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18">
-        <v>63561100</v>
-      </c>
-      <c r="G18">
-        <v>8707000</v>
-      </c>
-      <c r="H18" t="s">
-        <v>62</v>
-      </c>
-      <c r="I18">
-        <v>5000</v>
-      </c>
-      <c r="J18">
-        <v>6300</v>
-      </c>
-      <c r="K18" t="s">
-        <v>62</v>
-      </c>
-      <c r="L18">
-        <v>7300</v>
-      </c>
-      <c r="M18" t="s">
-        <v>62</v>
-      </c>
-      <c r="N18" t="s">
-        <v>62</v>
-      </c>
-      <c r="O18">
-        <v>40.00229700241185</v>
-      </c>
-      <c r="P18" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>62</v>
-      </c>
-      <c r="R18" t="s">
-        <v>110</v>
-      </c>
-      <c r="S18" t="s">
-        <v>62</v>
-      </c>
-      <c r="T18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2920,7 +2799,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2928,16 +2807,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -2949,10 +2828,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -2961,30 +2840,30 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
         <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H2">
         <v>8000</v>
@@ -3004,25 +2883,25 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
         <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H3">
         <v>14202</v>
@@ -3042,25 +2921,25 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
         <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H4">
         <v>15300</v>
@@ -3080,25 +2959,25 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
         <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H5">
         <v>8000</v>
@@ -3118,25 +2997,25 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
         <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
         <v>18</v>
-      </c>
-      <c r="G6" t="s">
-        <v>17</v>
       </c>
       <c r="H6">
         <v>19800</v>
@@ -3156,25 +3035,25 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H7">
         <v>14202</v>
@@ -3194,25 +3073,25 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
         <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H8">
         <v>7000</v>
@@ -3232,25 +3111,25 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" t="s">
         <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" t="s">
         <v>22</v>
-      </c>
-      <c r="G9" t="s">
-        <v>21</v>
       </c>
       <c r="H9">
         <v>8000</v>
@@ -3270,34 +3149,34 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H10">
-        <v>63561.1</v>
+        <v>42000</v>
       </c>
       <c r="I10">
-        <v>8707000</v>
+        <v>3000000</v>
       </c>
       <c r="J10">
-        <v>7300</v>
+        <v>14000</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -3308,34 +3187,34 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F11" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="G11" t="s">
         <v>26</v>
       </c>
       <c r="H11">
-        <v>42000</v>
+        <v>9150</v>
       </c>
       <c r="I11">
-        <v>3000000</v>
+        <v>4575000</v>
       </c>
       <c r="J11">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -3346,107 +3225,107 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="F12" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="G12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H12">
-        <v>9150</v>
+        <v>75800</v>
       </c>
       <c r="I12">
-        <v>4575000</v>
+        <v>379000</v>
       </c>
       <c r="J12">
-        <v>2000</v>
+        <v>250000</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>114</v>
+        <v>50</v>
       </c>
       <c r="F13" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="G13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H13">
-        <v>75800</v>
+        <v>13000</v>
       </c>
       <c r="I13">
-        <v>379000</v>
+        <v>6500000</v>
       </c>
       <c r="J13">
-        <v>250000</v>
+        <v>2000</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="L13">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
         <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F14" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H14">
-        <v>13000</v>
+        <v>8000</v>
       </c>
       <c r="I14">
-        <v>6500000</v>
+        <v>4000000</v>
       </c>
       <c r="J14">
         <v>2000</v>
@@ -3466,7 +3345,7 @@
         <v>67</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
         <v>54</v>
@@ -3475,19 +3354,19 @@
         <v>54</v>
       </c>
       <c r="F15" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="G15" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H15">
-        <v>8000</v>
+        <v>9600</v>
       </c>
       <c r="I15">
-        <v>4000000</v>
+        <v>600000</v>
       </c>
       <c r="J15">
-        <v>2000</v>
+        <v>16000</v>
       </c>
       <c r="K15">
         <v>0</v>
@@ -3498,34 +3377,34 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E16" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F16" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="G16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H16">
-        <v>9600</v>
+        <v>10000</v>
       </c>
       <c r="I16">
-        <v>600000</v>
+        <v>5000000</v>
       </c>
       <c r="J16">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="K16">
         <v>0</v>
@@ -3536,153 +3415,115 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E17" t="s">
-        <v>50</v>
+        <v>112</v>
       </c>
       <c r="F17" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="G17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H17">
-        <v>27000</v>
+        <v>18950</v>
       </c>
       <c r="I17">
-        <v>1500000</v>
+        <v>379000</v>
       </c>
       <c r="J17">
-        <v>18000</v>
+        <v>250000</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E18" t="s">
-        <v>114</v>
+        <v>46</v>
       </c>
       <c r="F18" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="G18" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H18">
-        <v>18950</v>
+        <v>60000</v>
       </c>
       <c r="I18">
-        <v>379000</v>
+        <v>2000000</v>
       </c>
       <c r="J18">
-        <v>250000</v>
+        <v>30000</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D19" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E19" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="F19" t="s">
+        <v>72</v>
+      </c>
+      <c r="G19" t="s">
         <v>23</v>
       </c>
-      <c r="G19" t="s">
-        <v>19</v>
-      </c>
       <c r="H19">
-        <v>10000</v>
+        <v>22600</v>
       </c>
       <c r="I19">
-        <v>5000000</v>
+        <v>1130000</v>
       </c>
       <c r="J19">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="K19">
         <v>0</v>
       </c>
       <c r="L19">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" t="s">
-        <v>57</v>
-      </c>
-      <c r="F20" t="s">
-        <v>73</v>
-      </c>
-      <c r="G20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H20">
-        <v>22600</v>
-      </c>
-      <c r="I20">
-        <v>1130000</v>
-      </c>
-      <c r="J20">
-        <v>20000</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2024-03-27
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="109">
   <si>
     <t>상장일</t>
   </si>
@@ -69,6 +69,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2024-03-26</t>
+  </si>
+  <si>
     <t>2024-03-21</t>
   </si>
   <si>
@@ -99,7 +102,7 @@
     <t>2024-02-06</t>
   </si>
   <si>
-    <t>2024-02-01</t>
+    <t>엔젤로보틱스</t>
   </si>
   <si>
     <t>삼현</t>
@@ -144,24 +147,18 @@
     <t>스튜디오삼익</t>
   </si>
   <si>
-    <t>이닉스</t>
-  </si>
-  <si>
-    <t>IBKS제24호스팩</t>
-  </si>
-  <si>
     <t>코스닥</t>
   </si>
   <si>
     <t>코스피</t>
   </si>
   <si>
+    <t>NH</t>
+  </si>
+  <si>
     <t>한국</t>
   </si>
   <si>
-    <t>NH</t>
-  </si>
-  <si>
     <t>DB</t>
   </si>
   <si>
@@ -192,12 +189,6 @@
     <t>신영</t>
   </si>
   <si>
-    <t>삼성</t>
-  </si>
-  <si>
-    <t>IBK</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -207,6 +198,9 @@
     <t>공동</t>
   </si>
   <si>
+    <t>2024-03-14</t>
+  </si>
+  <si>
     <t>2024-03-12</t>
   </si>
   <si>
@@ -228,7 +222,7 @@
     <t>2024-01-25</t>
   </si>
   <si>
-    <t>2024-01-23</t>
+    <t>2024-03-19</t>
   </si>
   <si>
     <t>2024-03-15</t>
@@ -240,9 +234,6 @@
     <t>2024-01-30</t>
   </si>
   <si>
-    <t>2024-01-26</t>
-  </si>
-  <si>
     <t>회사명</t>
   </si>
   <si>
@@ -297,6 +288,9 @@
     <t>DB, NH</t>
   </si>
   <si>
+    <t>2242.016 : 1</t>
+  </si>
+  <si>
     <t>1645.13 : 1</t>
   </si>
   <si>
@@ -337,12 +331,6 @@
   </si>
   <si>
     <t>2650.33 : 1</t>
-  </si>
-  <si>
-    <t>1997.39 : 1</t>
-  </si>
-  <si>
-    <t>940.84 : 1</t>
   </si>
   <si>
     <t>인수기관</t>
@@ -712,7 +700,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -779,49 +767,49 @@
         <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2">
-        <v>600</v>
+        <v>320</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F2">
-        <v>600</v>
+        <v>320</v>
       </c>
       <c r="G2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M2">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="N2">
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="P2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="Q2">
-        <v>1368000</v>
+        <v>880000</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -832,49 +820,49 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3">
-        <v>198</v>
+        <v>600</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F3">
-        <v>198</v>
+        <v>600</v>
       </c>
       <c r="G3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M3">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="N3">
         <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="P3" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="Q3">
-        <v>742500</v>
+        <v>1368000</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -885,87 +873,87 @@
         <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4">
-        <v>284.04</v>
+        <v>198</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F4">
-        <v>142.02</v>
+        <v>198</v>
       </c>
       <c r="G4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M4">
-        <v>13500</v>
+        <v>20000</v>
       </c>
       <c r="N4">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="P4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q4">
-        <v>2916000</v>
+        <v>742500</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5">
         <v>284.04</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F5">
         <v>142.02</v>
       </c>
       <c r="G5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M5">
         <v>13500</v>
@@ -974,10 +962,10 @@
         <v>50</v>
       </c>
       <c r="O5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="P5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q5">
         <v>2916000</v>
@@ -991,49 +979,49 @@
         <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6">
-        <v>100</v>
+        <v>284.04</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F6">
-        <v>100</v>
+        <v>142.02</v>
       </c>
       <c r="G6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="L6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M6">
-        <v>2000</v>
+        <v>13500</v>
       </c>
       <c r="N6">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O6" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="P6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="Q6">
-        <v>3750000</v>
+        <v>2916000</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1044,34 +1032,34 @@
         <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F7">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="G7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M7">
         <v>2000</v>
@@ -1080,13 +1068,13 @@
         <v>100</v>
       </c>
       <c r="O7" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="P7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="Q7">
-        <v>4875000</v>
+        <v>3750000</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1097,34 +1085,34 @@
         <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="E8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F8">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="G8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M8">
         <v>2000</v>
@@ -1133,51 +1121,51 @@
         <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="P8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q8">
-        <v>3000000</v>
+        <v>4875000</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
         <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9">
         <v>80</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F9">
         <v>80</v>
       </c>
       <c r="G9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M9">
         <v>2000</v>
@@ -1186,10 +1174,10 @@
         <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="P9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q9">
         <v>3000000</v>
@@ -1203,34 +1191,34 @@
         <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10">
         <v>80</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F10">
         <v>80</v>
       </c>
       <c r="G10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M10">
         <v>2000</v>
@@ -1239,10 +1227,10 @@
         <v>100</v>
       </c>
       <c r="O10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="P10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="Q10">
         <v>3000000</v>
@@ -1250,55 +1238,55 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
         <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F11">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="G11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M11">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="N11">
         <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="P11" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="Q11">
-        <v>420000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1309,99 +1297,99 @@
         <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D12">
-        <v>947.5</v>
+        <v>96</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F12">
-        <v>758</v>
+        <v>96</v>
       </c>
       <c r="G12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M12">
-        <v>250000</v>
+        <v>16000</v>
       </c>
       <c r="N12">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="O12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="P12" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="Q12">
-        <v>416900</v>
+        <v>420000</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D13">
         <v>947.5</v>
       </c>
       <c r="E13" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="F13">
-        <v>189.5</v>
+        <v>758</v>
       </c>
       <c r="G13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M13">
         <v>250000</v>
       </c>
       <c r="N13">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="O13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="P13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q13">
         <v>416900</v>
@@ -1418,205 +1406,205 @@
         <v>44</v>
       </c>
       <c r="D14">
-        <v>70</v>
+        <v>947.5</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F14">
-        <v>70</v>
+        <v>189.5</v>
       </c>
       <c r="G14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M14">
-        <v>7000</v>
+        <v>250000</v>
       </c>
       <c r="N14">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="O14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P14" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="Q14">
-        <v>750000</v>
+        <v>416900</v>
       </c>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
         <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15">
-        <v>226</v>
+        <v>70</v>
       </c>
       <c r="E15" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F15">
-        <v>226</v>
+        <v>70</v>
       </c>
       <c r="G15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M15">
-        <v>20000</v>
+        <v>7000</v>
       </c>
       <c r="N15">
         <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="P15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Q15">
-        <v>827500</v>
+        <v>750000</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
         <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16">
-        <v>91.5</v>
+        <v>226</v>
       </c>
       <c r="E16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F16">
-        <v>91.5</v>
+        <v>226</v>
       </c>
       <c r="G16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K16" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M16">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="N16">
         <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="P16" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="Q16">
-        <v>3431250</v>
+        <v>827500</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
         <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D17">
-        <v>153</v>
+        <v>91.5</v>
       </c>
       <c r="E17" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="F17">
-        <v>153</v>
+        <v>91.5</v>
       </c>
       <c r="G17" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H17" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I17" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J17" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L17" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M17">
-        <v>18000</v>
+        <v>2000</v>
       </c>
       <c r="N17">
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="Q17">
-        <v>637500</v>
+        <v>3431250</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -1627,102 +1615,49 @@
         <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D18">
-        <v>420</v>
+        <v>153</v>
       </c>
       <c r="E18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18">
+        <v>153</v>
+      </c>
+      <c r="G18" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18" t="s">
+        <v>57</v>
+      </c>
+      <c r="I18" t="s">
+        <v>57</v>
+      </c>
+      <c r="J18" t="s">
+        <v>57</v>
+      </c>
+      <c r="K18" t="s">
         <v>58</v>
       </c>
-      <c r="F18">
-        <v>420</v>
-      </c>
-      <c r="G18" t="s">
-        <v>60</v>
-      </c>
-      <c r="H18" t="s">
-        <v>60</v>
-      </c>
-      <c r="I18" t="s">
-        <v>60</v>
-      </c>
-      <c r="J18" t="s">
-        <v>60</v>
-      </c>
-      <c r="K18" t="s">
-        <v>61</v>
-      </c>
       <c r="L18" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M18">
-        <v>14000</v>
+        <v>18000</v>
       </c>
       <c r="N18">
         <v>100</v>
       </c>
       <c r="O18" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="P18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="Q18">
-        <v>2100000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
-      <c r="A19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19">
-        <v>80</v>
-      </c>
-      <c r="E19" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19">
-        <v>80</v>
-      </c>
-      <c r="G19" t="s">
-        <v>60</v>
-      </c>
-      <c r="H19" t="s">
-        <v>60</v>
-      </c>
-      <c r="I19" t="s">
-        <v>60</v>
-      </c>
-      <c r="J19" t="s">
-        <v>60</v>
-      </c>
-      <c r="K19" t="s">
-        <v>61</v>
-      </c>
-      <c r="L19" t="s">
-        <v>60</v>
-      </c>
-      <c r="M19">
-        <v>2000</v>
-      </c>
-      <c r="N19">
-        <v>100</v>
-      </c>
-      <c r="O19" t="s">
-        <v>70</v>
-      </c>
-      <c r="P19" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q19">
-        <v>3000000</v>
+        <v>637500</v>
       </c>
     </row>
   </sheetData>
@@ -1732,7 +1667,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1743,10 +1678,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -1755,323 +1690,323 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
         <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
       </c>
       <c r="F2">
-        <v>60000000</v>
+        <v>32000000</v>
       </c>
       <c r="G2">
-        <v>2000000</v>
+        <v>1600000</v>
       </c>
       <c r="H2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I2">
+        <v>11000</v>
+      </c>
+      <c r="J2">
+        <v>15000</v>
+      </c>
+      <c r="K2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L2">
         <v>20000</v>
       </c>
-      <c r="J2">
-        <v>25000</v>
-      </c>
-      <c r="K2" t="s">
-        <v>60</v>
-      </c>
-      <c r="L2">
-        <v>30000</v>
-      </c>
       <c r="M2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Q2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="R2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="S2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="T2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
       </c>
       <c r="F3">
-        <v>19800000</v>
+        <v>60000000</v>
       </c>
       <c r="G3">
-        <v>990000</v>
+        <v>2000000</v>
       </c>
       <c r="H3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I3">
-        <v>13000</v>
+        <v>20000</v>
       </c>
       <c r="J3">
-        <v>15000</v>
+        <v>25000</v>
       </c>
       <c r="K3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L3">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="M3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Q3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="R3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="S3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="T3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
       </c>
       <c r="F4">
-        <v>28404000</v>
+        <v>19800000</v>
       </c>
       <c r="G4">
-        <v>2104000</v>
+        <v>990000</v>
       </c>
       <c r="H4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I4">
-        <v>9000</v>
+        <v>13000</v>
       </c>
       <c r="J4">
-        <v>11000</v>
+        <v>15000</v>
       </c>
       <c r="K4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L4">
-        <v>13500</v>
+        <v>20000</v>
       </c>
       <c r="M4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Q4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="R4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="S4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="T4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
         <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
       </c>
       <c r="F5">
-        <v>10000000</v>
+        <v>28404000</v>
       </c>
       <c r="G5">
-        <v>5000000</v>
+        <v>2104000</v>
       </c>
       <c r="H5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I5">
-        <v>2000</v>
+        <v>9000</v>
       </c>
       <c r="J5">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="K5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L5">
-        <v>2000</v>
+        <v>13500</v>
       </c>
       <c r="M5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Q5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="R5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="S5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="T5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
         <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
       </c>
       <c r="F6">
-        <v>13000000</v>
+        <v>10000000</v>
       </c>
       <c r="G6">
-        <v>6500000</v>
+        <v>5000000</v>
       </c>
       <c r="H6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I6">
         <v>2000</v>
@@ -2080,60 +2015,60 @@
         <v>2000</v>
       </c>
       <c r="K6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L6">
         <v>2000</v>
       </c>
       <c r="M6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Q6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="R6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="S6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="T6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
         <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
         <v>22</v>
       </c>
       <c r="F7">
-        <v>8000000</v>
+        <v>13000000</v>
       </c>
       <c r="G7">
-        <v>4000000</v>
+        <v>6500000</v>
       </c>
       <c r="H7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I7">
         <v>2000</v>
@@ -2142,51 +2077,51 @@
         <v>2000</v>
       </c>
       <c r="K7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L7">
         <v>2000</v>
       </c>
       <c r="M7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Q7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="R7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="S7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="T7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
         <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F8">
         <v>8000000</v>
@@ -2195,7 +2130,7 @@
         <v>4000000</v>
       </c>
       <c r="H8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I8">
         <v>2000</v>
@@ -2204,48 +2139,48 @@
         <v>2000</v>
       </c>
       <c r="K8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L8">
         <v>2000</v>
       </c>
       <c r="M8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Q8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="R8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="S8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="T8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
         <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
         <v>21</v>
@@ -2257,7 +2192,7 @@
         <v>4000000</v>
       </c>
       <c r="H9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I9">
         <v>2000</v>
@@ -2266,530 +2201,468 @@
         <v>2000</v>
       </c>
       <c r="K9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L9">
         <v>2000</v>
       </c>
       <c r="M9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Q9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="R9" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="S9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="T9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
         <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10">
-        <v>9600000</v>
+        <v>8000000</v>
       </c>
       <c r="G10">
-        <v>600000</v>
+        <v>4000000</v>
       </c>
       <c r="H10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I10">
-        <v>12000</v>
+        <v>2000</v>
       </c>
       <c r="J10">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="K10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L10">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="M10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Q10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="R10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="S10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="T10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
         <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E11" t="s">
         <v>24</v>
       </c>
       <c r="F11">
-        <v>94750000</v>
+        <v>9600000</v>
       </c>
       <c r="G11">
-        <v>379000</v>
+        <v>600000</v>
       </c>
       <c r="H11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I11">
-        <v>147000</v>
+        <v>12000</v>
       </c>
       <c r="J11">
-        <v>200000</v>
+        <v>14000</v>
       </c>
       <c r="K11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L11">
-        <v>250000</v>
+        <v>16000</v>
       </c>
       <c r="M11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="O11">
-        <v>18.46965699208443</v>
+        <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Q11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="R11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="S11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="T11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" t="s">
         <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E12" t="s">
         <v>25</v>
       </c>
       <c r="F12">
-        <v>7000000</v>
+        <v>94750000</v>
       </c>
       <c r="G12">
-        <v>1000000</v>
+        <v>379000</v>
       </c>
       <c r="H12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I12">
-        <v>4800</v>
+        <v>147000</v>
       </c>
       <c r="J12">
-        <v>5800</v>
+        <v>200000</v>
       </c>
       <c r="K12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L12">
-        <v>7000</v>
+        <v>250000</v>
       </c>
       <c r="M12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="O12">
-        <v>0</v>
+        <v>18.46965699208443</v>
       </c>
       <c r="P12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Q12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="R12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="S12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="T12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
         <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F13">
-        <v>22600000</v>
+        <v>7000000</v>
       </c>
       <c r="G13">
-        <v>1130000</v>
+        <v>1000000</v>
       </c>
       <c r="H13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I13">
-        <v>14500</v>
+        <v>4800</v>
       </c>
       <c r="J13">
-        <v>18500</v>
+        <v>5800</v>
       </c>
       <c r="K13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L13">
-        <v>20000</v>
+        <v>7000</v>
       </c>
       <c r="M13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Q13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="R13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="S13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="T13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B14" t="s">
         <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F14">
-        <v>9150000</v>
+        <v>22600000</v>
       </c>
       <c r="G14">
-        <v>4575000</v>
+        <v>1130000</v>
       </c>
       <c r="H14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I14">
-        <v>2000</v>
+        <v>14500</v>
       </c>
       <c r="J14">
-        <v>2000</v>
+        <v>18500</v>
       </c>
       <c r="K14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L14">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="M14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Q14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="R14" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="S14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="T14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B15" t="s">
         <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F15">
-        <v>15300000</v>
+        <v>9150000</v>
       </c>
       <c r="G15">
-        <v>850000</v>
+        <v>4575000</v>
       </c>
       <c r="H15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I15">
-        <v>14500</v>
+        <v>2000</v>
       </c>
       <c r="J15">
-        <v>16500</v>
+        <v>2000</v>
       </c>
       <c r="K15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L15">
-        <v>18000</v>
+        <v>2000</v>
       </c>
       <c r="M15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Q15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="R15" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="S15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="T15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
         <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E16" t="s">
         <v>27</v>
       </c>
       <c r="F16">
-        <v>42000000</v>
+        <v>15300000</v>
       </c>
       <c r="G16">
-        <v>3000000</v>
+        <v>850000</v>
       </c>
       <c r="H16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I16">
-        <v>9200</v>
+        <v>14500</v>
       </c>
       <c r="J16">
-        <v>11000</v>
+        <v>16500</v>
       </c>
       <c r="K16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="L16">
-        <v>14000</v>
+        <v>18000</v>
       </c>
       <c r="M16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Q16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="R16" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="S16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="T16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20">
-      <c r="A17" t="s">
-        <v>70</v>
-      </c>
-      <c r="B17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17">
-        <v>8000000</v>
-      </c>
-      <c r="G17">
-        <v>4000000</v>
-      </c>
-      <c r="H17" t="s">
-        <v>60</v>
-      </c>
-      <c r="I17">
-        <v>2000</v>
-      </c>
-      <c r="J17">
-        <v>2000</v>
-      </c>
-      <c r="K17" t="s">
-        <v>60</v>
-      </c>
-      <c r="L17">
-        <v>2000</v>
-      </c>
-      <c r="M17" t="s">
-        <v>60</v>
-      </c>
-      <c r="N17" t="s">
-        <v>60</v>
-      </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>60</v>
-      </c>
-      <c r="R17" t="s">
-        <v>108</v>
-      </c>
-      <c r="S17" t="s">
-        <v>60</v>
-      </c>
-      <c r="T17" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2799,7 +2672,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2807,16 +2680,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -2828,10 +2701,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -2840,30 +2713,30 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2">
         <v>8000</v>
@@ -2883,25 +2756,25 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H3">
         <v>14202</v>
@@ -2921,25 +2794,25 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H4">
         <v>15300</v>
@@ -2959,72 +2832,72 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="F5" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="H5">
-        <v>8000</v>
+        <v>14202</v>
       </c>
       <c r="I5">
-        <v>4000000</v>
+        <v>2104000</v>
       </c>
       <c r="J5">
-        <v>2000</v>
+        <v>13500</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="H6">
-        <v>19800</v>
+        <v>7000</v>
       </c>
       <c r="I6">
-        <v>990000</v>
+        <v>1000000</v>
       </c>
       <c r="J6">
-        <v>20000</v>
+        <v>7000</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -3035,72 +2908,72 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="E7" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G7" t="s">
         <v>19</v>
       </c>
       <c r="H7">
-        <v>14202</v>
+        <v>19800</v>
       </c>
       <c r="I7">
-        <v>2104000</v>
+        <v>990000</v>
       </c>
       <c r="J7">
-        <v>13500</v>
+        <v>20000</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="H8">
-        <v>7000</v>
+        <v>32000</v>
       </c>
       <c r="I8">
-        <v>1000000</v>
+        <v>1600000</v>
       </c>
       <c r="J8">
-        <v>7000</v>
+        <v>20000</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -3111,25 +2984,25 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" t="s">
         <v>23</v>
-      </c>
-      <c r="G9" t="s">
-        <v>22</v>
       </c>
       <c r="H9">
         <v>8000</v>
@@ -3149,34 +3022,34 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G10" t="s">
         <v>27</v>
       </c>
       <c r="H10">
-        <v>42000</v>
+        <v>9150</v>
       </c>
       <c r="I10">
-        <v>3000000</v>
+        <v>4575000</v>
       </c>
       <c r="J10">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -3187,107 +3060,107 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E11" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="F11" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H11">
-        <v>9150</v>
+        <v>75800</v>
       </c>
       <c r="I11">
-        <v>4575000</v>
+        <v>379000</v>
       </c>
       <c r="J11">
-        <v>2000</v>
+        <v>250000</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>112</v>
+        <v>49</v>
       </c>
       <c r="F12" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="G12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H12">
-        <v>75800</v>
+        <v>13000</v>
       </c>
       <c r="I12">
-        <v>379000</v>
+        <v>6500000</v>
       </c>
       <c r="J12">
-        <v>250000</v>
+        <v>2000</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F13" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H13">
-        <v>13000</v>
+        <v>8000</v>
       </c>
       <c r="I13">
-        <v>6500000</v>
+        <v>4000000</v>
       </c>
       <c r="J13">
         <v>2000</v>
@@ -3304,10 +3177,10 @@
         <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
         <v>53</v>
@@ -3316,19 +3189,19 @@
         <v>53</v>
       </c>
       <c r="F14" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="G14" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H14">
-        <v>8000</v>
+        <v>9600</v>
       </c>
       <c r="I14">
-        <v>4000000</v>
+        <v>600000</v>
       </c>
       <c r="J14">
-        <v>2000</v>
+        <v>16000</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -3339,34 +3212,34 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F15" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="G15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H15">
-        <v>9600</v>
+        <v>10000</v>
       </c>
       <c r="I15">
-        <v>600000</v>
+        <v>5000000</v>
       </c>
       <c r="J15">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="K15">
         <v>0</v>
@@ -3377,153 +3250,115 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" t="s">
+        <v>108</v>
+      </c>
+      <c r="F16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" t="s">
         <v>25</v>
       </c>
-      <c r="C16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" t="s">
-        <v>20</v>
-      </c>
       <c r="H16">
-        <v>10000</v>
+        <v>18950</v>
       </c>
       <c r="I16">
-        <v>5000000</v>
+        <v>379000</v>
       </c>
       <c r="J16">
-        <v>2000</v>
+        <v>250000</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E17" t="s">
-        <v>112</v>
+        <v>46</v>
       </c>
       <c r="F17" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G17" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H17">
-        <v>18950</v>
+        <v>60000</v>
       </c>
       <c r="I17">
-        <v>379000</v>
+        <v>2000000</v>
       </c>
       <c r="J17">
-        <v>250000</v>
+        <v>30000</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E18" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="F18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G18" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="H18">
-        <v>60000</v>
+        <v>22600</v>
       </c>
       <c r="I18">
-        <v>2000000</v>
+        <v>1130000</v>
       </c>
       <c r="J18">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" t="s">
-        <v>67</v>
-      </c>
-      <c r="C19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" t="s">
-        <v>72</v>
-      </c>
-      <c r="G19" t="s">
-        <v>23</v>
-      </c>
-      <c r="H19">
-        <v>22600</v>
-      </c>
-      <c r="I19">
-        <v>1130000</v>
-      </c>
-      <c r="J19">
-        <v>20000</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2024-03-28
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="113">
   <si>
     <t>상장일</t>
   </si>
@@ -69,6 +69,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2024-03-27</t>
+  </si>
+  <si>
     <t>2024-03-26</t>
   </si>
   <si>
@@ -102,6 +105,9 @@
     <t>2024-02-06</t>
   </si>
   <si>
+    <t>하나32호스팩</t>
+  </si>
+  <si>
     <t>엔젤로보틱스</t>
   </si>
   <si>
@@ -153,6 +159,9 @@
     <t>코스피</t>
   </si>
   <si>
+    <t>하나</t>
+  </si>
+  <si>
     <t>NH</t>
   </si>
   <si>
@@ -162,9 +171,6 @@
     <t>DB</t>
   </si>
   <si>
-    <t>하나</t>
-  </si>
-  <si>
     <t>유안타</t>
   </si>
   <si>
@@ -198,6 +204,9 @@
     <t>공동</t>
   </si>
   <si>
+    <t>2024-03-18</t>
+  </si>
+  <si>
     <t>2024-03-14</t>
   </si>
   <si>
@@ -286,6 +295,9 @@
   </si>
   <si>
     <t>DB, NH</t>
+  </si>
+  <si>
+    <t>2389.8 : 1</t>
   </si>
   <si>
     <t>2242.016 : 1</t>
@@ -700,7 +712,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q18"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -764,52 +776,52 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D2">
-        <v>320</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F2">
-        <v>320</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M2">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="N2">
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="P2" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="Q2">
-        <v>880000</v>
+        <v>2250000</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -817,52 +829,52 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D3">
-        <v>600</v>
+        <v>320</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F3">
-        <v>600</v>
+        <v>320</v>
       </c>
       <c r="G3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M3">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="N3">
         <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="P3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="Q3">
-        <v>1368000</v>
+        <v>880000</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -870,52 +882,52 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D4">
-        <v>198</v>
+        <v>600</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F4">
-        <v>198</v>
+        <v>600</v>
       </c>
       <c r="G4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M4">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="N4">
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="P4" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="Q4">
-        <v>742500</v>
+        <v>1368000</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -923,90 +935,90 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D5">
-        <v>284.04</v>
+        <v>198</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F5">
-        <v>142.02</v>
+        <v>198</v>
       </c>
       <c r="G5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="L5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M5">
-        <v>13500</v>
+        <v>20000</v>
       </c>
       <c r="N5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="P5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q5">
-        <v>2916000</v>
+        <v>742500</v>
       </c>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D6">
         <v>284.04</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F6">
         <v>142.02</v>
       </c>
       <c r="G6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M6">
         <v>13500</v>
@@ -1015,10 +1027,10 @@
         <v>50</v>
       </c>
       <c r="O6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="P6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Q6">
         <v>2916000</v>
@@ -1029,52 +1041,52 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D7">
-        <v>100</v>
+        <v>284.04</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F7">
-        <v>100</v>
+        <v>142.02</v>
       </c>
       <c r="G7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M7">
-        <v>2000</v>
+        <v>13500</v>
       </c>
       <c r="N7">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O7" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="P7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="Q7">
-        <v>3750000</v>
+        <v>2916000</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1082,37 +1094,37 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D8">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F8">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="G8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M8">
         <v>2000</v>
@@ -1121,13 +1133,13 @@
         <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="P8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="Q8">
-        <v>4875000</v>
+        <v>3750000</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1135,37 +1147,37 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D9">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="E9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F9">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="G9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M9">
         <v>2000</v>
@@ -1174,51 +1186,51 @@
         <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="P9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q9">
-        <v>3000000</v>
+        <v>4875000</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D10">
         <v>80</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F10">
         <v>80</v>
       </c>
       <c r="G10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M10">
         <v>2000</v>
@@ -1227,10 +1239,10 @@
         <v>100</v>
       </c>
       <c r="O10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="P10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q10">
         <v>3000000</v>
@@ -1241,37 +1253,37 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D11">
         <v>80</v>
       </c>
       <c r="E11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F11">
         <v>80</v>
       </c>
       <c r="G11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M11">
         <v>2000</v>
@@ -1280,10 +1292,10 @@
         <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="P11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q11">
         <v>3000000</v>
@@ -1291,55 +1303,55 @@
     </row>
     <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D12">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F12">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="G12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M12">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="N12">
         <v>100</v>
       </c>
       <c r="O12" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="P12" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="Q12">
-        <v>420000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1347,102 +1359,102 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D13">
-        <v>947.5</v>
+        <v>96</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F13">
-        <v>758</v>
+        <v>96</v>
       </c>
       <c r="G13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M13">
-        <v>250000</v>
+        <v>16000</v>
       </c>
       <c r="N13">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="P13" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="Q13">
-        <v>416900</v>
+        <v>420000</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D14">
         <v>947.5</v>
       </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="F14">
-        <v>189.5</v>
+        <v>758</v>
       </c>
       <c r="G14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M14">
         <v>250000</v>
       </c>
       <c r="N14">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="O14" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="P14" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="Q14">
         <v>416900</v>
@@ -1453,210 +1465,263 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D15">
-        <v>70</v>
+        <v>947.5</v>
       </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F15">
-        <v>70</v>
+        <v>189.5</v>
       </c>
       <c r="G15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K15" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="L15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M15">
-        <v>7000</v>
+        <v>250000</v>
       </c>
       <c r="N15">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="O15" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="P15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="Q15">
-        <v>750000</v>
+        <v>416900</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D16">
-        <v>226</v>
+        <v>70</v>
       </c>
       <c r="E16" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F16">
-        <v>226</v>
+        <v>70</v>
       </c>
       <c r="G16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M16">
-        <v>20000</v>
+        <v>7000</v>
       </c>
       <c r="N16">
         <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="P16" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="Q16">
-        <v>827500</v>
+        <v>750000</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D17">
-        <v>91.5</v>
+        <v>226</v>
       </c>
       <c r="E17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F17">
-        <v>91.5</v>
+        <v>226</v>
       </c>
       <c r="G17" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H17" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I17" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J17" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L17" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M17">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="N17">
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="P17" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="Q17">
-        <v>3431250</v>
+        <v>827500</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D18">
-        <v>153</v>
+        <v>91.5</v>
       </c>
       <c r="E18" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="F18">
-        <v>153</v>
+        <v>91.5</v>
       </c>
       <c r="G18" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H18" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I18" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J18" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L18" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M18">
-        <v>18000</v>
+        <v>2000</v>
       </c>
       <c r="N18">
         <v>100</v>
       </c>
       <c r="O18" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="P18" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="Q18">
+        <v>3431250</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19">
+        <v>153</v>
+      </c>
+      <c r="E19" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19">
+        <v>153</v>
+      </c>
+      <c r="G19" t="s">
+        <v>59</v>
+      </c>
+      <c r="H19" t="s">
+        <v>59</v>
+      </c>
+      <c r="I19" t="s">
+        <v>59</v>
+      </c>
+      <c r="J19" t="s">
+        <v>59</v>
+      </c>
+      <c r="K19" t="s">
+        <v>60</v>
+      </c>
+      <c r="L19" t="s">
+        <v>59</v>
+      </c>
+      <c r="M19">
+        <v>18000</v>
+      </c>
+      <c r="N19">
+        <v>100</v>
+      </c>
+      <c r="O19" t="s">
+        <v>70</v>
+      </c>
+      <c r="P19" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q19">
         <v>637500</v>
       </c>
     </row>
@@ -1667,7 +1732,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1678,10 +1743,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -1690,385 +1755,385 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
       </c>
       <c r="F2">
-        <v>32000000</v>
+        <v>6000000</v>
       </c>
       <c r="G2">
-        <v>1600000</v>
+        <v>3000000</v>
       </c>
       <c r="H2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I2">
-        <v>11000</v>
+        <v>2000</v>
       </c>
       <c r="J2">
-        <v>15000</v>
+        <v>2000</v>
       </c>
       <c r="K2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L2">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="M2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="Q2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="S2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="T2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
       </c>
       <c r="F3">
-        <v>60000000</v>
+        <v>32000000</v>
       </c>
       <c r="G3">
-        <v>2000000</v>
+        <v>1600000</v>
       </c>
       <c r="H3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I3">
+        <v>11000</v>
+      </c>
+      <c r="J3">
+        <v>15000</v>
+      </c>
+      <c r="K3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3">
         <v>20000</v>
       </c>
-      <c r="J3">
-        <v>25000</v>
-      </c>
-      <c r="K3" t="s">
-        <v>57</v>
-      </c>
-      <c r="L3">
-        <v>30000</v>
-      </c>
       <c r="M3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="Q3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="S3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="T3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
       </c>
       <c r="F4">
-        <v>19800000</v>
+        <v>60000000</v>
       </c>
       <c r="G4">
-        <v>990000</v>
+        <v>2000000</v>
       </c>
       <c r="H4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I4">
-        <v>13000</v>
+        <v>20000</v>
       </c>
       <c r="J4">
-        <v>15000</v>
+        <v>25000</v>
       </c>
       <c r="K4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L4">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="M4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="Q4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R4" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="S4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="T4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
       </c>
       <c r="F5">
-        <v>28404000</v>
+        <v>19800000</v>
       </c>
       <c r="G5">
-        <v>2104000</v>
+        <v>990000</v>
       </c>
       <c r="H5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I5">
-        <v>9000</v>
+        <v>13000</v>
       </c>
       <c r="J5">
-        <v>11000</v>
+        <v>15000</v>
       </c>
       <c r="K5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L5">
-        <v>13500</v>
+        <v>20000</v>
       </c>
       <c r="M5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="Q5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="S5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="T5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
       </c>
       <c r="F6">
-        <v>10000000</v>
+        <v>28404000</v>
       </c>
       <c r="G6">
-        <v>5000000</v>
+        <v>2104000</v>
       </c>
       <c r="H6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I6">
-        <v>2000</v>
+        <v>9000</v>
       </c>
       <c r="J6">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="K6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L6">
-        <v>2000</v>
+        <v>13500</v>
       </c>
       <c r="M6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="Q6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R6" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="S6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="T6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
         <v>22</v>
       </c>
       <c r="F7">
-        <v>13000000</v>
+        <v>10000000</v>
       </c>
       <c r="G7">
-        <v>6500000</v>
+        <v>5000000</v>
       </c>
       <c r="H7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I7">
         <v>2000</v>
@@ -2077,60 +2142,60 @@
         <v>2000</v>
       </c>
       <c r="K7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L7">
         <v>2000</v>
       </c>
       <c r="M7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="Q7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R7" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="S7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="T7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
         <v>23</v>
       </c>
       <c r="F8">
-        <v>8000000</v>
+        <v>13000000</v>
       </c>
       <c r="G8">
-        <v>4000000</v>
+        <v>6500000</v>
       </c>
       <c r="H8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I8">
         <v>2000</v>
@@ -2139,51 +2204,51 @@
         <v>2000</v>
       </c>
       <c r="K8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L8">
         <v>2000</v>
       </c>
       <c r="M8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="Q8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R8" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="S8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="T8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F9">
         <v>8000000</v>
@@ -2192,7 +2257,7 @@
         <v>4000000</v>
       </c>
       <c r="H9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I9">
         <v>2000</v>
@@ -2201,48 +2266,48 @@
         <v>2000</v>
       </c>
       <c r="K9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L9">
         <v>2000</v>
       </c>
       <c r="M9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="Q9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R9" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="S9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="T9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
         <v>22</v>
@@ -2254,7 +2319,7 @@
         <v>4000000</v>
       </c>
       <c r="H10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I10">
         <v>2000</v>
@@ -2263,406 +2328,468 @@
         <v>2000</v>
       </c>
       <c r="K10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L10">
         <v>2000</v>
       </c>
       <c r="M10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="Q10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R10" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="S10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="T10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F11">
-        <v>9600000</v>
+        <v>8000000</v>
       </c>
       <c r="G11">
-        <v>600000</v>
+        <v>4000000</v>
       </c>
       <c r="H11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I11">
-        <v>12000</v>
+        <v>2000</v>
       </c>
       <c r="J11">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="K11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L11">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="M11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="Q11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R11" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="S11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="T11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="E12" t="s">
         <v>25</v>
       </c>
       <c r="F12">
-        <v>94750000</v>
+        <v>9600000</v>
       </c>
       <c r="G12">
-        <v>379000</v>
+        <v>600000</v>
       </c>
       <c r="H12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I12">
-        <v>147000</v>
+        <v>12000</v>
       </c>
       <c r="J12">
-        <v>200000</v>
+        <v>14000</v>
       </c>
       <c r="K12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L12">
-        <v>250000</v>
+        <v>16000</v>
       </c>
       <c r="M12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="O12">
-        <v>18.46965699208443</v>
+        <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="Q12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R12" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="S12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="T12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E13" t="s">
         <v>26</v>
       </c>
       <c r="F13">
-        <v>7000000</v>
+        <v>94750000</v>
       </c>
       <c r="G13">
-        <v>1000000</v>
+        <v>379000</v>
       </c>
       <c r="H13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I13">
-        <v>4800</v>
+        <v>147000</v>
       </c>
       <c r="J13">
-        <v>5800</v>
+        <v>200000</v>
       </c>
       <c r="K13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L13">
-        <v>7000</v>
+        <v>250000</v>
       </c>
       <c r="M13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="O13">
-        <v>0</v>
+        <v>18.46965699208443</v>
       </c>
       <c r="P13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="Q13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R13" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="S13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="T13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E14" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F14">
-        <v>22600000</v>
+        <v>7000000</v>
       </c>
       <c r="G14">
-        <v>1130000</v>
+        <v>1000000</v>
       </c>
       <c r="H14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I14">
-        <v>14500</v>
+        <v>4800</v>
       </c>
       <c r="J14">
-        <v>18500</v>
+        <v>5800</v>
       </c>
       <c r="K14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L14">
-        <v>20000</v>
+        <v>7000</v>
       </c>
       <c r="M14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="Q14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R14" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="S14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="T14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F15">
-        <v>9150000</v>
+        <v>22600000</v>
       </c>
       <c r="G15">
-        <v>4575000</v>
+        <v>1130000</v>
       </c>
       <c r="H15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I15">
-        <v>2000</v>
+        <v>14500</v>
       </c>
       <c r="J15">
-        <v>2000</v>
+        <v>18500</v>
       </c>
       <c r="K15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L15">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="M15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="Q15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R15" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="S15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="T15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F16">
-        <v>15300000</v>
+        <v>9150000</v>
       </c>
       <c r="G16">
-        <v>850000</v>
+        <v>4575000</v>
       </c>
       <c r="H16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I16">
-        <v>14500</v>
+        <v>2000</v>
       </c>
       <c r="J16">
-        <v>16500</v>
+        <v>2000</v>
       </c>
       <c r="K16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L16">
-        <v>18000</v>
+        <v>2000</v>
       </c>
       <c r="M16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="Q16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R16" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="S16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="T16" t="s">
-        <v>57</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17">
+        <v>15300000</v>
+      </c>
+      <c r="G17">
+        <v>850000</v>
+      </c>
+      <c r="H17" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17">
+        <v>14500</v>
+      </c>
+      <c r="J17">
+        <v>16500</v>
+      </c>
+      <c r="K17" t="s">
+        <v>59</v>
+      </c>
+      <c r="L17">
+        <v>18000</v>
+      </c>
+      <c r="M17" t="s">
+        <v>59</v>
+      </c>
+      <c r="N17" t="s">
+        <v>59</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>59</v>
+      </c>
+      <c r="R17" t="s">
+        <v>108</v>
+      </c>
+      <c r="S17" t="s">
+        <v>59</v>
+      </c>
+      <c r="T17" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2672,7 +2799,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2680,16 +2807,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -2701,10 +2828,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -2713,30 +2840,30 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H2">
         <v>8000</v>
@@ -2756,139 +2883,139 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="H3">
-        <v>14202</v>
+        <v>15300</v>
       </c>
       <c r="I3">
-        <v>2104000</v>
+        <v>850000</v>
       </c>
       <c r="J3">
-        <v>13500</v>
+        <v>18000</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="F4" t="s">
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H4">
-        <v>15300</v>
+        <v>14202</v>
       </c>
       <c r="I4">
-        <v>850000</v>
+        <v>2104000</v>
       </c>
       <c r="J4">
-        <v>18000</v>
+        <v>13500</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H5">
-        <v>14202</v>
+        <v>32000</v>
       </c>
       <c r="I5">
-        <v>2104000</v>
+        <v>1600000</v>
       </c>
       <c r="J5">
-        <v>13500</v>
+        <v>20000</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F6" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H6">
         <v>7000</v>
@@ -2908,25 +3035,25 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
         <v>20</v>
-      </c>
-      <c r="G7" t="s">
-        <v>19</v>
       </c>
       <c r="H7">
         <v>19800</v>
@@ -2946,63 +3073,63 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="F8" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="G8" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H8">
-        <v>32000</v>
+        <v>14202</v>
       </c>
       <c r="I8">
-        <v>1600000</v>
+        <v>2104000</v>
       </c>
       <c r="J8">
-        <v>20000</v>
+        <v>13500</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" t="s">
         <v>24</v>
-      </c>
-      <c r="G9" t="s">
-        <v>23</v>
       </c>
       <c r="H9">
         <v>8000</v>
@@ -3022,25 +3149,25 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F10" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H10">
         <v>9150</v>
@@ -3060,25 +3187,25 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E11" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="F11" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H11">
         <v>75800</v>
@@ -3098,25 +3225,25 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H12">
         <v>13000</v>
@@ -3136,25 +3263,25 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H13">
         <v>8000</v>
@@ -3174,25 +3301,25 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E14" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F14" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H14">
         <v>9600</v>
@@ -3212,25 +3339,25 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" t="s">
         <v>26</v>
       </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" t="s">
-        <v>25</v>
-      </c>
       <c r="G15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H15">
         <v>10000</v>
@@ -3250,25 +3377,25 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E16" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="F16" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H16">
         <v>18950</v>
@@ -3288,34 +3415,34 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C17" t="s">
         <v>29</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F17" t="s">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="G17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H17">
-        <v>60000</v>
+        <v>6000</v>
       </c>
       <c r="I17">
-        <v>2000000</v>
+        <v>3000000</v>
       </c>
       <c r="J17">
-        <v>30000</v>
+        <v>2000</v>
       </c>
       <c r="K17">
         <v>0</v>
@@ -3326,39 +3453,77 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E18" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F18" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G18" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H18">
-        <v>22600</v>
+        <v>60000</v>
       </c>
       <c r="I18">
-        <v>1130000</v>
+        <v>2000000</v>
       </c>
       <c r="J18">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" t="s">
+        <v>73</v>
+      </c>
+      <c r="G19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19">
+        <v>22600</v>
+      </c>
+      <c r="I19">
+        <v>1130000</v>
+      </c>
+      <c r="J19">
+        <v>20000</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2024-03-31
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="105">
   <si>
     <t>상장일</t>
   </si>
@@ -102,9 +102,6 @@
     <t>2024-02-22</t>
   </si>
   <si>
-    <t>2024-02-06</t>
-  </si>
-  <si>
     <t>하나32호스팩</t>
   </si>
   <si>
@@ -147,12 +144,6 @@
     <t>이에이트</t>
   </si>
   <si>
-    <t>신영스팩10호</t>
-  </si>
-  <si>
-    <t>스튜디오삼익</t>
-  </si>
-  <si>
     <t>코스닥</t>
   </si>
   <si>
@@ -192,9 +183,6 @@
     <t>한화</t>
   </si>
   <si>
-    <t>신영</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -228,9 +216,6 @@
     <t>2024-02-14</t>
   </si>
   <si>
-    <t>2024-01-25</t>
-  </si>
-  <si>
     <t>2024-03-19</t>
   </si>
   <si>
@@ -240,9 +225,6 @@
     <t>2024-02-16</t>
   </si>
   <si>
-    <t>2024-01-30</t>
-  </si>
-  <si>
     <t>회사명</t>
   </si>
   <si>
@@ -337,12 +319,6 @@
   </si>
   <si>
     <t>381.16 : 1</t>
-  </si>
-  <si>
-    <t>817.09 : 1</t>
-  </si>
-  <si>
-    <t>2650.33 : 1</t>
   </si>
   <si>
     <t>인수기관</t>
@@ -712,7 +688,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -776,37 +752,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D2">
         <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F2">
         <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="L2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="M2">
         <v>2000</v>
@@ -815,7 +791,7 @@
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="P2" t="s">
         <v>19</v>
@@ -829,37 +805,37 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D3">
         <v>320</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F3">
         <v>320</v>
       </c>
       <c r="G3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="L3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="M3">
         <v>20000</v>
@@ -868,10 +844,10 @@
         <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="P3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="Q3">
         <v>880000</v>
@@ -882,37 +858,37 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D4">
         <v>600</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F4">
         <v>600</v>
       </c>
       <c r="G4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="L4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="M4">
         <v>30000</v>
@@ -921,10 +897,10 @@
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="P4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="Q4">
         <v>1368000</v>
@@ -935,37 +911,37 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D5">
         <v>198</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F5">
         <v>198</v>
       </c>
       <c r="G5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="L5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="M5">
         <v>20000</v>
@@ -988,37 +964,37 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D6">
         <v>284.04</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F6">
         <v>142.02</v>
       </c>
       <c r="G6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="M6">
         <v>13500</v>
@@ -1027,7 +1003,7 @@
         <v>50</v>
       </c>
       <c r="O6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="P6" t="s">
         <v>23</v>
@@ -1041,37 +1017,37 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D7">
         <v>284.04</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F7">
         <v>142.02</v>
       </c>
       <c r="G7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="M7">
         <v>13500</v>
@@ -1080,7 +1056,7 @@
         <v>50</v>
       </c>
       <c r="O7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="P7" t="s">
         <v>23</v>
@@ -1094,37 +1070,37 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D8">
         <v>100</v>
       </c>
       <c r="E8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F8">
         <v>100</v>
       </c>
       <c r="G8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="L8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="M8">
         <v>2000</v>
@@ -1147,37 +1123,37 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D9">
         <v>130</v>
       </c>
       <c r="E9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F9">
         <v>130</v>
       </c>
       <c r="G9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K9" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="L9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="M9">
         <v>2000</v>
@@ -1186,7 +1162,7 @@
         <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="P9" t="s">
         <v>25</v>
@@ -1200,37 +1176,37 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D10">
         <v>80</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F10">
         <v>80</v>
       </c>
       <c r="G10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K10" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="L10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="M10">
         <v>2000</v>
@@ -1239,7 +1215,7 @@
         <v>100</v>
       </c>
       <c r="O10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="P10" t="s">
         <v>25</v>
@@ -1253,37 +1229,37 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D11">
         <v>80</v>
       </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F11">
         <v>80</v>
       </c>
       <c r="G11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="L11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="M11">
         <v>2000</v>
@@ -1292,7 +1268,7 @@
         <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="P11" t="s">
         <v>27</v>
@@ -1306,37 +1282,37 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D12">
         <v>80</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F12">
         <v>80</v>
       </c>
       <c r="G12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="L12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="M12">
         <v>2000</v>
@@ -1345,7 +1321,7 @@
         <v>100</v>
       </c>
       <c r="O12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="P12" t="s">
         <v>27</v>
@@ -1359,37 +1335,37 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D13">
         <v>96</v>
       </c>
       <c r="E13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F13">
         <v>96</v>
       </c>
       <c r="G13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="L13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="M13">
         <v>16000</v>
@@ -1398,10 +1374,10 @@
         <v>100</v>
       </c>
       <c r="O13" t="s">
+        <v>64</v>
+      </c>
+      <c r="P13" t="s">
         <v>68</v>
-      </c>
-      <c r="P13" t="s">
-        <v>73</v>
       </c>
       <c r="Q13">
         <v>420000</v>
@@ -1412,37 +1388,37 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D14">
         <v>947.5</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F14">
         <v>758</v>
       </c>
       <c r="G14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="L14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="M14">
         <v>250000</v>
@@ -1451,10 +1427,10 @@
         <v>80</v>
       </c>
       <c r="O14" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="P14" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="Q14">
         <v>416900</v>
@@ -1465,37 +1441,37 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D15">
         <v>947.5</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F15">
         <v>189.5</v>
       </c>
       <c r="G15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="L15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="M15">
         <v>250000</v>
@@ -1504,10 +1480,10 @@
         <v>20</v>
       </c>
       <c r="O15" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="P15" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="Q15">
         <v>416900</v>
@@ -1518,37 +1494,37 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D16">
         <v>70</v>
       </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F16">
         <v>70</v>
       </c>
       <c r="G16" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H16" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I16" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J16" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K16" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="L16" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="M16">
         <v>7000</v>
@@ -1557,10 +1533,10 @@
         <v>100</v>
       </c>
       <c r="O16" t="s">
+        <v>64</v>
+      </c>
+      <c r="P16" t="s">
         <v>68</v>
-      </c>
-      <c r="P16" t="s">
-        <v>73</v>
       </c>
       <c r="Q16">
         <v>750000</v>
@@ -1571,37 +1547,37 @@
         <v>25</v>
       </c>
       <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
         <v>42</v>
-      </c>
-      <c r="C17" t="s">
-        <v>45</v>
       </c>
       <c r="D17">
         <v>226</v>
       </c>
       <c r="E17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F17">
         <v>226</v>
       </c>
       <c r="G17" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H17" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I17" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J17" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K17" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="L17" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="M17">
         <v>20000</v>
@@ -1610,119 +1586,13 @@
         <v>100</v>
       </c>
       <c r="O17" t="s">
+        <v>64</v>
+      </c>
+      <c r="P17" t="s">
         <v>68</v>
-      </c>
-      <c r="P17" t="s">
-        <v>73</v>
       </c>
       <c r="Q17">
         <v>827500</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17">
-      <c r="A18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18">
-        <v>91.5</v>
-      </c>
-      <c r="E18" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18">
-        <v>91.5</v>
-      </c>
-      <c r="G18" t="s">
-        <v>59</v>
-      </c>
-      <c r="H18" t="s">
-        <v>59</v>
-      </c>
-      <c r="I18" t="s">
-        <v>59</v>
-      </c>
-      <c r="J18" t="s">
-        <v>59</v>
-      </c>
-      <c r="K18" t="s">
-        <v>60</v>
-      </c>
-      <c r="L18" t="s">
-        <v>59</v>
-      </c>
-      <c r="M18">
-        <v>2000</v>
-      </c>
-      <c r="N18">
-        <v>100</v>
-      </c>
-      <c r="O18" t="s">
-        <v>70</v>
-      </c>
-      <c r="P18" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q18">
-        <v>3431250</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
-      <c r="A19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19">
-        <v>153</v>
-      </c>
-      <c r="E19" t="s">
-        <v>50</v>
-      </c>
-      <c r="F19">
-        <v>153</v>
-      </c>
-      <c r="G19" t="s">
-        <v>59</v>
-      </c>
-      <c r="H19" t="s">
-        <v>59</v>
-      </c>
-      <c r="I19" t="s">
-        <v>59</v>
-      </c>
-      <c r="J19" t="s">
-        <v>59</v>
-      </c>
-      <c r="K19" t="s">
-        <v>60</v>
-      </c>
-      <c r="L19" t="s">
-        <v>59</v>
-      </c>
-      <c r="M19">
-        <v>18000</v>
-      </c>
-      <c r="N19">
-        <v>100</v>
-      </c>
-      <c r="O19" t="s">
-        <v>70</v>
-      </c>
-      <c r="P19" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q19">
-        <v>637500</v>
       </c>
     </row>
   </sheetData>
@@ -1732,7 +1602,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1743,10 +1613,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -1755,60 +1625,60 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -1823,7 +1693,7 @@
         <v>3000000</v>
       </c>
       <c r="H2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I2">
         <v>2000</v>
@@ -1832,48 +1702,48 @@
         <v>2000</v>
       </c>
       <c r="K2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L2">
         <v>2000</v>
       </c>
       <c r="M2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="N2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="Q2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="R2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="S2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="T2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
@@ -1885,7 +1755,7 @@
         <v>1600000</v>
       </c>
       <c r="H3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I3">
         <v>11000</v>
@@ -1894,48 +1764,48 @@
         <v>15000</v>
       </c>
       <c r="K3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L3">
         <v>20000</v>
       </c>
       <c r="M3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="N3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="Q3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="R3" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="S3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="T3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
@@ -1947,7 +1817,7 @@
         <v>2000000</v>
       </c>
       <c r="H4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I4">
         <v>20000</v>
@@ -1956,34 +1826,34 @@
         <v>25000</v>
       </c>
       <c r="K4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L4">
         <v>30000</v>
       </c>
       <c r="M4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="N4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="Q4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="R4" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="S4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="T4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -1991,10 +1861,10 @@
         <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -2009,7 +1879,7 @@
         <v>990000</v>
       </c>
       <c r="H5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I5">
         <v>13000</v>
@@ -2018,45 +1888,45 @@
         <v>15000</v>
       </c>
       <c r="K5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L5">
         <v>20000</v>
       </c>
       <c r="M5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="N5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="Q5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="R5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="S5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="T5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D6" t="s">
         <v>23</v>
@@ -2071,7 +1941,7 @@
         <v>2104000</v>
       </c>
       <c r="H6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I6">
         <v>9000</v>
@@ -2080,34 +1950,34 @@
         <v>11000</v>
       </c>
       <c r="K6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L6">
         <v>13500</v>
       </c>
       <c r="M6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="N6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="Q6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="R6" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="S6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="T6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -2115,10 +1985,10 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
         <v>26</v>
@@ -2133,7 +2003,7 @@
         <v>5000000</v>
       </c>
       <c r="H7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I7">
         <v>2000</v>
@@ -2142,45 +2012,45 @@
         <v>2000</v>
       </c>
       <c r="K7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L7">
         <v>2000</v>
       </c>
       <c r="M7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="N7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="Q7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="R7" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="S7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="T7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
         <v>25</v>
@@ -2195,7 +2065,7 @@
         <v>6500000</v>
       </c>
       <c r="H8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I8">
         <v>2000</v>
@@ -2204,45 +2074,45 @@
         <v>2000</v>
       </c>
       <c r="K8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L8">
         <v>2000</v>
       </c>
       <c r="M8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="N8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="Q8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="R8" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="S8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="T8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
         <v>25</v>
@@ -2257,7 +2127,7 @@
         <v>4000000</v>
       </c>
       <c r="H9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I9">
         <v>2000</v>
@@ -2266,45 +2136,45 @@
         <v>2000</v>
       </c>
       <c r="K9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L9">
         <v>2000</v>
       </c>
       <c r="M9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="N9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="Q9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="R9" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="S9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="T9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
         <v>27</v>
@@ -2319,7 +2189,7 @@
         <v>4000000</v>
       </c>
       <c r="H10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I10">
         <v>2000</v>
@@ -2328,45 +2198,45 @@
         <v>2000</v>
       </c>
       <c r="K10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L10">
         <v>2000</v>
       </c>
       <c r="M10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="N10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="Q10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="R10" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="S10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="T10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D11" t="s">
         <v>27</v>
@@ -2381,7 +2251,7 @@
         <v>4000000</v>
       </c>
       <c r="H11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I11">
         <v>2000</v>
@@ -2390,48 +2260,48 @@
         <v>2000</v>
       </c>
       <c r="K11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L11">
         <v>2000</v>
       </c>
       <c r="M11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="N11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="Q11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="R11" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="S11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="T11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" t="s">
         <v>68</v>
-      </c>
-      <c r="B12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" t="s">
-        <v>73</v>
       </c>
       <c r="E12" t="s">
         <v>25</v>
@@ -2443,7 +2313,7 @@
         <v>600000</v>
       </c>
       <c r="H12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I12">
         <v>12000</v>
@@ -2452,48 +2322,48 @@
         <v>14000</v>
       </c>
       <c r="K12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L12">
         <v>16000</v>
       </c>
       <c r="M12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="N12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="Q12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="R12" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="S12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="T12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E13" t="s">
         <v>26</v>
@@ -2505,7 +2375,7 @@
         <v>379000</v>
       </c>
       <c r="H13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I13">
         <v>147000</v>
@@ -2514,48 +2384,48 @@
         <v>200000</v>
       </c>
       <c r="K13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L13">
         <v>250000</v>
       </c>
       <c r="M13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="N13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="O13">
         <v>18.46965699208443</v>
       </c>
       <c r="P13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="Q13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="R13" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="S13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="T13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" t="s">
         <v>68</v>
-      </c>
-      <c r="B14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" t="s">
-        <v>73</v>
       </c>
       <c r="E14" t="s">
         <v>27</v>
@@ -2567,7 +2437,7 @@
         <v>1000000</v>
       </c>
       <c r="H14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I14">
         <v>4800</v>
@@ -2576,48 +2446,48 @@
         <v>5800</v>
       </c>
       <c r="K14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L14">
         <v>7000</v>
       </c>
       <c r="M14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="N14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="Q14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="R14" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="S14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="T14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" t="s">
         <v>68</v>
-      </c>
-      <c r="B15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" t="s">
-        <v>73</v>
       </c>
       <c r="E15" t="s">
         <v>25</v>
@@ -2629,7 +2499,7 @@
         <v>1130000</v>
       </c>
       <c r="H15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I15">
         <v>14500</v>
@@ -2638,158 +2508,34 @@
         <v>18500</v>
       </c>
       <c r="K15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L15">
         <v>20000</v>
       </c>
       <c r="M15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="N15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="Q15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="R15" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="S15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="T15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20">
-      <c r="A16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" t="s">
-        <v>74</v>
-      </c>
-      <c r="E16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16">
-        <v>9150000</v>
-      </c>
-      <c r="G16">
-        <v>4575000</v>
-      </c>
-      <c r="H16" t="s">
-        <v>59</v>
-      </c>
-      <c r="I16">
-        <v>2000</v>
-      </c>
-      <c r="J16">
-        <v>2000</v>
-      </c>
-      <c r="K16" t="s">
-        <v>59</v>
-      </c>
-      <c r="L16">
-        <v>2000</v>
-      </c>
-      <c r="M16" t="s">
-        <v>59</v>
-      </c>
-      <c r="N16" t="s">
-        <v>59</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>59</v>
-      </c>
-      <c r="R16" t="s">
-        <v>107</v>
-      </c>
-      <c r="S16" t="s">
-        <v>59</v>
-      </c>
-      <c r="T16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20">
-      <c r="A17" t="s">
-        <v>70</v>
-      </c>
-      <c r="B17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17">
-        <v>15300000</v>
-      </c>
-      <c r="G17">
-        <v>850000</v>
-      </c>
-      <c r="H17" t="s">
-        <v>59</v>
-      </c>
-      <c r="I17">
-        <v>14500</v>
-      </c>
-      <c r="J17">
-        <v>16500</v>
-      </c>
-      <c r="K17" t="s">
-        <v>59</v>
-      </c>
-      <c r="L17">
-        <v>18000</v>
-      </c>
-      <c r="M17" t="s">
-        <v>59</v>
-      </c>
-      <c r="N17" t="s">
-        <v>59</v>
-      </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>59</v>
-      </c>
-      <c r="R17" t="s">
-        <v>108</v>
-      </c>
-      <c r="S17" t="s">
-        <v>59</v>
-      </c>
-      <c r="T17" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2799,7 +2545,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2807,16 +2553,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -2828,10 +2574,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -2840,24 +2586,24 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
         <v>27</v>
@@ -2883,107 +2629,107 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="F3" t="s">
-        <v>74</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H3">
-        <v>15300</v>
+        <v>14202</v>
       </c>
       <c r="I3">
-        <v>850000</v>
+        <v>2104000</v>
       </c>
       <c r="J3">
-        <v>18000</v>
+        <v>13500</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H4">
-        <v>14202</v>
+        <v>32000</v>
       </c>
       <c r="I4">
-        <v>2104000</v>
+        <v>1600000</v>
       </c>
       <c r="J4">
-        <v>13500</v>
+        <v>20000</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H5">
-        <v>32000</v>
+        <v>19800</v>
       </c>
       <c r="I5">
-        <v>1600000</v>
+        <v>990000</v>
       </c>
       <c r="J5">
         <v>20000</v>
@@ -2997,72 +2743,72 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="F6" t="s">
-        <v>73</v>
+        <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H6">
-        <v>7000</v>
+        <v>14202</v>
       </c>
       <c r="I6">
-        <v>1000000</v>
+        <v>2104000</v>
       </c>
       <c r="J6">
-        <v>7000</v>
+        <v>13500</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H7">
-        <v>19800</v>
+        <v>7000</v>
       </c>
       <c r="I7">
-        <v>990000</v>
+        <v>1000000</v>
       </c>
       <c r="J7">
-        <v>20000</v>
+        <v>7000</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -3073,107 +2819,107 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>92</v>
+        <v>49</v>
       </c>
       <c r="E8" t="s">
-        <v>92</v>
+        <v>49</v>
       </c>
       <c r="F8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H8">
-        <v>14202</v>
+        <v>8000</v>
       </c>
       <c r="I8">
-        <v>2104000</v>
+        <v>4000000</v>
       </c>
       <c r="J8">
-        <v>13500</v>
+        <v>2000</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>104</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="G9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H9">
-        <v>8000</v>
+        <v>75800</v>
       </c>
       <c r="I9">
-        <v>4000000</v>
+        <v>379000</v>
       </c>
       <c r="J9">
-        <v>2000</v>
+        <v>250000</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="F10" t="s">
-        <v>74</v>
+        <v>25</v>
       </c>
       <c r="G10" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="H10">
-        <v>9150</v>
+        <v>13000</v>
       </c>
       <c r="I10">
-        <v>4575000</v>
+        <v>6500000</v>
       </c>
       <c r="J10">
         <v>2000</v>
@@ -3187,72 +2933,72 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E11" t="s">
-        <v>112</v>
+        <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H11">
-        <v>75800</v>
+        <v>8000</v>
       </c>
       <c r="I11">
-        <v>379000</v>
+        <v>4000000</v>
       </c>
       <c r="J11">
-        <v>250000</v>
+        <v>2000</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" t="s">
         <v>25</v>
       </c>
-      <c r="G12" t="s">
-        <v>23</v>
-      </c>
       <c r="H12">
-        <v>13000</v>
+        <v>9600</v>
       </c>
       <c r="I12">
-        <v>6500000</v>
+        <v>600000</v>
       </c>
       <c r="J12">
-        <v>2000</v>
+        <v>16000</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -3263,31 +3009,31 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="F13" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="G13" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H13">
-        <v>8000</v>
+        <v>6000</v>
       </c>
       <c r="I13">
-        <v>4000000</v>
+        <v>3000000</v>
       </c>
       <c r="J13">
         <v>2000</v>
@@ -3301,34 +3047,34 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F14" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="G14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H14">
-        <v>9600</v>
+        <v>10000</v>
       </c>
       <c r="I14">
-        <v>600000</v>
+        <v>5000000</v>
       </c>
       <c r="J14">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -3339,191 +3085,115 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>104</v>
       </c>
       <c r="F15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" t="s">
         <v>26</v>
       </c>
-      <c r="G15" t="s">
-        <v>22</v>
-      </c>
       <c r="H15">
-        <v>10000</v>
+        <v>18950</v>
       </c>
       <c r="I15">
-        <v>5000000</v>
+        <v>379000</v>
       </c>
       <c r="J15">
-        <v>2000</v>
+        <v>250000</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>112</v>
+        <v>46</v>
       </c>
       <c r="F16" t="s">
         <v>67</v>
       </c>
       <c r="G16" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H16">
-        <v>18950</v>
+        <v>60000</v>
       </c>
       <c r="I16">
-        <v>379000</v>
+        <v>2000000</v>
       </c>
       <c r="J16">
-        <v>250000</v>
+        <v>30000</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="F17" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="G17" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="H17">
-        <v>6000</v>
+        <v>22600</v>
       </c>
       <c r="I17">
-        <v>3000000</v>
+        <v>1130000</v>
       </c>
       <c r="J17">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" t="s">
-        <v>72</v>
-      </c>
-      <c r="G18" t="s">
-        <v>19</v>
-      </c>
-      <c r="H18">
-        <v>60000</v>
-      </c>
-      <c r="I18">
-        <v>2000000</v>
-      </c>
-      <c r="J18">
-        <v>30000</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" t="s">
-        <v>57</v>
-      </c>
-      <c r="E19" t="s">
-        <v>57</v>
-      </c>
-      <c r="F19" t="s">
-        <v>73</v>
-      </c>
-      <c r="G19" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19">
-        <v>22600</v>
-      </c>
-      <c r="I19">
-        <v>1130000</v>
-      </c>
-      <c r="J19">
-        <v>20000</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2024-04-04
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="111">
   <si>
     <t>상장일</t>
   </si>
@@ -69,6 +69,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2024-04-03</t>
+  </si>
+  <si>
     <t>2024-03-27</t>
   </si>
   <si>
@@ -102,6 +105,9 @@
     <t>2024-02-22</t>
   </si>
   <si>
+    <t>아이엠비디엑스</t>
+  </si>
+  <si>
     <t>하나32호스팩</t>
   </si>
   <si>
@@ -150,6 +156,9 @@
     <t>코스피</t>
   </si>
   <si>
+    <t>미래</t>
+  </si>
+  <si>
     <t>하나</t>
   </si>
   <si>
@@ -192,6 +201,9 @@
     <t>공동</t>
   </si>
   <si>
+    <t>2024-03-25</t>
+  </si>
+  <si>
     <t>2024-03-18</t>
   </si>
   <si>
@@ -216,6 +228,9 @@
     <t>2024-02-14</t>
   </si>
   <si>
+    <t>2024-03-28</t>
+  </si>
+  <si>
     <t>2024-03-19</t>
   </si>
   <si>
@@ -277,6 +292,9 @@
   </si>
   <si>
     <t>DB, NH</t>
+  </si>
+  <si>
+    <t>2654.2 : 1</t>
   </si>
   <si>
     <t>2389.8 : 1</t>
@@ -688,7 +706,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -752,52 +770,52 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D2">
-        <v>60</v>
+        <v>325</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F2">
-        <v>60</v>
+        <v>325</v>
       </c>
       <c r="G2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="L2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="M2">
-        <v>2000</v>
+        <v>13000</v>
       </c>
       <c r="N2">
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="P2" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="Q2">
-        <v>2250000</v>
+        <v>1875000</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -805,52 +823,52 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D3">
-        <v>320</v>
+        <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F3">
-        <v>320</v>
+        <v>60</v>
       </c>
       <c r="G3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="L3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="M3">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="N3">
         <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="P3" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="Q3">
-        <v>880000</v>
+        <v>2250000</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -858,52 +876,52 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D4">
-        <v>600</v>
+        <v>320</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F4">
-        <v>600</v>
+        <v>320</v>
       </c>
       <c r="G4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="L4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="M4">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="N4">
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="P4" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="Q4">
-        <v>1368000</v>
+        <v>880000</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -911,52 +929,52 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D5">
-        <v>198</v>
+        <v>600</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F5">
-        <v>198</v>
+        <v>600</v>
       </c>
       <c r="G5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="L5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="M5">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="N5">
         <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="P5" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="Q5">
-        <v>742500</v>
+        <v>1368000</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -964,90 +982,90 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D6">
-        <v>284.04</v>
+        <v>198</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F6">
-        <v>142.02</v>
+        <v>198</v>
       </c>
       <c r="G6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K6" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="L6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="M6">
-        <v>13500</v>
+        <v>20000</v>
       </c>
       <c r="N6">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="P6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q6">
-        <v>2916000</v>
+        <v>742500</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D7">
         <v>284.04</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F7">
         <v>142.02</v>
       </c>
       <c r="G7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="L7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="M7">
         <v>13500</v>
@@ -1056,10 +1074,10 @@
         <v>50</v>
       </c>
       <c r="O7" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="P7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q7">
         <v>2916000</v>
@@ -1070,52 +1088,52 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D8">
-        <v>100</v>
+        <v>284.04</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F8">
-        <v>100</v>
+        <v>142.02</v>
       </c>
       <c r="G8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="L8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="M8">
-        <v>2000</v>
+        <v>13500</v>
       </c>
       <c r="N8">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O8" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="P8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="Q8">
-        <v>3750000</v>
+        <v>2916000</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1123,37 +1141,37 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D9">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F9">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="G9" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H9" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I9" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J9" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K9" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="L9" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="M9">
         <v>2000</v>
@@ -1162,13 +1180,13 @@
         <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="P9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q9">
-        <v>4875000</v>
+        <v>3750000</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1176,37 +1194,37 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D10">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="E10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F10">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="G10" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H10" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I10" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J10" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K10" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="L10" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="M10">
         <v>2000</v>
@@ -1215,51 +1233,51 @@
         <v>100</v>
       </c>
       <c r="O10" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="P10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="Q10">
-        <v>3000000</v>
+        <v>4875000</v>
       </c>
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D11">
         <v>80</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F11">
         <v>80</v>
       </c>
       <c r="G11" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H11" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I11" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J11" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K11" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="L11" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="M11">
         <v>2000</v>
@@ -1268,10 +1286,10 @@
         <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="P11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q11">
         <v>3000000</v>
@@ -1282,37 +1300,37 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D12">
         <v>80</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F12">
         <v>80</v>
       </c>
       <c r="G12" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H12" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I12" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J12" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K12" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="L12" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="M12">
         <v>2000</v>
@@ -1321,10 +1339,10 @@
         <v>100</v>
       </c>
       <c r="O12" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="P12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q12">
         <v>3000000</v>
@@ -1332,55 +1350,55 @@
     </row>
     <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D13">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F13">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="G13" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H13" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I13" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J13" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K13" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="L13" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="M13">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="N13">
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="P13" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="Q13">
-        <v>420000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1388,102 +1406,102 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D14">
-        <v>947.5</v>
+        <v>96</v>
       </c>
       <c r="E14" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F14">
-        <v>758</v>
+        <v>96</v>
       </c>
       <c r="G14" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H14" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I14" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J14" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K14" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="L14" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="M14">
-        <v>250000</v>
+        <v>16000</v>
       </c>
       <c r="N14">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="P14" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="Q14">
-        <v>416900</v>
+        <v>420000</v>
       </c>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D15">
         <v>947.5</v>
       </c>
       <c r="E15" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="F15">
-        <v>189.5</v>
+        <v>758</v>
       </c>
       <c r="G15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="M15">
         <v>250000</v>
       </c>
       <c r="N15">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="O15" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="P15" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="Q15">
         <v>416900</v>
@@ -1494,104 +1512,157 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D16">
-        <v>70</v>
+        <v>947.5</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F16">
-        <v>70</v>
+        <v>189.5</v>
       </c>
       <c r="G16" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H16" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I16" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J16" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K16" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="L16" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="M16">
-        <v>7000</v>
+        <v>250000</v>
       </c>
       <c r="N16">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="O16" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="P16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q16">
-        <v>750000</v>
+        <v>416900</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D17">
-        <v>226</v>
+        <v>70</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F17">
-        <v>226</v>
+        <v>70</v>
       </c>
       <c r="G17" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H17" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I17" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J17" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K17" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="L17" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="M17">
-        <v>20000</v>
+        <v>7000</v>
       </c>
       <c r="N17">
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="P17" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q17">
+        <v>750000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18">
+        <v>226</v>
+      </c>
+      <c r="E18" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18">
+        <v>226</v>
+      </c>
+      <c r="G18" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" t="s">
+        <v>58</v>
+      </c>
+      <c r="J18" t="s">
+        <v>58</v>
+      </c>
+      <c r="K18" t="s">
+        <v>59</v>
+      </c>
+      <c r="L18" t="s">
+        <v>58</v>
+      </c>
+      <c r="M18">
+        <v>20000</v>
+      </c>
+      <c r="N18">
+        <v>100</v>
+      </c>
+      <c r="O18" t="s">
         <v>68</v>
       </c>
-      <c r="Q17">
+      <c r="P18" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q18">
         <v>827500</v>
       </c>
     </row>
@@ -1602,7 +1673,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T15"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1613,10 +1684,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -1625,447 +1696,447 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
       </c>
       <c r="F2">
-        <v>6000000</v>
+        <v>32500000</v>
       </c>
       <c r="G2">
-        <v>3000000</v>
+        <v>2500000</v>
       </c>
       <c r="H2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I2">
-        <v>2000</v>
+        <v>7700</v>
       </c>
       <c r="J2">
-        <v>2000</v>
+        <v>9900</v>
       </c>
       <c r="K2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="L2">
-        <v>2000</v>
+        <v>13000</v>
       </c>
       <c r="M2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="Q2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="R2" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="S2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="T2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
       </c>
       <c r="F3">
-        <v>32000000</v>
+        <v>6000000</v>
       </c>
       <c r="G3">
-        <v>1600000</v>
+        <v>3000000</v>
       </c>
       <c r="H3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I3">
-        <v>11000</v>
+        <v>2000</v>
       </c>
       <c r="J3">
-        <v>15000</v>
+        <v>2000</v>
       </c>
       <c r="K3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="L3">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="M3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="Q3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="R3" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="S3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="T3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
       </c>
       <c r="F4">
-        <v>60000000</v>
+        <v>32000000</v>
       </c>
       <c r="G4">
-        <v>2000000</v>
+        <v>1600000</v>
       </c>
       <c r="H4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I4">
+        <v>11000</v>
+      </c>
+      <c r="J4">
+        <v>15000</v>
+      </c>
+      <c r="K4" t="s">
+        <v>58</v>
+      </c>
+      <c r="L4">
         <v>20000</v>
       </c>
-      <c r="J4">
-        <v>25000</v>
-      </c>
-      <c r="K4" t="s">
-        <v>55</v>
-      </c>
-      <c r="L4">
-        <v>30000</v>
-      </c>
       <c r="M4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="Q4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="R4" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="S4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="T4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
       </c>
       <c r="F5">
-        <v>19800000</v>
+        <v>60000000</v>
       </c>
       <c r="G5">
-        <v>990000</v>
+        <v>2000000</v>
       </c>
       <c r="H5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I5">
-        <v>13000</v>
+        <v>20000</v>
       </c>
       <c r="J5">
-        <v>15000</v>
+        <v>25000</v>
       </c>
       <c r="K5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="L5">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="M5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="Q5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="R5" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="S5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="T5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
       </c>
       <c r="F6">
-        <v>28404000</v>
+        <v>19800000</v>
       </c>
       <c r="G6">
-        <v>2104000</v>
+        <v>990000</v>
       </c>
       <c r="H6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I6">
-        <v>9000</v>
+        <v>13000</v>
       </c>
       <c r="J6">
-        <v>11000</v>
+        <v>15000</v>
       </c>
       <c r="K6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="L6">
-        <v>13500</v>
+        <v>20000</v>
       </c>
       <c r="M6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="Q6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="R6" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="S6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="T6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
         <v>22</v>
       </c>
       <c r="F7">
-        <v>10000000</v>
+        <v>28404000</v>
       </c>
       <c r="G7">
-        <v>5000000</v>
+        <v>2104000</v>
       </c>
       <c r="H7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I7">
-        <v>2000</v>
+        <v>9000</v>
       </c>
       <c r="J7">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="K7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="L7">
-        <v>2000</v>
+        <v>13500</v>
       </c>
       <c r="M7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="Q7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="R7" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="S7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="T7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
         <v>23</v>
       </c>
       <c r="F8">
-        <v>13000000</v>
+        <v>10000000</v>
       </c>
       <c r="G8">
-        <v>6500000</v>
+        <v>5000000</v>
       </c>
       <c r="H8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I8">
         <v>2000</v>
@@ -2074,60 +2145,60 @@
         <v>2000</v>
       </c>
       <c r="K8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="L8">
         <v>2000</v>
       </c>
       <c r="M8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="Q8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="R8" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="S8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="T8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
       </c>
       <c r="F9">
-        <v>8000000</v>
+        <v>13000000</v>
       </c>
       <c r="G9">
-        <v>4000000</v>
+        <v>6500000</v>
       </c>
       <c r="H9" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I9">
         <v>2000</v>
@@ -2136,51 +2207,51 @@
         <v>2000</v>
       </c>
       <c r="K9" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="L9">
         <v>2000</v>
       </c>
       <c r="M9" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N9" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="Q9" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="R9" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="S9" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="T9" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F10">
         <v>8000000</v>
@@ -2189,7 +2260,7 @@
         <v>4000000</v>
       </c>
       <c r="H10" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I10">
         <v>2000</v>
@@ -2198,48 +2269,48 @@
         <v>2000</v>
       </c>
       <c r="K10" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="L10">
         <v>2000</v>
       </c>
       <c r="M10" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N10" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="Q10" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="R10" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="S10" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="T10" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
         <v>23</v>
@@ -2251,7 +2322,7 @@
         <v>4000000</v>
       </c>
       <c r="H11" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I11">
         <v>2000</v>
@@ -2260,282 +2331,344 @@
         <v>2000</v>
       </c>
       <c r="K11" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="L11">
         <v>2000</v>
       </c>
       <c r="M11" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N11" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="Q11" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="R11" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="S11" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="T11" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12">
-        <v>9600000</v>
+        <v>8000000</v>
       </c>
       <c r="G12">
-        <v>600000</v>
+        <v>4000000</v>
       </c>
       <c r="H12" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I12">
-        <v>12000</v>
+        <v>2000</v>
       </c>
       <c r="J12">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="K12" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="L12">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="M12" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N12" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="Q12" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="R12" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="S12" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="T12" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E13" t="s">
         <v>26</v>
       </c>
       <c r="F13">
-        <v>94750000</v>
+        <v>9600000</v>
       </c>
       <c r="G13">
-        <v>379000</v>
+        <v>600000</v>
       </c>
       <c r="H13" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I13">
-        <v>147000</v>
+        <v>12000</v>
       </c>
       <c r="J13">
-        <v>200000</v>
+        <v>14000</v>
       </c>
       <c r="K13" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="L13">
-        <v>250000</v>
+        <v>16000</v>
       </c>
       <c r="M13" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N13" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="O13">
-        <v>18.46965699208443</v>
+        <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="Q13" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="R13" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="S13" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="T13" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E14" t="s">
         <v>27</v>
       </c>
       <c r="F14">
-        <v>7000000</v>
+        <v>94750000</v>
       </c>
       <c r="G14">
-        <v>1000000</v>
+        <v>379000</v>
       </c>
       <c r="H14" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I14">
-        <v>4800</v>
+        <v>147000</v>
       </c>
       <c r="J14">
-        <v>5800</v>
+        <v>200000</v>
       </c>
       <c r="K14" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="L14">
-        <v>7000</v>
+        <v>250000</v>
       </c>
       <c r="M14" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N14" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="O14">
-        <v>0</v>
+        <v>18.46965699208443</v>
       </c>
       <c r="P14" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="Q14" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="R14" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="S14" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="T14" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F15">
-        <v>22600000</v>
+        <v>7000000</v>
       </c>
       <c r="G15">
-        <v>1130000</v>
+        <v>1000000</v>
       </c>
       <c r="H15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I15">
-        <v>14500</v>
+        <v>4800</v>
       </c>
       <c r="J15">
-        <v>18500</v>
+        <v>5800</v>
       </c>
       <c r="K15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="L15">
-        <v>20000</v>
+        <v>7000</v>
       </c>
       <c r="M15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="Q15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="R15" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="S15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="T15" t="s">
-        <v>55</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16">
+        <v>22600000</v>
+      </c>
+      <c r="G16">
+        <v>1130000</v>
+      </c>
+      <c r="H16" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16">
+        <v>14500</v>
+      </c>
+      <c r="J16">
+        <v>18500</v>
+      </c>
+      <c r="K16" t="s">
+        <v>58</v>
+      </c>
+      <c r="L16">
+        <v>20000</v>
+      </c>
+      <c r="M16" t="s">
+        <v>58</v>
+      </c>
+      <c r="N16" t="s">
+        <v>58</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>58</v>
+      </c>
+      <c r="R16" t="s">
+        <v>106</v>
+      </c>
+      <c r="S16" t="s">
+        <v>58</v>
+      </c>
+      <c r="T16" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2545,7 +2678,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2553,16 +2686,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -2574,10 +2707,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -2586,30 +2719,30 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2">
         <v>8000</v>
@@ -2629,25 +2762,25 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="E3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H3">
         <v>14202</v>
@@ -2667,25 +2800,25 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H4">
         <v>32000</v>
@@ -2705,25 +2838,25 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
         <v>21</v>
-      </c>
-      <c r="G5" t="s">
-        <v>20</v>
       </c>
       <c r="H5">
         <v>19800</v>
@@ -2743,25 +2876,25 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="E6" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H6">
         <v>14202</v>
@@ -2781,25 +2914,25 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F7" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H7">
         <v>7000</v>
@@ -2819,25 +2952,25 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" t="s">
         <v>25</v>
-      </c>
-      <c r="G8" t="s">
-        <v>24</v>
       </c>
       <c r="H8">
         <v>8000</v>
@@ -2857,78 +2990,78 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>104</v>
+        <v>46</v>
       </c>
       <c r="F9" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="H9">
-        <v>75800</v>
+        <v>32500</v>
       </c>
       <c r="I9">
-        <v>379000</v>
+        <v>2500000</v>
       </c>
       <c r="J9">
-        <v>250000</v>
+        <v>13000</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>110</v>
       </c>
       <c r="F10" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="G10" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H10">
-        <v>13000</v>
+        <v>75800</v>
       </c>
       <c r="I10">
-        <v>6500000</v>
+        <v>379000</v>
       </c>
       <c r="J10">
-        <v>2000</v>
+        <v>250000</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -2936,10 +3069,10 @@
         <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
         <v>51</v>
@@ -2948,16 +3081,16 @@
         <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H11">
-        <v>8000</v>
+        <v>13000</v>
       </c>
       <c r="I11">
-        <v>4000000</v>
+        <v>6500000</v>
       </c>
       <c r="J11">
         <v>2000</v>
@@ -2971,34 +3104,34 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F12" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="G12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H12">
-        <v>9600</v>
+        <v>8000</v>
       </c>
       <c r="I12">
-        <v>600000</v>
+        <v>4000000</v>
       </c>
       <c r="J12">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -3009,34 +3142,34 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="E13" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="F13" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="G13" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="H13">
-        <v>6000</v>
+        <v>9600</v>
       </c>
       <c r="I13">
-        <v>3000000</v>
+        <v>600000</v>
       </c>
       <c r="J13">
-        <v>2000</v>
+        <v>16000</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -3047,31 +3180,31 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E14" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F14" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G14" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H14">
-        <v>10000</v>
+        <v>6000</v>
       </c>
       <c r="I14">
-        <v>5000000</v>
+        <v>3000000</v>
       </c>
       <c r="J14">
         <v>2000</v>
@@ -3085,25 +3218,25 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E15" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F15" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="G15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H15">
         <v>18950</v>
@@ -3123,34 +3256,34 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F16" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="G16" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H16">
-        <v>60000</v>
+        <v>10000</v>
       </c>
       <c r="I16">
-        <v>2000000</v>
+        <v>5000000</v>
       </c>
       <c r="J16">
-        <v>30000</v>
+        <v>2000</v>
       </c>
       <c r="K16">
         <v>0</v>
@@ -3161,39 +3294,77 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
         <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F17" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G17" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H17">
-        <v>22600</v>
+        <v>60000</v>
       </c>
       <c r="I17">
-        <v>1130000</v>
+        <v>2000000</v>
       </c>
       <c r="J17">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" t="s">
+        <v>73</v>
+      </c>
+      <c r="G18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18">
+        <v>22600</v>
+      </c>
+      <c r="I18">
+        <v>1130000</v>
+      </c>
+      <c r="J18">
+        <v>20000</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2024-04-20
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="105">
   <si>
     <t>상장일</t>
   </si>
@@ -102,144 +102,132 @@
     <t>2024-02-23</t>
   </si>
   <si>
+    <t>신한제12호스팩</t>
+  </si>
+  <si>
+    <t>아이엠비디엑스</t>
+  </si>
+  <si>
+    <t>하나32호스팩</t>
+  </si>
+  <si>
+    <t>엔젤로보틱스</t>
+  </si>
+  <si>
+    <t>삼현</t>
+  </si>
+  <si>
+    <t>오상헬스케어</t>
+  </si>
+  <si>
+    <t>케이엔알시스템</t>
+  </si>
+  <si>
+    <t>하나31호스팩</t>
+  </si>
+  <si>
+    <t>유안타제15호스팩</t>
+  </si>
+  <si>
+    <t>SK증권제11호스팩</t>
+  </si>
+  <si>
+    <t>비엔케이제2호스팩</t>
+  </si>
+  <si>
+    <t>유진스팩10호</t>
+  </si>
+  <si>
+    <t>코셈</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>신한</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>한국</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>유안타</t>
+  </si>
+  <si>
+    <t>SK</t>
+  </si>
+  <si>
+    <t>BNK</t>
+  </si>
+  <si>
+    <t>유진</t>
+  </si>
+  <si>
+    <t>키움</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>2024-04-02</t>
+  </si>
+  <si>
+    <t>2024-03-25</t>
+  </si>
+  <si>
+    <t>2024-03-18</t>
+  </si>
+  <si>
+    <t>2024-03-14</t>
+  </si>
+  <si>
+    <t>2024-03-12</t>
+  </si>
+  <si>
+    <t>2024-02-26</t>
+  </si>
+  <si>
+    <t>2024-02-22</t>
+  </si>
+  <si>
+    <t>2024-02-20</t>
+  </si>
+  <si>
+    <t>2024-02-19</t>
+  </si>
+  <si>
+    <t>2024-02-13</t>
+  </si>
+  <si>
+    <t>2024-04-05</t>
+  </si>
+  <si>
+    <t>2024-03-28</t>
+  </si>
+  <si>
+    <t>2024-03-19</t>
+  </si>
+  <si>
+    <t>2024-03-15</t>
+  </si>
+  <si>
     <t>2024-02-27</t>
   </si>
   <si>
-    <t>신한제12호스팩</t>
-  </si>
-  <si>
-    <t>아이엠비디엑스</t>
-  </si>
-  <si>
-    <t>하나32호스팩</t>
-  </si>
-  <si>
-    <t>엔젤로보틱스</t>
-  </si>
-  <si>
-    <t>삼현</t>
-  </si>
-  <si>
-    <t>오상헬스케어</t>
-  </si>
-  <si>
-    <t>케이엔알시스템</t>
-  </si>
-  <si>
-    <t>하나31호스팩</t>
-  </si>
-  <si>
-    <t>유안타제15호스팩</t>
-  </si>
-  <si>
-    <t>SK증권제11호스팩</t>
-  </si>
-  <si>
-    <t>비엔케이제2호스팩</t>
-  </si>
-  <si>
-    <t>유진스팩10호</t>
-  </si>
-  <si>
-    <t>코셈</t>
-  </si>
-  <si>
-    <t>에이피알</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>코스피</t>
-  </si>
-  <si>
-    <t>신한</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>한국</t>
-  </si>
-  <si>
-    <t>DB</t>
-  </si>
-  <si>
-    <t>유안타</t>
-  </si>
-  <si>
-    <t>SK</t>
-  </si>
-  <si>
-    <t>BNK</t>
-  </si>
-  <si>
-    <t>유진</t>
-  </si>
-  <si>
-    <t>키움</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>공동</t>
-  </si>
-  <si>
-    <t>2024-04-02</t>
-  </si>
-  <si>
-    <t>2024-03-25</t>
-  </si>
-  <si>
-    <t>2024-03-18</t>
-  </si>
-  <si>
-    <t>2024-03-14</t>
-  </si>
-  <si>
-    <t>2024-03-12</t>
-  </si>
-  <si>
-    <t>2024-02-26</t>
-  </si>
-  <si>
-    <t>2024-02-22</t>
-  </si>
-  <si>
-    <t>2024-02-20</t>
-  </si>
-  <si>
-    <t>2024-02-19</t>
-  </si>
-  <si>
-    <t>2024-02-13</t>
-  </si>
-  <si>
-    <t>2024-02-14</t>
-  </si>
-  <si>
-    <t>2024-04-05</t>
-  </si>
-  <si>
-    <t>2024-03-28</t>
-  </si>
-  <si>
-    <t>2024-03-19</t>
-  </si>
-  <si>
-    <t>2024-03-15</t>
-  </si>
-  <si>
     <t>2024-02-16</t>
   </si>
   <si>
@@ -336,9 +324,6 @@
     <t>2518.4 : 1</t>
   </si>
   <si>
-    <t>1113 : 1</t>
-  </si>
-  <si>
     <t>인수기관</t>
   </si>
   <si>
@@ -346,9 +331,6 @@
   </si>
   <si>
     <t>인수비율</t>
-  </si>
-  <si>
-    <t>신한, 하나</t>
   </si>
 </sst>
 </file>
@@ -706,7 +688,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -770,37 +752,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D2">
         <v>100</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F2">
         <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="M2">
         <v>2000</v>
@@ -809,10 +791,10 @@
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="P2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="Q2">
         <v>3750000</v>
@@ -823,37 +805,37 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D3">
         <v>325</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F3">
         <v>325</v>
       </c>
       <c r="G3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="M3">
         <v>13000</v>
@@ -862,10 +844,10 @@
         <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="P3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="Q3">
         <v>1875000</v>
@@ -876,37 +858,37 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D4">
         <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F4">
         <v>60</v>
       </c>
       <c r="G4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="M4">
         <v>2000</v>
@@ -915,7 +897,7 @@
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="P4" t="s">
         <v>21</v>
@@ -929,37 +911,37 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D5">
         <v>320</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F5">
         <v>320</v>
       </c>
       <c r="G5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="M5">
         <v>20000</v>
@@ -968,10 +950,10 @@
         <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="P5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="Q5">
         <v>880000</v>
@@ -982,37 +964,37 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D6">
         <v>600</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F6">
         <v>600</v>
       </c>
       <c r="G6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="M6">
         <v>30000</v>
@@ -1021,10 +1003,10 @@
         <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="P6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="Q6">
         <v>1368000</v>
@@ -1035,37 +1017,37 @@
         <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D7">
         <v>198</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F7">
         <v>198</v>
       </c>
       <c r="G7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="M7">
         <v>20000</v>
@@ -1088,37 +1070,37 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D8">
         <v>284.04</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F8">
         <v>142.02</v>
       </c>
       <c r="G8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="M8">
         <v>13500</v>
@@ -1127,7 +1109,7 @@
         <v>50</v>
       </c>
       <c r="O8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="P8" t="s">
         <v>25</v>
@@ -1141,37 +1123,37 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D9">
         <v>284.04</v>
       </c>
       <c r="E9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F9">
         <v>142.02</v>
       </c>
       <c r="G9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="M9">
         <v>13500</v>
@@ -1180,7 +1162,7 @@
         <v>50</v>
       </c>
       <c r="O9" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="P9" t="s">
         <v>25</v>
@@ -1194,37 +1176,37 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D10">
         <v>100</v>
       </c>
       <c r="E10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F10">
         <v>100</v>
       </c>
       <c r="G10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="M10">
         <v>2000</v>
@@ -1233,10 +1215,10 @@
         <v>100</v>
       </c>
       <c r="O10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="P10" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="Q10">
         <v>3750000</v>
@@ -1247,37 +1229,37 @@
         <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D11">
         <v>130</v>
       </c>
       <c r="E11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F11">
         <v>130</v>
       </c>
       <c r="G11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="M11">
         <v>2000</v>
@@ -1286,7 +1268,7 @@
         <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="P11" t="s">
         <v>27</v>
@@ -1300,37 +1282,37 @@
         <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D12">
         <v>80</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F12">
         <v>80</v>
       </c>
       <c r="G12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="M12">
         <v>2000</v>
@@ -1339,7 +1321,7 @@
         <v>100</v>
       </c>
       <c r="O12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="P12" t="s">
         <v>27</v>
@@ -1353,37 +1335,37 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D13">
         <v>80</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F13">
         <v>80</v>
       </c>
       <c r="G13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="M13">
         <v>2000</v>
@@ -1392,10 +1374,10 @@
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="P13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="Q13">
         <v>3000000</v>
@@ -1406,37 +1388,37 @@
         <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D14">
         <v>80</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F14">
         <v>80</v>
       </c>
       <c r="G14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K14" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="M14">
         <v>2000</v>
@@ -1445,10 +1427,10 @@
         <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="P14" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="Q14">
         <v>3000000</v>
@@ -1459,37 +1441,37 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
         <v>41</v>
-      </c>
-      <c r="C15" t="s">
-        <v>43</v>
       </c>
       <c r="D15">
         <v>96</v>
       </c>
       <c r="E15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F15">
         <v>96</v>
       </c>
       <c r="G15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="M15">
         <v>16000</v>
@@ -1498,119 +1480,13 @@
         <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="P15" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="Q15">
         <v>420000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16">
-        <v>947.5</v>
-      </c>
-      <c r="E16" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16">
-        <v>758</v>
-      </c>
-      <c r="G16" t="s">
-        <v>56</v>
-      </c>
-      <c r="H16" t="s">
-        <v>56</v>
-      </c>
-      <c r="I16" t="s">
-        <v>56</v>
-      </c>
-      <c r="J16" t="s">
-        <v>56</v>
-      </c>
-      <c r="K16" t="s">
-        <v>57</v>
-      </c>
-      <c r="L16" t="s">
-        <v>56</v>
-      </c>
-      <c r="M16">
-        <v>250000</v>
-      </c>
-      <c r="N16">
-        <v>80</v>
-      </c>
-      <c r="O16" t="s">
-        <v>69</v>
-      </c>
-      <c r="P16" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q16">
-        <v>416900</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
-      <c r="A17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17">
-        <v>947.5</v>
-      </c>
-      <c r="E17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17">
-        <v>189.5</v>
-      </c>
-      <c r="G17" t="s">
-        <v>56</v>
-      </c>
-      <c r="H17" t="s">
-        <v>56</v>
-      </c>
-      <c r="I17" t="s">
-        <v>56</v>
-      </c>
-      <c r="J17" t="s">
-        <v>56</v>
-      </c>
-      <c r="K17" t="s">
-        <v>58</v>
-      </c>
-      <c r="L17" t="s">
-        <v>56</v>
-      </c>
-      <c r="M17">
-        <v>250000</v>
-      </c>
-      <c r="N17">
-        <v>20</v>
-      </c>
-      <c r="O17" t="s">
-        <v>69</v>
-      </c>
-      <c r="P17" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q17">
-        <v>416900</v>
       </c>
     </row>
   </sheetData>
@@ -1620,7 +1496,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T15"/>
+  <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1631,10 +1507,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -1643,63 +1519,63 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
@@ -1711,7 +1587,7 @@
         <v>5000000</v>
       </c>
       <c r="H2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I2">
         <v>2000</v>
@@ -1720,48 +1596,48 @@
         <v>2000</v>
       </c>
       <c r="K2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L2">
         <v>2000</v>
       </c>
       <c r="M2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="R2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="S2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="T2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
@@ -1773,7 +1649,7 @@
         <v>2500000</v>
       </c>
       <c r="H3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I3">
         <v>7700</v>
@@ -1782,45 +1658,45 @@
         <v>9900</v>
       </c>
       <c r="K3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L3">
         <v>13000</v>
       </c>
       <c r="M3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="R3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="S3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="T3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -1835,7 +1711,7 @@
         <v>3000000</v>
       </c>
       <c r="H4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I4">
         <v>2000</v>
@@ -1844,48 +1720,48 @@
         <v>2000</v>
       </c>
       <c r="K4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L4">
         <v>2000</v>
       </c>
       <c r="M4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="R4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="S4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="T4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
@@ -1897,7 +1773,7 @@
         <v>1600000</v>
       </c>
       <c r="H5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I5">
         <v>11000</v>
@@ -1906,48 +1782,48 @@
         <v>15000</v>
       </c>
       <c r="K5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L5">
         <v>20000</v>
       </c>
       <c r="M5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="R5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="S5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="T5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
@@ -1959,7 +1835,7 @@
         <v>2000000</v>
       </c>
       <c r="H6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I6">
         <v>20000</v>
@@ -1968,34 +1844,34 @@
         <v>25000</v>
       </c>
       <c r="K6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L6">
         <v>30000</v>
       </c>
       <c r="M6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="R6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="S6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="T6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -2003,10 +1879,10 @@
         <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
         <v>23</v>
@@ -2021,7 +1897,7 @@
         <v>990000</v>
       </c>
       <c r="H7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I7">
         <v>13000</v>
@@ -2030,45 +1906,45 @@
         <v>15000</v>
       </c>
       <c r="K7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L7">
         <v>20000</v>
       </c>
       <c r="M7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="R7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="S7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="T7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D8" t="s">
         <v>25</v>
@@ -2083,7 +1959,7 @@
         <v>2104000</v>
       </c>
       <c r="H8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I8">
         <v>9000</v>
@@ -2092,48 +1968,48 @@
         <v>11000</v>
       </c>
       <c r="K8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L8">
         <v>13500</v>
       </c>
       <c r="M8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="R8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="S8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="T8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
@@ -2145,7 +2021,7 @@
         <v>5000000</v>
       </c>
       <c r="H9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I9">
         <v>2000</v>
@@ -2154,45 +2030,45 @@
         <v>2000</v>
       </c>
       <c r="K9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L9">
         <v>2000</v>
       </c>
       <c r="M9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="R9" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="S9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="T9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
         <v>27</v>
@@ -2207,7 +2083,7 @@
         <v>6500000</v>
       </c>
       <c r="H10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I10">
         <v>2000</v>
@@ -2216,45 +2092,45 @@
         <v>2000</v>
       </c>
       <c r="K10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L10">
         <v>2000</v>
       </c>
       <c r="M10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="R10" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="S10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="T10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
         <v>27</v>
@@ -2269,7 +2145,7 @@
         <v>4000000</v>
       </c>
       <c r="H11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I11">
         <v>2000</v>
@@ -2278,48 +2154,48 @@
         <v>2000</v>
       </c>
       <c r="K11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L11">
         <v>2000</v>
       </c>
       <c r="M11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="R11" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="S11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="T11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
         <v>24</v>
@@ -2331,7 +2207,7 @@
         <v>4000000</v>
       </c>
       <c r="H12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I12">
         <v>2000</v>
@@ -2340,48 +2216,48 @@
         <v>2000</v>
       </c>
       <c r="K12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L12">
         <v>2000</v>
       </c>
       <c r="M12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="R12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="S12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="T12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E13" t="s">
         <v>25</v>
@@ -2393,7 +2269,7 @@
         <v>4000000</v>
       </c>
       <c r="H13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I13">
         <v>2000</v>
@@ -2402,48 +2278,48 @@
         <v>2000</v>
       </c>
       <c r="K13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L13">
         <v>2000</v>
       </c>
       <c r="M13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="R13" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="S13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="T13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E14" t="s">
         <v>27</v>
@@ -2455,7 +2331,7 @@
         <v>600000</v>
       </c>
       <c r="H14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I14">
         <v>12000</v>
@@ -2464,96 +2340,34 @@
         <v>14000</v>
       </c>
       <c r="K14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L14">
         <v>16000</v>
       </c>
       <c r="M14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="R14" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="S14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="T14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20">
-      <c r="A15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15">
-        <v>94750000</v>
-      </c>
-      <c r="G15">
-        <v>379000</v>
-      </c>
-      <c r="H15" t="s">
-        <v>56</v>
-      </c>
-      <c r="I15">
-        <v>147000</v>
-      </c>
-      <c r="J15">
-        <v>200000</v>
-      </c>
-      <c r="K15" t="s">
-        <v>56</v>
-      </c>
-      <c r="L15">
-        <v>250000</v>
-      </c>
-      <c r="M15" t="s">
-        <v>56</v>
-      </c>
-      <c r="N15" t="s">
-        <v>56</v>
-      </c>
-      <c r="O15">
-        <v>18.46965699208443</v>
-      </c>
-      <c r="P15" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>56</v>
-      </c>
-      <c r="R15" t="s">
-        <v>106</v>
-      </c>
-      <c r="S15" t="s">
-        <v>56</v>
-      </c>
-      <c r="T15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -2563,7 +2377,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2571,16 +2385,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -2592,10 +2406,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -2604,27 +2418,27 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G2" t="s">
         <v>24</v>
@@ -2647,19 +2461,19 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F3" t="s">
         <v>25</v>
@@ -2685,22 +2499,22 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G4" t="s">
         <v>20</v>
@@ -2723,19 +2537,19 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
         <v>23</v>
@@ -2761,19 +2575,19 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F6" t="s">
         <v>25</v>
@@ -2799,19 +2613,19 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F7" t="s">
         <v>27</v>
@@ -2837,22 +2651,22 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F8" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G8" t="s">
         <v>18</v>
@@ -2875,22 +2689,22 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F9" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G9" t="s">
         <v>17</v>
@@ -2913,40 +2727,40 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E10" t="s">
-        <v>110</v>
+        <v>48</v>
       </c>
       <c r="F10" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="G10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H10">
-        <v>75800</v>
+        <v>13000</v>
       </c>
       <c r="I10">
-        <v>379000</v>
+        <v>6500000</v>
       </c>
       <c r="J10">
-        <v>250000</v>
+        <v>2000</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -2954,10 +2768,10 @@
         <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
         <v>51</v>
@@ -2966,16 +2780,16 @@
         <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="G11" t="s">
         <v>25</v>
       </c>
       <c r="H11">
-        <v>13000</v>
+        <v>8000</v>
       </c>
       <c r="I11">
-        <v>6500000</v>
+        <v>4000000</v>
       </c>
       <c r="J11">
         <v>2000</v>
@@ -2989,34 +2803,34 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C12" t="s">
         <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F12" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="G12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H12">
-        <v>8000</v>
+        <v>9600</v>
       </c>
       <c r="I12">
-        <v>4000000</v>
+        <v>600000</v>
       </c>
       <c r="J12">
-        <v>2000</v>
+        <v>16000</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -3027,34 +2841,34 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="E13" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F13" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="G13" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H13">
-        <v>9600</v>
+        <v>6000</v>
       </c>
       <c r="I13">
-        <v>600000</v>
+        <v>3000000</v>
       </c>
       <c r="J13">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -3065,31 +2879,31 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
         <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="G14" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="H14">
-        <v>6000</v>
+        <v>10000</v>
       </c>
       <c r="I14">
-        <v>3000000</v>
+        <v>5000000</v>
       </c>
       <c r="J14">
         <v>2000</v>
@@ -3103,115 +2917,39 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F15" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="G15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H15">
-        <v>10000</v>
+        <v>60000</v>
       </c>
       <c r="I15">
-        <v>5000000</v>
+        <v>2000000</v>
       </c>
       <c r="J15">
-        <v>2000</v>
+        <v>30000</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" t="s">
-        <v>110</v>
-      </c>
-      <c r="F16" t="s">
-        <v>67</v>
-      </c>
-      <c r="G16" t="s">
-        <v>28</v>
-      </c>
-      <c r="H16">
-        <v>18950</v>
-      </c>
-      <c r="I16">
-        <v>379000</v>
-      </c>
-      <c r="J16">
-        <v>250000</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" t="s">
-        <v>73</v>
-      </c>
-      <c r="G17" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17">
-        <v>60000</v>
-      </c>
-      <c r="I17">
-        <v>2000000</v>
-      </c>
-      <c r="J17">
-        <v>30000</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2024-04-22
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="100">
   <si>
     <t>상장일</t>
   </si>
@@ -99,138 +99,126 @@
     <t>2024-03-04</t>
   </si>
   <si>
+    <t>신한제12호스팩</t>
+  </si>
+  <si>
+    <t>아이엠비디엑스</t>
+  </si>
+  <si>
+    <t>하나32호스팩</t>
+  </si>
+  <si>
+    <t>엔젤로보틱스</t>
+  </si>
+  <si>
+    <t>삼현</t>
+  </si>
+  <si>
+    <t>오상헬스케어</t>
+  </si>
+  <si>
+    <t>케이엔알시스템</t>
+  </si>
+  <si>
+    <t>하나31호스팩</t>
+  </si>
+  <si>
+    <t>유안타제15호스팩</t>
+  </si>
+  <si>
+    <t>SK증권제11호스팩</t>
+  </si>
+  <si>
+    <t>비엔케이제2호스팩</t>
+  </si>
+  <si>
+    <t>유진스팩10호</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>신한</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>한국</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>유안타</t>
+  </si>
+  <si>
+    <t>SK</t>
+  </si>
+  <si>
+    <t>BNK</t>
+  </si>
+  <si>
+    <t>유진</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>2024-04-02</t>
+  </si>
+  <si>
+    <t>2024-03-25</t>
+  </si>
+  <si>
+    <t>2024-03-18</t>
+  </si>
+  <si>
+    <t>2024-03-14</t>
+  </si>
+  <si>
+    <t>2024-03-12</t>
+  </si>
+  <si>
+    <t>2024-02-26</t>
+  </si>
+  <si>
+    <t>2024-02-22</t>
+  </si>
+  <si>
+    <t>2024-02-20</t>
+  </si>
+  <si>
+    <t>2024-02-19</t>
+  </si>
+  <si>
+    <t>2024-04-05</t>
+  </si>
+  <si>
+    <t>2024-03-28</t>
+  </si>
+  <si>
+    <t>2024-03-19</t>
+  </si>
+  <si>
+    <t>2024-03-15</t>
+  </si>
+  <si>
+    <t>2024-02-27</t>
+  </si>
+  <si>
     <t>2024-02-23</t>
   </si>
   <si>
-    <t>신한제12호스팩</t>
-  </si>
-  <si>
-    <t>아이엠비디엑스</t>
-  </si>
-  <si>
-    <t>하나32호스팩</t>
-  </si>
-  <si>
-    <t>엔젤로보틱스</t>
-  </si>
-  <si>
-    <t>삼현</t>
-  </si>
-  <si>
-    <t>오상헬스케어</t>
-  </si>
-  <si>
-    <t>케이엔알시스템</t>
-  </si>
-  <si>
-    <t>하나31호스팩</t>
-  </si>
-  <si>
-    <t>유안타제15호스팩</t>
-  </si>
-  <si>
-    <t>SK증권제11호스팩</t>
-  </si>
-  <si>
-    <t>비엔케이제2호스팩</t>
-  </si>
-  <si>
-    <t>유진스팩10호</t>
-  </si>
-  <si>
-    <t>코셈</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>신한</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>한국</t>
-  </si>
-  <si>
-    <t>DB</t>
-  </si>
-  <si>
-    <t>유안타</t>
-  </si>
-  <si>
-    <t>SK</t>
-  </si>
-  <si>
-    <t>BNK</t>
-  </si>
-  <si>
-    <t>유진</t>
-  </si>
-  <si>
-    <t>키움</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>2024-04-02</t>
-  </si>
-  <si>
-    <t>2024-03-25</t>
-  </si>
-  <si>
-    <t>2024-03-18</t>
-  </si>
-  <si>
-    <t>2024-03-14</t>
-  </si>
-  <si>
-    <t>2024-03-12</t>
-  </si>
-  <si>
-    <t>2024-02-26</t>
-  </si>
-  <si>
-    <t>2024-02-22</t>
-  </si>
-  <si>
-    <t>2024-02-20</t>
-  </si>
-  <si>
-    <t>2024-02-19</t>
-  </si>
-  <si>
-    <t>2024-02-13</t>
-  </si>
-  <si>
-    <t>2024-04-05</t>
-  </si>
-  <si>
-    <t>2024-03-28</t>
-  </si>
-  <si>
-    <t>2024-03-19</t>
-  </si>
-  <si>
-    <t>2024-03-15</t>
-  </si>
-  <si>
-    <t>2024-02-27</t>
-  </si>
-  <si>
-    <t>2024-02-16</t>
-  </si>
-  <si>
     <t>회사명</t>
   </si>
   <si>
@@ -319,9 +307,6 @@
   </si>
   <si>
     <t>986.89 : 1</t>
-  </si>
-  <si>
-    <t>2518.4 : 1</t>
   </si>
   <si>
     <t>인수기관</t>
@@ -688,7 +673,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -752,37 +737,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D2">
         <v>100</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F2">
         <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M2">
         <v>2000</v>
@@ -791,10 +776,10 @@
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="P2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="Q2">
         <v>3750000</v>
@@ -805,37 +790,37 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D3">
         <v>325</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F3">
         <v>325</v>
       </c>
       <c r="G3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M3">
         <v>13000</v>
@@ -844,10 +829,10 @@
         <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="P3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="Q3">
         <v>1875000</v>
@@ -858,37 +843,37 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4">
         <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F4">
         <v>60</v>
       </c>
       <c r="G4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M4">
         <v>2000</v>
@@ -897,7 +882,7 @@
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="P4" t="s">
         <v>21</v>
@@ -911,37 +896,37 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D5">
         <v>320</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F5">
         <v>320</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M5">
         <v>20000</v>
@@ -950,10 +935,10 @@
         <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="P5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="Q5">
         <v>880000</v>
@@ -964,37 +949,37 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D6">
         <v>600</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F6">
         <v>600</v>
       </c>
       <c r="G6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M6">
         <v>30000</v>
@@ -1003,10 +988,10 @@
         <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="P6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="Q6">
         <v>1368000</v>
@@ -1017,37 +1002,37 @@
         <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D7">
         <v>198</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F7">
         <v>198</v>
       </c>
       <c r="G7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M7">
         <v>20000</v>
@@ -1070,37 +1055,37 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D8">
         <v>284.04</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F8">
         <v>142.02</v>
       </c>
       <c r="G8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M8">
         <v>13500</v>
@@ -1109,7 +1094,7 @@
         <v>50</v>
       </c>
       <c r="O8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="P8" t="s">
         <v>25</v>
@@ -1123,37 +1108,37 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D9">
         <v>284.04</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F9">
         <v>142.02</v>
       </c>
       <c r="G9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M9">
         <v>13500</v>
@@ -1162,7 +1147,7 @@
         <v>50</v>
       </c>
       <c r="O9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="P9" t="s">
         <v>25</v>
@@ -1176,37 +1161,37 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D10">
         <v>100</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F10">
         <v>100</v>
       </c>
       <c r="G10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M10">
         <v>2000</v>
@@ -1215,10 +1200,10 @@
         <v>100</v>
       </c>
       <c r="O10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="P10" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="Q10">
         <v>3750000</v>
@@ -1229,37 +1214,37 @@
         <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D11">
         <v>130</v>
       </c>
       <c r="E11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F11">
         <v>130</v>
       </c>
       <c r="G11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M11">
         <v>2000</v>
@@ -1268,10 +1253,10 @@
         <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="P11" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="Q11">
         <v>4875000</v>
@@ -1282,37 +1267,37 @@
         <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D12">
         <v>80</v>
       </c>
       <c r="E12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F12">
         <v>80</v>
       </c>
       <c r="G12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M12">
         <v>2000</v>
@@ -1321,10 +1306,10 @@
         <v>100</v>
       </c>
       <c r="O12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="P12" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="Q12">
         <v>3000000</v>
@@ -1335,37 +1320,37 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D13">
         <v>80</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F13">
         <v>80</v>
       </c>
       <c r="G13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M13">
         <v>2000</v>
@@ -1374,10 +1359,10 @@
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="P13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="Q13">
         <v>3000000</v>
@@ -1388,37 +1373,37 @@
         <v>25</v>
       </c>
       <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
         <v>39</v>
-      </c>
-      <c r="C14" t="s">
-        <v>41</v>
       </c>
       <c r="D14">
         <v>80</v>
       </c>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F14">
         <v>80</v>
       </c>
       <c r="G14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M14">
         <v>2000</v>
@@ -1427,66 +1412,13 @@
         <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="P14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="Q14">
         <v>3000000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
-      <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15">
-        <v>96</v>
-      </c>
-      <c r="E15" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15">
-        <v>96</v>
-      </c>
-      <c r="G15" t="s">
-        <v>53</v>
-      </c>
-      <c r="H15" t="s">
-        <v>53</v>
-      </c>
-      <c r="I15" t="s">
-        <v>53</v>
-      </c>
-      <c r="J15" t="s">
-        <v>53</v>
-      </c>
-      <c r="K15" t="s">
-        <v>54</v>
-      </c>
-      <c r="L15" t="s">
-        <v>53</v>
-      </c>
-      <c r="M15">
-        <v>16000</v>
-      </c>
-      <c r="N15">
-        <v>100</v>
-      </c>
-      <c r="O15" t="s">
-        <v>64</v>
-      </c>
-      <c r="P15" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q15">
-        <v>420000</v>
       </c>
     </row>
   </sheetData>
@@ -1496,7 +1428,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T14"/>
+  <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1507,10 +1439,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -1519,63 +1451,63 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
@@ -1587,7 +1519,7 @@
         <v>5000000</v>
       </c>
       <c r="H2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I2">
         <v>2000</v>
@@ -1596,48 +1528,48 @@
         <v>2000</v>
       </c>
       <c r="K2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L2">
         <v>2000</v>
       </c>
       <c r="M2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="N2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="Q2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="R2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="S2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="T2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
@@ -1649,7 +1581,7 @@
         <v>2500000</v>
       </c>
       <c r="H3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I3">
         <v>7700</v>
@@ -1658,45 +1590,45 @@
         <v>9900</v>
       </c>
       <c r="K3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L3">
         <v>13000</v>
       </c>
       <c r="M3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="N3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="Q3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="R3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="S3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="T3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -1711,7 +1643,7 @@
         <v>3000000</v>
       </c>
       <c r="H4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I4">
         <v>2000</v>
@@ -1720,48 +1652,48 @@
         <v>2000</v>
       </c>
       <c r="K4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L4">
         <v>2000</v>
       </c>
       <c r="M4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="N4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="Q4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="R4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="S4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="T4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
@@ -1773,7 +1705,7 @@
         <v>1600000</v>
       </c>
       <c r="H5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I5">
         <v>11000</v>
@@ -1782,48 +1714,48 @@
         <v>15000</v>
       </c>
       <c r="K5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L5">
         <v>20000</v>
       </c>
       <c r="M5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="N5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="Q5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="R5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="S5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="T5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
@@ -1835,7 +1767,7 @@
         <v>2000000</v>
       </c>
       <c r="H6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I6">
         <v>20000</v>
@@ -1844,34 +1776,34 @@
         <v>25000</v>
       </c>
       <c r="K6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L6">
         <v>30000</v>
       </c>
       <c r="M6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="N6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="Q6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="R6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="S6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="T6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -1879,10 +1811,10 @@
         <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
         <v>23</v>
@@ -1897,7 +1829,7 @@
         <v>990000</v>
       </c>
       <c r="H7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I7">
         <v>13000</v>
@@ -1906,45 +1838,45 @@
         <v>15000</v>
       </c>
       <c r="K7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L7">
         <v>20000</v>
       </c>
       <c r="M7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="N7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="Q7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="R7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="S7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="T7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D8" t="s">
         <v>25</v>
@@ -1959,7 +1891,7 @@
         <v>2104000</v>
       </c>
       <c r="H8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I8">
         <v>9000</v>
@@ -1968,48 +1900,48 @@
         <v>11000</v>
       </c>
       <c r="K8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L8">
         <v>13500</v>
       </c>
       <c r="M8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="N8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="Q8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="R8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="S8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="T8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
@@ -2021,7 +1953,7 @@
         <v>5000000</v>
       </c>
       <c r="H9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I9">
         <v>2000</v>
@@ -2030,48 +1962,48 @@
         <v>2000</v>
       </c>
       <c r="K9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L9">
         <v>2000</v>
       </c>
       <c r="M9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="N9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="Q9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="R9" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="S9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="T9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="E10" t="s">
         <v>25</v>
@@ -2083,7 +2015,7 @@
         <v>6500000</v>
       </c>
       <c r="H10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I10">
         <v>2000</v>
@@ -2092,48 +2024,48 @@
         <v>2000</v>
       </c>
       <c r="K10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L10">
         <v>2000</v>
       </c>
       <c r="M10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="N10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="Q10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="R10" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="S10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="T10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="E11" t="s">
         <v>26</v>
@@ -2145,7 +2077,7 @@
         <v>4000000</v>
       </c>
       <c r="H11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I11">
         <v>2000</v>
@@ -2154,48 +2086,48 @@
         <v>2000</v>
       </c>
       <c r="K11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L11">
         <v>2000</v>
       </c>
       <c r="M11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="N11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="Q11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="R11" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="S11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="T11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E12" t="s">
         <v>24</v>
@@ -2207,7 +2139,7 @@
         <v>4000000</v>
       </c>
       <c r="H12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I12">
         <v>2000</v>
@@ -2216,48 +2148,48 @@
         <v>2000</v>
       </c>
       <c r="K12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L12">
         <v>2000</v>
       </c>
       <c r="M12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="N12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="Q12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="R12" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="S12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="T12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E13" t="s">
         <v>25</v>
@@ -2269,7 +2201,7 @@
         <v>4000000</v>
       </c>
       <c r="H13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I13">
         <v>2000</v>
@@ -2278,96 +2210,34 @@
         <v>2000</v>
       </c>
       <c r="K13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L13">
         <v>2000</v>
       </c>
       <c r="M13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="N13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="Q13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="R13" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="S13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="T13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20">
-      <c r="A14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14">
-        <v>9600000</v>
-      </c>
-      <c r="G14">
-        <v>600000</v>
-      </c>
-      <c r="H14" t="s">
-        <v>53</v>
-      </c>
-      <c r="I14">
-        <v>12000</v>
-      </c>
-      <c r="J14">
-        <v>14000</v>
-      </c>
-      <c r="K14" t="s">
-        <v>53</v>
-      </c>
-      <c r="L14">
-        <v>16000</v>
-      </c>
-      <c r="M14" t="s">
-        <v>53</v>
-      </c>
-      <c r="N14" t="s">
-        <v>53</v>
-      </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>53</v>
-      </c>
-      <c r="R14" t="s">
-        <v>101</v>
-      </c>
-      <c r="S14" t="s">
-        <v>53</v>
-      </c>
-      <c r="T14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2377,7 +2247,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2385,16 +2255,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -2406,10 +2276,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -2418,27 +2288,27 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G2" t="s">
         <v>24</v>
@@ -2461,19 +2331,19 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F3" t="s">
         <v>25</v>
@@ -2499,22 +2369,22 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G4" t="s">
         <v>20</v>
@@ -2537,19 +2407,19 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
         <v>23</v>
@@ -2575,19 +2445,19 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F6" t="s">
         <v>25</v>
@@ -2613,22 +2483,22 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="G7" t="s">
         <v>26</v>
@@ -2651,22 +2521,22 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G8" t="s">
         <v>18</v>
@@ -2689,22 +2559,22 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F9" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G9" t="s">
         <v>17</v>
@@ -2727,22 +2597,22 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="G10" t="s">
         <v>25</v>
@@ -2765,22 +2635,22 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G11" t="s">
         <v>25</v>
@@ -2803,34 +2673,34 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>70</v>
+        <v>21</v>
       </c>
       <c r="G12" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H12">
-        <v>9600</v>
+        <v>6000</v>
       </c>
       <c r="I12">
-        <v>600000</v>
+        <v>3000000</v>
       </c>
       <c r="J12">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -2841,31 +2711,31 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F13" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="G13" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="H13">
-        <v>6000</v>
+        <v>10000</v>
       </c>
       <c r="I13">
-        <v>3000000</v>
+        <v>5000000</v>
       </c>
       <c r="J13">
         <v>2000</v>
@@ -2882,10 +2752,10 @@
         <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
         <v>44</v>
@@ -2894,62 +2764,24 @@
         <v>44</v>
       </c>
       <c r="F14" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H14">
-        <v>10000</v>
+        <v>60000</v>
       </c>
       <c r="I14">
-        <v>5000000</v>
+        <v>2000000</v>
       </c>
       <c r="J14">
-        <v>2000</v>
+        <v>30000</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" t="s">
-        <v>68</v>
-      </c>
-      <c r="G15" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15">
-        <v>60000</v>
-      </c>
-      <c r="I15">
-        <v>2000000</v>
-      </c>
-      <c r="J15">
-        <v>30000</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2024-04-23
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="97">
   <si>
     <t>상장일</t>
   </si>
@@ -69,6 +69,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2024-04-22</t>
+  </si>
+  <si>
     <t>2024-04-15</t>
   </si>
   <si>
@@ -99,6 +102,9 @@
     <t>2024-03-04</t>
   </si>
   <si>
+    <t>신한제13호스팩</t>
+  </si>
+  <si>
     <t>신한제12호스팩</t>
   </si>
   <si>
@@ -129,12 +135,6 @@
     <t>SK증권제11호스팩</t>
   </si>
   <si>
-    <t>비엔케이제2호스팩</t>
-  </si>
-  <si>
-    <t>유진스팩10호</t>
-  </si>
-  <si>
     <t>코스닥</t>
   </si>
   <si>
@@ -162,18 +162,15 @@
     <t>SK</t>
   </si>
   <si>
-    <t>BNK</t>
-  </si>
-  <si>
-    <t>유진</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
     <t>대표</t>
   </si>
   <si>
+    <t>2024-04-11</t>
+  </si>
+  <si>
     <t>2024-04-02</t>
   </si>
   <si>
@@ -198,9 +195,6 @@
     <t>2024-02-20</t>
   </si>
   <si>
-    <t>2024-02-19</t>
-  </si>
-  <si>
     <t>2024-04-05</t>
   </si>
   <si>
@@ -273,6 +267,9 @@
     <t>DB, NH</t>
   </si>
   <si>
+    <t>1337.88 : 1</t>
+  </si>
+  <si>
     <t>1698.24 : 1</t>
   </si>
   <si>
@@ -301,12 +298,6 @@
   </si>
   <si>
     <t>1245.3 : 1</t>
-  </si>
-  <si>
-    <t>327.3249 : 1</t>
-  </si>
-  <si>
-    <t>986.89 : 1</t>
   </si>
   <si>
     <t>인수기관</t>
@@ -673,7 +664,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -737,37 +728,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
         <v>40</v>
       </c>
       <c r="F2">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M2">
         <v>2000</v>
@@ -776,13 +767,13 @@
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P2" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="Q2">
-        <v>3750000</v>
+        <v>2250000</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -790,52 +781,52 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
         <v>39</v>
       </c>
       <c r="D3">
-        <v>325</v>
+        <v>100</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F3">
-        <v>325</v>
+        <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M3">
-        <v>13000</v>
+        <v>2000</v>
       </c>
       <c r="N3">
         <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="Q3">
-        <v>1875000</v>
+        <v>3750000</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -843,52 +834,52 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
         <v>39</v>
       </c>
       <c r="D4">
-        <v>60</v>
+        <v>325</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F4">
-        <v>60</v>
+        <v>325</v>
       </c>
       <c r="G4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M4">
-        <v>2000</v>
+        <v>13000</v>
       </c>
       <c r="N4">
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="P4" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="Q4">
-        <v>2250000</v>
+        <v>1875000</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -896,52 +887,52 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
         <v>39</v>
       </c>
       <c r="D5">
-        <v>320</v>
+        <v>60</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5">
-        <v>320</v>
+        <v>60</v>
       </c>
       <c r="G5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M5">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="N5">
         <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P5" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="Q5">
-        <v>880000</v>
+        <v>2250000</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -949,52 +940,52 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
         <v>39</v>
       </c>
       <c r="D6">
-        <v>600</v>
+        <v>320</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F6">
-        <v>600</v>
+        <v>320</v>
       </c>
       <c r="G6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M6">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="N6">
         <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="P6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="Q6">
-        <v>1368000</v>
+        <v>880000</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1002,52 +993,52 @@
         <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
         <v>39</v>
       </c>
       <c r="D7">
-        <v>198</v>
+        <v>600</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F7">
-        <v>198</v>
+        <v>600</v>
       </c>
       <c r="G7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M7">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="N7">
         <v>100</v>
       </c>
       <c r="O7" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="P7" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="Q7">
-        <v>742500</v>
+        <v>1368000</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1055,60 +1046,60 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
         <v>39</v>
       </c>
       <c r="D8">
-        <v>284.04</v>
+        <v>198</v>
       </c>
       <c r="E8" t="s">
         <v>43</v>
       </c>
       <c r="F8">
-        <v>142.02</v>
+        <v>198</v>
       </c>
       <c r="G8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M8">
-        <v>13500</v>
+        <v>20000</v>
       </c>
       <c r="N8">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="P8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q8">
-        <v>2916000</v>
+        <v>742500</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
         <v>39</v>
@@ -1117,28 +1108,28 @@
         <v>284.04</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F9">
         <v>142.02</v>
       </c>
       <c r="G9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M9">
         <v>13500</v>
@@ -1147,10 +1138,10 @@
         <v>50</v>
       </c>
       <c r="O9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="Q9">
         <v>2916000</v>
@@ -1161,52 +1152,52 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
         <v>39</v>
       </c>
       <c r="D10">
-        <v>100</v>
+        <v>284.04</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F10">
-        <v>100</v>
+        <v>142.02</v>
       </c>
       <c r="G10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" t="s">
+        <v>48</v>
+      </c>
+      <c r="J10" t="s">
+        <v>48</v>
+      </c>
+      <c r="K10" t="s">
+        <v>48</v>
+      </c>
+      <c r="L10" t="s">
+        <v>48</v>
+      </c>
+      <c r="M10">
+        <v>13500</v>
+      </c>
+      <c r="N10">
         <v>50</v>
       </c>
-      <c r="H10" t="s">
-        <v>50</v>
-      </c>
-      <c r="I10" t="s">
-        <v>50</v>
-      </c>
-      <c r="J10" t="s">
-        <v>50</v>
-      </c>
-      <c r="K10" t="s">
-        <v>51</v>
-      </c>
-      <c r="L10" t="s">
-        <v>50</v>
-      </c>
-      <c r="M10">
-        <v>2000</v>
-      </c>
-      <c r="N10">
-        <v>100</v>
-      </c>
       <c r="O10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="P10" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="Q10">
-        <v>3750000</v>
+        <v>2916000</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1214,37 +1205,37 @@
         <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
         <v>39</v>
       </c>
       <c r="D11">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F11">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="G11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M11">
         <v>2000</v>
@@ -1253,13 +1244,13 @@
         <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="P11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q11">
-        <v>4875000</v>
+        <v>3750000</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1267,37 +1258,37 @@
         <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
         <v>39</v>
       </c>
       <c r="D12">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F12">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="G12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M12">
         <v>2000</v>
@@ -1306,21 +1297,21 @@
         <v>100</v>
       </c>
       <c r="O12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q12">
-        <v>3000000</v>
+        <v>4875000</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
         <v>39</v>
@@ -1329,28 +1320,28 @@
         <v>80</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F13">
         <v>80</v>
       </c>
       <c r="G13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M13">
         <v>2000</v>
@@ -1359,65 +1350,12 @@
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="P13" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="Q13">
-        <v>3000000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14">
-        <v>80</v>
-      </c>
-      <c r="E14" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14">
-        <v>80</v>
-      </c>
-      <c r="G14" t="s">
-        <v>50</v>
-      </c>
-      <c r="H14" t="s">
-        <v>50</v>
-      </c>
-      <c r="I14" t="s">
-        <v>50</v>
-      </c>
-      <c r="J14" t="s">
-        <v>50</v>
-      </c>
-      <c r="K14" t="s">
-        <v>51</v>
-      </c>
-      <c r="L14" t="s">
-        <v>50</v>
-      </c>
-      <c r="M14">
-        <v>2000</v>
-      </c>
-      <c r="N14">
-        <v>100</v>
-      </c>
-      <c r="O14" t="s">
-        <v>60</v>
-      </c>
-      <c r="P14" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q14">
         <v>3000000</v>
       </c>
     </row>
@@ -1428,7 +1366,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T13"/>
+  <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1439,10 +1377,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -1451,75 +1389,75 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
         <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
       </c>
       <c r="F2">
-        <v>10000000</v>
+        <v>6000000</v>
       </c>
       <c r="G2">
-        <v>5000000</v>
+        <v>3000000</v>
       </c>
       <c r="H2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I2">
         <v>2000</v>
@@ -1528,494 +1466,494 @@
         <v>2000</v>
       </c>
       <c r="K2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L2">
         <v>2000</v>
       </c>
       <c r="M2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Q2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="R2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="S2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="T2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
       </c>
       <c r="F3">
-        <v>32500000</v>
+        <v>10000000</v>
       </c>
       <c r="G3">
-        <v>2500000</v>
+        <v>5000000</v>
       </c>
       <c r="H3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I3">
-        <v>7700</v>
+        <v>2000</v>
       </c>
       <c r="J3">
-        <v>9900</v>
+        <v>2000</v>
       </c>
       <c r="K3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L3">
-        <v>13000</v>
+        <v>2000</v>
       </c>
       <c r="M3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Q3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="R3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="S3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="T3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
       </c>
       <c r="F4">
-        <v>6000000</v>
+        <v>32500000</v>
       </c>
       <c r="G4">
-        <v>3000000</v>
+        <v>2500000</v>
       </c>
       <c r="H4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I4">
-        <v>2000</v>
+        <v>7700</v>
       </c>
       <c r="J4">
-        <v>2000</v>
+        <v>9900</v>
       </c>
       <c r="K4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L4">
-        <v>2000</v>
+        <v>13000</v>
       </c>
       <c r="M4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Q4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="R4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="S4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="T4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
       </c>
       <c r="F5">
-        <v>32000000</v>
+        <v>6000000</v>
       </c>
       <c r="G5">
-        <v>1600000</v>
+        <v>3000000</v>
       </c>
       <c r="H5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I5">
-        <v>11000</v>
+        <v>2000</v>
       </c>
       <c r="J5">
-        <v>15000</v>
+        <v>2000</v>
       </c>
       <c r="K5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L5">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="M5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Q5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="R5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="S5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="T5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
       </c>
       <c r="F6">
-        <v>60000000</v>
+        <v>32000000</v>
       </c>
       <c r="G6">
-        <v>2000000</v>
+        <v>1600000</v>
       </c>
       <c r="H6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I6">
+        <v>11000</v>
+      </c>
+      <c r="J6">
+        <v>15000</v>
+      </c>
+      <c r="K6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6">
         <v>20000</v>
       </c>
-      <c r="J6">
-        <v>25000</v>
-      </c>
-      <c r="K6" t="s">
-        <v>50</v>
-      </c>
-      <c r="L6">
-        <v>30000</v>
-      </c>
       <c r="M6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Q6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="R6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="T6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="E7" t="s">
         <v>22</v>
       </c>
       <c r="F7">
-        <v>19800000</v>
+        <v>60000000</v>
       </c>
       <c r="G7">
-        <v>990000</v>
+        <v>2000000</v>
       </c>
       <c r="H7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I7">
-        <v>13000</v>
+        <v>20000</v>
       </c>
       <c r="J7">
-        <v>15000</v>
+        <v>25000</v>
       </c>
       <c r="K7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L7">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="M7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Q7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="R7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="S7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="T7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
         <v>23</v>
       </c>
       <c r="F8">
-        <v>28404000</v>
+        <v>19800000</v>
       </c>
       <c r="G8">
-        <v>2104000</v>
+        <v>990000</v>
       </c>
       <c r="H8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I8">
-        <v>9000</v>
+        <v>13000</v>
       </c>
       <c r="J8">
-        <v>11000</v>
+        <v>15000</v>
       </c>
       <c r="K8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L8">
-        <v>13500</v>
+        <v>20000</v>
       </c>
       <c r="M8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Q8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="R8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="S8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="T8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
       </c>
       <c r="F9">
-        <v>10000000</v>
+        <v>28404000</v>
       </c>
       <c r="G9">
-        <v>5000000</v>
+        <v>2104000</v>
       </c>
       <c r="H9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I9">
-        <v>2000</v>
+        <v>9000</v>
       </c>
       <c r="J9">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="K9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L9">
-        <v>2000</v>
+        <v>13500</v>
       </c>
       <c r="M9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Q9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="R9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="S9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="T9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E10" t="s">
         <v>25</v>
       </c>
       <c r="F10">
-        <v>13000000</v>
+        <v>10000000</v>
       </c>
       <c r="G10">
-        <v>6500000</v>
+        <v>5000000</v>
       </c>
       <c r="H10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I10">
         <v>2000</v>
@@ -2024,60 +1962,60 @@
         <v>2000</v>
       </c>
       <c r="K10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L10">
         <v>2000</v>
       </c>
       <c r="M10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Q10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="R10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="S10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="T10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E11" t="s">
         <v>26</v>
       </c>
       <c r="F11">
-        <v>8000000</v>
+        <v>13000000</v>
       </c>
       <c r="G11">
-        <v>4000000</v>
+        <v>6500000</v>
       </c>
       <c r="H11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I11">
         <v>2000</v>
@@ -2086,51 +2024,51 @@
         <v>2000</v>
       </c>
       <c r="K11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L11">
         <v>2000</v>
       </c>
       <c r="M11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Q11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="R11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="S11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="T11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E12" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F12">
         <v>8000000</v>
@@ -2139,7 +2077,7 @@
         <v>4000000</v>
       </c>
       <c r="H12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I12">
         <v>2000</v>
@@ -2148,96 +2086,34 @@
         <v>2000</v>
       </c>
       <c r="K12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L12">
         <v>2000</v>
       </c>
       <c r="M12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Q12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="R12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="S12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="T12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20">
-      <c r="A13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13">
-        <v>8000000</v>
-      </c>
-      <c r="G13">
-        <v>4000000</v>
-      </c>
-      <c r="H13" t="s">
-        <v>50</v>
-      </c>
-      <c r="I13">
-        <v>2000</v>
-      </c>
-      <c r="J13">
-        <v>2000</v>
-      </c>
-      <c r="K13" t="s">
-        <v>50</v>
-      </c>
-      <c r="L13">
-        <v>2000</v>
-      </c>
-      <c r="M13" t="s">
-        <v>50</v>
-      </c>
-      <c r="N13" t="s">
-        <v>50</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>50</v>
-      </c>
-      <c r="R13" t="s">
-        <v>96</v>
-      </c>
-      <c r="S13" t="s">
-        <v>50</v>
-      </c>
-      <c r="T13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2247,7 +2123,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2255,16 +2131,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -2276,10 +2152,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -2288,83 +2164,83 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="G2" t="s">
         <v>24</v>
       </c>
       <c r="H2">
-        <v>8000</v>
+        <v>14202</v>
       </c>
       <c r="I2">
-        <v>4000000</v>
+        <v>2104000</v>
       </c>
       <c r="J2">
-        <v>2000</v>
+        <v>13500</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
       <c r="L2">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
-        <v>84</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H3">
-        <v>14202</v>
+        <v>32000</v>
       </c>
       <c r="I3">
-        <v>2104000</v>
+        <v>1600000</v>
       </c>
       <c r="J3">
-        <v>13500</v>
+        <v>20000</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -2372,10 +2248,10 @@
         <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
         <v>43</v>
@@ -2384,16 +2260,16 @@
         <v>43</v>
       </c>
       <c r="F4" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H4">
-        <v>32000</v>
+        <v>19800</v>
       </c>
       <c r="I4">
-        <v>1600000</v>
+        <v>990000</v>
       </c>
       <c r="J4">
         <v>20000</v>
@@ -2410,107 +2286,107 @@
         <v>43</v>
       </c>
       <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" t="s">
-        <v>23</v>
-      </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H5">
-        <v>19800</v>
+        <v>14202</v>
       </c>
       <c r="I5">
-        <v>990000</v>
+        <v>2104000</v>
       </c>
       <c r="J5">
-        <v>20000</v>
+        <v>13500</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="G6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H6">
-        <v>14202</v>
+        <v>8000</v>
       </c>
       <c r="I6">
-        <v>2104000</v>
+        <v>4000000</v>
       </c>
       <c r="J6">
-        <v>13500</v>
+        <v>2000</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H7">
-        <v>8000</v>
+        <v>32500</v>
       </c>
       <c r="I7">
-        <v>4000000</v>
+        <v>2500000</v>
       </c>
       <c r="J7">
-        <v>2000</v>
+        <v>13000</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -2521,34 +2397,34 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
         <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F8" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H8">
-        <v>32500</v>
+        <v>6000</v>
       </c>
       <c r="I8">
-        <v>2500000</v>
+        <v>3000000</v>
       </c>
       <c r="J8">
-        <v>13000</v>
+        <v>2000</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -2562,10 +2438,10 @@
         <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
         <v>40</v>
@@ -2574,10 +2450,10 @@
         <v>40</v>
       </c>
       <c r="F9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H9">
         <v>10000</v>
@@ -2600,10 +2476,10 @@
         <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
         <v>46</v>
@@ -2612,10 +2488,10 @@
         <v>46</v>
       </c>
       <c r="F10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H10">
         <v>13000</v>
@@ -2635,31 +2511,31 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F11" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H11">
-        <v>8000</v>
+        <v>6000</v>
       </c>
       <c r="I11">
-        <v>4000000</v>
+        <v>3000000</v>
       </c>
       <c r="J11">
         <v>2000</v>
@@ -2676,10 +2552,10 @@
         <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
         <v>42</v>
@@ -2688,16 +2564,16 @@
         <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="G12" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H12">
-        <v>6000</v>
+        <v>10000</v>
       </c>
       <c r="I12">
-        <v>3000000</v>
+        <v>5000000</v>
       </c>
       <c r="J12">
         <v>2000</v>
@@ -2711,77 +2587,39 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H13">
-        <v>10000</v>
+        <v>60000</v>
       </c>
       <c r="I13">
-        <v>5000000</v>
+        <v>2000000</v>
       </c>
       <c r="J13">
-        <v>2000</v>
+        <v>30000</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="L13">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" t="s">
-        <v>64</v>
-      </c>
-      <c r="G14" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14">
-        <v>60000</v>
-      </c>
-      <c r="I14">
-        <v>2000000</v>
-      </c>
-      <c r="J14">
-        <v>30000</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2024-04-24
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="89">
   <si>
     <t>상장일</t>
   </si>
@@ -96,123 +96,105 @@
     <t>2024-03-05</t>
   </si>
   <si>
+    <t>신한제13호스팩</t>
+  </si>
+  <si>
+    <t>신한제12호스팩</t>
+  </si>
+  <si>
+    <t>아이엠비디엑스</t>
+  </si>
+  <si>
+    <t>하나32호스팩</t>
+  </si>
+  <si>
+    <t>엔젤로보틱스</t>
+  </si>
+  <si>
+    <t>삼현</t>
+  </si>
+  <si>
+    <t>오상헬스케어</t>
+  </si>
+  <si>
+    <t>케이엔알시스템</t>
+  </si>
+  <si>
+    <t>하나31호스팩</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>신한</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>한국</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>2024-04-11</t>
+  </si>
+  <si>
+    <t>2024-04-02</t>
+  </si>
+  <si>
+    <t>2024-03-25</t>
+  </si>
+  <si>
+    <t>2024-03-18</t>
+  </si>
+  <si>
+    <t>2024-03-14</t>
+  </si>
+  <si>
+    <t>2024-03-12</t>
+  </si>
+  <si>
+    <t>2024-03-04</t>
+  </si>
+  <si>
+    <t>2024-02-26</t>
+  </si>
+  <si>
+    <t>2024-02-22</t>
+  </si>
+  <si>
+    <t>2024-04-05</t>
+  </si>
+  <si>
+    <t>2024-03-28</t>
+  </si>
+  <si>
+    <t>2024-03-19</t>
+  </si>
+  <si>
+    <t>2024-03-15</t>
+  </si>
+  <si>
     <t>2024-02-29</t>
   </si>
   <si>
-    <t>2024-03-04</t>
-  </si>
-  <si>
-    <t>신한제13호스팩</t>
-  </si>
-  <si>
-    <t>신한제12호스팩</t>
-  </si>
-  <si>
-    <t>아이엠비디엑스</t>
-  </si>
-  <si>
-    <t>하나32호스팩</t>
-  </si>
-  <si>
-    <t>엔젤로보틱스</t>
-  </si>
-  <si>
-    <t>삼현</t>
-  </si>
-  <si>
-    <t>오상헬스케어</t>
-  </si>
-  <si>
-    <t>케이엔알시스템</t>
-  </si>
-  <si>
-    <t>하나31호스팩</t>
-  </si>
-  <si>
-    <t>유안타제15호스팩</t>
-  </si>
-  <si>
-    <t>SK증권제11호스팩</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>신한</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>한국</t>
-  </si>
-  <si>
-    <t>DB</t>
-  </si>
-  <si>
-    <t>유안타</t>
-  </si>
-  <si>
-    <t>SK</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>2024-04-11</t>
-  </si>
-  <si>
-    <t>2024-04-02</t>
-  </si>
-  <si>
-    <t>2024-03-25</t>
-  </si>
-  <si>
-    <t>2024-03-18</t>
-  </si>
-  <si>
-    <t>2024-03-14</t>
-  </si>
-  <si>
-    <t>2024-03-12</t>
-  </si>
-  <si>
-    <t>2024-02-26</t>
-  </si>
-  <si>
-    <t>2024-02-22</t>
-  </si>
-  <si>
-    <t>2024-02-20</t>
-  </si>
-  <si>
-    <t>2024-04-05</t>
-  </si>
-  <si>
-    <t>2024-03-28</t>
-  </si>
-  <si>
-    <t>2024-03-19</t>
-  </si>
-  <si>
-    <t>2024-03-15</t>
-  </si>
-  <si>
     <t>2024-02-27</t>
   </si>
   <si>
-    <t>2024-02-23</t>
-  </si>
-  <si>
     <t>회사명</t>
   </si>
   <si>
@@ -292,12 +274,6 @@
   </si>
   <si>
     <t>1896.1033 : 1</t>
-  </si>
-  <si>
-    <t>288 : 1</t>
-  </si>
-  <si>
-    <t>1245.3 : 1</t>
   </si>
   <si>
     <t>인수기관</t>
@@ -664,7 +640,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -728,37 +704,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D2">
         <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F2">
         <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="J2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="K2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="M2">
         <v>2000</v>
@@ -767,7 +743,7 @@
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="P2" t="s">
         <v>18</v>
@@ -781,37 +757,37 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D3">
         <v>100</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F3">
         <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="J3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="K3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="M3">
         <v>2000</v>
@@ -820,10 +796,10 @@
         <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="P3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="Q3">
         <v>3750000</v>
@@ -834,37 +810,37 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D4">
         <v>325</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F4">
         <v>325</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="J4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="K4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="M4">
         <v>13000</v>
@@ -873,10 +849,10 @@
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="P4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="Q4">
         <v>1875000</v>
@@ -887,37 +863,37 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D5">
         <v>60</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F5">
         <v>60</v>
       </c>
       <c r="G5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="J5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="K5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="M5">
         <v>2000</v>
@@ -926,7 +902,7 @@
         <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="P5" t="s">
         <v>22</v>
@@ -940,37 +916,37 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D6">
         <v>320</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F6">
         <v>320</v>
       </c>
       <c r="G6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="J6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="K6" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="M6">
         <v>20000</v>
@@ -979,10 +955,10 @@
         <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="P6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="Q6">
         <v>880000</v>
@@ -993,37 +969,37 @@
         <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D7">
         <v>600</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F7">
         <v>600</v>
       </c>
       <c r="G7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="J7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="K7" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="M7">
         <v>30000</v>
@@ -1032,10 +1008,10 @@
         <v>100</v>
       </c>
       <c r="O7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="P7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="Q7">
         <v>1368000</v>
@@ -1046,37 +1022,37 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D8">
         <v>198</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F8">
         <v>198</v>
       </c>
       <c r="G8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="J8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="K8" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="M8">
         <v>20000</v>
@@ -1085,7 +1061,7 @@
         <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="P8" t="s">
         <v>24</v>
@@ -1099,37 +1075,37 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
         <v>35</v>
-      </c>
-      <c r="C9" t="s">
-        <v>39</v>
       </c>
       <c r="D9">
         <v>284.04</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F9">
         <v>142.02</v>
       </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="J9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="K9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="L9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="M9">
         <v>13500</v>
@@ -1138,10 +1114,10 @@
         <v>50</v>
       </c>
       <c r="O9" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="P9" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="Q9">
         <v>2916000</v>
@@ -1152,37 +1128,37 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
         <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>39</v>
       </c>
       <c r="D10">
         <v>284.04</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F10">
         <v>142.02</v>
       </c>
       <c r="G10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="J10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="K10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="L10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="M10">
         <v>13500</v>
@@ -1191,10 +1167,10 @@
         <v>50</v>
       </c>
       <c r="O10" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="P10" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="Q10">
         <v>2916000</v>
@@ -1205,37 +1181,37 @@
         <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D11">
         <v>100</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F11">
         <v>100</v>
       </c>
       <c r="G11" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H11" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I11" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="J11" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="K11" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L11" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="M11">
         <v>2000</v>
@@ -1244,119 +1220,13 @@
         <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="P11" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="Q11">
         <v>3750000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
-      <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12">
-        <v>130</v>
-      </c>
-      <c r="E12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12">
-        <v>130</v>
-      </c>
-      <c r="G12" t="s">
-        <v>48</v>
-      </c>
-      <c r="H12" t="s">
-        <v>48</v>
-      </c>
-      <c r="I12" t="s">
-        <v>48</v>
-      </c>
-      <c r="J12" t="s">
-        <v>48</v>
-      </c>
-      <c r="K12" t="s">
-        <v>49</v>
-      </c>
-      <c r="L12" t="s">
-        <v>48</v>
-      </c>
-      <c r="M12">
-        <v>2000</v>
-      </c>
-      <c r="N12">
-        <v>100</v>
-      </c>
-      <c r="O12" t="s">
-        <v>58</v>
-      </c>
-      <c r="P12" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q12">
-        <v>4875000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13">
-        <v>80</v>
-      </c>
-      <c r="E13" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13">
-        <v>80</v>
-      </c>
-      <c r="G13" t="s">
-        <v>48</v>
-      </c>
-      <c r="H13" t="s">
-        <v>48</v>
-      </c>
-      <c r="I13" t="s">
-        <v>48</v>
-      </c>
-      <c r="J13" t="s">
-        <v>48</v>
-      </c>
-      <c r="K13" t="s">
-        <v>49</v>
-      </c>
-      <c r="L13" t="s">
-        <v>48</v>
-      </c>
-      <c r="M13">
-        <v>2000</v>
-      </c>
-      <c r="N13">
-        <v>100</v>
-      </c>
-      <c r="O13" t="s">
-        <v>58</v>
-      </c>
-      <c r="P13" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q13">
-        <v>3000000</v>
       </c>
     </row>
   </sheetData>
@@ -1366,7 +1236,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1377,10 +1247,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -1389,60 +1259,60 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -1457,7 +1327,7 @@
         <v>3000000</v>
       </c>
       <c r="H2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I2">
         <v>2000</v>
@@ -1466,48 +1336,48 @@
         <v>2000</v>
       </c>
       <c r="K2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="L2">
         <v>2000</v>
       </c>
       <c r="M2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="N2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="Q2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="R2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="S2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="T2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
@@ -1519,7 +1389,7 @@
         <v>5000000</v>
       </c>
       <c r="H3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I3">
         <v>2000</v>
@@ -1528,48 +1398,48 @@
         <v>2000</v>
       </c>
       <c r="K3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="L3">
         <v>2000</v>
       </c>
       <c r="M3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="N3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="Q3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="R3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="S3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="T3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
@@ -1581,7 +1451,7 @@
         <v>2500000</v>
       </c>
       <c r="H4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I4">
         <v>7700</v>
@@ -1590,45 +1460,45 @@
         <v>9900</v>
       </c>
       <c r="K4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="L4">
         <v>13000</v>
       </c>
       <c r="M4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="N4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="Q4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="R4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="S4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="T4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
         <v>22</v>
@@ -1643,7 +1513,7 @@
         <v>3000000</v>
       </c>
       <c r="H5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I5">
         <v>2000</v>
@@ -1652,48 +1522,48 @@
         <v>2000</v>
       </c>
       <c r="K5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="L5">
         <v>2000</v>
       </c>
       <c r="M5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="N5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="Q5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="R5" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="S5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="T5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
@@ -1705,7 +1575,7 @@
         <v>1600000</v>
       </c>
       <c r="H6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I6">
         <v>11000</v>
@@ -1714,48 +1584,48 @@
         <v>15000</v>
       </c>
       <c r="K6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="L6">
         <v>20000</v>
       </c>
       <c r="M6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="N6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="Q6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="R6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="S6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="T6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s">
         <v>22</v>
@@ -1767,7 +1637,7 @@
         <v>2000000</v>
       </c>
       <c r="H7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I7">
         <v>20000</v>
@@ -1776,45 +1646,45 @@
         <v>25000</v>
       </c>
       <c r="K7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="L7">
         <v>30000</v>
       </c>
       <c r="M7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="N7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="Q7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="R7" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="S7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="T7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
         <v>24</v>
@@ -1829,7 +1699,7 @@
         <v>990000</v>
       </c>
       <c r="H8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I8">
         <v>13000</v>
@@ -1838,48 +1708,48 @@
         <v>15000</v>
       </c>
       <c r="K8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="L8">
         <v>20000</v>
       </c>
       <c r="M8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="N8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="Q8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="R8" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="S8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="T8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
@@ -1891,7 +1761,7 @@
         <v>2104000</v>
       </c>
       <c r="H9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I9">
         <v>9000</v>
@@ -1900,48 +1770,48 @@
         <v>11000</v>
       </c>
       <c r="K9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="L9">
         <v>13500</v>
       </c>
       <c r="M9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="N9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="Q9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="R9" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="S9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="T9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
         <v>25</v>
@@ -1953,7 +1823,7 @@
         <v>5000000</v>
       </c>
       <c r="H10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I10">
         <v>2000</v>
@@ -1962,158 +1832,34 @@
         <v>2000</v>
       </c>
       <c r="K10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="L10">
         <v>2000</v>
       </c>
       <c r="M10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="N10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="Q10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="R10" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="S10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="T10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20">
-      <c r="A11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11">
-        <v>13000000</v>
-      </c>
-      <c r="G11">
-        <v>6500000</v>
-      </c>
-      <c r="H11" t="s">
-        <v>48</v>
-      </c>
-      <c r="I11">
-        <v>2000</v>
-      </c>
-      <c r="J11">
-        <v>2000</v>
-      </c>
-      <c r="K11" t="s">
-        <v>48</v>
-      </c>
-      <c r="L11">
-        <v>2000</v>
-      </c>
-      <c r="M11" t="s">
-        <v>48</v>
-      </c>
-      <c r="N11" t="s">
-        <v>48</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>48</v>
-      </c>
-      <c r="R11" t="s">
-        <v>92</v>
-      </c>
-      <c r="S11" t="s">
-        <v>48</v>
-      </c>
-      <c r="T11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20">
-      <c r="A12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" t="s">
-        <v>64</v>
-      </c>
-      <c r="E12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12">
-        <v>8000000</v>
-      </c>
-      <c r="G12">
-        <v>4000000</v>
-      </c>
-      <c r="H12" t="s">
-        <v>48</v>
-      </c>
-      <c r="I12">
-        <v>2000</v>
-      </c>
-      <c r="J12">
-        <v>2000</v>
-      </c>
-      <c r="K12" t="s">
-        <v>48</v>
-      </c>
-      <c r="L12">
-        <v>2000</v>
-      </c>
-      <c r="M12" t="s">
-        <v>48</v>
-      </c>
-      <c r="N12" t="s">
-        <v>48</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>48</v>
-      </c>
-      <c r="R12" t="s">
-        <v>93</v>
-      </c>
-      <c r="S12" t="s">
-        <v>48</v>
-      </c>
-      <c r="T12" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2123,7 +1869,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2131,16 +1877,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -2152,10 +1898,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -2164,27 +1910,27 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="G2" t="s">
         <v>24</v>
@@ -2207,22 +1953,22 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G3" t="s">
         <v>21</v>
@@ -2245,19 +1991,19 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s">
         <v>24</v>
@@ -2283,22 +2029,22 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="G5" t="s">
         <v>24</v>
@@ -2321,34 +2067,34 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H6">
-        <v>8000</v>
+        <v>32500</v>
       </c>
       <c r="I6">
-        <v>4000000</v>
+        <v>2500000</v>
       </c>
       <c r="J6">
-        <v>2000</v>
+        <v>13000</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -2359,34 +2105,34 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H7">
-        <v>32500</v>
+        <v>6000</v>
       </c>
       <c r="I7">
-        <v>2500000</v>
+        <v>3000000</v>
       </c>
       <c r="J7">
-        <v>13000</v>
+        <v>2000</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -2397,31 +2143,31 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" t="s">
         <v>18</v>
       </c>
-      <c r="G8" t="s">
-        <v>17</v>
-      </c>
       <c r="H8">
-        <v>6000</v>
+        <v>10000</v>
       </c>
       <c r="I8">
-        <v>3000000</v>
+        <v>5000000</v>
       </c>
       <c r="J8">
         <v>2000</v>
@@ -2435,31 +2181,31 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
         <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H9">
-        <v>10000</v>
+        <v>6000</v>
       </c>
       <c r="I9">
-        <v>5000000</v>
+        <v>3000000</v>
       </c>
       <c r="J9">
         <v>2000</v>
@@ -2473,31 +2219,31 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" t="s">
         <v>58</v>
       </c>
-      <c r="C10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" t="s">
-        <v>64</v>
-      </c>
       <c r="G10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H10">
-        <v>13000</v>
+        <v>10000</v>
       </c>
       <c r="I10">
-        <v>6500000</v>
+        <v>5000000</v>
       </c>
       <c r="J10">
         <v>2000</v>
@@ -2511,115 +2257,39 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
         <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" t="s">
         <v>22</v>
       </c>
-      <c r="G11" t="s">
-        <v>20</v>
-      </c>
       <c r="H11">
-        <v>6000</v>
+        <v>60000</v>
       </c>
       <c r="I11">
-        <v>3000000</v>
+        <v>2000000</v>
       </c>
       <c r="J11">
-        <v>2000</v>
+        <v>30000</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" t="s">
-        <v>63</v>
-      </c>
-      <c r="G12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12">
-        <v>10000</v>
-      </c>
-      <c r="I12">
-        <v>5000000</v>
-      </c>
-      <c r="J12">
-        <v>2000</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" t="s">
-        <v>62</v>
-      </c>
-      <c r="G13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13">
-        <v>60000</v>
-      </c>
-      <c r="I13">
-        <v>2000000</v>
-      </c>
-      <c r="J13">
-        <v>30000</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2024-04-27
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="93">
   <si>
     <t>상장일</t>
   </si>
@@ -69,6 +69,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2024-04-24</t>
+  </si>
+  <si>
     <t>2024-04-22</t>
   </si>
   <si>
@@ -96,6 +99,9 @@
     <t>2024-03-05</t>
   </si>
   <si>
+    <t>하나33호스팩</t>
+  </si>
+  <si>
     <t>신한제13호스팩</t>
   </si>
   <si>
@@ -126,15 +132,15 @@
     <t>코스닥</t>
   </si>
   <si>
+    <t>하나</t>
+  </si>
+  <si>
     <t>신한</t>
   </si>
   <si>
     <t>미래</t>
   </si>
   <si>
-    <t>하나</t>
-  </si>
-  <si>
     <t>NH</t>
   </si>
   <si>
@@ -177,6 +183,9 @@
     <t>2024-02-22</t>
   </si>
   <si>
+    <t>2024-04-18</t>
+  </si>
+  <si>
     <t>2024-04-05</t>
   </si>
   <si>
@@ -247,6 +256,9 @@
   </si>
   <si>
     <t>DB, NH</t>
+  </si>
+  <si>
+    <t>2248.41 : 1</t>
   </si>
   <si>
     <t>1337.88 : 1</t>
@@ -640,7 +652,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -704,37 +716,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D2">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F2">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M2">
         <v>2000</v>
@@ -743,13 +755,13 @@
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="P2" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="Q2">
-        <v>2250000</v>
+        <v>2625000</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -757,37 +769,37 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D3">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F3">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M3">
         <v>2000</v>
@@ -796,13 +808,13 @@
         <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="P3" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="Q3">
-        <v>3750000</v>
+        <v>2250000</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -810,52 +822,52 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D4">
-        <v>325</v>
+        <v>100</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F4">
-        <v>325</v>
+        <v>100</v>
       </c>
       <c r="G4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M4">
-        <v>13000</v>
+        <v>2000</v>
       </c>
       <c r="N4">
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="P4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="Q4">
-        <v>1875000</v>
+        <v>3750000</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -863,52 +875,52 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D5">
-        <v>60</v>
+        <v>325</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F5">
-        <v>60</v>
+        <v>325</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M5">
-        <v>2000</v>
+        <v>13000</v>
       </c>
       <c r="N5">
         <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P5" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="Q5">
-        <v>2250000</v>
+        <v>1875000</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -916,52 +928,52 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D6">
-        <v>320</v>
+        <v>60</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F6">
-        <v>320</v>
+        <v>60</v>
       </c>
       <c r="G6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M6">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="N6">
         <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="P6" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="Q6">
-        <v>880000</v>
+        <v>2250000</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -969,52 +981,52 @@
         <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D7">
-        <v>600</v>
+        <v>320</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F7">
-        <v>600</v>
+        <v>320</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M7">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="N7">
         <v>100</v>
       </c>
       <c r="O7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="P7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q7">
-        <v>1368000</v>
+        <v>880000</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1022,52 +1034,52 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D8">
-        <v>198</v>
+        <v>600</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F8">
-        <v>198</v>
+        <v>600</v>
       </c>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M8">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="N8">
         <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="P8" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="Q8">
-        <v>742500</v>
+        <v>1368000</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1075,63 +1087,63 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D9">
-        <v>284.04</v>
+        <v>198</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F9">
-        <v>142.02</v>
+        <v>198</v>
       </c>
       <c r="G9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K9" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="L9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M9">
-        <v>13500</v>
+        <v>20000</v>
       </c>
       <c r="N9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P9" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="Q9">
-        <v>2916000</v>
+        <v>742500</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D10">
         <v>284.04</v>
@@ -1143,22 +1155,22 @@
         <v>142.02</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M10">
         <v>13500</v>
@@ -1167,10 +1179,10 @@
         <v>50</v>
       </c>
       <c r="O10" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="P10" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="Q10">
         <v>2916000</v>
@@ -1181,51 +1193,104 @@
         <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D11">
+        <v>284.04</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11">
+        <v>142.02</v>
+      </c>
+      <c r="G11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" t="s">
+        <v>44</v>
+      </c>
+      <c r="K11" t="s">
+        <v>44</v>
+      </c>
+      <c r="L11" t="s">
+        <v>44</v>
+      </c>
+      <c r="M11">
+        <v>13500</v>
+      </c>
+      <c r="N11">
+        <v>50</v>
+      </c>
+      <c r="O11" t="s">
+        <v>53</v>
+      </c>
+      <c r="P11" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q11">
+        <v>2916000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12">
         <v>100</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>38</v>
       </c>
-      <c r="F11">
+      <c r="F12">
         <v>100</v>
       </c>
-      <c r="G11" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11" t="s">
-        <v>42</v>
-      </c>
-      <c r="J11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K11" t="s">
-        <v>43</v>
-      </c>
-      <c r="L11" t="s">
-        <v>42</v>
-      </c>
-      <c r="M11">
+      <c r="G12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" t="s">
+        <v>44</v>
+      </c>
+      <c r="J12" t="s">
+        <v>44</v>
+      </c>
+      <c r="K12" t="s">
+        <v>45</v>
+      </c>
+      <c r="L12" t="s">
+        <v>44</v>
+      </c>
+      <c r="M12">
         <v>2000</v>
       </c>
-      <c r="N11">
+      <c r="N12">
         <v>100</v>
       </c>
-      <c r="O11" t="s">
-        <v>52</v>
-      </c>
-      <c r="P11" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q11">
+      <c r="O12" t="s">
+        <v>54</v>
+      </c>
+      <c r="P12" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q12">
         <v>3750000</v>
       </c>
     </row>
@@ -1236,7 +1301,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1247,10 +1312,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -1259,75 +1324,75 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
       </c>
       <c r="F2">
-        <v>6000000</v>
+        <v>7000000</v>
       </c>
       <c r="G2">
-        <v>3000000</v>
+        <v>3500000</v>
       </c>
       <c r="H2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I2">
         <v>2000</v>
@@ -1336,60 +1401,60 @@
         <v>2000</v>
       </c>
       <c r="K2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L2">
         <v>2000</v>
       </c>
       <c r="M2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="N2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="Q2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="R2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="S2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="T2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
       </c>
       <c r="F3">
-        <v>10000000</v>
+        <v>6000000</v>
       </c>
       <c r="G3">
-        <v>5000000</v>
+        <v>3000000</v>
       </c>
       <c r="H3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I3">
         <v>2000</v>
@@ -1398,468 +1463,530 @@
         <v>2000</v>
       </c>
       <c r="K3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L3">
         <v>2000</v>
       </c>
       <c r="M3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="N3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="Q3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="R3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="S3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="T3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
       </c>
       <c r="F4">
-        <v>32500000</v>
+        <v>10000000</v>
       </c>
       <c r="G4">
-        <v>2500000</v>
+        <v>5000000</v>
       </c>
       <c r="H4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I4">
-        <v>7700</v>
+        <v>2000</v>
       </c>
       <c r="J4">
-        <v>9900</v>
+        <v>2000</v>
       </c>
       <c r="K4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L4">
-        <v>13000</v>
+        <v>2000</v>
       </c>
       <c r="M4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="N4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="Q4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="R4" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="S4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="T4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
       </c>
       <c r="F5">
-        <v>6000000</v>
+        <v>32500000</v>
       </c>
       <c r="G5">
-        <v>3000000</v>
+        <v>2500000</v>
       </c>
       <c r="H5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I5">
-        <v>2000</v>
+        <v>7700</v>
       </c>
       <c r="J5">
-        <v>2000</v>
+        <v>9900</v>
       </c>
       <c r="K5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L5">
-        <v>2000</v>
+        <v>13000</v>
       </c>
       <c r="M5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="N5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="Q5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="R5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="S5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="T5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
       </c>
       <c r="F6">
-        <v>32000000</v>
+        <v>6000000</v>
       </c>
       <c r="G6">
-        <v>1600000</v>
+        <v>3000000</v>
       </c>
       <c r="H6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I6">
-        <v>11000</v>
+        <v>2000</v>
       </c>
       <c r="J6">
-        <v>15000</v>
+        <v>2000</v>
       </c>
       <c r="K6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L6">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="M6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="N6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="Q6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="R6" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="S6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="T6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E7" t="s">
         <v>22</v>
       </c>
       <c r="F7">
-        <v>60000000</v>
+        <v>32000000</v>
       </c>
       <c r="G7">
-        <v>2000000</v>
+        <v>1600000</v>
       </c>
       <c r="H7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I7">
+        <v>11000</v>
+      </c>
+      <c r="J7">
+        <v>15000</v>
+      </c>
+      <c r="K7" t="s">
+        <v>44</v>
+      </c>
+      <c r="L7">
         <v>20000</v>
       </c>
-      <c r="J7">
-        <v>25000</v>
-      </c>
-      <c r="K7" t="s">
-        <v>42</v>
-      </c>
-      <c r="L7">
-        <v>30000</v>
-      </c>
       <c r="M7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="N7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="Q7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="R7" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="S7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="T7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="E8" t="s">
         <v>23</v>
       </c>
       <c r="F8">
-        <v>19800000</v>
+        <v>60000000</v>
       </c>
       <c r="G8">
-        <v>990000</v>
+        <v>2000000</v>
       </c>
       <c r="H8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I8">
-        <v>13000</v>
+        <v>20000</v>
       </c>
       <c r="J8">
-        <v>15000</v>
+        <v>25000</v>
       </c>
       <c r="K8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L8">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="M8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="N8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="Q8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="R8" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="S8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="T8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
       </c>
       <c r="F9">
-        <v>28404000</v>
+        <v>19800000</v>
       </c>
       <c r="G9">
-        <v>2104000</v>
+        <v>990000</v>
       </c>
       <c r="H9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I9">
-        <v>9000</v>
+        <v>13000</v>
       </c>
       <c r="J9">
-        <v>11000</v>
+        <v>15000</v>
       </c>
       <c r="K9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L9">
-        <v>13500</v>
+        <v>20000</v>
       </c>
       <c r="M9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="N9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="Q9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="R9" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="S9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="T9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E10" t="s">
         <v>25</v>
       </c>
       <c r="F10">
-        <v>10000000</v>
+        <v>28404000</v>
       </c>
       <c r="G10">
-        <v>5000000</v>
+        <v>2104000</v>
       </c>
       <c r="H10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I10">
-        <v>2000</v>
+        <v>9000</v>
       </c>
       <c r="J10">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="K10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L10">
-        <v>2000</v>
+        <v>13500</v>
       </c>
       <c r="M10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="N10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="Q10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="R10" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="S10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="T10" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11">
+        <v>10000000</v>
+      </c>
+      <c r="G11">
+        <v>5000000</v>
+      </c>
+      <c r="H11" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11">
+        <v>2000</v>
+      </c>
+      <c r="J11">
+        <v>2000</v>
+      </c>
+      <c r="K11" t="s">
+        <v>44</v>
+      </c>
+      <c r="L11">
+        <v>2000</v>
+      </c>
+      <c r="M11" t="s">
+        <v>44</v>
+      </c>
+      <c r="N11" t="s">
+        <v>44</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>44</v>
+      </c>
+      <c r="R11" t="s">
+        <v>89</v>
+      </c>
+      <c r="S11" t="s">
+        <v>44</v>
+      </c>
+      <c r="T11" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1869,7 +1996,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1877,16 +2004,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -1898,10 +2025,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -1910,30 +2037,30 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H2">
         <v>14202</v>
@@ -1953,25 +2080,25 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H3">
         <v>32000</v>
@@ -1991,25 +2118,25 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
         <v>24</v>
-      </c>
-      <c r="G4" t="s">
-        <v>23</v>
       </c>
       <c r="H4">
         <v>19800</v>
@@ -2029,25 +2156,25 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H5">
         <v>14202</v>
@@ -2067,25 +2194,25 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H6">
         <v>32500</v>
@@ -2105,25 +2232,25 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
         <v>18</v>
-      </c>
-      <c r="G7" t="s">
-        <v>17</v>
       </c>
       <c r="H7">
         <v>6000</v>
@@ -2143,25 +2270,25 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F8" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H8">
         <v>10000</v>
@@ -2184,10 +2311,10 @@
         <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
         <v>38</v>
@@ -2196,16 +2323,16 @@
         <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="G9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H9">
-        <v>6000</v>
+        <v>7000</v>
       </c>
       <c r="I9">
-        <v>3000000</v>
+        <v>3500000</v>
       </c>
       <c r="J9">
         <v>2000</v>
@@ -2222,10 +2349,10 @@
         <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
         <v>38</v>
@@ -2234,16 +2361,16 @@
         <v>38</v>
       </c>
       <c r="F10" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="G10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H10">
-        <v>10000</v>
+        <v>6000</v>
       </c>
       <c r="I10">
-        <v>5000000</v>
+        <v>3000000</v>
       </c>
       <c r="J10">
         <v>2000</v>
@@ -2257,39 +2384,77 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F11" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="G11" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H11">
-        <v>60000</v>
+        <v>10000</v>
       </c>
       <c r="I11">
-        <v>2000000</v>
+        <v>5000000</v>
       </c>
       <c r="J11">
-        <v>30000</v>
+        <v>2000</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12">
+        <v>60000</v>
+      </c>
+      <c r="I12">
+        <v>2000000</v>
+      </c>
+      <c r="J12">
+        <v>30000</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2024-04-28
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="88">
   <si>
     <t>상장일</t>
   </si>
@@ -96,9 +96,6 @@
     <t>2024-03-07</t>
   </si>
   <si>
-    <t>2024-03-05</t>
-  </si>
-  <si>
     <t>하나33호스팩</t>
   </si>
   <si>
@@ -126,9 +123,6 @@
     <t>케이엔알시스템</t>
   </si>
   <si>
-    <t>하나31호스팩</t>
-  </si>
-  <si>
     <t>코스닥</t>
   </si>
   <si>
@@ -180,9 +174,6 @@
     <t>2024-02-26</t>
   </si>
   <si>
-    <t>2024-02-22</t>
-  </si>
-  <si>
     <t>2024-04-18</t>
   </si>
   <si>
@@ -201,9 +192,6 @@
     <t>2024-02-29</t>
   </si>
   <si>
-    <t>2024-02-27</t>
-  </si>
-  <si>
     <t>회사명</t>
   </si>
   <si>
@@ -283,9 +271,6 @@
   </si>
   <si>
     <t>2266.72 : 1</t>
-  </si>
-  <si>
-    <t>1896.1033 : 1</t>
   </si>
   <si>
     <t>인수기관</t>
@@ -652,7 +637,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -716,37 +701,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D2">
         <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F2">
         <v>70</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M2">
         <v>2000</v>
@@ -758,7 +743,7 @@
         <v>19</v>
       </c>
       <c r="P2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="Q2">
         <v>2625000</v>
@@ -769,37 +754,37 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D3">
         <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F3">
         <v>60</v>
       </c>
       <c r="G3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M3">
         <v>2000</v>
@@ -808,7 +793,7 @@
         <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P3" t="s">
         <v>19</v>
@@ -822,37 +807,37 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D4">
         <v>100</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F4">
         <v>100</v>
       </c>
       <c r="G4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M4">
         <v>2000</v>
@@ -861,10 +846,10 @@
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="P4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q4">
         <v>3750000</v>
@@ -875,37 +860,37 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D5">
         <v>325</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F5">
         <v>325</v>
       </c>
       <c r="G5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M5">
         <v>13000</v>
@@ -914,10 +899,10 @@
         <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="P5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="Q5">
         <v>1875000</v>
@@ -928,37 +913,37 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D6">
         <v>60</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F6">
         <v>60</v>
       </c>
       <c r="G6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M6">
         <v>2000</v>
@@ -967,7 +952,7 @@
         <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P6" t="s">
         <v>23</v>
@@ -981,37 +966,37 @@
         <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D7">
         <v>320</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F7">
         <v>320</v>
       </c>
       <c r="G7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M7">
         <v>20000</v>
@@ -1020,10 +1005,10 @@
         <v>100</v>
       </c>
       <c r="O7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="P7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="Q7">
         <v>880000</v>
@@ -1034,37 +1019,37 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D8">
         <v>600</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F8">
         <v>600</v>
       </c>
       <c r="G8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M8">
         <v>30000</v>
@@ -1073,10 +1058,10 @@
         <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="P8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="Q8">
         <v>1368000</v>
@@ -1087,37 +1072,37 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D9">
         <v>198</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F9">
         <v>198</v>
       </c>
       <c r="G9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M9">
         <v>20000</v>
@@ -1126,7 +1111,7 @@
         <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P9" t="s">
         <v>25</v>
@@ -1140,37 +1125,37 @@
         <v>25</v>
       </c>
       <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
         <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>37</v>
       </c>
       <c r="D10">
         <v>284.04</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F10">
         <v>142.02</v>
       </c>
       <c r="G10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M10">
         <v>13500</v>
@@ -1179,10 +1164,10 @@
         <v>50</v>
       </c>
       <c r="O10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Q10">
         <v>2916000</v>
@@ -1193,37 +1178,37 @@
         <v>25</v>
       </c>
       <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
         <v>35</v>
-      </c>
-      <c r="C11" t="s">
-        <v>37</v>
       </c>
       <c r="D11">
         <v>284.04</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F11">
         <v>142.02</v>
       </c>
       <c r="G11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M11">
         <v>13500</v>
@@ -1232,66 +1217,13 @@
         <v>50</v>
       </c>
       <c r="O11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Q11">
         <v>2916000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
-      <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12">
-        <v>100</v>
-      </c>
-      <c r="E12" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12">
-        <v>100</v>
-      </c>
-      <c r="G12" t="s">
-        <v>44</v>
-      </c>
-      <c r="H12" t="s">
-        <v>44</v>
-      </c>
-      <c r="I12" t="s">
-        <v>44</v>
-      </c>
-      <c r="J12" t="s">
-        <v>44</v>
-      </c>
-      <c r="K12" t="s">
-        <v>45</v>
-      </c>
-      <c r="L12" t="s">
-        <v>44</v>
-      </c>
-      <c r="M12">
-        <v>2000</v>
-      </c>
-      <c r="N12">
-        <v>100</v>
-      </c>
-      <c r="O12" t="s">
-        <v>54</v>
-      </c>
-      <c r="P12" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q12">
-        <v>3750000</v>
       </c>
     </row>
   </sheetData>
@@ -1301,7 +1233,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T11"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1312,10 +1244,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -1324,49 +1256,49 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -1374,13 +1306,13 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
@@ -1392,7 +1324,7 @@
         <v>3500000</v>
       </c>
       <c r="H2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I2">
         <v>2000</v>
@@ -1401,45 +1333,45 @@
         <v>2000</v>
       </c>
       <c r="K2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L2">
         <v>2000</v>
       </c>
       <c r="M2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="S2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="T2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
@@ -1454,7 +1386,7 @@
         <v>3000000</v>
       </c>
       <c r="H3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I3">
         <v>2000</v>
@@ -1463,48 +1395,48 @@
         <v>2000</v>
       </c>
       <c r="K3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L3">
         <v>2000</v>
       </c>
       <c r="M3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="S3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="T3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
@@ -1516,7 +1448,7 @@
         <v>5000000</v>
       </c>
       <c r="H4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I4">
         <v>2000</v>
@@ -1525,48 +1457,48 @@
         <v>2000</v>
       </c>
       <c r="K4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L4">
         <v>2000</v>
       </c>
       <c r="M4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="S4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="T4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
@@ -1578,7 +1510,7 @@
         <v>2500000</v>
       </c>
       <c r="H5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I5">
         <v>7700</v>
@@ -1587,45 +1519,45 @@
         <v>9900</v>
       </c>
       <c r="K5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L5">
         <v>13000</v>
       </c>
       <c r="M5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="S5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="T5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
         <v>23</v>
@@ -1640,7 +1572,7 @@
         <v>3000000</v>
       </c>
       <c r="H6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I6">
         <v>2000</v>
@@ -1649,48 +1581,48 @@
         <v>2000</v>
       </c>
       <c r="K6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L6">
         <v>2000</v>
       </c>
       <c r="M6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="S6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="T6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
         <v>22</v>
@@ -1702,7 +1634,7 @@
         <v>1600000</v>
       </c>
       <c r="H7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I7">
         <v>11000</v>
@@ -1711,48 +1643,48 @@
         <v>15000</v>
       </c>
       <c r="K7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L7">
         <v>20000</v>
       </c>
       <c r="M7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="S7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="T7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E8" t="s">
         <v>23</v>
@@ -1764,7 +1696,7 @@
         <v>2000000</v>
       </c>
       <c r="H8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I8">
         <v>20000</v>
@@ -1773,45 +1705,45 @@
         <v>25000</v>
       </c>
       <c r="K8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L8">
         <v>30000</v>
       </c>
       <c r="M8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="S8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="T8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
         <v>25</v>
@@ -1826,7 +1758,7 @@
         <v>990000</v>
       </c>
       <c r="H9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I9">
         <v>13000</v>
@@ -1835,48 +1767,48 @@
         <v>15000</v>
       </c>
       <c r="K9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L9">
         <v>20000</v>
       </c>
       <c r="M9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="S9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="T9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s">
         <v>25</v>
@@ -1888,7 +1820,7 @@
         <v>2104000</v>
       </c>
       <c r="H10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I10">
         <v>9000</v>
@@ -1897,96 +1829,34 @@
         <v>11000</v>
       </c>
       <c r="K10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L10">
         <v>13500</v>
       </c>
       <c r="M10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R10" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="S10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="T10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20">
-      <c r="A11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11">
-        <v>10000000</v>
-      </c>
-      <c r="G11">
-        <v>5000000</v>
-      </c>
-      <c r="H11" t="s">
-        <v>44</v>
-      </c>
-      <c r="I11">
-        <v>2000</v>
-      </c>
-      <c r="J11">
-        <v>2000</v>
-      </c>
-      <c r="K11" t="s">
-        <v>44</v>
-      </c>
-      <c r="L11">
-        <v>2000</v>
-      </c>
-      <c r="M11" t="s">
-        <v>44</v>
-      </c>
-      <c r="N11" t="s">
-        <v>44</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>44</v>
-      </c>
-      <c r="R11" t="s">
-        <v>89</v>
-      </c>
-      <c r="S11" t="s">
-        <v>44</v>
-      </c>
-      <c r="T11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1996,7 +1866,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2004,16 +1874,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -2025,10 +1895,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -2037,27 +1907,27 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G2" t="s">
         <v>25</v>
@@ -2080,22 +1950,22 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G3" t="s">
         <v>22</v>
@@ -2118,19 +1988,19 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s">
         <v>25</v>
@@ -2156,22 +2026,22 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G5" t="s">
         <v>25</v>
@@ -2194,22 +2064,22 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G6" t="s">
         <v>20</v>
@@ -2232,19 +2102,19 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
         <v>19</v>
@@ -2270,22 +2140,22 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G8" t="s">
         <v>19</v>
@@ -2308,22 +2178,22 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G9" t="s">
         <v>17</v>
@@ -2346,19 +2216,19 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
         <v>23</v>
@@ -2384,77 +2254,39 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H11">
-        <v>10000</v>
+        <v>60000</v>
       </c>
       <c r="I11">
-        <v>5000000</v>
+        <v>2000000</v>
       </c>
       <c r="J11">
-        <v>2000</v>
+        <v>30000</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12">
-        <v>60000</v>
-      </c>
-      <c r="I12">
-        <v>2000000</v>
-      </c>
-      <c r="J12">
-        <v>30000</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2024-04-30
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="82">
   <si>
     <t>상장일</t>
   </si>
@@ -93,105 +93,93 @@
     <t>2024-03-13</t>
   </si>
   <si>
+    <t>하나33호스팩</t>
+  </si>
+  <si>
+    <t>신한제13호스팩</t>
+  </si>
+  <si>
+    <t>신한제12호스팩</t>
+  </si>
+  <si>
+    <t>아이엠비디엑스</t>
+  </si>
+  <si>
+    <t>하나32호스팩</t>
+  </si>
+  <si>
+    <t>엔젤로보틱스</t>
+  </si>
+  <si>
+    <t>삼현</t>
+  </si>
+  <si>
+    <t>오상헬스케어</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>신한</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>한국</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>2024-04-11</t>
+  </si>
+  <si>
+    <t>2024-04-02</t>
+  </si>
+  <si>
+    <t>2024-03-25</t>
+  </si>
+  <si>
+    <t>2024-03-18</t>
+  </si>
+  <si>
+    <t>2024-03-14</t>
+  </si>
+  <si>
+    <t>2024-03-12</t>
+  </si>
+  <si>
+    <t>2024-03-04</t>
+  </si>
+  <si>
+    <t>2024-04-18</t>
+  </si>
+  <si>
+    <t>2024-04-05</t>
+  </si>
+  <si>
+    <t>2024-03-28</t>
+  </si>
+  <si>
+    <t>2024-03-19</t>
+  </si>
+  <si>
+    <t>2024-03-15</t>
+  </si>
+  <si>
     <t>2024-03-07</t>
   </si>
   <si>
-    <t>하나33호스팩</t>
-  </si>
-  <si>
-    <t>신한제13호스팩</t>
-  </si>
-  <si>
-    <t>신한제12호스팩</t>
-  </si>
-  <si>
-    <t>아이엠비디엑스</t>
-  </si>
-  <si>
-    <t>하나32호스팩</t>
-  </si>
-  <si>
-    <t>엔젤로보틱스</t>
-  </si>
-  <si>
-    <t>삼현</t>
-  </si>
-  <si>
-    <t>오상헬스케어</t>
-  </si>
-  <si>
-    <t>케이엔알시스템</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>신한</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>한국</t>
-  </si>
-  <si>
-    <t>DB</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>2024-04-11</t>
-  </si>
-  <si>
-    <t>2024-04-02</t>
-  </si>
-  <si>
-    <t>2024-03-25</t>
-  </si>
-  <si>
-    <t>2024-03-18</t>
-  </si>
-  <si>
-    <t>2024-03-14</t>
-  </si>
-  <si>
-    <t>2024-03-12</t>
-  </si>
-  <si>
-    <t>2024-03-04</t>
-  </si>
-  <si>
-    <t>2024-02-26</t>
-  </si>
-  <si>
-    <t>2024-04-18</t>
-  </si>
-  <si>
-    <t>2024-04-05</t>
-  </si>
-  <si>
-    <t>2024-03-28</t>
-  </si>
-  <si>
-    <t>2024-03-19</t>
-  </si>
-  <si>
-    <t>2024-03-15</t>
-  </si>
-  <si>
-    <t>2024-02-29</t>
-  </si>
-  <si>
     <t>회사명</t>
   </si>
   <si>
@@ -243,9 +231,6 @@
     <t>수수료율</t>
   </si>
   <si>
-    <t>DB, NH</t>
-  </si>
-  <si>
     <t>2248.41 : 1</t>
   </si>
   <si>
@@ -268,9 +253,6 @@
   </si>
   <si>
     <t>2126.13 : 1</t>
-  </si>
-  <si>
-    <t>2266.72 : 1</t>
   </si>
   <si>
     <t>인수기관</t>
@@ -637,7 +619,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -701,37 +683,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2">
         <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F2">
         <v>70</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="M2">
         <v>2000</v>
@@ -743,7 +725,7 @@
         <v>19</v>
       </c>
       <c r="P2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="Q2">
         <v>2625000</v>
@@ -754,37 +736,37 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D3">
         <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F3">
         <v>60</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="M3">
         <v>2000</v>
@@ -793,7 +775,7 @@
         <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P3" t="s">
         <v>19</v>
@@ -807,37 +789,37 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D4">
         <v>100</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F4">
         <v>100</v>
       </c>
       <c r="G4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="M4">
         <v>2000</v>
@@ -846,10 +828,10 @@
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="P4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="Q4">
         <v>3750000</v>
@@ -860,37 +842,37 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D5">
         <v>325</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F5">
         <v>325</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="M5">
         <v>13000</v>
@@ -899,10 +881,10 @@
         <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="P5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="Q5">
         <v>1875000</v>
@@ -913,37 +895,37 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6">
         <v>60</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F6">
         <v>60</v>
       </c>
       <c r="G6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="M6">
         <v>2000</v>
@@ -952,7 +934,7 @@
         <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P6" t="s">
         <v>23</v>
@@ -966,37 +948,37 @@
         <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D7">
         <v>320</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F7">
         <v>320</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="M7">
         <v>20000</v>
@@ -1005,10 +987,10 @@
         <v>100</v>
       </c>
       <c r="O7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="P7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="Q7">
         <v>880000</v>
@@ -1019,37 +1001,37 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D8">
         <v>600</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F8">
         <v>600</v>
       </c>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="M8">
         <v>30000</v>
@@ -1058,10 +1040,10 @@
         <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="P8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="Q8">
         <v>1368000</v>
@@ -1072,37 +1054,37 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
         <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>35</v>
       </c>
       <c r="D9">
         <v>198</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F9">
         <v>198</v>
       </c>
       <c r="G9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="M9">
         <v>20000</v>
@@ -1111,119 +1093,13 @@
         <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="P9" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="Q9">
         <v>742500</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10">
-        <v>284.04</v>
-      </c>
-      <c r="E10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10">
-        <v>142.02</v>
-      </c>
-      <c r="G10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10" t="s">
-        <v>42</v>
-      </c>
-      <c r="J10" t="s">
-        <v>42</v>
-      </c>
-      <c r="K10" t="s">
-        <v>42</v>
-      </c>
-      <c r="L10" t="s">
-        <v>42</v>
-      </c>
-      <c r="M10">
-        <v>13500</v>
-      </c>
-      <c r="N10">
-        <v>50</v>
-      </c>
-      <c r="O10" t="s">
-        <v>51</v>
-      </c>
-      <c r="P10" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q10">
-        <v>2916000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11">
-        <v>284.04</v>
-      </c>
-      <c r="E11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11">
-        <v>142.02</v>
-      </c>
-      <c r="G11" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11" t="s">
-        <v>42</v>
-      </c>
-      <c r="J11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K11" t="s">
-        <v>42</v>
-      </c>
-      <c r="L11" t="s">
-        <v>42</v>
-      </c>
-      <c r="M11">
-        <v>13500</v>
-      </c>
-      <c r="N11">
-        <v>50</v>
-      </c>
-      <c r="O11" t="s">
-        <v>51</v>
-      </c>
-      <c r="P11" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q11">
-        <v>2916000</v>
       </c>
     </row>
   </sheetData>
@@ -1233,7 +1109,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1244,10 +1120,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -1256,49 +1132,49 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -1306,13 +1182,13 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
@@ -1324,7 +1200,7 @@
         <v>3500000</v>
       </c>
       <c r="H2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I2">
         <v>2000</v>
@@ -1333,45 +1209,45 @@
         <v>2000</v>
       </c>
       <c r="K2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L2">
         <v>2000</v>
       </c>
       <c r="M2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="N2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="Q2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="R2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="S2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="T2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
@@ -1386,7 +1262,7 @@
         <v>3000000</v>
       </c>
       <c r="H3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I3">
         <v>2000</v>
@@ -1395,48 +1271,48 @@
         <v>2000</v>
       </c>
       <c r="K3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L3">
         <v>2000</v>
       </c>
       <c r="M3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="N3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="Q3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="R3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="S3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="T3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
@@ -1448,7 +1324,7 @@
         <v>5000000</v>
       </c>
       <c r="H4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I4">
         <v>2000</v>
@@ -1457,48 +1333,48 @@
         <v>2000</v>
       </c>
       <c r="K4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L4">
         <v>2000</v>
       </c>
       <c r="M4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="N4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="Q4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="R4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="S4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="T4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
@@ -1510,7 +1386,7 @@
         <v>2500000</v>
       </c>
       <c r="H5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I5">
         <v>7700</v>
@@ -1519,45 +1395,45 @@
         <v>9900</v>
       </c>
       <c r="K5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L5">
         <v>13000</v>
       </c>
       <c r="M5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="N5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="Q5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="R5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="S5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="T5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
         <v>23</v>
@@ -1572,7 +1448,7 @@
         <v>3000000</v>
       </c>
       <c r="H6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I6">
         <v>2000</v>
@@ -1581,48 +1457,48 @@
         <v>2000</v>
       </c>
       <c r="K6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L6">
         <v>2000</v>
       </c>
       <c r="M6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="N6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="Q6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="R6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="S6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="T6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E7" t="s">
         <v>22</v>
@@ -1634,7 +1510,7 @@
         <v>1600000</v>
       </c>
       <c r="H7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I7">
         <v>11000</v>
@@ -1643,48 +1519,48 @@
         <v>15000</v>
       </c>
       <c r="K7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L7">
         <v>20000</v>
       </c>
       <c r="M7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="N7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="Q7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="R7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="S7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="T7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E8" t="s">
         <v>23</v>
@@ -1696,7 +1572,7 @@
         <v>2000000</v>
       </c>
       <c r="H8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I8">
         <v>20000</v>
@@ -1705,48 +1581,48 @@
         <v>25000</v>
       </c>
       <c r="K8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L8">
         <v>30000</v>
       </c>
       <c r="M8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="N8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="Q8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="R8" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="S8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="T8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
@@ -1758,7 +1634,7 @@
         <v>990000</v>
       </c>
       <c r="H9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I9">
         <v>13000</v>
@@ -1767,96 +1643,34 @@
         <v>15000</v>
       </c>
       <c r="K9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L9">
         <v>20000</v>
       </c>
       <c r="M9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="N9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="Q9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="R9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="S9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="T9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20">
-      <c r="A10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10">
-        <v>28404000</v>
-      </c>
-      <c r="G10">
-        <v>2104000</v>
-      </c>
-      <c r="H10" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10">
-        <v>9000</v>
-      </c>
-      <c r="J10">
-        <v>11000</v>
-      </c>
-      <c r="K10" t="s">
-        <v>42</v>
-      </c>
-      <c r="L10">
-        <v>13500</v>
-      </c>
-      <c r="M10" t="s">
-        <v>42</v>
-      </c>
-      <c r="N10" t="s">
-        <v>42</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>42</v>
-      </c>
-      <c r="R10" t="s">
-        <v>84</v>
-      </c>
-      <c r="S10" t="s">
-        <v>42</v>
-      </c>
-      <c r="T10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1866,7 +1680,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1874,16 +1688,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -1895,10 +1709,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -1907,74 +1721,74 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
         <v>51</v>
       </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" t="s">
-        <v>57</v>
-      </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H2">
-        <v>14202</v>
+        <v>32000</v>
       </c>
       <c r="I2">
-        <v>2104000</v>
+        <v>1600000</v>
       </c>
       <c r="J2">
-        <v>13500</v>
+        <v>20000</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
       <c r="L2">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H3">
-        <v>32000</v>
+        <v>19800</v>
       </c>
       <c r="I3">
-        <v>1600000</v>
+        <v>990000</v>
       </c>
       <c r="J3">
         <v>20000</v>
@@ -1988,34 +1802,34 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
         <v>50</v>
       </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H4">
-        <v>19800</v>
+        <v>32500</v>
       </c>
       <c r="I4">
-        <v>990000</v>
+        <v>2500000</v>
       </c>
       <c r="J4">
-        <v>20000</v>
+        <v>13000</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -2026,72 +1840,72 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="F5" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H5">
-        <v>14202</v>
+        <v>6000</v>
       </c>
       <c r="I5">
-        <v>2104000</v>
+        <v>3000000</v>
       </c>
       <c r="J5">
-        <v>13500</v>
+        <v>2000</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H6">
-        <v>32500</v>
+        <v>10000</v>
       </c>
       <c r="I6">
-        <v>2500000</v>
+        <v>5000000</v>
       </c>
       <c r="J6">
-        <v>13000</v>
+        <v>2000</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -2102,31 +1916,31 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H7">
-        <v>6000</v>
+        <v>7000</v>
       </c>
       <c r="I7">
-        <v>3000000</v>
+        <v>3500000</v>
       </c>
       <c r="J7">
         <v>2000</v>
@@ -2140,31 +1954,31 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="G8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H8">
-        <v>10000</v>
+        <v>6000</v>
       </c>
       <c r="I8">
-        <v>5000000</v>
+        <v>3000000</v>
       </c>
       <c r="J8">
         <v>2000</v>
@@ -2178,115 +1992,39 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s">
         <v>52</v>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H9">
-        <v>7000</v>
+        <v>60000</v>
       </c>
       <c r="I9">
-        <v>3500000</v>
+        <v>2000000</v>
       </c>
       <c r="J9">
-        <v>2000</v>
+        <v>30000</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10">
-        <v>6000</v>
-      </c>
-      <c r="I10">
-        <v>3000000</v>
-      </c>
-      <c r="J10">
-        <v>2000</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11">
-        <v>60000</v>
-      </c>
-      <c r="I11">
-        <v>2000000</v>
-      </c>
-      <c r="J11">
-        <v>30000</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2024-05-01
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="87">
   <si>
     <t>상장일</t>
   </si>
@@ -69,6 +69,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2024-04-30</t>
+  </si>
+  <si>
     <t>2024-04-24</t>
   </si>
   <si>
@@ -93,6 +96,9 @@
     <t>2024-03-13</t>
   </si>
   <si>
+    <t>제일엠앤에스</t>
+  </si>
+  <si>
     <t>하나33호스팩</t>
   </si>
   <si>
@@ -120,6 +126,9 @@
     <t>코스닥</t>
   </si>
   <si>
+    <t>KB</t>
+  </si>
+  <si>
     <t>하나</t>
   </si>
   <si>
@@ -141,6 +150,9 @@
     <t>대표</t>
   </si>
   <si>
+    <t>2024-04-18</t>
+  </si>
+  <si>
     <t>2024-04-11</t>
   </si>
   <si>
@@ -162,7 +174,7 @@
     <t>2024-03-04</t>
   </si>
   <si>
-    <t>2024-04-18</t>
+    <t>2024-04-23</t>
   </si>
   <si>
     <t>2024-04-05</t>
@@ -229,6 +241,9 @@
   </si>
   <si>
     <t>수수료율</t>
+  </si>
+  <si>
+    <t>1438.96 : 1</t>
   </si>
   <si>
     <t>2248.41 : 1</t>
@@ -619,7 +634,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -683,52 +698,52 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D2">
-        <v>70</v>
+        <v>528</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F2">
-        <v>70</v>
+        <v>528</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="L2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="M2">
-        <v>2000</v>
+        <v>22000</v>
       </c>
       <c r="N2">
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="P2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="Q2">
-        <v>2625000</v>
+        <v>1800000</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -736,37 +751,37 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D3">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F3">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="G3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="L3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="M3">
         <v>2000</v>
@@ -775,13 +790,13 @@
         <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="P3" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="Q3">
-        <v>2250000</v>
+        <v>2625000</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -789,37 +804,37 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D4">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F4">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="G4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="L4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="M4">
         <v>2000</v>
@@ -828,13 +843,13 @@
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="P4" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="Q4">
-        <v>3750000</v>
+        <v>2250000</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -842,52 +857,52 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D5">
-        <v>325</v>
+        <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F5">
-        <v>325</v>
+        <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="L5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="M5">
-        <v>13000</v>
+        <v>2000</v>
       </c>
       <c r="N5">
         <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="P5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="Q5">
-        <v>1875000</v>
+        <v>3750000</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -895,52 +910,52 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D6">
-        <v>60</v>
+        <v>325</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F6">
-        <v>60</v>
+        <v>325</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K6" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="L6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="M6">
-        <v>2000</v>
+        <v>13000</v>
       </c>
       <c r="N6">
         <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P6" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="Q6">
-        <v>2250000</v>
+        <v>1875000</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -948,52 +963,52 @@
         <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D7">
-        <v>320</v>
+        <v>60</v>
       </c>
       <c r="E7" t="s">
         <v>37</v>
       </c>
       <c r="F7">
-        <v>320</v>
+        <v>60</v>
       </c>
       <c r="G7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="L7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="M7">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="N7">
         <v>100</v>
       </c>
       <c r="O7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="P7" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="Q7">
-        <v>880000</v>
+        <v>2250000</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1001,52 +1016,52 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D8">
-        <v>600</v>
+        <v>320</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F8">
-        <v>600</v>
+        <v>320</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K8" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="L8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="M8">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="N8">
         <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P8" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q8">
-        <v>1368000</v>
+        <v>880000</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1054,51 +1069,104 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D9">
-        <v>198</v>
+        <v>600</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F9">
-        <v>198</v>
+        <v>600</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K9" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="L9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="M9">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="N9">
         <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="P9" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="Q9">
+        <v>1368000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10">
+        <v>198</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10">
+        <v>198</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" t="s">
+        <v>42</v>
+      </c>
+      <c r="K10" t="s">
+        <v>43</v>
+      </c>
+      <c r="L10" t="s">
+        <v>42</v>
+      </c>
+      <c r="M10">
+        <v>20000</v>
+      </c>
+      <c r="N10">
+        <v>100</v>
+      </c>
+      <c r="O10" t="s">
+        <v>51</v>
+      </c>
+      <c r="P10" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q10">
         <v>742500</v>
       </c>
     </row>
@@ -1109,7 +1177,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1120,10 +1188,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -1132,137 +1200,137 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
       </c>
       <c r="F2">
-        <v>7000000</v>
+        <v>52800000</v>
       </c>
       <c r="G2">
-        <v>3500000</v>
+        <v>2400000</v>
       </c>
       <c r="H2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I2">
-        <v>2000</v>
+        <v>15000</v>
       </c>
       <c r="J2">
-        <v>2000</v>
+        <v>18000</v>
       </c>
       <c r="K2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L2">
-        <v>2000</v>
+        <v>22000</v>
       </c>
       <c r="M2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="N2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="Q2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="R2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="S2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="T2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
       </c>
       <c r="F3">
-        <v>6000000</v>
+        <v>7000000</v>
       </c>
       <c r="G3">
-        <v>3000000</v>
+        <v>3500000</v>
       </c>
       <c r="H3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I3">
         <v>2000</v>
@@ -1271,60 +1339,60 @@
         <v>2000</v>
       </c>
       <c r="K3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L3">
         <v>2000</v>
       </c>
       <c r="M3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="N3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="Q3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="R3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="S3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="T3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
       </c>
       <c r="F4">
-        <v>10000000</v>
+        <v>6000000</v>
       </c>
       <c r="G4">
-        <v>5000000</v>
+        <v>3000000</v>
       </c>
       <c r="H4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I4">
         <v>2000</v>
@@ -1333,344 +1401,406 @@
         <v>2000</v>
       </c>
       <c r="K4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L4">
         <v>2000</v>
       </c>
       <c r="M4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="N4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="Q4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="R4" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="S4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="T4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
       </c>
       <c r="F5">
-        <v>32500000</v>
+        <v>10000000</v>
       </c>
       <c r="G5">
-        <v>2500000</v>
+        <v>5000000</v>
       </c>
       <c r="H5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I5">
-        <v>7700</v>
+        <v>2000</v>
       </c>
       <c r="J5">
-        <v>9900</v>
+        <v>2000</v>
       </c>
       <c r="K5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L5">
-        <v>13000</v>
+        <v>2000</v>
       </c>
       <c r="M5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="N5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="Q5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="R5" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="S5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="T5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
       </c>
       <c r="F6">
-        <v>6000000</v>
+        <v>32500000</v>
       </c>
       <c r="G6">
-        <v>3000000</v>
+        <v>2500000</v>
       </c>
       <c r="H6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I6">
-        <v>2000</v>
+        <v>7700</v>
       </c>
       <c r="J6">
-        <v>2000</v>
+        <v>9900</v>
       </c>
       <c r="K6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L6">
-        <v>2000</v>
+        <v>13000</v>
       </c>
       <c r="M6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="N6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="Q6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="R6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="S6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="T6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
         <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
         <v>22</v>
       </c>
       <c r="F7">
-        <v>32000000</v>
+        <v>6000000</v>
       </c>
       <c r="G7">
-        <v>1600000</v>
+        <v>3000000</v>
       </c>
       <c r="H7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I7">
-        <v>11000</v>
+        <v>2000</v>
       </c>
       <c r="J7">
-        <v>15000</v>
+        <v>2000</v>
       </c>
       <c r="K7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L7">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="M7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="N7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="Q7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="R7" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="S7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="T7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
         <v>23</v>
       </c>
       <c r="F8">
-        <v>60000000</v>
+        <v>32000000</v>
       </c>
       <c r="G8">
-        <v>2000000</v>
+        <v>1600000</v>
       </c>
       <c r="H8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I8">
+        <v>11000</v>
+      </c>
+      <c r="J8">
+        <v>15000</v>
+      </c>
+      <c r="K8" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8">
         <v>20000</v>
       </c>
-      <c r="J8">
-        <v>25000</v>
-      </c>
-      <c r="K8" t="s">
-        <v>39</v>
-      </c>
-      <c r="L8">
-        <v>30000</v>
-      </c>
       <c r="M8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="N8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="Q8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="R8" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="S8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="T8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
       </c>
       <c r="F9">
-        <v>19800000</v>
+        <v>60000000</v>
       </c>
       <c r="G9">
-        <v>990000</v>
+        <v>2000000</v>
       </c>
       <c r="H9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I9">
-        <v>13000</v>
+        <v>20000</v>
       </c>
       <c r="J9">
-        <v>15000</v>
+        <v>25000</v>
       </c>
       <c r="K9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L9">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="M9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="N9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="Q9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="R9" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="S9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="T9" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10">
+        <v>19800000</v>
+      </c>
+      <c r="G10">
+        <v>990000</v>
+      </c>
+      <c r="H10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10">
+        <v>13000</v>
+      </c>
+      <c r="J10">
+        <v>15000</v>
+      </c>
+      <c r="K10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L10">
+        <v>20000</v>
+      </c>
+      <c r="M10" t="s">
+        <v>42</v>
+      </c>
+      <c r="N10" t="s">
+        <v>42</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>42</v>
+      </c>
+      <c r="R10" t="s">
+        <v>83</v>
+      </c>
+      <c r="S10" t="s">
+        <v>42</v>
+      </c>
+      <c r="T10" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1680,7 +1810,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1688,16 +1818,16 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -1709,10 +1839,10 @@
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>12</v>
@@ -1721,39 +1851,39 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="H2">
-        <v>32000</v>
+        <v>52800</v>
       </c>
       <c r="I2">
-        <v>1600000</v>
+        <v>2400000</v>
       </c>
       <c r="J2">
-        <v>20000</v>
+        <v>22000</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1764,31 +1894,31 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
         <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3">
-        <v>19800</v>
+        <v>32000</v>
       </c>
       <c r="I3">
-        <v>990000</v>
+        <v>1600000</v>
       </c>
       <c r="J3">
         <v>20000</v>
@@ -1802,34 +1932,34 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H4">
-        <v>32500</v>
+        <v>19800</v>
       </c>
       <c r="I4">
-        <v>2500000</v>
+        <v>990000</v>
       </c>
       <c r="J4">
-        <v>13000</v>
+        <v>20000</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -1840,34 +1970,34 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H5">
-        <v>6000</v>
+        <v>32500</v>
       </c>
       <c r="I5">
-        <v>3000000</v>
+        <v>2500000</v>
       </c>
       <c r="J5">
-        <v>2000</v>
+        <v>13000</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -1878,31 +2008,31 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F6" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="G6" t="s">
         <v>19</v>
       </c>
       <c r="H6">
-        <v>10000</v>
+        <v>6000</v>
       </c>
       <c r="I6">
-        <v>5000000</v>
+        <v>3000000</v>
       </c>
       <c r="J6">
         <v>2000</v>
@@ -1916,31 +2046,31 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="G7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H7">
-        <v>7000</v>
+        <v>10000</v>
       </c>
       <c r="I7">
-        <v>3500000</v>
+        <v>5000000</v>
       </c>
       <c r="J7">
         <v>2000</v>
@@ -1954,31 +2084,31 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" t="s">
         <v>44</v>
       </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" t="s">
-        <v>23</v>
-      </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H8">
-        <v>6000</v>
+        <v>7000</v>
       </c>
       <c r="I8">
-        <v>3000000</v>
+        <v>3500000</v>
       </c>
       <c r="J8">
         <v>2000</v>
@@ -1992,39 +2122,77 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
         <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="G9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H9">
-        <v>60000</v>
+        <v>6000</v>
       </c>
       <c r="I9">
-        <v>2000000</v>
+        <v>3000000</v>
       </c>
       <c r="J9">
-        <v>30000</v>
+        <v>2000</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10">
+        <v>60000</v>
+      </c>
+      <c r="I10">
+        <v>2000000</v>
+      </c>
+      <c r="J10">
+        <v>30000</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2024-05-03
</commit_message>
<xml_diff>
--- a/datasets/corporate-finance-data.xlsx
+++ b/datasets/corporate-finance-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="94">
   <si>
     <t>상장일</t>
   </si>
@@ -69,6 +69,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2024-05-02</t>
+  </si>
+  <si>
     <t>2024-04-30</t>
   </si>
   <si>
@@ -96,6 +99,12 @@
     <t>2024-03-13</t>
   </si>
   <si>
+    <t>디앤디파마텍</t>
+  </si>
+  <si>
+    <t>유안타제16호스팩</t>
+  </si>
+  <si>
     <t>제일엠앤에스</t>
   </si>
   <si>
@@ -126,6 +135,12 @@
     <t>코스닥</t>
   </si>
   <si>
+    <t>한국</t>
+  </si>
+  <si>
+    <t>유안타</t>
+  </si>
+  <si>
     <t>KB</t>
   </si>
   <si>
@@ -141,9 +156,6 @@
     <t>NH</t>
   </si>
   <si>
-    <t>한국</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -174,6 +186,9 @@
     <t>2024-03-04</t>
   </si>
   <si>
+    <t>2024-04-25</t>
+  </si>
+  <si>
     <t>2024-04-23</t>
   </si>
   <si>
@@ -241,6 +256,12 @@
   </si>
   <si>
     <t>수수료율</t>
+  </si>
+  <si>
+    <t>1544 : 1</t>
+  </si>
+  <si>
+    <t>334 : 1</t>
   </si>
   <si>
     <t>1438.96 : 1</t>
@@ -634,7 +655,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -698,90 +719,90 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D2">
-        <v>528</v>
+        <v>363</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F2">
-        <v>528</v>
+        <v>363</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="I2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="J2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="K2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="L2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="M2">
-        <v>22000</v>
+        <v>33000</v>
       </c>
       <c r="N2">
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="P2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="Q2">
-        <v>1800000</v>
+        <v>805400</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D3">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F3">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="I3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="J3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="K3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="L3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="M3">
         <v>2000</v>
@@ -793,101 +814,101 @@
         <v>20</v>
       </c>
       <c r="P3" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="Q3">
-        <v>2625000</v>
+        <v>3862500</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D4">
-        <v>60</v>
+        <v>528</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F4">
-        <v>60</v>
+        <v>528</v>
       </c>
       <c r="G4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="I4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="J4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="K4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="L4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="M4">
-        <v>2000</v>
+        <v>22000</v>
       </c>
       <c r="N4">
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="P4" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="Q4">
-        <v>2250000</v>
+        <v>1800000</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D5">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F5">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="I5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     